<commit_message>
finalize customizing of standard components for gdv
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47153EA4-C717-42D2-BFE2-1E6BC87DA971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF07EA-87EA-47B4-B986-9112B5863A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1012,7 +1012,7 @@
     <t>A; B; C; D; E; F; G; H; L</t>
   </si>
   <si>
-    <t>$File Activity, import { Activity } from "@clients/backend"</t>
+    <t>EuTaxonomyActivityOptions</t>
   </si>
 </sst>
 </file>
@@ -1636,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -4318,18 +4318,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4542,14 +4542,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4562,6 +4554,14 @@
     <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
make iso questions single fields
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CDE2DB-C69B-4691-902B-9EF2FEB10941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDF6055-14E4-4D12-9F49-24393BB45E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="322">
   <si>
     <t>Unit</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Master Data</t>
   </si>
   <si>
-    <t>30.1</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -117,39 +114,12 @@
     <t>4.2</t>
   </si>
   <si>
-    <t>6.1</t>
-  </si>
-  <si>
-    <t>6.2</t>
-  </si>
-  <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>9.1</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
     <t>10.1</t>
   </si>
   <si>
     <t>10.2</t>
   </si>
   <si>
-    <t>10.3</t>
-  </si>
-  <si>
-    <t>11.1</t>
-  </si>
-  <si>
-    <t>11.2</t>
-  </si>
-  <si>
-    <t>11.3</t>
-  </si>
-  <si>
     <t>12.1</t>
   </si>
   <si>
@@ -159,27 +129,12 @@
     <t>10.1.2</t>
   </si>
   <si>
-    <t>18.1</t>
-  </si>
-  <si>
-    <t>32.1</t>
-  </si>
-  <si>
-    <t>45.1</t>
-  </si>
-  <si>
-    <t>45.2</t>
-  </si>
-  <si>
     <t>49.1</t>
   </si>
   <si>
     <t>49.2</t>
   </si>
   <si>
-    <t>51.1</t>
-  </si>
-  <si>
     <t>Field Identifier</t>
   </si>
   <si>
@@ -289,15 +244,6 @@
   </si>
   <si>
     <t>Akkreditierungen</t>
-  </si>
-  <si>
-    <t>Welche der folgenden Akkreditierungen haben Sie? Bitte teilen Sie die entsprechenden Zertifikate mit uns. Bitte führen Sie weitere Akkreditierungen auf, sofern diese nicht gelistet sind.</t>
-  </si>
-  <si>
-    <t>ISO 14001, ISO 45001, ISO 27001, ISO 50001</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>Mechanismen zur Überwachung der Einhaltung UN Global Compact Prinzipien und/oder OECD Leitsätze</t>
@@ -619,9 +565,6 @@
     <t>Bitte teilen Sie mit uns wieviele unbefristete Verträge es insgesamt in Deutschland und in der Gesamtgruppe gibt und wieviele unbefristete Verträge von der Änderung betroffen sind (Verkauf oder Akquisition).</t>
   </si>
   <si>
-    <t>36.2</t>
-  </si>
-  <si>
     <t>Auswirkungen auf Anteil befrister Verträge und Fluktuation</t>
   </si>
   <si>
@@ -718,9 +661,6 @@
     <t>Hat sich das Unternehmen im aktuellen Jahr der Berichterstattung von CEO/Vorsitzenden getrennt?</t>
   </si>
   <si>
-    <t>48.1</t>
-  </si>
-  <si>
     <t>Amtszeit</t>
   </si>
   <si>
@@ -781,18 +721,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>6.1.1</t>
-  </si>
-  <si>
-    <t>6.1.2</t>
-  </si>
-  <si>
-    <t>6.2.1</t>
-  </si>
-  <si>
-    <t>6.2.2</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -811,12 +739,6 @@
     <t>10.2.2</t>
   </si>
   <si>
-    <t>10.3.1</t>
-  </si>
-  <si>
-    <t>10.3.2</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -880,9 +802,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>31.1</t>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
@@ -1013,6 +932,117 @@
   </si>
   <si>
     <t>EuTaxonomyActivityOptions</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>13.2</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>14.1.1</t>
+  </si>
+  <si>
+    <t>14.1.2</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>14.2.1</t>
+  </si>
+  <si>
+    <t>14.2.2</t>
+  </si>
+  <si>
+    <t>14.3</t>
+  </si>
+  <si>
+    <t>14.3.1</t>
+  </si>
+  <si>
+    <t>14.3.2</t>
+  </si>
+  <si>
+    <t>15.1</t>
+  </si>
+  <si>
+    <t>15.2</t>
+  </si>
+  <si>
+    <t>15.3</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>22.1</t>
+  </si>
+  <si>
+    <t>34.1</t>
+  </si>
+  <si>
+    <t>35.1</t>
+  </si>
+  <si>
+    <t>40.1</t>
+  </si>
+  <si>
+    <t>40.2</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>52.1</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>53.1</t>
+  </si>
+  <si>
+    <t>53.2</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>55.1</t>
+  </si>
+  <si>
+    <t>ISO 14001</t>
+  </si>
+  <si>
+    <t>ISO 45001</t>
+  </si>
+  <si>
+    <t>ISO 27001</t>
+  </si>
+  <si>
+    <t>ISO 50001</t>
+  </si>
+  <si>
+    <t>Haben Sie eine ISO 14001 Akkreditierung? Bitte teilen Sie das entsprechende Zertifikat mit uns.</t>
+  </si>
+  <si>
+    <t>Haben Sie eine ISO 45001 Akkreditierung? Bitte teilen Sie das entsprechende Zertifikat mit uns.</t>
+  </si>
+  <si>
+    <t>Haben Sie eine ISO 27001 Akkreditierung? Bitte teilen Sie das entsprechende Zertifikat mit uns.</t>
+  </si>
+  <si>
+    <t>Haben Sie eine ISO 50001 Akkreditierung? Bitte teilen Sie das entsprechende Zertifikat mit uns.</t>
+  </si>
+  <si>
+    <t>Bitte führen Sie weitere Akkreditierungen auf, sofern diese nicht bereits gelistet sind, und teilen Sie entsprechende Zertifikate mit uns.</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1292,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1385,9 +1415,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1416,6 +1443,18 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1634,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -1652,45 +1691,45 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="36" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="J1" s="39" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="37" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1699,13 +1738,13 @@
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="45" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>28</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="11"/>
@@ -1715,8 +1754,8 @@
       <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="43" t="s">
-        <v>7</v>
+      <c r="A3" s="42" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1725,15 +1764,15 @@
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="45"/>
+        <v>5</v>
+      </c>
+      <c r="G3" s="44"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="40"/>
@@ -1742,2575 +1781,2675 @@
     </row>
     <row r="4" spans="1:12" ht="26">
       <c r="A4" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="8" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="44" t="s">
-        <v>229</v>
+      <c r="A5" s="43" t="s">
+        <v>209</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="8" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="9"/>
       <c r="J5" s="41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="37" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="8" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="9"/>
       <c r="J6" s="41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="26">
       <c r="A7" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="26">
       <c r="A8" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="51" t="s">
-        <v>310</v>
+        <v>48</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>283</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
       <c r="J8" s="41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="37" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="8" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="8" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>305</v>
+        <v>52</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>278</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="41" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="8" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="J11" s="41" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:12" ht="38.5">
-      <c r="A12" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>44</v>
-      </c>
+    <row r="12" spans="1:12" ht="26">
+      <c r="A12" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="51"/>
+      <c r="D12" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="41"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:12" ht="38.5">
-      <c r="A13" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>44</v>
-      </c>
+    <row r="13" spans="1:12" ht="26">
+      <c r="A13" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="51"/>
+      <c r="D13" s="44" t="s">
+        <v>314</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="41"/>
+      <c r="K13" s="9"/>
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="26">
-      <c r="A14" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="A14" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="51"/>
+      <c r="D14" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="F14" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="41"/>
+      <c r="K14" s="9"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" ht="26">
-      <c r="A15" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="A15" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="51"/>
+      <c r="D15" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>320</v>
+      </c>
+      <c r="F15" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="41"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:12" ht="28.5">
-      <c r="A16" s="37" t="s">
-        <v>235</v>
+    <row r="16" spans="1:12" ht="26">
+      <c r="A16" s="52" t="s">
+        <v>216</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C16" s="12"/>
-      <c r="D16" s="45" t="s">
-        <v>288</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>80</v>
+      <c r="D16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>321</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="G16" s="8"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="7"/>
       <c r="J16" s="41" t="s">
-        <v>13</v>
+        <v>208</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="1:12" ht="26">
-      <c r="A17" s="37" t="s">
-        <v>14</v>
+    <row r="17" spans="1:12" ht="38.5">
+      <c r="A17" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="8" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="9"/>
       <c r="J17" s="41" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="37" t="s">
-        <v>236</v>
+    <row r="18" spans="1:12" ht="26">
+      <c r="A18" s="52" t="s">
+        <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="16"/>
+        <v>58</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="I18" s="9"/>
       <c r="J18" s="41" t="s">
-        <v>14</v>
+        <v>217</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="1:12" ht="28.5">
-      <c r="A19" s="37" t="s">
-        <v>237</v>
+    <row r="19" spans="1:12" ht="26">
+      <c r="A19" s="52" t="s">
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C19" s="12"/>
-      <c r="D19" s="45" t="s">
-        <v>289</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="D19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="16"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="J19" s="41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" ht="38.5">
-      <c r="A20" s="37" t="s">
-        <v>238</v>
+    <row r="20" spans="1:12" ht="28.5">
+      <c r="A20" s="52" t="s">
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C20" s="12"/>
-      <c r="D20" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>42</v>
+      <c r="D20" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="9"/>
       <c r="J20" s="41" t="s">
-        <v>228</v>
+        <v>12</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" ht="26">
-      <c r="A21" s="37" t="s">
-        <v>239</v>
+      <c r="A21" s="52" t="s">
+        <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="8" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>43</v>
+        <v>64</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="9"/>
       <c r="J21" s="41" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="37" t="s">
-        <v>15</v>
+      <c r="A22" s="52" t="s">
+        <v>218</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>42</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="16"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="J22" s="41" t="s">
-        <v>239</v>
+        <v>13</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="1:12" ht="26">
-      <c r="A23" s="37" t="s">
-        <v>240</v>
+    <row r="23" spans="1:12" ht="28.5">
+      <c r="A23" s="52" t="s">
+        <v>219</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>43</v>
+      <c r="D23" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="41" t="s">
-        <v>228</v>
+        <v>13</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12" ht="38.5">
-      <c r="A24" s="37" t="s">
-        <v>16</v>
+      <c r="A24" s="52" t="s">
+        <v>220</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>94</v>
+        <v>67</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="49" t="s">
-        <v>304</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="41" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="38.5">
-      <c r="A25" s="37" t="s">
-        <v>17</v>
+    <row r="25" spans="1:12" ht="26">
+      <c r="A25" s="52" t="s">
+        <v>221</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>96</v>
+        <v>69</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>304</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="41" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" ht="26">
-      <c r="A26" s="37" t="s">
-        <v>241</v>
+    <row r="26" spans="1:12">
+      <c r="A26" s="52" t="s">
+        <v>14</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="8" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="41" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="37" t="s">
-        <v>18</v>
+    <row r="27" spans="1:12" ht="26">
+      <c r="A27" s="52" t="s">
+        <v>222</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="45" t="s">
-        <v>293</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>99</v>
+      <c r="D27" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="41" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L27" s="9"/>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="37" t="s">
-        <v>25</v>
+    <row r="28" spans="1:12" ht="38.5">
+      <c r="A28" s="52" t="s">
+        <v>285</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="8" t="s">
-        <v>302</v>
+        <v>75</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>306</v>
+        <v>52</v>
+      </c>
+      <c r="G28" s="48" t="s">
+        <v>277</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="41" t="s">
-        <v>18</v>
+        <v>222</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L28" s="9"/>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="37" t="s">
-        <v>26</v>
+    <row r="29" spans="1:12" ht="38.5">
+      <c r="A29" s="52" t="s">
+        <v>286</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="45" t="s">
-        <v>290</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="11"/>
+      <c r="G29" s="19" t="s">
+        <v>277</v>
+      </c>
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="41" t="s">
-        <v>18</v>
+        <v>222</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L29" s="9"/>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="37" t="s">
-        <v>19</v>
+    <row r="30" spans="1:12" ht="26">
+      <c r="A30" s="52" t="s">
+        <v>223</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>102</v>
+      <c r="D30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="41" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="37" t="s">
-        <v>242</v>
+      <c r="A31" s="52" t="s">
+        <v>287</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>103</v>
+      <c r="D31" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>81</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>306</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="41" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="37" t="s">
-        <v>243</v>
+      <c r="A32" s="52" t="s">
+        <v>288</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="45" t="s">
-        <v>291</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="11"/>
+      <c r="G32" s="8" t="s">
+        <v>279</v>
+      </c>
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="41" t="s">
-        <v>19</v>
+        <v>287</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="37" t="s">
-        <v>20</v>
+      <c r="A33" s="52" t="s">
+        <v>289</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C33" s="12"/>
-      <c r="D33" s="45" t="s">
-        <v>295</v>
+      <c r="D33" s="44" t="s">
+        <v>263</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="41" t="s">
-        <v>241</v>
+        <v>287</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="37" t="s">
-        <v>244</v>
+      <c r="A34" s="52" t="s">
+        <v>290</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>105</v>
+      <c r="D34" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>306</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="41" t="s">
-        <v>20</v>
+        <v>223</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L34" s="9"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="37" t="s">
-        <v>245</v>
+      <c r="A35" s="52" t="s">
+        <v>291</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="45" t="s">
-        <v>292</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G35" s="11"/>
+      <c r="G35" s="8" t="s">
+        <v>279</v>
+      </c>
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="41" t="s">
-        <v>20</v>
+        <v>290</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="37" t="s">
-        <v>246</v>
+      <c r="A36" s="52" t="s">
+        <v>292</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>107</v>
+      <c r="D36" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="41" t="s">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L36" s="9"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="37" t="s">
-        <v>21</v>
+      <c r="A37" s="52" t="s">
+        <v>293</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>109</v>
+      <c r="D37" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>86</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="41" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="37" t="s">
-        <v>22</v>
+      <c r="A38" s="52" t="s">
+        <v>294</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>111</v>
+        <v>276</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>279</v>
+      </c>
       <c r="H38" s="11"/>
-      <c r="I38" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="I38" s="9"/>
       <c r="J38" s="41" t="s">
-        <v>246</v>
+        <v>293</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L38" s="9"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="37" t="s">
-        <v>23</v>
+      <c r="A39" s="52" t="s">
+        <v>295</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C39" s="12"/>
-      <c r="D39" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>113</v>
+      <c r="D39" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="41" t="s">
-        <v>246</v>
+        <v>293</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L39" s="9"/>
     </row>
-    <row r="40" spans="1:12" ht="26">
-      <c r="A40" s="37" t="s">
-        <v>247</v>
+    <row r="40" spans="1:12">
+      <c r="A40" s="52" t="s">
+        <v>224</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="8" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L40" s="9"/>
     </row>
-    <row r="41" spans="1:12" ht="26">
-      <c r="A41" s="37" t="s">
-        <v>24</v>
+    <row r="41" spans="1:12">
+      <c r="A41" s="52" t="s">
+        <v>296</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>117</v>
+        <v>90</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
       <c r="I41" s="9"/>
       <c r="J41" s="41" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L41" s="9"/>
     </row>
-    <row r="42" spans="1:12" ht="26">
-      <c r="A42" s="37" t="s">
-        <v>248</v>
+    <row r="42" spans="1:12">
+      <c r="A42" s="52" t="s">
+        <v>297</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>119</v>
+        <v>92</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="9"/>
+      <c r="I42" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="J42" s="41" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L42" s="9"/>
     </row>
-    <row r="43" spans="1:12" ht="26">
-      <c r="A43" s="37" t="s">
-        <v>249</v>
+    <row r="43" spans="1:12">
+      <c r="A43" s="52" t="s">
+        <v>298</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="8" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="41" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L43" s="9"/>
     </row>
-    <row r="44" spans="1:12" ht="51">
-      <c r="A44" s="37" t="s">
-        <v>250</v>
+    <row r="44" spans="1:12" ht="26">
+      <c r="A44" s="52" t="s">
+        <v>225</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C44" s="12"/>
       <c r="D44" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>125</v>
+        <v>96</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L44" s="9"/>
     </row>
-    <row r="45" spans="1:12" ht="38.5">
-      <c r="A45" s="37" t="s">
-        <v>251</v>
+    <row r="45" spans="1:12" ht="26">
+      <c r="A45" s="52" t="s">
+        <v>299</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>296</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>126</v>
+        <v>37</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="41" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L45" s="9"/>
     </row>
-    <row r="46" spans="1:12" ht="51">
-      <c r="A46" s="37" t="s">
-        <v>252</v>
+    <row r="46" spans="1:12" ht="26">
+      <c r="A46" s="52" t="s">
+        <v>226</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C46" s="12"/>
       <c r="D46" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>128</v>
+        <v>100</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12" ht="26">
-      <c r="A47" s="37" t="s">
-        <v>253</v>
+      <c r="A47" s="52" t="s">
+        <v>227</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="8" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12" ht="51">
+      <c r="A48" s="52" t="s">
         <v>228</v>
       </c>
-      <c r="K47" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L47" s="9"/>
-    </row>
-    <row r="48" spans="1:12" ht="26">
-      <c r="A48" s="37" t="s">
-        <v>27</v>
-      </c>
       <c r="B48" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D48" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>132</v>
+        <v>106</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="41" t="s">
-        <v>253</v>
+        <v>208</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L48" s="9"/>
     </row>
-    <row r="49" spans="1:12" ht="26">
-      <c r="A49" s="37" t="s">
-        <v>254</v>
+    <row r="49" spans="1:12" ht="38.5">
+      <c r="A49" s="52" t="s">
+        <v>229</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>134</v>
+        <v>104</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L49" s="9"/>
     </row>
-    <row r="50" spans="1:12" ht="56.5">
-      <c r="A50" s="37" t="s">
-        <v>255</v>
+    <row r="50" spans="1:12" ht="51">
+      <c r="A50" s="52" t="s">
+        <v>230</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>137</v>
+        <v>109</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="1:12" ht="42.5">
-      <c r="A51" s="37" t="s">
-        <v>256</v>
+    <row r="51" spans="1:12" ht="26">
+      <c r="A51" s="52" t="s">
+        <v>231</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D51" s="45" t="s">
-        <v>298</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>138</v>
+        <v>104</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L51" s="9"/>
     </row>
-    <row r="52" spans="1:12" ht="42.5">
-      <c r="A52" s="37" t="s">
-        <v>257</v>
+    <row r="52" spans="1:12" ht="26">
+      <c r="A52" s="52" t="s">
+        <v>300</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>139</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C52" s="12"/>
       <c r="D52" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>141</v>
+        <v>113</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="41" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="1:12" ht="42.5">
-      <c r="A53" s="37" t="s">
-        <v>258</v>
+    <row r="53" spans="1:12" ht="26">
+      <c r="A53" s="52" t="s">
+        <v>232</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" s="47" t="s">
-        <v>299</v>
-      </c>
-      <c r="E53" s="24" t="s">
-        <v>138</v>
+        <v>104</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="1:12" ht="42.5">
-      <c r="A54" s="37" t="s">
-        <v>259</v>
+    <row r="54" spans="1:12" ht="56.5">
+      <c r="A54" s="52" t="s">
+        <v>233</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>143</v>
+        <v>117</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L54" s="9"/>
     </row>
     <row r="55" spans="1:12" ht="42.5">
-      <c r="A55" s="37" t="s">
-        <v>260</v>
+      <c r="A55" s="52" t="s">
+        <v>234</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D55" s="46" t="s">
-        <v>297</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>138</v>
+        <v>117</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L55" s="9"/>
     </row>
-    <row r="56" spans="1:12" ht="56.5">
-      <c r="A56" s="37" t="s">
-        <v>261</v>
+    <row r="56" spans="1:12" ht="42.5">
+      <c r="A56" s="52" t="s">
+        <v>235</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>146</v>
-      </c>
       <c r="E56" s="22" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:12">
-      <c r="A57" s="37" t="s">
-        <v>262</v>
+    <row r="57" spans="1:12" ht="42.5">
+      <c r="A57" s="52" t="s">
+        <v>236</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D57" s="48" t="s">
-        <v>300</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>138</v>
+        <v>121</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>272</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L57" s="9"/>
     </row>
-    <row r="58" spans="1:12" ht="51">
-      <c r="A58" s="37" t="s">
-        <v>263</v>
+    <row r="58" spans="1:12" ht="42.5">
+      <c r="A58" s="52" t="s">
+        <v>237</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>149</v>
+        <v>124</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>126</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L58" s="9"/>
     </row>
-    <row r="59" spans="1:12" ht="26">
-      <c r="A59" s="37" t="s">
-        <v>264</v>
+    <row r="59" spans="1:12" ht="42.5">
+      <c r="A59" s="52" t="s">
+        <v>238</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>152</v>
+        <v>124</v>
+      </c>
+      <c r="D59" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L59" s="9"/>
     </row>
-    <row r="60" spans="1:12">
-      <c r="A60" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="B60" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="52" t="s">
-        <v>155</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="E60" s="30" t="s">
-        <v>154</v>
+    <row r="60" spans="1:12" ht="56.5">
+      <c r="A60" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:12" ht="51">
-      <c r="A61" s="37" t="s">
-        <v>5</v>
+    <row r="61" spans="1:12">
+      <c r="A61" s="52" t="s">
+        <v>240</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>157</v>
+        <v>127</v>
+      </c>
+      <c r="D61" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>120</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="41" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L61" s="9"/>
     </row>
-    <row r="62" spans="1:12">
-      <c r="A62" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="B62" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="C62" s="52" t="s">
-        <v>155</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="E62" s="31" t="s">
-        <v>159</v>
+    <row r="62" spans="1:12" ht="51">
+      <c r="A62" s="52" t="s">
+        <v>241</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>131</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L62" s="9"/>
     </row>
-    <row r="63" spans="1:12" ht="51">
-      <c r="A63" s="37" t="s">
-        <v>267</v>
+    <row r="63" spans="1:12" ht="26">
+      <c r="A63" s="52" t="s">
+        <v>242</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="41" t="s">
-        <v>266</v>
+        <v>208</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L63" s="9"/>
     </row>
-    <row r="64" spans="1:12" ht="51">
-      <c r="A64" s="37" t="s">
-        <v>268</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>164</v>
+    <row r="64" spans="1:12">
+      <c r="A64" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="B64" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>136</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L64" s="9"/>
     </row>
-    <row r="65" spans="1:12" ht="42.5">
-      <c r="A65" s="37" t="s">
-        <v>28</v>
+    <row r="65" spans="1:12" ht="51">
+      <c r="A65" s="52" t="s">
+        <v>301</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>166</v>
+        <v>138</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="41" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L65" s="9"/>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>169</v>
+      <c r="A66" s="52" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E66" s="31" t="s">
+        <v>141</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>309</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L66" s="9"/>
     </row>
-    <row r="67" spans="1:12">
-      <c r="A67" s="37" t="s">
-        <v>270</v>
+    <row r="67" spans="1:12" ht="51">
+      <c r="A67" s="52" t="s">
+        <v>302</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>311</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G67" s="11"/>
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="41" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L67" s="9"/>
     </row>
-    <row r="68" spans="1:12" ht="63.5">
-      <c r="A68" s="37" t="s">
-        <v>271</v>
+    <row r="68" spans="1:12" ht="51">
+      <c r="A68" s="52" t="s">
+        <v>245</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>173</v>
+        <v>145</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L68" s="9"/>
     </row>
-    <row r="69" spans="1:12" ht="26">
-      <c r="A69" s="37" t="s">
-        <v>272</v>
+    <row r="69" spans="1:12" ht="42.5">
+      <c r="A69" s="52" t="s">
+        <v>159</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C69" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="D69" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E69" s="13" t="s">
-        <v>176</v>
+        <v>147</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>148</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="41" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L69" s="9"/>
     </row>
-    <row r="70" spans="1:12" ht="38.5">
-      <c r="A70" s="37" t="s">
-        <v>177</v>
+    <row r="70" spans="1:12">
+      <c r="A70" s="52" t="s">
+        <v>246</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C70" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="D70" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>179</v>
+        <v>150</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G70" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>282</v>
+      </c>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="41" t="s">
-        <v>272</v>
+        <v>208</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:12" ht="26">
-      <c r="A71" s="37" t="s">
-        <v>180</v>
+    <row r="71" spans="1:12">
+      <c r="A71" s="52" t="s">
+        <v>247</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C71" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="D71" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>182</v>
+        <v>152</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G71" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>284</v>
+      </c>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="41" t="s">
-        <v>272</v>
+        <v>208</v>
       </c>
       <c r="K71" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L71" s="9"/>
     </row>
-    <row r="72" spans="1:12" ht="26">
-      <c r="A72" s="37" t="s">
-        <v>273</v>
+    <row r="72" spans="1:12" ht="63.5">
+      <c r="A72" s="52" t="s">
+        <v>248</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C72" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="D72" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>184</v>
+        <v>154</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>155</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L72" s="9"/>
     </row>
-    <row r="73" spans="1:12">
-      <c r="A73" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="B73" s="28"/>
+    <row r="73" spans="1:12" ht="26">
+      <c r="A73" s="52" t="s">
+        <v>249</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="C73" s="12"/>
       <c r="D73" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E73" s="32" t="s">
-        <v>186</v>
+        <v>157</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>158</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L73" s="9"/>
     </row>
-    <row r="74" spans="1:12" ht="26">
-      <c r="A74" s="37" t="s">
-        <v>275</v>
+    <row r="74" spans="1:12" ht="38.5">
+      <c r="A74" s="52" t="s">
+        <v>303</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="8" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="41" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L74" s="9"/>
     </row>
-    <row r="75" spans="1:12" ht="38.5">
-      <c r="A75" s="37" t="s">
-        <v>276</v>
+    <row r="75" spans="1:12" ht="26">
+      <c r="A75" s="52" t="s">
+        <v>304</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>189</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C75" s="12"/>
       <c r="D75" s="8" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="41" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L75" s="9"/>
     </row>
     <row r="76" spans="1:12" ht="26">
-      <c r="A76" s="37" t="s">
-        <v>277</v>
+      <c r="A76" s="52" t="s">
+        <v>250</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>189</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C76" s="12"/>
       <c r="D76" s="8" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L76" s="9"/>
     </row>
-    <row r="77" spans="1:12" ht="26">
-      <c r="A77" s="37" t="s">
-        <v>278</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>194</v>
-      </c>
+    <row r="77" spans="1:12">
+      <c r="A77" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="B77" s="28"/>
+      <c r="C77" s="12"/>
       <c r="D77" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>196</v>
+        <v>166</v>
+      </c>
+      <c r="E77" s="32" t="s">
+        <v>167</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K77" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L77" s="9"/>
     </row>
-    <row r="78" spans="1:12">
-      <c r="A78" s="37" t="s">
-        <v>279</v>
+    <row r="78" spans="1:12" ht="26">
+      <c r="A78" s="52" t="s">
+        <v>252</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>194</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C78" s="12"/>
       <c r="D78" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E78" s="13" t="s">
-        <v>198</v>
+        <v>168</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>169</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K78" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L78" s="9"/>
     </row>
-    <row r="79" spans="1:12">
-      <c r="A79" s="37" t="s">
-        <v>280</v>
+    <row r="79" spans="1:12" ht="38.5">
+      <c r="A79" s="52" t="s">
+        <v>253</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E79" s="29" t="s">
-        <v>200</v>
+        <v>171</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L79" s="9"/>
     </row>
     <row r="80" spans="1:12" ht="26">
-      <c r="A80" s="37" t="s">
-        <v>281</v>
+      <c r="A80" s="52" t="s">
+        <v>254</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E80" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="E80" s="13" t="s">
-        <v>203</v>
-      </c>
       <c r="F80" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K80" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L80" s="9"/>
     </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="37" t="s">
-        <v>29</v>
+    <row r="81" spans="1:12" ht="26">
+      <c r="A81" s="52" t="s">
+        <v>255</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E81" s="33"/>
+        <v>176</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>177</v>
+      </c>
       <c r="F81" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G81" s="50" t="s">
-        <v>307</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="41" t="s">
-        <v>281</v>
+        <v>208</v>
       </c>
       <c r="K81" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L81" s="9"/>
     </row>
     <row r="82" spans="1:12">
-      <c r="A82" s="37" t="s">
-        <v>30</v>
+      <c r="A82" s="52" t="s">
+        <v>256</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E82" s="29" t="s">
-        <v>206</v>
+        <v>178</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="41" t="s">
-        <v>281</v>
+        <v>208</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L82" s="9"/>
     </row>
     <row r="83" spans="1:12">
-      <c r="A83" s="37" t="s">
-        <v>282</v>
+      <c r="A83" s="52" t="s">
+        <v>257</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C83" s="12"/>
+        <v>156</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="D83" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="E83" s="34" t="s">
-        <v>209</v>
+        <v>180</v>
+      </c>
+      <c r="E83" s="29" t="s">
+        <v>181</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L83" s="9"/>
     </row>
-    <row r="84" spans="1:12">
-      <c r="A84" s="37" t="s">
-        <v>283</v>
+    <row r="84" spans="1:12" ht="26">
+      <c r="A84" s="52" t="s">
+        <v>258</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C84" s="12"/>
+        <v>156</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="D84" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="E84" s="9"/>
+        <v>183</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="F84" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L84" s="9"/>
     </row>
     <row r="85" spans="1:12">
-      <c r="A85" s="37" t="s">
-        <v>284</v>
+      <c r="A85" s="52" t="s">
+        <v>17</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C85" s="12"/>
+        <v>156</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="D85" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>212</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="E85" s="33"/>
       <c r="F85" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G85" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="G85" s="49" t="s">
+        <v>280</v>
+      </c>
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="41" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L85" s="9"/>
     </row>
     <row r="86" spans="1:12">
-      <c r="A86" s="37" t="s">
-        <v>213</v>
+      <c r="A86" s="52" t="s">
+        <v>18</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C86" s="12"/>
+        <v>156</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="D86" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>215</v>
+        <v>186</v>
+      </c>
+      <c r="E86" s="29" t="s">
+        <v>187</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="41" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L86" s="9"/>
     </row>
-    <row r="87" spans="1:12" ht="51">
-      <c r="A87" s="37" t="s">
-        <v>285</v>
+    <row r="87" spans="1:12">
+      <c r="A87" s="52" t="s">
+        <v>259</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="E87" s="13" t="s">
-        <v>217</v>
+        <v>189</v>
+      </c>
+      <c r="E87" s="34" t="s">
+        <v>190</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L87" s="9"/>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="37" t="s">
-        <v>31</v>
+      <c r="A88" s="52" t="s">
+        <v>260</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C88" s="12"/>
-      <c r="D88" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="E88" s="29" t="s">
-        <v>219</v>
-      </c>
+      <c r="D88" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E88" s="9"/>
       <c r="F88" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="41" t="s">
-        <v>285</v>
+        <v>208</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L88" s="9"/>
     </row>
-    <row r="89" spans="1:12" ht="38.5">
-      <c r="A89" s="37" t="s">
-        <v>32</v>
+    <row r="89" spans="1:12">
+      <c r="A89" s="52" t="s">
+        <v>305</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="E89" s="13" t="s">
-        <v>221</v>
+        <v>192</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="41" t="s">
-        <v>285</v>
+        <v>208</v>
       </c>
       <c r="K89" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L89" s="9"/>
     </row>
-    <row r="90" spans="1:12" ht="26">
-      <c r="A90" s="37" t="s">
-        <v>286</v>
+    <row r="90" spans="1:12">
+      <c r="A90" s="52" t="s">
+        <v>306</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="E90" s="10" t="s">
-        <v>223</v>
+        <v>194</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G90" s="45" t="s">
-        <v>308</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="41" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L90" s="9"/>
     </row>
-    <row r="91" spans="1:12" ht="26">
-      <c r="A91" s="37" t="s">
-        <v>287</v>
+    <row r="91" spans="1:12" ht="51">
+      <c r="A91" s="52" t="s">
+        <v>307</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C91" s="12"/>
       <c r="D91" s="8" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="41" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K91" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L91" s="9"/>
     </row>
-    <row r="92" spans="1:12" ht="51">
-      <c r="A92" s="37" t="s">
-        <v>33</v>
+    <row r="92" spans="1:12">
+      <c r="A92" s="52" t="s">
+        <v>308</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C92" s="35"/>
-      <c r="D92" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="E92" s="13" t="s">
-        <v>227</v>
+        <v>188</v>
+      </c>
+      <c r="C92" s="12"/>
+      <c r="D92" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>199</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
-      <c r="I92" s="15"/>
-      <c r="J92" s="42" t="s">
-        <v>287</v>
+      <c r="I92" s="9"/>
+      <c r="J92" s="41" t="s">
+        <v>307</v>
       </c>
       <c r="K92" s="9" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L92" s="9"/>
+    </row>
+    <row r="93" spans="1:12" ht="38.5">
+      <c r="A93" s="52" t="s">
+        <v>309</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C93" s="12"/>
+      <c r="D93" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="41" t="s">
+        <v>307</v>
+      </c>
+      <c r="K93" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L93" s="9"/>
+    </row>
+    <row r="94" spans="1:12" ht="26">
+      <c r="A94" s="52" t="s">
+        <v>310</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="12"/>
+      <c r="D94" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F94" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G94" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="H94" s="11"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="K94" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L94" s="9"/>
+    </row>
+    <row r="95" spans="1:12" ht="26">
+      <c r="A95" s="52" t="s">
+        <v>311</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="12"/>
+      <c r="D95" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L95" s="9"/>
+    </row>
+    <row r="96" spans="1:12" ht="51">
+      <c r="A96" s="52" t="s">
+        <v>312</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96" s="35"/>
+      <c r="D96" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="55" t="s">
+        <v>311</v>
+      </c>
+      <c r="K96" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L96" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4318,18 +4457,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4542,14 +4681,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4562,6 +4693,14 @@
     <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
progress on custom field for "weitere akkreditierungen"
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDF6055-14E4-4D12-9F49-24393BB45E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDEC1D4-FE8C-4E3B-8AA1-63301D0B54F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="326">
   <si>
     <t>Unit</t>
   </si>
@@ -126,9 +126,6 @@
     <t>10.1.1</t>
   </si>
   <si>
-    <t>10.1.2</t>
-  </si>
-  <si>
     <t>49.1</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>Bitte teilen Sie die letzten Berichte mit uns (vorzugsweise die letzten drei).</t>
   </si>
   <si>
-    <t>Akkreditierungen</t>
-  </si>
-  <si>
     <t>Mechanismen zur Überwachung der Einhaltung UN Global Compact Prinzipien und/oder OECD Leitsätze</t>
   </si>
   <si>
@@ -255,22 +249,10 @@
     <t>UNCG Prinzipien</t>
   </si>
   <si>
-    <t>Hat das Unternehmen Überwachungsmechanismen für die UNGC Prinzipien eingerichtet ?</t>
-  </si>
-  <si>
-    <t>Richtlinien Einhaltung UNGC</t>
-  </si>
-  <si>
-    <t>Bitte teilen Sie die Richtlinien mit uns die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung des UNGC (alle vier Säulen) überwacht.</t>
-  </si>
-  <si>
     <t>Bitte geben Sie eine Erklärung ab, dass keine Verstöße gegen diese Grundsätze vorliegen.</t>
   </si>
   <si>
     <t>OECD Leitsätze</t>
-  </si>
-  <si>
-    <t>Hat das Unternehmen Überwachungsmechanismen für die OECD Leitsätze eingerichtet ?</t>
   </si>
   <si>
     <t>Richtlinien Einhaltung OECD</t>
@@ -1043,6 +1025,36 @@
   </si>
   <si>
     <t>Bitte führen Sie weitere Akkreditierungen auf, sofern diese nicht bereits gelistet sind, und teilen Sie entsprechende Zertifikate mit uns.</t>
+  </si>
+  <si>
+    <t>In welchen Zeitabständen werden die Berichte erstellt?</t>
+  </si>
+  <si>
+    <t>Custom - List of BaseDocumentReference</t>
+  </si>
+  <si>
+    <t>Custom - Sollte in mehrere Fragen aufgebrochen werden =&gt; Ausstehende Emissionen einmal für "Nachhaltige Emissionen" und für "SLD" =&gt; Dann kann beides jeweils ein DecimalField mit € als (feste) unit sein</t>
+  </si>
+  <si>
+    <t>Custom - Rolling Window</t>
+  </si>
+  <si>
+    <t>Weitere Akkreditierungen</t>
+  </si>
+  <si>
+    <t>New Component - Yes/No with multiple basedocumentreferences</t>
+  </si>
+  <si>
+    <t>Hat das Unternehmen Überwachungsmechanismen für die OECD Leitsätze eingerichtet ? Wenn ja, bitte teilen Sie die Richtlinien mit uns, die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der OECD Leitsätze überwacht.</t>
+  </si>
+  <si>
+    <t>Hat das Unternehmen Überwachungsmechanismen für die UNGC Prinzipien eingerichtet ? Wenn ja bitte, teilen Sie die Richtlinien mit uns, die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung des UNGC (alle vier Säulen) überwacht.</t>
+  </si>
+  <si>
+    <t>Custom - Rolling Window mit vorangestellter Freitext (oder List of Strings) Frage zu den Sektoren</t>
+  </si>
+  <si>
+    <t>Custom - Tabellencomponent?</t>
   </si>
 </sst>
 </file>
@@ -1339,9 +1351,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
@@ -1455,6 +1464,9 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1673,63 +1685,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="38"/>
+    <col min="1" max="1" width="12.54296875" style="37"/>
     <col min="4" max="4" width="38.1796875" customWidth="1"/>
-    <col min="5" max="5" width="71" customWidth="1"/>
+    <col min="5" max="5" width="85.54296875" customWidth="1"/>
     <col min="6" max="6" width="65.54296875" customWidth="1"/>
     <col min="7" max="7" width="31.6328125" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" style="38"/>
+    <col min="10" max="10" width="12.54296875" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="36" t="s">
-        <v>19</v>
+      <c r="A1" s="35" t="s">
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="37" t="s">
-        <v>208</v>
+      <c r="A2" s="36" t="s">
+        <v>202</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1738,23 +1750,23 @@
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="44" t="s">
-        <v>28</v>
+      <c r="F2" s="43" t="s">
+        <v>27</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="11"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="40"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1764,588 +1776,596 @@
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="44"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="40"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="9"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="26">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="41" t="s">
-        <v>208</v>
+      <c r="J4" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="43" t="s">
-        <v>209</v>
+      <c r="A5" s="42" t="s">
+        <v>203</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>41</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="40" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="26">
-      <c r="A6" s="37" t="s">
-        <v>210</v>
+      <c r="A6" s="36" t="s">
+        <v>204</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="41" t="s">
+      <c r="J6" s="40" t="s">
         <v>7</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="26">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="41" t="s">
-        <v>208</v>
+      <c r="J7" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="26">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>283</v>
+      <c r="G8" s="49" t="s">
+        <v>277</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="40" t="s">
         <v>8</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="37" t="s">
-        <v>211</v>
+      <c r="A9" s="36" t="s">
+        <v>205</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>50</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="41" t="s">
-        <v>208</v>
+      <c r="J9" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="44" t="s">
-        <v>278</v>
+      <c r="G10" s="43" t="s">
+        <v>272</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="41" t="s">
-        <v>211</v>
+      <c r="J10" s="40" t="s">
+        <v>205</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="50" t="s">
+        <v>317</v>
+      </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>211</v>
+        <v>29</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>205</v>
       </c>
       <c r="K11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" ht="26">
+      <c r="A12" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="50"/>
+      <c r="D12" s="43" t="s">
+        <v>307</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>311</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" ht="26">
-      <c r="A12" s="52" t="s">
-        <v>212</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="44" t="s">
-        <v>313</v>
-      </c>
-      <c r="E12" s="54" t="s">
-        <v>317</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="41"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12" ht="26">
-      <c r="A13" s="52" t="s">
-        <v>213</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="44" t="s">
-        <v>314</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>318</v>
-      </c>
-      <c r="F13" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="41"/>
+      <c r="A13" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="43" t="s">
+        <v>308</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>312</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="40"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="26">
-      <c r="A14" s="52" t="s">
-        <v>214</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="44" t="s">
-        <v>315</v>
-      </c>
-      <c r="E14" s="54" t="s">
-        <v>319</v>
-      </c>
-      <c r="F14" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="41"/>
+      <c r="A14" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="43" t="s">
+        <v>309</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>313</v>
+      </c>
+      <c r="F14" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="40"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" ht="26">
-      <c r="A15" s="52" t="s">
-        <v>215</v>
-      </c>
-      <c r="B15" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="44" t="s">
-        <v>316</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>320</v>
-      </c>
-      <c r="F15" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="J15" s="41"/>
+      <c r="A15" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>314</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="40"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="26">
-      <c r="A16" s="52" t="s">
-        <v>216</v>
+      <c r="A16" s="51" t="s">
+        <v>210</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="8" t="s">
-        <v>55</v>
+        <v>320</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>36</v>
+        <v>315</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>35</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="41" t="s">
-        <v>208</v>
+      <c r="I16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" ht="38.5">
-      <c r="A17" s="52" t="s">
-        <v>217</v>
+      <c r="A17" s="51" t="s">
+        <v>211</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="41" t="s">
-        <v>208</v>
+      <c r="J17" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" ht="38.5">
+      <c r="A18" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="50"/>
+      <c r="D18" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="F18" s="43" t="s">
+        <v>321</v>
+      </c>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="9"/>
-    </row>
-    <row r="18" spans="1:12" ht="26">
-      <c r="A18" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" ht="26">
-      <c r="A19" s="52" t="s">
+      <c r="J18" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="K18" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="50"/>
+    </row>
+    <row r="19" spans="1:12" ht="28.5">
+      <c r="A19" s="51" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="12"/>
-      <c r="D19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="16"/>
+      <c r="D19" s="43" t="s">
+        <v>255</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" s="41" t="s">
-        <v>12</v>
-      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="40"/>
       <c r="K19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" ht="28.5">
-      <c r="A20" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="44" t="s">
-        <v>261</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="5" t="s">
+    <row r="20" spans="1:12" ht="38.5">
+      <c r="A20" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>322</v>
+      </c>
+      <c r="F20" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="9"/>
-    </row>
-    <row r="21" spans="1:12" ht="26">
-      <c r="A21" s="52" t="s">
-        <v>13</v>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="K20" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="50"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="51" t="s">
+        <v>212</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>28</v>
+        <v>59</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="50" t="s">
+        <v>317</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="41" t="s">
-        <v>217</v>
+      <c r="I21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="40" t="s">
+        <v>13</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="52" t="s">
-        <v>218</v>
+    <row r="22" spans="1:12" ht="28.5">
+      <c r="A22" s="51" t="s">
+        <v>213</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="16"/>
+      <c r="D22" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J22" s="41" t="s">
+      <c r="I22" s="9"/>
+      <c r="J22" s="40" t="s">
         <v>13</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="1:12" ht="28.5">
-      <c r="A23" s="52" t="s">
-        <v>219</v>
+    <row r="23" spans="1:12" ht="38.5">
+      <c r="A23" s="51" t="s">
+        <v>214</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="44" t="s">
-        <v>262</v>
-      </c>
-      <c r="E23" s="17" t="s">
+      <c r="D23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>27</v>
+      <c r="F23" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="41" t="s">
-        <v>13</v>
+      <c r="J23" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="1:12" ht="38.5">
-      <c r="A24" s="52" t="s">
-        <v>220</v>
+    <row r="24" spans="1:12" ht="26">
+      <c r="A24" s="51" t="s">
+        <v>215</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>27</v>
@@ -2353,55 +2373,55 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="41" t="s">
-        <v>208</v>
+      <c r="J24" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="26">
-      <c r="A25" s="52" t="s">
-        <v>221</v>
+    <row r="25" spans="1:12">
+      <c r="A25" s="51" t="s">
+        <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="41" t="s">
-        <v>208</v>
+      <c r="J25" s="40" t="s">
+        <v>215</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="52" t="s">
-        <v>14</v>
+    <row r="26" spans="1:12" ht="26">
+      <c r="A26" s="51" t="s">
+        <v>216</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>27</v>
@@ -2409,201 +2429,201 @@
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="41" t="s">
-        <v>221</v>
+      <c r="J26" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:12" ht="26">
-      <c r="A27" s="52" t="s">
-        <v>222</v>
+    <row r="27" spans="1:12" ht="38.5">
+      <c r="A27" s="51" t="s">
+        <v>279</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="G27" s="47" t="s">
+        <v>271</v>
+      </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="41" t="s">
-        <v>208</v>
+      <c r="J27" s="40" t="s">
+        <v>216</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="1:12" ht="38.5">
-      <c r="A28" s="52" t="s">
-        <v>285</v>
+      <c r="A28" s="51" t="s">
+        <v>280</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="48" t="s">
-        <v>277</v>
+        <v>51</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>271</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="41" t="s">
-        <v>222</v>
+      <c r="J28" s="40" t="s">
+        <v>216</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L28" s="9"/>
     </row>
-    <row r="29" spans="1:12" ht="38.5">
-      <c r="A29" s="52" t="s">
-        <v>286</v>
+    <row r="29" spans="1:12" ht="26">
+      <c r="A29" s="51" t="s">
+        <v>217</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>277</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="41" t="s">
-        <v>222</v>
+      <c r="J29" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L29" s="9"/>
     </row>
-    <row r="30" spans="1:12" ht="26">
-      <c r="A30" s="52" t="s">
-        <v>223</v>
+    <row r="30" spans="1:12">
+      <c r="A30" s="51" t="s">
+        <v>281</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>80</v>
+      <c r="D30" s="43" t="s">
+        <v>260</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="41" t="s">
-        <v>208</v>
+      <c r="J30" s="40" t="s">
+        <v>217</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="52" t="s">
-        <v>287</v>
+      <c r="A31" s="51" t="s">
+        <v>282</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="44" t="s">
-        <v>266</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>81</v>
+      <c r="D31" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>273</v>
+      </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="41" t="s">
-        <v>223</v>
+      <c r="J31" s="40" t="s">
+        <v>281</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="52" t="s">
-        <v>288</v>
+      <c r="A32" s="51" t="s">
+        <v>283</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>82</v>
+      <c r="D32" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>279</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
-      <c r="J32" s="41" t="s">
-        <v>287</v>
+      <c r="J32" s="40" t="s">
+        <v>281</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="52" t="s">
-        <v>289</v>
+      <c r="A33" s="51" t="s">
+        <v>284</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="12"/>
-      <c r="D33" s="44" t="s">
-        <v>263</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>83</v>
+      <c r="D33" s="43" t="s">
+        <v>261</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>27</v>
@@ -2611,85 +2631,85 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="41" t="s">
-        <v>287</v>
+      <c r="J33" s="40" t="s">
+        <v>217</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="52" t="s">
-        <v>290</v>
+      <c r="A34" s="51" t="s">
+        <v>285</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="44" t="s">
-        <v>267</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>84</v>
+      <c r="D34" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>273</v>
+      </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="41" t="s">
-        <v>223</v>
+      <c r="J34" s="40" t="s">
+        <v>284</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L34" s="9"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="52" t="s">
-        <v>291</v>
+      <c r="A35" s="51" t="s">
+        <v>286</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>85</v>
+      <c r="D35" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>279</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="41" t="s">
-        <v>290</v>
+      <c r="J35" s="40" t="s">
+        <v>284</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="52" t="s">
-        <v>292</v>
+      <c r="A36" s="51" t="s">
+        <v>287</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="44" t="s">
-        <v>264</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>83</v>
+      <c r="D36" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>27</v>
@@ -2697,84 +2717,84 @@
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
-      <c r="J36" s="41" t="s">
-        <v>290</v>
+      <c r="J36" s="40" t="s">
+        <v>217</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L36" s="9"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="52" t="s">
-        <v>293</v>
+      <c r="A37" s="51" t="s">
+        <v>288</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>86</v>
+      <c r="D37" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>273</v>
+      </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
-      <c r="J37" s="41" t="s">
-        <v>223</v>
+      <c r="J37" s="40" t="s">
+        <v>287</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="52" t="s">
-        <v>294</v>
+      <c r="A38" s="51" t="s">
+        <v>289</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>87</v>
+      <c r="D38" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>279</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G38" s="11"/>
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
-      <c r="J38" s="41" t="s">
-        <v>293</v>
+      <c r="J38" s="40" t="s">
+        <v>287</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L38" s="9"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="52" t="s">
-        <v>295</v>
+      <c r="A39" s="51" t="s">
+        <v>218</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="12"/>
-      <c r="D39" s="44" t="s">
-        <v>265</v>
-      </c>
-      <c r="E39" s="20" t="s">
+      <c r="D39" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>83</v>
       </c>
       <c r="F39" s="7" t="s">
@@ -2783,113 +2803,113 @@
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="41" t="s">
-        <v>293</v>
+      <c r="J39" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L39" s="9"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="52" t="s">
-        <v>224</v>
+      <c r="A40" s="51" t="s">
+        <v>290</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
-      <c r="J40" s="41" t="s">
-        <v>208</v>
+      <c r="J40" s="40" t="s">
+        <v>218</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="52" t="s">
-        <v>296</v>
+      <c r="A41" s="51" t="s">
+        <v>291</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="41" t="s">
-        <v>224</v>
+      <c r="I41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41" s="40" t="s">
+        <v>218</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="52" t="s">
-        <v>297</v>
+      <c r="A42" s="51" t="s">
+        <v>292</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J42" s="41" t="s">
-        <v>224</v>
+      <c r="I42" s="9"/>
+      <c r="J42" s="40" t="s">
+        <v>218</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L42" s="9"/>
     </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="52" t="s">
-        <v>298</v>
+    <row r="43" spans="1:12" ht="26">
+      <c r="A43" s="51" t="s">
+        <v>219</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>27</v>
@@ -2897,201 +2917,201 @@
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
-      <c r="J43" s="41" t="s">
-        <v>224</v>
+      <c r="J43" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L43" s="9"/>
     </row>
     <row r="44" spans="1:12" ht="26">
-      <c r="A44" s="52" t="s">
-        <v>225</v>
+      <c r="A44" s="51" t="s">
+        <v>293</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>28</v>
+        <v>92</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="43" t="s">
+        <v>318</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
-      <c r="J44" s="41" t="s">
-        <v>208</v>
+      <c r="J44" s="40" t="s">
+        <v>219</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12" ht="26">
-      <c r="A45" s="52" t="s">
-        <v>299</v>
+      <c r="A45" s="51" t="s">
+        <v>220</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
-      <c r="J45" s="41" t="s">
-        <v>225</v>
+      <c r="J45" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12" ht="26">
-      <c r="A46" s="52" t="s">
-        <v>226</v>
+      <c r="A46" s="51" t="s">
+        <v>221</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
-      <c r="J46" s="41" t="s">
-        <v>208</v>
+      <c r="J46" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L46" s="9"/>
     </row>
-    <row r="47" spans="1:12" ht="26">
-      <c r="A47" s="52" t="s">
-        <v>227</v>
+    <row r="47" spans="1:12" ht="51">
+      <c r="A47" s="51" t="s">
+        <v>222</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D47" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>27</v>
+        <v>100</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="43" t="s">
+        <v>319</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
-      <c r="J47" s="41" t="s">
-        <v>208</v>
+      <c r="J47" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L47" s="9"/>
     </row>
-    <row r="48" spans="1:12" ht="51">
-      <c r="A48" s="52" t="s">
-        <v>228</v>
+    <row r="48" spans="1:12" ht="38.5">
+      <c r="A48" s="51" t="s">
+        <v>223</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>263</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
-      <c r="J48" s="41" t="s">
-        <v>208</v>
+      <c r="J48" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L48" s="9"/>
     </row>
-    <row r="49" spans="1:12" ht="38.5">
-      <c r="A49" s="52" t="s">
-        <v>229</v>
+    <row r="49" spans="1:12" ht="51">
+      <c r="A49" s="51" t="s">
+        <v>224</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="44" t="s">
-        <v>269</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="F49" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
-      <c r="J49" s="41" t="s">
-        <v>208</v>
+      <c r="J49" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L49" s="9"/>
     </row>
-    <row r="50" spans="1:12" ht="51">
-      <c r="A50" s="52" t="s">
-        <v>230</v>
+    <row r="50" spans="1:12" ht="26">
+      <c r="A50" s="51" t="s">
+        <v>225</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="E50" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>27</v>
@@ -3099,55 +3119,55 @@
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
-      <c r="J50" s="41" t="s">
-        <v>208</v>
+      <c r="J50" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12" ht="26">
-      <c r="A51" s="52" t="s">
-        <v>231</v>
+      <c r="A51" s="51" t="s">
+        <v>294</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
-      <c r="J51" s="41" t="s">
-        <v>208</v>
+      <c r="J51" s="40" t="s">
+        <v>225</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" ht="26">
-      <c r="A52" s="52" t="s">
-        <v>300</v>
+      <c r="A52" s="51" t="s">
+        <v>226</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>27</v>
@@ -3155,327 +3175,329 @@
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
-      <c r="J52" s="41" t="s">
-        <v>231</v>
+      <c r="J52" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="1:12" ht="26">
-      <c r="A53" s="52" t="s">
-        <v>232</v>
+    <row r="53" spans="1:12" ht="56.5">
+      <c r="A53" s="51" t="s">
+        <v>227</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="D53" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>28</v>
+        <v>112</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="F53" s="43" t="s">
+        <v>319</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
-      <c r="J53" s="41" t="s">
-        <v>208</v>
+      <c r="J53" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="1:12" ht="56.5">
-      <c r="A54" s="52" t="s">
-        <v>233</v>
+    <row r="54" spans="1:12" ht="42.5">
+      <c r="A54" s="51" t="s">
+        <v>228</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="D54" s="43" t="s">
+        <v>265</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
-      <c r="J54" s="41" t="s">
-        <v>208</v>
+      <c r="J54" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L54" s="9"/>
     </row>
     <row r="55" spans="1:12" ht="42.5">
-      <c r="A55" s="52" t="s">
-        <v>234</v>
+      <c r="A55" s="51" t="s">
+        <v>229</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C55" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="44" t="s">
-        <v>271</v>
-      </c>
-      <c r="E55" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>27</v>
+      <c r="F55" s="43" t="s">
+        <v>319</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
-      <c r="J55" s="41" t="s">
-        <v>208</v>
+      <c r="J55" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L55" s="9"/>
     </row>
     <row r="56" spans="1:12" ht="42.5">
-      <c r="A56" s="52" t="s">
-        <v>235</v>
+      <c r="A56" s="51" t="s">
+        <v>230</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>123</v>
+        <v>115</v>
+      </c>
+      <c r="D56" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
-      <c r="J56" s="41" t="s">
-        <v>208</v>
+      <c r="J56" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L56" s="9"/>
     </row>
     <row r="57" spans="1:12" ht="42.5">
-      <c r="A57" s="52" t="s">
-        <v>236</v>
+      <c r="A57" s="51" t="s">
+        <v>231</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D57" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="E57" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="F57" s="7" t="s">
-        <v>27</v>
+      <c r="F57" s="43" t="s">
+        <v>319</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
-      <c r="J57" s="41" t="s">
-        <v>208</v>
+      <c r="J57" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L57" s="9"/>
     </row>
     <row r="58" spans="1:12" ht="42.5">
-      <c r="A58" s="52" t="s">
-        <v>237</v>
+      <c r="A58" s="51" t="s">
+        <v>232</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>126</v>
+        <v>118</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
-      <c r="J58" s="41" t="s">
-        <v>208</v>
+      <c r="J58" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L58" s="9"/>
     </row>
-    <row r="59" spans="1:12" ht="42.5">
-      <c r="A59" s="52" t="s">
-        <v>238</v>
+    <row r="59" spans="1:12" ht="56.5">
+      <c r="A59" s="51" t="s">
+        <v>233</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D59" s="45" t="s">
-        <v>270</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>27</v>
+        <v>121</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F59" s="43" t="s">
+        <v>319</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
-      <c r="J59" s="41" t="s">
-        <v>208</v>
+      <c r="J59" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L59" s="9"/>
     </row>
-    <row r="60" spans="1:12" ht="56.5">
-      <c r="A60" s="52" t="s">
-        <v>239</v>
+    <row r="60" spans="1:12">
+      <c r="A60" s="51" t="s">
+        <v>234</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>129</v>
+        <v>121</v>
+      </c>
+      <c r="D60" s="46" t="s">
+        <v>267</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
-      <c r="J60" s="41" t="s">
-        <v>208</v>
+      <c r="J60" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:12">
-      <c r="A61" s="52" t="s">
-        <v>240</v>
+    <row r="61" spans="1:12" ht="51">
+      <c r="A61" s="51" t="s">
+        <v>235</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D61" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="E61" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>27</v>
+        <v>121</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F61" s="43" t="s">
+        <v>319</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
-      <c r="J61" s="41" t="s">
-        <v>208</v>
+      <c r="J61" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L61" s="9"/>
     </row>
-    <row r="62" spans="1:12" ht="51">
-      <c r="A62" s="52" t="s">
-        <v>241</v>
+    <row r="62" spans="1:12" ht="26">
+      <c r="A62" s="51" t="s">
+        <v>236</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D62" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D62" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="E62" s="27" t="s">
-        <v>131</v>
+      <c r="E62" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
-      <c r="J62" s="41" t="s">
-        <v>208</v>
+      <c r="J62" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L62" s="9"/>
     </row>
-    <row r="63" spans="1:12" ht="26">
-      <c r="A63" s="52" t="s">
-        <v>242</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>134</v>
+    <row r="63" spans="1:12">
+      <c r="A63" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="B63" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>130</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>27</v>
@@ -3483,59 +3505,59 @@
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
-      <c r="J63" s="41" t="s">
-        <v>208</v>
+      <c r="J63" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L63" s="9"/>
     </row>
-    <row r="64" spans="1:12">
-      <c r="A64" s="52" t="s">
-        <v>243</v>
-      </c>
-      <c r="B64" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E64" s="30" t="s">
-        <v>136</v>
+    <row r="64" spans="1:12" ht="51">
+      <c r="A64" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
-      <c r="J64" s="41" t="s">
-        <v>208</v>
+      <c r="J64" s="40" t="s">
+        <v>237</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L64" s="9"/>
     </row>
-    <row r="65" spans="1:12" ht="51">
-      <c r="A65" s="52" t="s">
-        <v>301</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>139</v>
+    <row r="65" spans="1:12">
+      <c r="A65" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="B65" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>135</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>27</v>
@@ -3543,59 +3565,59 @@
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
-      <c r="J65" s="41" t="s">
-        <v>243</v>
+      <c r="J65" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L65" s="9"/>
     </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="52" t="s">
-        <v>244</v>
-      </c>
-      <c r="B66" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="C66" s="51" t="s">
+    <row r="66" spans="1:12" ht="51">
+      <c r="A66" s="51" t="s">
+        <v>296</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E66" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D66" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="E66" s="31" t="s">
-        <v>141</v>
-      </c>
       <c r="F66" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
-      <c r="J66" s="41" t="s">
-        <v>208</v>
+      <c r="J66" s="40" t="s">
+        <v>238</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L66" s="9"/>
     </row>
     <row r="67" spans="1:12" ht="51">
-      <c r="A67" s="52" t="s">
-        <v>302</v>
+      <c r="A67" s="51" t="s">
+        <v>239</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>27</v>
@@ -3603,469 +3625,469 @@
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
-      <c r="J67" s="41" t="s">
-        <v>244</v>
+      <c r="J67" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L67" s="9"/>
     </row>
-    <row r="68" spans="1:12" ht="51">
-      <c r="A68" s="52" t="s">
-        <v>245</v>
+    <row r="68" spans="1:12" ht="42.5">
+      <c r="A68" s="51" t="s">
+        <v>153</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E68" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>28</v>
+        <v>141</v>
+      </c>
+      <c r="E68" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F68" s="43" t="s">
+        <v>319</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
-      <c r="J68" s="41" t="s">
-        <v>208</v>
+      <c r="J68" s="40" t="s">
+        <v>239</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L68" s="9"/>
     </row>
-    <row r="69" spans="1:12" ht="42.5">
-      <c r="A69" s="52" t="s">
-        <v>159</v>
+    <row r="69" spans="1:12">
+      <c r="A69" s="51" t="s">
+        <v>240</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D69" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>148</v>
+      <c r="E69" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G69" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>276</v>
+      </c>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
-      <c r="J69" s="41" t="s">
-        <v>245</v>
+      <c r="J69" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L69" s="9"/>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="52" t="s">
-        <v>246</v>
+      <c r="A70" s="51" t="s">
+        <v>241</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>151</v>
+        <v>146</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>282</v>
+        <v>47</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
-      <c r="J70" s="41" t="s">
-        <v>208</v>
+      <c r="J70" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:12">
-      <c r="A71" s="52" t="s">
-        <v>247</v>
+    <row r="71" spans="1:12" ht="63.5">
+      <c r="A71" s="51" t="s">
+        <v>242</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D71" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>284</v>
-      </c>
+      <c r="F71" s="43" t="s">
+        <v>324</v>
+      </c>
+      <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
-      <c r="J71" s="41" t="s">
-        <v>208</v>
+      <c r="J71" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K71" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L71" s="9"/>
     </row>
-    <row r="72" spans="1:12" ht="63.5">
-      <c r="A72" s="52" t="s">
-        <v>248</v>
+    <row r="72" spans="1:12" ht="26">
+      <c r="A72" s="51" t="s">
+        <v>243</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>149</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C72" s="12"/>
       <c r="D72" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>152</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
-      <c r="J72" s="41" t="s">
-        <v>208</v>
+      <c r="J72" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L72" s="9"/>
     </row>
-    <row r="73" spans="1:12" ht="26">
-      <c r="A73" s="52" t="s">
-        <v>249</v>
+    <row r="73" spans="1:12" ht="38.5">
+      <c r="A73" s="51" t="s">
+        <v>297</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>158</v>
+        <v>154</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>155</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>28</v>
+        <v>325</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
-      <c r="J73" s="41" t="s">
-        <v>208</v>
+      <c r="J73" s="40" t="s">
+        <v>243</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L73" s="9"/>
     </row>
-    <row r="74" spans="1:12" ht="38.5">
-      <c r="A74" s="52" t="s">
-        <v>303</v>
+    <row r="74" spans="1:12" ht="26">
+      <c r="A74" s="51" t="s">
+        <v>298</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>36</v>
+        <v>319</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
-      <c r="J74" s="41" t="s">
-        <v>249</v>
+      <c r="J74" s="40" t="s">
+        <v>243</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L74" s="9"/>
     </row>
     <row r="75" spans="1:12" ht="26">
-      <c r="A75" s="52" t="s">
-        <v>304</v>
+      <c r="A75" s="51" t="s">
+        <v>244</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
-      <c r="J75" s="41" t="s">
-        <v>249</v>
+      <c r="J75" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L75" s="9"/>
     </row>
-    <row r="76" spans="1:12" ht="26">
-      <c r="A76" s="52" t="s">
-        <v>250</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>156</v>
-      </c>
+    <row r="76" spans="1:12">
+      <c r="A76" s="51" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" s="27"/>
       <c r="C76" s="12"/>
       <c r="D76" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>161</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
-      <c r="J76" s="41" t="s">
-        <v>208</v>
+      <c r="J76" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L76" s="9"/>
     </row>
-    <row r="77" spans="1:12">
-      <c r="A77" s="52" t="s">
-        <v>251</v>
-      </c>
-      <c r="B77" s="28"/>
+    <row r="77" spans="1:12" ht="26">
+      <c r="A77" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="C77" s="12"/>
       <c r="D77" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E77" s="32" t="s">
-        <v>167</v>
+        <v>162</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
-      <c r="J77" s="41" t="s">
-        <v>208</v>
+      <c r="J77" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K77" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L77" s="9"/>
     </row>
-    <row r="78" spans="1:12" ht="26">
-      <c r="A78" s="52" t="s">
-        <v>252</v>
+    <row r="78" spans="1:12" ht="38.5">
+      <c r="A78" s="51" t="s">
+        <v>247</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" s="12"/>
+        <v>150</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="D78" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
-      <c r="J78" s="41" t="s">
-        <v>208</v>
+      <c r="J78" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K78" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L78" s="9"/>
     </row>
-    <row r="79" spans="1:12" ht="38.5">
-      <c r="A79" s="52" t="s">
-        <v>253</v>
+    <row r="79" spans="1:12" ht="26">
+      <c r="A79" s="51" t="s">
+        <v>248</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
-      <c r="J79" s="41" t="s">
-        <v>208</v>
+      <c r="J79" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L79" s="9"/>
     </row>
     <row r="80" spans="1:12" ht="26">
-      <c r="A80" s="52" t="s">
-        <v>254</v>
+      <c r="A80" s="51" t="s">
+        <v>249</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D80" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E80" s="13" t="s">
-        <v>174</v>
+      <c r="E80" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
-      <c r="J80" s="41" t="s">
-        <v>208</v>
+      <c r="J80" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K80" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L80" s="9"/>
     </row>
-    <row r="81" spans="1:12" ht="26">
-      <c r="A81" s="52" t="s">
-        <v>255</v>
+    <row r="81" spans="1:12">
+      <c r="A81" s="51" t="s">
+        <v>250</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>177</v>
+        <v>172</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
-      <c r="J81" s="41" t="s">
-        <v>208</v>
+      <c r="J81" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K81" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L81" s="9"/>
     </row>
     <row r="82" spans="1:12">
-      <c r="A82" s="52" t="s">
-        <v>256</v>
+      <c r="A82" s="51" t="s">
+        <v>251</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C82" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>179</v>
-      </c>
       <c r="F82" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
-      <c r="J82" s="41" t="s">
-        <v>208</v>
+      <c r="J82" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L82" s="9"/>
     </row>
-    <row r="83" spans="1:12">
-      <c r="A83" s="52" t="s">
-        <v>257</v>
+    <row r="83" spans="1:12" ht="26">
+      <c r="A83" s="51" t="s">
+        <v>252</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E83" s="29" t="s">
-        <v>181</v>
+        <v>177</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>27</v>
@@ -4073,199 +4095,197 @@
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
-      <c r="J83" s="41" t="s">
-        <v>208</v>
+      <c r="J83" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L83" s="9"/>
     </row>
-    <row r="84" spans="1:12" ht="26">
-      <c r="A84" s="52" t="s">
-        <v>258</v>
+    <row r="84" spans="1:12">
+      <c r="A84" s="51" t="s">
+        <v>16</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>184</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="E84" s="32"/>
       <c r="F84" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G84" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="G84" s="48" t="s">
+        <v>274</v>
+      </c>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
-      <c r="J84" s="41" t="s">
-        <v>208</v>
+      <c r="J84" s="40" t="s">
+        <v>252</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L84" s="9"/>
     </row>
     <row r="85" spans="1:12">
-      <c r="A85" s="52" t="s">
+      <c r="A85" s="51" t="s">
         <v>17</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E85" s="33"/>
+        <v>180</v>
+      </c>
+      <c r="E85" s="28" t="s">
+        <v>181</v>
+      </c>
       <c r="F85" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G85" s="49" t="s">
-        <v>280</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G85" s="11"/>
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
-      <c r="J85" s="41" t="s">
-        <v>258</v>
+      <c r="J85" s="40" t="s">
+        <v>252</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L85" s="9"/>
     </row>
     <row r="86" spans="1:12">
-      <c r="A86" s="52" t="s">
-        <v>18</v>
+      <c r="A86" s="51" t="s">
+        <v>253</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C86" s="4" t="s">
         <v>182</v>
       </c>
+      <c r="C86" s="12"/>
       <c r="D86" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E86" s="29" t="s">
-        <v>187</v>
+        <v>183</v>
+      </c>
+      <c r="E86" s="33" t="s">
+        <v>184</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
-      <c r="J86" s="41" t="s">
-        <v>258</v>
+      <c r="J86" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L86" s="9"/>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="52" t="s">
-        <v>259</v>
+      <c r="A87" s="51" t="s">
+        <v>254</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E87" s="34" t="s">
-        <v>190</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="E87" s="9"/>
       <c r="F87" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
-      <c r="J87" s="41" t="s">
-        <v>208</v>
+      <c r="J87" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L87" s="9"/>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="52" t="s">
-        <v>260</v>
+      <c r="A88" s="51" t="s">
+        <v>299</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E88" s="9"/>
+        <v>186</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>187</v>
+      </c>
       <c r="F88" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
-      <c r="J88" s="41" t="s">
-        <v>208</v>
+      <c r="J88" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L88" s="9"/>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="52" t="s">
-        <v>305</v>
+      <c r="A89" s="51" t="s">
+        <v>300</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
-      <c r="J89" s="41" t="s">
-        <v>208</v>
+      <c r="J89" s="40" t="s">
+        <v>299</v>
       </c>
       <c r="K89" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L89" s="9"/>
     </row>
-    <row r="90" spans="1:12">
-      <c r="A90" s="52" t="s">
-        <v>306</v>
+    <row r="90" spans="1:12" ht="51">
+      <c r="A90" s="51" t="s">
+        <v>301</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>27</v>
@@ -4273,183 +4293,155 @@
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
-      <c r="J90" s="41" t="s">
-        <v>305</v>
+      <c r="J90" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L90" s="9"/>
     </row>
-    <row r="91" spans="1:12" ht="51">
-      <c r="A91" s="52" t="s">
-        <v>307</v>
+    <row r="91" spans="1:12">
+      <c r="A91" s="51" t="s">
+        <v>302</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C91" s="12"/>
-      <c r="D91" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>197</v>
+      <c r="D91" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>193</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
-      <c r="J91" s="41" t="s">
-        <v>208</v>
+      <c r="J91" s="40" t="s">
+        <v>301</v>
       </c>
       <c r="K91" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L91" s="9"/>
     </row>
-    <row r="92" spans="1:12">
-      <c r="A92" s="52" t="s">
-        <v>308</v>
+    <row r="92" spans="1:12" ht="38.5">
+      <c r="A92" s="51" t="s">
+        <v>303</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C92" s="12"/>
-      <c r="D92" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="E92" s="29" t="s">
-        <v>199</v>
+      <c r="D92" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
-      <c r="J92" s="41" t="s">
-        <v>307</v>
+      <c r="J92" s="40" t="s">
+        <v>301</v>
       </c>
       <c r="K92" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L92" s="9"/>
     </row>
-    <row r="93" spans="1:12" ht="38.5">
-      <c r="A93" s="52" t="s">
-        <v>309</v>
+    <row r="93" spans="1:12" ht="26">
+      <c r="A93" s="51" t="s">
+        <v>304</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="F93" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G93" s="11"/>
+        <v>196</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F93" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="G93" s="43" t="s">
+        <v>275</v>
+      </c>
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
-      <c r="J93" s="41" t="s">
-        <v>307</v>
+      <c r="J93" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L93" s="9"/>
     </row>
     <row r="94" spans="1:12" ht="26">
-      <c r="A94" s="52" t="s">
-        <v>310</v>
+      <c r="A94" s="51" t="s">
+        <v>305</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="E94" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="F94" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G94" s="44" t="s">
-        <v>281</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="E94" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G94" s="11"/>
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
-      <c r="J94" s="41" t="s">
-        <v>208</v>
+      <c r="J94" s="40" t="s">
+        <v>202</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L94" s="9"/>
     </row>
-    <row r="95" spans="1:12" ht="26">
-      <c r="A95" s="52" t="s">
-        <v>311</v>
+    <row r="95" spans="1:12" ht="51">
+      <c r="A95" s="51" t="s">
+        <v>306</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C95" s="12"/>
+        <v>182</v>
+      </c>
+      <c r="C95" s="34"/>
       <c r="D95" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
-      <c r="I95" s="9"/>
-      <c r="J95" s="41" t="s">
-        <v>208</v>
+      <c r="I95" s="15"/>
+      <c r="J95" s="54" t="s">
+        <v>305</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L95" s="9"/>
-    </row>
-    <row r="96" spans="1:12" ht="51">
-      <c r="A96" s="52" t="s">
-        <v>312</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C96" s="35"/>
-      <c r="D96" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="E96" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="15"/>
-      <c r="J96" s="55" t="s">
-        <v>311</v>
-      </c>
-      <c r="K96" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L96" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish up certificates stuff
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDEC1D4-FE8C-4E3B-8AA1-63301D0B54F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBE25F2-D6C2-4A32-B55D-653A7A5C5DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="326">
   <si>
     <t>Unit</t>
   </si>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -1763,7 +1763,9 @@
       <c r="I2" s="9"/>
       <c r="J2" s="39"/>
       <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="L2" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="41" t="s">
@@ -2021,7 +2023,7 @@
       </c>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:12" ht="26">
+    <row r="12" spans="1:12">
       <c r="A12" s="51" t="s">
         <v>206</v>
       </c>
@@ -2047,7 +2049,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:12" ht="26">
+    <row r="13" spans="1:12">
       <c r="A13" s="51" t="s">
         <v>207</v>
       </c>
@@ -2073,7 +2075,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:12" ht="26">
+    <row r="14" spans="1:12">
       <c r="A14" s="51" t="s">
         <v>208</v>
       </c>
@@ -2099,7 +2101,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:12" ht="26">
+    <row r="15" spans="1:12">
       <c r="A15" s="51" t="s">
         <v>209</v>
       </c>
@@ -2213,7 +2215,7 @@
       </c>
       <c r="L18" s="50"/>
     </row>
-    <row r="19" spans="1:12" ht="28.5">
+    <row r="19" spans="1:12">
       <c r="A19" s="51" t="s">
         <v>15</v>
       </c>
@@ -2297,7 +2299,7 @@
       </c>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="1:12" ht="28.5">
+    <row r="22" spans="1:12">
       <c r="A22" s="51" t="s">
         <v>213</v>
       </c>
@@ -2409,7 +2411,7 @@
       </c>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" ht="26">
+    <row r="26" spans="1:12">
       <c r="A26" s="51" t="s">
         <v>216</v>
       </c>
@@ -2437,7 +2439,7 @@
       </c>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:12" ht="38.5">
+    <row r="27" spans="1:12" ht="26">
       <c r="A27" s="51" t="s">
         <v>279</v>
       </c>
@@ -2467,7 +2469,7 @@
       </c>
       <c r="L27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="38.5">
+    <row r="28" spans="1:12" ht="26">
       <c r="A28" s="51" t="s">
         <v>280</v>
       </c>
@@ -3099,7 +3101,7 @@
       </c>
       <c r="L49" s="9"/>
     </row>
-    <row r="50" spans="1:12" ht="26">
+    <row r="50" spans="1:12">
       <c r="A50" s="51" t="s">
         <v>225</v>
       </c>
@@ -3127,7 +3129,7 @@
       </c>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="1:12" ht="26">
+    <row r="51" spans="1:12">
       <c r="A51" s="51" t="s">
         <v>294</v>
       </c>
@@ -3183,7 +3185,7 @@
       </c>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="1:12" ht="56.5">
+    <row r="53" spans="1:12" ht="42.5">
       <c r="A53" s="51" t="s">
         <v>227</v>
       </c>
@@ -3243,7 +3245,7 @@
       </c>
       <c r="L54" s="9"/>
     </row>
-    <row r="55" spans="1:12" ht="42.5">
+    <row r="55" spans="1:12" ht="28.5">
       <c r="A55" s="51" t="s">
         <v>229</v>
       </c>
@@ -3423,7 +3425,7 @@
       </c>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:12" ht="51">
+    <row r="61" spans="1:12" ht="38.5">
       <c r="A61" s="51" t="s">
         <v>235</v>
       </c>
@@ -3603,7 +3605,7 @@
       </c>
       <c r="L66" s="9"/>
     </row>
-    <row r="67" spans="1:12" ht="51">
+    <row r="67" spans="1:12" ht="38.5">
       <c r="A67" s="51" t="s">
         <v>239</v>
       </c>
@@ -3727,7 +3729,7 @@
       </c>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:12" ht="63.5">
+    <row r="71" spans="1:12" ht="51">
       <c r="A71" s="51" t="s">
         <v>242</v>
       </c>
@@ -4273,7 +4275,7 @@
       </c>
       <c r="L89" s="9"/>
     </row>
-    <row r="90" spans="1:12" ht="51">
+    <row r="90" spans="1:12" ht="38.5">
       <c r="A90" s="51" t="s">
         <v>301</v>
       </c>
@@ -4449,18 +4451,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4673,6 +4675,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4685,14 +4695,6 @@
     <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
progress on "weitere Berichte"
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8D5C8F-C200-47B0-A98F-B30BA567099D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B05B482-F212-4992-A321-1AA9B4732E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="331">
   <si>
     <t>Unit</t>
   </si>
@@ -189,31 +189,16 @@
     <t>Allgemein</t>
   </si>
   <si>
-    <t>ESG-Ziele</t>
-  </si>
-  <si>
     <t>Hat das Unternehmen spezifische ESG-Ziele/Engagements? Werden bspw. spezifische Ziele / Maßnahmen ergriffen, um das 1,5 Grad Ziel zu erreichen?</t>
   </si>
   <si>
-    <t>Ziele</t>
-  </si>
-  <si>
     <t>Bitte geben Sie eine genaue Beschreibung der ESG-Ziele.</t>
   </si>
   <si>
-    <t>Investitionen</t>
-  </si>
-  <si>
     <t>Bitte geben Sie an wieviele Budgets/Vollzeitäquivalente für das Erreichen der ESG-Ziele zugewiesen wurden.</t>
   </si>
   <si>
-    <t>Sektor mit hohen Klimaauswirkungen</t>
-  </si>
-  <si>
     <t>Kann das Unternehmen einem oder mehreren Sektoren mit hohen Klimaauswirkungen zugeordnet werden?</t>
-  </si>
-  <si>
-    <t>Sektor</t>
   </si>
   <si>
     <t>Bitte geben Sie an, zu welchen Sektoren (mit hohen Klimaauswirkungen) das Unternehmen zugeordnet werden kann.</t>
@@ -1055,6 +1040,36 @@
   </si>
   <si>
     <t>Custom - Tabellencomponent?</t>
+  </si>
+  <si>
+    <t>Akkreditierungen</t>
+  </si>
+  <si>
+    <t>Beschreibung der ESG-Ziele</t>
+  </si>
+  <si>
+    <t>ESG Berichte</t>
+  </si>
+  <si>
+    <t>Sektoren</t>
+  </si>
+  <si>
+    <t>Auflistung der Sektoren</t>
+  </si>
+  <si>
+    <t>ESG Ziele</t>
+  </si>
+  <si>
+    <t>Existenz von ESG-Zielen</t>
+  </si>
+  <si>
+    <t>Investitionen in Zielerreichung</t>
+  </si>
+  <si>
+    <t>Sektoren mit hohen Klimaauswirkungen</t>
+  </si>
+  <si>
+    <t>Custom - List of BaseDataPoint&lt;string&gt;</t>
   </si>
 </sst>
 </file>
@@ -1685,7 +1700,7 @@
   <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -1738,7 +1753,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="35" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1797,12 +1812,14 @@
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12" t="s">
+        <v>326</v>
+      </c>
       <c r="D4" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>27</v>
@@ -1811,7 +1828,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>28</v>
@@ -1820,17 +1837,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="41" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>326</v>
+      </c>
       <c r="D5" s="8" t="s">
-        <v>39</v>
+        <v>322</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>26</v>
@@ -1848,17 +1867,19 @@
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="35" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12" t="s">
+        <v>326</v>
+      </c>
       <c r="D6" s="8" t="s">
-        <v>41</v>
+        <v>328</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>26</v>
@@ -1881,12 +1902,14 @@
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>324</v>
+      </c>
       <c r="D7" s="8" t="s">
-        <v>43</v>
+        <v>329</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>27</v>
@@ -1895,7 +1918,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>28</v>
@@ -1909,18 +1932,20 @@
       <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>324</v>
+      </c>
       <c r="D8" s="8" t="s">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -1934,17 +1959,19 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="35" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>323</v>
+      </c>
       <c r="D9" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>27</v>
@@ -1953,7 +1980,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>28</v>
@@ -1967,23 +1994,25 @@
       <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>323</v>
+      </c>
       <c r="D10" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="39" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>28</v>
@@ -1997,15 +2026,17 @@
       <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>323</v>
+      </c>
       <c r="D11" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2013,7 +2044,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>28</v>
@@ -2022,17 +2053,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="50" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B12" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="49" t="s">
+        <v>321</v>
+      </c>
       <c r="D12" s="42" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F12" s="49" t="s">
         <v>27</v>
@@ -2048,17 +2081,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="50" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B13" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="49"/>
+      <c r="C13" s="49" t="s">
+        <v>321</v>
+      </c>
       <c r="D13" s="42" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F13" s="49" t="s">
         <v>27</v>
@@ -2074,17 +2109,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="50" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B14" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="49" t="s">
+        <v>321</v>
+      </c>
       <c r="D14" s="42" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F14" s="49" t="s">
         <v>27</v>
@@ -2100,17 +2137,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="50" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B15" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="49" t="s">
+        <v>321</v>
+      </c>
       <c r="D15" s="42" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F15" s="49" t="s">
         <v>27</v>
@@ -2126,20 +2165,22 @@
     </row>
     <row r="16" spans="1:12" ht="26">
       <c r="A16" s="50" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="49" t="s">
+        <v>321</v>
+      </c>
       <c r="D16" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>35</v>
+        <v>330</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
@@ -2147,7 +2188,7 @@
         <v>29</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>28</v>
@@ -2156,17 +2197,17 @@
     </row>
     <row r="17" spans="1:12" ht="38.5">
       <c r="A17" s="50" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>27</v>
@@ -2175,7 +2216,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="9"/>
       <c r="J17" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>28</v>
@@ -2191,13 +2232,13 @@
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="42" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -2205,7 +2246,7 @@
         <v>29</v>
       </c>
       <c r="J18" s="54" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="K18" s="49" t="s">
         <v>28</v>
@@ -2221,10 +2262,10 @@
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="42" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>26</v>
@@ -2247,10 +2288,10 @@
       </c>
       <c r="C20" s="49"/>
       <c r="D20" s="42" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>27</v>
@@ -2259,7 +2300,7 @@
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
       <c r="J20" s="54" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="K20" s="49" t="s">
         <v>28</v>
@@ -2268,20 +2309,20 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="50" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F21" s="49" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2298,17 +2339,17 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="50" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="42" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>26</v>
@@ -2326,17 +2367,17 @@
     </row>
     <row r="23" spans="1:12" ht="38.5">
       <c r="A23" s="50" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>26</v>
@@ -2345,7 +2386,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>28</v>
@@ -2354,17 +2395,17 @@
     </row>
     <row r="24" spans="1:12" ht="26">
       <c r="A24" s="50" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>27</v>
@@ -2373,7 +2414,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>28</v>
@@ -2389,10 +2430,10 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>26</v>
@@ -2401,7 +2442,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="39" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>28</v>
@@ -2410,17 +2451,17 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="50" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>27</v>
@@ -2429,7 +2470,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>28</v>
@@ -2438,28 +2479,28 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="50" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G27" s="46" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="39" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>28</v>
@@ -2468,28 +2509,28 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="50" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="39" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>28</v>
@@ -2498,17 +2539,17 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="50" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>27</v>
@@ -2517,7 +2558,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>28</v>
@@ -2526,17 +2567,17 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="50" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="42" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>27</v>
@@ -2545,7 +2586,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="39" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>28</v>
@@ -2554,28 +2595,28 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="50" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="8" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="39" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>28</v>
@@ -2584,17 +2625,17 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="50" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="42" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>26</v>
@@ -2603,7 +2644,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="39" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>28</v>
@@ -2612,17 +2653,17 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="50" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="42" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>27</v>
@@ -2631,7 +2672,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="39" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>28</v>
@@ -2640,28 +2681,28 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="50" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>273</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="39" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>28</v>
@@ -2670,17 +2711,17 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="50" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="42" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>26</v>
@@ -2689,7 +2730,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="39" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>28</v>
@@ -2698,17 +2739,17 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="50" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="42" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>27</v>
@@ -2717,7 +2758,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="39" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>28</v>
@@ -2726,28 +2767,28 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="50" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="8" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="39" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>28</v>
@@ -2756,17 +2797,17 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="50" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="42" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>26</v>
@@ -2775,7 +2816,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="39" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>28</v>
@@ -2784,17 +2825,17 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="50" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>27</v>
@@ -2803,7 +2844,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>28</v>
@@ -2812,17 +2853,17 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="50" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>26</v>
@@ -2831,7 +2872,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>28</v>
@@ -2840,17 +2881,17 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="50" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>26</v>
@@ -2861,7 +2902,7 @@
         <v>29</v>
       </c>
       <c r="J41" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>28</v>
@@ -2870,17 +2911,17 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="50" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>26</v>
@@ -2889,7 +2930,7 @@
       <c r="H42" s="11"/>
       <c r="I42" s="9"/>
       <c r="J42" s="39" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>28</v>
@@ -2898,17 +2939,17 @@
     </row>
     <row r="43" spans="1:12" ht="26">
       <c r="A43" s="50" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>27</v>
@@ -2917,7 +2958,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>28</v>
@@ -2926,26 +2967,26 @@
     </row>
     <row r="44" spans="1:12" ht="26">
       <c r="A44" s="50" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="39" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>28</v>
@@ -2954,17 +2995,17 @@
     </row>
     <row r="45" spans="1:12" ht="26">
       <c r="A45" s="50" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>26</v>
@@ -2973,7 +3014,7 @@
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>28</v>
@@ -2982,17 +3023,17 @@
     </row>
     <row r="46" spans="1:12" ht="26">
       <c r="A46" s="50" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>26</v>
@@ -3001,7 +3042,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>28</v>
@@ -3010,28 +3051,28 @@
     </row>
     <row r="47" spans="1:12" ht="51">
       <c r="A47" s="50" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F47" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>28</v>
@@ -3040,19 +3081,19 @@
     </row>
     <row r="48" spans="1:12" ht="38.5">
       <c r="A48" s="50" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>26</v>
@@ -3061,7 +3102,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>28</v>
@@ -3070,19 +3111,19 @@
     </row>
     <row r="49" spans="1:12" ht="51">
       <c r="A49" s="50" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="E49" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>26</v>
@@ -3091,7 +3132,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>28</v>
@@ -3100,17 +3141,17 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="50" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>27</v>
@@ -3119,7 +3160,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>28</v>
@@ -3128,17 +3169,17 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="50" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>26</v>
@@ -3147,7 +3188,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="39" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>28</v>
@@ -3156,17 +3197,17 @@
     </row>
     <row r="52" spans="1:12" ht="26">
       <c r="A52" s="50" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>27</v>
@@ -3175,7 +3216,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>28</v>
@@ -3184,28 +3225,28 @@
     </row>
     <row r="53" spans="1:12" ht="42.5">
       <c r="A53" s="50" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>28</v>
@@ -3214,19 +3255,19 @@
     </row>
     <row r="54" spans="1:12" ht="42.5">
       <c r="A54" s="50" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>26</v>
@@ -3235,7 +3276,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>28</v>
@@ -3244,28 +3285,28 @@
     </row>
     <row r="55" spans="1:12" ht="28.5">
       <c r="A55" s="50" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F55" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>28</v>
@@ -3274,19 +3315,19 @@
     </row>
     <row r="56" spans="1:12" ht="42.5">
       <c r="A56" s="50" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>26</v>
@@ -3295,7 +3336,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>28</v>
@@ -3304,28 +3345,28 @@
     </row>
     <row r="57" spans="1:12" ht="42.5">
       <c r="A57" s="50" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F57" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>28</v>
@@ -3334,19 +3375,19 @@
     </row>
     <row r="58" spans="1:12" ht="42.5">
       <c r="A58" s="50" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>26</v>
@@ -3355,7 +3396,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>28</v>
@@ -3364,28 +3405,28 @@
     </row>
     <row r="59" spans="1:12" ht="56.5">
       <c r="A59" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F59" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>28</v>
@@ -3394,19 +3435,19 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="50" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D60" s="45" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>26</v>
@@ -3415,7 +3456,7 @@
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>28</v>
@@ -3424,28 +3465,28 @@
     </row>
     <row r="61" spans="1:12" ht="38.5">
       <c r="A61" s="50" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F61" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>28</v>
@@ -3454,19 +3495,19 @@
     </row>
     <row r="62" spans="1:12" ht="26">
       <c r="A62" s="50" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>26</v>
@@ -3475,7 +3516,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>28</v>
@@ -3484,19 +3525,19 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B63" s="49" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C63" s="49" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>27</v>
@@ -3505,7 +3546,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>28</v>
@@ -3514,19 +3555,19 @@
     </row>
     <row r="64" spans="1:12" ht="51">
       <c r="A64" s="50" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>26</v>
@@ -3535,7 +3576,7 @@
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="39" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>28</v>
@@ -3544,19 +3585,19 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="50" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B65" s="49" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C65" s="49" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>27</v>
@@ -3565,7 +3606,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>28</v>
@@ -3574,19 +3615,19 @@
     </row>
     <row r="66" spans="1:12" ht="51">
       <c r="A66" s="50" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D66" s="8" t="s">
-        <v>136</v>
-      </c>
       <c r="E66" s="13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>26</v>
@@ -3595,7 +3636,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="39" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>28</v>
@@ -3604,19 +3645,19 @@
     </row>
     <row r="67" spans="1:12" ht="38.5">
       <c r="A67" s="50" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>27</v>
@@ -3625,7 +3666,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>28</v>
@@ -3634,28 +3675,28 @@
     </row>
     <row r="68" spans="1:12" ht="42.5">
       <c r="A68" s="50" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F68" s="42" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="39" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>28</v>
@@ -3664,30 +3705,30 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="50" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>28</v>
@@ -3696,30 +3737,30 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="50" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>28</v>
@@ -3728,28 +3769,28 @@
     </row>
     <row r="71" spans="1:12" ht="51">
       <c r="A71" s="50" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D71" s="8" t="s">
-        <v>148</v>
-      </c>
       <c r="E71" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F71" s="42" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>28</v>
@@ -3758,17 +3799,17 @@
     </row>
     <row r="72" spans="1:12" ht="26">
       <c r="A72" s="50" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>27</v>
@@ -3777,7 +3818,7 @@
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>28</v>
@@ -3786,26 +3827,26 @@
     </row>
     <row r="73" spans="1:12" ht="38.5">
       <c r="A73" s="50" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="39" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>28</v>
@@ -3814,26 +3855,26 @@
     </row>
     <row r="74" spans="1:12" ht="26">
       <c r="A74" s="50" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="39" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>28</v>
@@ -3842,17 +3883,17 @@
     </row>
     <row r="75" spans="1:12" ht="26">
       <c r="A75" s="50" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>26</v>
@@ -3861,7 +3902,7 @@
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>28</v>
@@ -3870,17 +3911,17 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="50" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B76" s="49" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>35</v>
@@ -3889,7 +3930,7 @@
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>28</v>
@@ -3898,17 +3939,17 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="50" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>35</v>
@@ -3917,7 +3958,7 @@
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>28</v>
@@ -3926,19 +3967,19 @@
     </row>
     <row r="78" spans="1:12" ht="38.5">
       <c r="A78" s="50" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>35</v>
@@ -3947,7 +3988,7 @@
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>28</v>
@@ -3956,19 +3997,19 @@
     </row>
     <row r="79" spans="1:12" ht="26">
       <c r="A79" s="50" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>26</v>
@@ -3977,7 +4018,7 @@
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>28</v>
@@ -3986,19 +4027,19 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="50" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>35</v>
@@ -4007,7 +4048,7 @@
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>28</v>
@@ -4016,19 +4057,19 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="50" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -4037,7 +4078,7 @@
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>28</v>
@@ -4046,19 +4087,19 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="50" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C82" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>174</v>
-      </c>
       <c r="E82" s="27" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>26</v>
@@ -4067,7 +4108,7 @@
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>28</v>
@@ -4076,19 +4117,19 @@
     </row>
     <row r="83" spans="1:12" ht="26">
       <c r="A83" s="50" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>27</v>
@@ -4097,7 +4138,7 @@
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>28</v>
@@ -4109,25 +4150,25 @@
         <v>16</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E84" s="31"/>
       <c r="F84" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G84" s="47" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="39" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>28</v>
@@ -4139,16 +4180,16 @@
         <v>17</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E85" s="27" t="s">
         <v>176</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>181</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>26</v>
@@ -4157,7 +4198,7 @@
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="39" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>28</v>
@@ -4166,17 +4207,17 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="50" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E86" s="32" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>35</v>
@@ -4185,7 +4226,7 @@
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>28</v>
@@ -4194,14 +4235,14 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="50" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E87" s="9"/>
       <c r="F87" s="7" t="s">
@@ -4211,7 +4252,7 @@
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>28</v>
@@ -4220,17 +4261,17 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="50" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>27</v>
@@ -4239,7 +4280,7 @@
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>28</v>
@@ -4248,17 +4289,17 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="50" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>26</v>
@@ -4267,7 +4308,7 @@
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="39" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>28</v>
@@ -4276,17 +4317,17 @@
     </row>
     <row r="90" spans="1:12" ht="38.5">
       <c r="A90" s="50" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>27</v>
@@ -4295,7 +4336,7 @@
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>28</v>
@@ -4304,17 +4345,17 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="50" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C91" s="12"/>
       <c r="D91" s="27" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>26</v>
@@ -4323,7 +4364,7 @@
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="39" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>28</v>
@@ -4332,17 +4373,17 @@
     </row>
     <row r="92" spans="1:12" ht="38.5">
       <c r="A92" s="50" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C92" s="12"/>
       <c r="D92" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>26</v>
@@ -4351,7 +4392,7 @@
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
       <c r="J92" s="39" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>28</v>
@@ -4360,28 +4401,28 @@
     </row>
     <row r="93" spans="1:12" ht="26">
       <c r="A93" s="50" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F93" s="42" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G93" s="42" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>28</v>
@@ -4390,17 +4431,17 @@
     </row>
     <row r="94" spans="1:12" ht="26">
       <c r="A94" s="50" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>27</v>
@@ -4409,7 +4450,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
       <c r="J94" s="39" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>28</v>
@@ -4418,17 +4459,17 @@
     </row>
     <row r="95" spans="1:12" ht="51">
       <c r="A95" s="50" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C95" s="33"/>
       <c r="D95" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>26</v>
@@ -4437,7 +4478,7 @@
       <c r="H95" s="11"/>
       <c r="I95" s="15"/>
       <c r="J95" s="53" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>28</v>
@@ -4450,21 +4491,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -4673,32 +4699,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4715,4 +4731,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
take care of some todos
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B05B482-F212-4992-A321-1AA9B4732E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D4A4A7-EF2A-45C3-A733-4BABB62048E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1700,7 +1700,7 @@
   <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -4491,6 +4491,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -4699,22 +4714,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4731,29 +4756,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
rework OECD and UNGC + use custom fields
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D4A4A7-EF2A-45C3-A733-4BABB62048E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB62EEBE-5A7A-4F17-9658-1005911C28E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="330">
   <si>
     <t>Unit</t>
   </si>
@@ -225,25 +225,10 @@
     <t>Bitte teilen Sie die letzten Berichte mit uns (vorzugsweise die letzten drei).</t>
   </si>
   <si>
-    <t>Mechanismen zur Überwachung der Einhaltung UN Global Compact Prinzipien und/oder OECD Leitsätze</t>
-  </si>
-  <si>
-    <t>Verfügt das Unternehmen über Prozesse und Compliance-Mechanismen, um die Einhaltung der Prinzipien des UN Global Compact und/oder der OECD-Leitsätze für multinationale Unternehmen (OECD MNE-Leitsätze) zu überwachen?</t>
-  </si>
-  <si>
-    <t>UNCG Prinzipien</t>
-  </si>
-  <si>
     <t>Bitte geben Sie eine Erklärung ab, dass keine Verstöße gegen diese Grundsätze vorliegen.</t>
   </si>
   <si>
     <t>OECD Leitsätze</t>
-  </si>
-  <si>
-    <t>Richtlinien Einhaltung OECD</t>
-  </si>
-  <si>
-    <t>Bitte teilen Sie die Richtlinien mit uns die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der OECD Leitsätze überwacht.</t>
   </si>
   <si>
     <t>Ausrichtung auf die UN SDGs und aktives Verfolgen</t>
@@ -697,15 +682,9 @@
     <t>9</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>10.2.1</t>
   </si>
   <si>
-    <t>10.2.2</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -829,9 +808,6 @@
     <t>51</t>
   </si>
   <si>
-    <t>Erklärung UNGC</t>
-  </si>
-  <si>
     <t>Erklärung OECD</t>
   </si>
   <si>
@@ -1015,9 +991,6 @@
     <t>In welchen Zeitabständen werden die Berichte erstellt?</t>
   </si>
   <si>
-    <t>Custom - List of BaseDocumentReference</t>
-  </si>
-  <si>
     <t>Custom - Sollte in mehrere Fragen aufgebrochen werden =&gt; Ausstehende Emissionen einmal für "Nachhaltige Emissionen" und für "SLD" =&gt; Dann kann beides jeweils ein DecimalField mit € als (feste) unit sein</t>
   </si>
   <si>
@@ -1027,15 +1000,6 @@
     <t>Weitere Akkreditierungen</t>
   </si>
   <si>
-    <t>New Component - Yes/No with multiple basedocumentreferences</t>
-  </si>
-  <si>
-    <t>Hat das Unternehmen Überwachungsmechanismen für die OECD Leitsätze eingerichtet ? Wenn ja, bitte teilen Sie die Richtlinien mit uns, die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der OECD Leitsätze überwacht.</t>
-  </si>
-  <si>
-    <t>Hat das Unternehmen Überwachungsmechanismen für die UNGC Prinzipien eingerichtet ? Wenn ja bitte, teilen Sie die Richtlinien mit uns, die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung des UNGC (alle vier Säulen) überwacht.</t>
-  </si>
-  <si>
     <t>Custom - Rolling Window mit vorangestellter Freitext (oder List of Strings) Frage zu den Sektoren</t>
   </si>
   <si>
@@ -1070,6 +1034,39 @@
   </si>
   <si>
     <t>Custom - List of BaseDataPoint&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>Verfügt das Unternehmen über Prozesse und Compliance-Mechanismen, um die Einhaltung der Prinzipien des UN Global Compact zu überwachen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erklärung der Einhaltung </t>
+  </si>
+  <si>
+    <t>Mechanismen zur Überwachung der Einhaltung der UN Global Compact Prinzipien</t>
+  </si>
+  <si>
+    <t>Richtlinien zur Einhaltung</t>
+  </si>
+  <si>
+    <t>Bitte teilen Sie die Richtlinien mit uns die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der UN Global Compact Prinzipien überwacht.</t>
+  </si>
+  <si>
+    <t>UN Global Concept Prinzipien</t>
+  </si>
+  <si>
+    <t>Verfügt das Unternehmen über Prozesse und Compliance-Mechanismen, um die Einhaltung der OECD-Leitsätze für multinationale Unternehmen (OECD MNE Guidelines) zu überwachen?</t>
+  </si>
+  <si>
+    <t>Mechanismen zur Überwachung der Einhaltung der OECD-Leitsätze</t>
+  </si>
+  <si>
+    <t>Bitte teilen Sie die Richtlinien mit uns die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der OECD-Leitsätze überwacht.</t>
+  </si>
+  <si>
+    <t>10.1.1.1</t>
+  </si>
+  <si>
+    <t>10.2.1.1</t>
   </si>
 </sst>
 </file>
@@ -1699,14 +1696,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="12.54296875" style="36"/>
-    <col min="4" max="4" width="38.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="62.6328125" customWidth="1"/>
     <col min="5" max="5" width="85.54296875" customWidth="1"/>
     <col min="6" max="6" width="65.54296875" customWidth="1"/>
     <col min="7" max="7" width="31.6328125" customWidth="1"/>
@@ -1753,7 +1751,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="35" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1813,10 +1811,10 @@
         <v>36</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>37</v>
@@ -1828,7 +1826,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>28</v>
@@ -1837,16 +1835,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="41" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>38</v>
@@ -1867,16 +1865,16 @@
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="35" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>39</v>
@@ -1903,10 +1901,10 @@
         <v>36</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>40</v>
@@ -1918,7 +1916,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>28</v>
@@ -1933,10 +1931,10 @@
         <v>36</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>41</v>
@@ -1945,7 +1943,7 @@
         <v>42</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -1959,13 +1957,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="35" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>43</v>
@@ -1980,7 +1978,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>28</v>
@@ -1995,24 +1993,24 @@
         <v>36</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="39" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>28</v>
@@ -2027,7 +2025,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>47</v>
@@ -2036,15 +2034,13 @@
         <v>48</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="I11" s="7"/>
       <c r="J11" s="39" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>28</v>
@@ -2053,19 +2049,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="50" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B12" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F12" s="49" t="s">
         <v>27</v>
@@ -2081,19 +2077,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="50" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B13" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F13" s="49" t="s">
         <v>27</v>
@@ -2109,19 +2105,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="50" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B14" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="F14" s="49" t="s">
         <v>27</v>
@@ -2137,19 +2133,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="50" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B15" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="F15" s="49" t="s">
         <v>27</v>
@@ -2165,133 +2161,139 @@
     </row>
     <row r="16" spans="1:12" ht="26">
       <c r="A16" s="50" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="I16" s="7"/>
       <c r="J16" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="1:12" ht="38.5">
+    <row r="17" spans="1:12" ht="26">
       <c r="A17" s="50" t="s">
-        <v>206</v>
-      </c>
-      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="49" t="s">
+        <v>324</v>
+      </c>
       <c r="D17" s="8" t="s">
-        <v>49</v>
+        <v>321</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F17" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="9"/>
+      <c r="I17" s="7"/>
       <c r="J17" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="1:12" ht="38.5">
+    <row r="18" spans="1:12">
       <c r="A18" s="50" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B18" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="52" t="s">
+      <c r="C18" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="F18" s="42" t="s">
         <v>318</v>
       </c>
-      <c r="F18" s="42" t="s">
-        <v>316</v>
-      </c>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="K18" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="L18" s="49"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B19" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="42" t="s">
-        <v>250</v>
+      <c r="C19" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>320</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="39"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="39" t="s">
+        <v>12</v>
+      </c>
       <c r="K19" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" ht="38.5">
+    <row r="20" spans="1:12" ht="26">
       <c r="A20" s="50" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="52" t="s">
-        <v>317</v>
+      <c r="C20" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>325</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>27</v>
@@ -2300,7 +2302,7 @@
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
       <c r="J20" s="54" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="K20" s="49" t="s">
         <v>28</v>
@@ -2309,26 +2311,26 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="50" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="49" t="s">
+        <v>50</v>
+      </c>
       <c r="D21" s="8" t="s">
-        <v>54</v>
+        <v>322</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="49" t="s">
-        <v>312</v>
+        <v>327</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>318</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="I21" s="7"/>
       <c r="J21" s="39" t="s">
         <v>13</v>
       </c>
@@ -2339,17 +2341,19 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="50" t="s">
-        <v>208</v>
+        <v>329</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="49" t="s">
+        <v>50</v>
+      </c>
       <c r="D22" s="42" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>26</v>
@@ -2367,17 +2371,17 @@
     </row>
     <row r="23" spans="1:12" ht="38.5">
       <c r="A23" s="50" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>26</v>
@@ -2386,7 +2390,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>28</v>
@@ -2395,17 +2399,17 @@
     </row>
     <row r="24" spans="1:12" ht="26">
       <c r="A24" s="50" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>27</v>
@@ -2414,7 +2418,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>28</v>
@@ -2430,10 +2434,10 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>26</v>
@@ -2442,7 +2446,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="39" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>28</v>
@@ -2451,17 +2455,17 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="50" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>27</v>
@@ -2470,7 +2474,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>28</v>
@@ -2479,28 +2483,28 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="50" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G27" s="46" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="39" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>28</v>
@@ -2509,28 +2513,28 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="50" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="39" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>28</v>
@@ -2539,17 +2543,17 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="50" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>27</v>
@@ -2558,7 +2562,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>28</v>
@@ -2567,17 +2571,17 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="50" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="42" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>27</v>
@@ -2586,7 +2590,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="39" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>28</v>
@@ -2595,28 +2599,28 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="50" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="8" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="39" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>28</v>
@@ -2625,17 +2629,17 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="50" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="42" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>26</v>
@@ -2644,7 +2648,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="39" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>28</v>
@@ -2653,17 +2657,17 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="50" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="42" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>27</v>
@@ -2672,7 +2676,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="39" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>28</v>
@@ -2681,28 +2685,28 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="50" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="8" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="39" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>28</v>
@@ -2711,17 +2715,17 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="50" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="42" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>26</v>
@@ -2730,7 +2734,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="39" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>28</v>
@@ -2739,17 +2743,17 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="50" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="42" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>27</v>
@@ -2758,7 +2762,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="39" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>28</v>
@@ -2767,28 +2771,28 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="50" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="8" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="39" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>28</v>
@@ -2797,17 +2801,17 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="50" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="42" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>26</v>
@@ -2816,7 +2820,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="39" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>28</v>
@@ -2825,17 +2829,17 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="50" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>27</v>
@@ -2844,7 +2848,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>28</v>
@@ -2853,17 +2857,17 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="50" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>26</v>
@@ -2872,7 +2876,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="39" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>28</v>
@@ -2881,17 +2885,17 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="50" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>26</v>
@@ -2902,7 +2906,7 @@
         <v>29</v>
       </c>
       <c r="J41" s="39" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>28</v>
@@ -2911,17 +2915,17 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="50" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>26</v>
@@ -2930,7 +2934,7 @@
       <c r="H42" s="11"/>
       <c r="I42" s="9"/>
       <c r="J42" s="39" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>28</v>
@@ -2939,17 +2943,17 @@
     </row>
     <row r="43" spans="1:12" ht="26">
       <c r="A43" s="50" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>27</v>
@@ -2958,7 +2962,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>28</v>
@@ -2967,26 +2971,26 @@
     </row>
     <row r="44" spans="1:12" ht="26">
       <c r="A44" s="50" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="39" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>28</v>
@@ -2995,17 +2999,17 @@
     </row>
     <row r="45" spans="1:12" ht="26">
       <c r="A45" s="50" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>26</v>
@@ -3014,7 +3018,7 @@
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>28</v>
@@ -3023,17 +3027,17 @@
     </row>
     <row r="46" spans="1:12" ht="26">
       <c r="A46" s="50" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>26</v>
@@ -3042,7 +3046,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>28</v>
@@ -3051,28 +3055,28 @@
     </row>
     <row r="47" spans="1:12" ht="51">
       <c r="A47" s="50" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F47" s="42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>28</v>
@@ -3081,19 +3085,19 @@
     </row>
     <row r="48" spans="1:12" ht="38.5">
       <c r="A48" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>26</v>
@@ -3102,7 +3106,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>28</v>
@@ -3111,19 +3115,19 @@
     </row>
     <row r="49" spans="1:12" ht="51">
       <c r="A49" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="E49" s="13" t="s">
         <v>94</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>26</v>
@@ -3132,7 +3136,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>28</v>
@@ -3141,17 +3145,17 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>27</v>
@@ -3160,7 +3164,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>28</v>
@@ -3169,17 +3173,17 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="50" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>26</v>
@@ -3188,7 +3192,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="39" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>28</v>
@@ -3197,17 +3201,17 @@
     </row>
     <row r="52" spans="1:12" ht="26">
       <c r="A52" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>27</v>
@@ -3216,7 +3220,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>28</v>
@@ -3225,28 +3229,28 @@
     </row>
     <row r="53" spans="1:12" ht="42.5">
       <c r="A53" s="50" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>28</v>
@@ -3255,19 +3259,19 @@
     </row>
     <row r="54" spans="1:12" ht="42.5">
       <c r="A54" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>26</v>
@@ -3276,7 +3280,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>28</v>
@@ -3285,28 +3289,28 @@
     </row>
     <row r="55" spans="1:12" ht="28.5">
       <c r="A55" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F55" s="42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>28</v>
@@ -3315,19 +3319,19 @@
     </row>
     <row r="56" spans="1:12" ht="42.5">
       <c r="A56" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>26</v>
@@ -3336,7 +3340,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>28</v>
@@ -3345,28 +3349,28 @@
     </row>
     <row r="57" spans="1:12" ht="42.5">
       <c r="A57" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F57" s="42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>28</v>
@@ -3375,19 +3379,19 @@
     </row>
     <row r="58" spans="1:12" ht="42.5">
       <c r="A58" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>26</v>
@@ -3396,7 +3400,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>28</v>
@@ -3405,28 +3409,28 @@
     </row>
     <row r="59" spans="1:12" ht="56.5">
       <c r="A59" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F59" s="42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>28</v>
@@ -3435,19 +3439,19 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="50" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D60" s="45" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>26</v>
@@ -3456,7 +3460,7 @@
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>28</v>
@@ -3465,28 +3469,28 @@
     </row>
     <row r="61" spans="1:12" ht="38.5">
       <c r="A61" s="50" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F61" s="42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>28</v>
@@ -3495,19 +3499,19 @@
     </row>
     <row r="62" spans="1:12" ht="26">
       <c r="A62" s="50" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>26</v>
@@ -3516,7 +3520,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>28</v>
@@ -3525,19 +3529,19 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="50" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B63" s="49" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C63" s="49" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>27</v>
@@ -3546,7 +3550,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>28</v>
@@ -3555,19 +3559,19 @@
     </row>
     <row r="64" spans="1:12" ht="51">
       <c r="A64" s="50" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>26</v>
@@ -3576,7 +3580,7 @@
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="39" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>28</v>
@@ -3585,19 +3589,19 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="50" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B65" s="49" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C65" s="49" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>27</v>
@@ -3606,7 +3610,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>28</v>
@@ -3615,19 +3619,19 @@
     </row>
     <row r="66" spans="1:12" ht="51">
       <c r="A66" s="50" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="8" t="s">
-        <v>131</v>
-      </c>
       <c r="E66" s="13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>26</v>
@@ -3636,7 +3640,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="39" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>28</v>
@@ -3645,19 +3649,19 @@
     </row>
     <row r="67" spans="1:12" ht="38.5">
       <c r="A67" s="50" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>27</v>
@@ -3666,7 +3670,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>28</v>
@@ -3675,28 +3679,28 @@
     </row>
     <row r="68" spans="1:12" ht="42.5">
       <c r="A68" s="50" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F68" s="42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="39" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>28</v>
@@ -3705,30 +3709,30 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="50" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>28</v>
@@ -3737,30 +3741,30 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="50" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>28</v>
@@ -3769,28 +3773,28 @@
     </row>
     <row r="71" spans="1:12" ht="51">
       <c r="A71" s="50" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D71" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="E71" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F71" s="42" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>28</v>
@@ -3799,17 +3803,17 @@
     </row>
     <row r="72" spans="1:12" ht="26">
       <c r="A72" s="50" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>27</v>
@@ -3818,7 +3822,7 @@
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>28</v>
@@ -3827,26 +3831,26 @@
     </row>
     <row r="73" spans="1:12" ht="38.5">
       <c r="A73" s="50" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="39" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>28</v>
@@ -3855,26 +3859,26 @@
     </row>
     <row r="74" spans="1:12" ht="26">
       <c r="A74" s="50" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="39" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>28</v>
@@ -3883,17 +3887,17 @@
     </row>
     <row r="75" spans="1:12" ht="26">
       <c r="A75" s="50" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>26</v>
@@ -3902,7 +3906,7 @@
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>28</v>
@@ -3911,17 +3915,17 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="50" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B76" s="49" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>35</v>
@@ -3930,7 +3934,7 @@
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>28</v>
@@ -3939,17 +3943,17 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="50" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>35</v>
@@ -3958,7 +3962,7 @@
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>28</v>
@@ -3967,19 +3971,19 @@
     </row>
     <row r="78" spans="1:12" ht="38.5">
       <c r="A78" s="50" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>35</v>
@@ -3988,7 +3992,7 @@
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>28</v>
@@ -3997,19 +4001,19 @@
     </row>
     <row r="79" spans="1:12" ht="26">
       <c r="A79" s="50" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>26</v>
@@ -4018,7 +4022,7 @@
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>28</v>
@@ -4027,19 +4031,19 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="50" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>35</v>
@@ -4048,7 +4052,7 @@
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>28</v>
@@ -4057,19 +4061,19 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="50" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -4078,7 +4082,7 @@
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>28</v>
@@ -4087,19 +4091,19 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="50" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C82" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="E82" s="27" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>26</v>
@@ -4108,7 +4112,7 @@
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>28</v>
@@ -4117,19 +4121,19 @@
     </row>
     <row r="83" spans="1:12" ht="26">
       <c r="A83" s="50" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>27</v>
@@ -4138,7 +4142,7 @@
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>28</v>
@@ -4150,25 +4154,25 @@
         <v>16</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E84" s="31"/>
       <c r="F84" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G84" s="47" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="39" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>28</v>
@@ -4180,16 +4184,16 @@
         <v>17</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E85" s="27" t="s">
         <v>171</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>176</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>26</v>
@@ -4198,7 +4202,7 @@
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="39" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>28</v>
@@ -4207,17 +4211,17 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="50" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="8" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E86" s="32" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>35</v>
@@ -4226,7 +4230,7 @@
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>28</v>
@@ -4235,14 +4239,14 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="50" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E87" s="9"/>
       <c r="F87" s="7" t="s">
@@ -4252,7 +4256,7 @@
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>28</v>
@@ -4261,17 +4265,17 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="50" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>27</v>
@@ -4280,7 +4284,7 @@
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>28</v>
@@ -4289,17 +4293,17 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="50" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>26</v>
@@ -4308,7 +4312,7 @@
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="39" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>28</v>
@@ -4317,17 +4321,17 @@
     </row>
     <row r="90" spans="1:12" ht="38.5">
       <c r="A90" s="50" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>27</v>
@@ -4336,7 +4340,7 @@
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>28</v>
@@ -4345,17 +4349,17 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="50" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C91" s="12"/>
       <c r="D91" s="27" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>26</v>
@@ -4364,7 +4368,7 @@
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="39" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>28</v>
@@ -4373,17 +4377,17 @@
     </row>
     <row r="92" spans="1:12" ht="38.5">
       <c r="A92" s="50" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C92" s="12"/>
       <c r="D92" s="8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>26</v>
@@ -4392,7 +4396,7 @@
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
       <c r="J92" s="39" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>28</v>
@@ -4401,28 +4405,28 @@
     </row>
     <row r="93" spans="1:12" ht="26">
       <c r="A93" s="50" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F93" s="42" t="s">
         <v>42</v>
       </c>
       <c r="G93" s="42" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>28</v>
@@ -4431,17 +4435,17 @@
     </row>
     <row r="94" spans="1:12" ht="26">
       <c r="A94" s="50" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>27</v>
@@ -4450,7 +4454,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
       <c r="J94" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>28</v>
@@ -4459,17 +4463,17 @@
     </row>
     <row r="95" spans="1:12" ht="51">
       <c r="A95" s="50" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C95" s="33"/>
       <c r="D95" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>26</v>
@@ -4478,7 +4482,7 @@
       <c r="H95" s="11"/>
       <c r="I95" s="15"/>
       <c r="J95" s="53" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>28</v>
@@ -4497,15 +4501,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -4714,6 +4709,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
@@ -4732,14 +4736,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4756,4 +4752,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add dependencies to custom field + some refactoring
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB62EEBE-5A7A-4F17-9658-1005911C28E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8839BA-EE40-4FA7-8583-97975164AF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="330">
   <si>
     <t>Unit</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Multi-Select Dropdown</t>
-  </si>
-  <si>
-    <t>Nachhaltigkeitsbericht</t>
   </si>
   <si>
     <t>Erstellt das Unternehmen Nachhaltigkeits- oder ESG-Berichte?</t>
@@ -1067,6 +1064,9 @@
   </si>
   <si>
     <t>10.2.1.1</t>
+  </si>
+  <si>
+    <t>Nachhaltigkeitsberichte</t>
   </si>
 </sst>
 </file>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1811,10 +1811,10 @@
         <v>36</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>314</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>315</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>37</v>
@@ -1826,7 +1826,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>28</v>
@@ -1835,16 +1835,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>38</v>
@@ -1865,16 +1865,16 @@
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>39</v>
@@ -1901,10 +1901,10 @@
         <v>36</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>40</v>
@@ -1916,7 +1916,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>28</v>
@@ -1931,10 +1931,10 @@
         <v>36</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>312</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>313</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>41</v>
@@ -1943,7 +1943,7 @@
         <v>42</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -1957,19 +1957,19 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>27</v>
@@ -1978,7 +1978,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>28</v>
@@ -1993,24 +1993,24 @@
         <v>36</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="G10" s="42" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>28</v>
@@ -2025,22 +2025,22 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="F11" s="49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7"/>
       <c r="J11" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>28</v>
@@ -2049,19 +2049,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F12" s="49" t="s">
         <v>27</v>
@@ -2071,25 +2071,29 @@
       <c r="I12" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="39"/>
-      <c r="K12" s="9"/>
+      <c r="J12" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F13" s="49" t="s">
         <v>27</v>
@@ -2099,25 +2103,29 @@
       <c r="I13" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="39"/>
-      <c r="K13" s="9"/>
+      <c r="J13" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B14" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F14" s="49" t="s">
         <v>27</v>
@@ -2127,25 +2135,29 @@
       <c r="I14" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="39"/>
-      <c r="K14" s="9"/>
+      <c r="J14" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B15" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F15" s="49" t="s">
         <v>27</v>
@@ -2155,34 +2167,38 @@
       <c r="I15" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="39"/>
-      <c r="K15" s="9"/>
+      <c r="J15" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="26">
       <c r="A16" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
       <c r="I16" s="7"/>
       <c r="J16" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>28</v>
@@ -2197,13 +2213,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>27</v>
@@ -2212,7 +2228,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="7"/>
       <c r="J17" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>28</v>
@@ -2227,16 +2243,16 @@
         <v>36</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>323</v>
-      </c>
       <c r="F18" s="42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -2251,19 +2267,19 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="50" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B19" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>26</v>
@@ -2287,13 +2303,13 @@
         <v>36</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>27</v>
@@ -2302,7 +2318,7 @@
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
       <c r="J20" s="54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K20" s="49" t="s">
         <v>28</v>
@@ -2311,22 +2327,22 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2341,19 +2357,19 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="50" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>26</v>
@@ -2371,17 +2387,17 @@
     </row>
     <row r="23" spans="1:12" ht="38.5">
       <c r="A23" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>52</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>26</v>
@@ -2390,7 +2406,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>28</v>
@@ -2399,17 +2415,17 @@
     </row>
     <row r="24" spans="1:12" ht="26">
       <c r="A24" s="50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>27</v>
@@ -2418,7 +2434,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>28</v>
@@ -2434,10 +2450,10 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>26</v>
@@ -2446,7 +2462,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>28</v>
@@ -2455,17 +2471,17 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>27</v>
@@ -2474,7 +2490,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>28</v>
@@ -2483,28 +2499,28 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="F27" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G27" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>28</v>
@@ -2513,28 +2529,28 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="F28" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>28</v>
@@ -2543,17 +2559,17 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>64</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>27</v>
@@ -2562,7 +2578,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>28</v>
@@ -2571,17 +2587,17 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>27</v>
@@ -2590,7 +2606,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>28</v>
@@ -2599,28 +2615,28 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>28</v>
@@ -2629,17 +2645,17 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>26</v>
@@ -2648,7 +2664,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>28</v>
@@ -2657,17 +2673,17 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>27</v>
@@ -2676,7 +2692,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>28</v>
@@ -2685,28 +2701,28 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="50" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>28</v>
@@ -2715,17 +2731,17 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="50" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>26</v>
@@ -2734,7 +2750,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>28</v>
@@ -2743,17 +2759,17 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="50" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="42" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>27</v>
@@ -2762,7 +2778,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>28</v>
@@ -2771,28 +2787,28 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="50" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>28</v>
@@ -2801,17 +2817,17 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="50" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="42" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>26</v>
@@ -2820,7 +2836,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>28</v>
@@ -2829,17 +2845,17 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>72</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>73</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>27</v>
@@ -2848,7 +2864,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>28</v>
@@ -2857,17 +2873,17 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="50" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>75</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>26</v>
@@ -2876,7 +2892,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>28</v>
@@ -2885,17 +2901,17 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="50" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>26</v>
@@ -2906,7 +2922,7 @@
         <v>29</v>
       </c>
       <c r="J41" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>28</v>
@@ -2915,17 +2931,17 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>26</v>
@@ -2934,7 +2950,7 @@
       <c r="H42" s="11"/>
       <c r="I42" s="9"/>
       <c r="J42" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>28</v>
@@ -2943,17 +2959,17 @@
     </row>
     <row r="43" spans="1:12" ht="26">
       <c r="A43" s="50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>27</v>
@@ -2962,7 +2978,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>28</v>
@@ -2971,26 +2987,26 @@
     </row>
     <row r="44" spans="1:12" ht="26">
       <c r="A44" s="50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="20" t="s">
-        <v>83</v>
-      </c>
       <c r="F44" s="42" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>28</v>
@@ -2999,17 +3015,17 @@
     </row>
     <row r="45" spans="1:12" ht="26">
       <c r="A45" s="50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="19" t="s">
         <v>84</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>85</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>26</v>
@@ -3018,7 +3034,7 @@
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>28</v>
@@ -3027,17 +3043,17 @@
     </row>
     <row r="46" spans="1:12" ht="26">
       <c r="A46" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>26</v>
@@ -3046,7 +3062,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>28</v>
@@ -3055,28 +3071,28 @@
     </row>
     <row r="47" spans="1:12" ht="51">
       <c r="A47" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D47" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="F47" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>28</v>
@@ -3085,19 +3101,19 @@
     </row>
     <row r="48" spans="1:12" ht="38.5">
       <c r="A48" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="D48" s="42" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>26</v>
@@ -3106,7 +3122,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>28</v>
@@ -3115,19 +3131,19 @@
     </row>
     <row r="49" spans="1:12" ht="51">
       <c r="A49" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="D49" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>94</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>26</v>
@@ -3136,7 +3152,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>28</v>
@@ -3145,17 +3161,17 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>96</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>27</v>
@@ -3164,7 +3180,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>28</v>
@@ -3173,17 +3189,17 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>98</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>26</v>
@@ -3192,7 +3208,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>28</v>
@@ -3201,17 +3217,17 @@
     </row>
     <row r="52" spans="1:12" ht="26">
       <c r="A52" s="50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>100</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>27</v>
@@ -3220,7 +3236,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>28</v>
@@ -3229,28 +3245,28 @@
     </row>
     <row r="53" spans="1:12" ht="42.5">
       <c r="A53" s="50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="E53" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E53" s="21" t="s">
-        <v>103</v>
-      </c>
       <c r="F53" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>28</v>
@@ -3259,19 +3275,19 @@
     </row>
     <row r="54" spans="1:12" ht="42.5">
       <c r="A54" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>26</v>
@@ -3280,7 +3296,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>28</v>
@@ -3289,28 +3305,28 @@
     </row>
     <row r="55" spans="1:12" ht="28.5">
       <c r="A55" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C55" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="E55" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="21" t="s">
-        <v>107</v>
-      </c>
       <c r="F55" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>28</v>
@@ -3319,19 +3335,19 @@
     </row>
     <row r="56" spans="1:12" ht="42.5">
       <c r="A56" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>26</v>
@@ -3340,7 +3356,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>28</v>
@@ -3349,28 +3365,28 @@
     </row>
     <row r="57" spans="1:12" ht="42.5">
       <c r="A57" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C57" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="E57" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E57" s="21" t="s">
-        <v>110</v>
-      </c>
       <c r="F57" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>28</v>
@@ -3379,19 +3395,19 @@
     </row>
     <row r="58" spans="1:12" ht="42.5">
       <c r="A58" s="50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>26</v>
@@ -3400,7 +3416,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>28</v>
@@ -3409,28 +3425,28 @@
     </row>
     <row r="59" spans="1:12" ht="56.5">
       <c r="A59" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="E59" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E59" s="21" t="s">
-        <v>113</v>
-      </c>
       <c r="F59" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>28</v>
@@ -3439,19 +3455,19 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D60" s="45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>26</v>
@@ -3460,7 +3476,7 @@
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>28</v>
@@ -3469,28 +3485,28 @@
     </row>
     <row r="61" spans="1:12" ht="38.5">
       <c r="A61" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D61" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E61" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="26" t="s">
-        <v>115</v>
-      </c>
       <c r="F61" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>28</v>
@@ -3499,19 +3515,19 @@
     </row>
     <row r="62" spans="1:12" ht="26">
       <c r="A62" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="E62" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>118</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>26</v>
@@ -3520,7 +3536,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>28</v>
@@ -3529,19 +3545,19 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B63" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D63" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" s="28" t="s">
         <v>119</v>
-      </c>
-      <c r="E63" s="28" t="s">
-        <v>120</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>27</v>
@@ -3550,7 +3566,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>28</v>
@@ -3559,19 +3575,19 @@
     </row>
     <row r="64" spans="1:12" ht="51">
       <c r="A64" s="50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="E64" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>26</v>
@@ -3580,7 +3596,7 @@
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>28</v>
@@ -3589,19 +3605,19 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B65" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C65" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D65" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E65" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="E65" s="29" t="s">
-        <v>125</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>27</v>
@@ -3610,7 +3626,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>28</v>
@@ -3619,19 +3635,19 @@
     </row>
     <row r="66" spans="1:12" ht="51">
       <c r="A66" s="50" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D66" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E66" s="13" t="s">
         <v>126</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>127</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>26</v>
@@ -3640,7 +3656,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>28</v>
@@ -3649,19 +3665,19 @@
     </row>
     <row r="67" spans="1:12" ht="38.5">
       <c r="A67" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="E67" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>27</v>
@@ -3670,7 +3686,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>28</v>
@@ -3679,28 +3695,28 @@
     </row>
     <row r="68" spans="1:12" ht="42.5">
       <c r="A68" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D68" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E68" s="21" t="s">
-        <v>132</v>
-      </c>
       <c r="F68" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>28</v>
@@ -3709,30 +3725,30 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="E69" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E69" s="14" t="s">
-        <v>135</v>
-      </c>
       <c r="F69" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>28</v>
@@ -3741,30 +3757,30 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D70" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" s="13" t="s">
         <v>136</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>137</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>28</v>
@@ -3773,28 +3789,28 @@
     </row>
     <row r="71" spans="1:12" ht="51">
       <c r="A71" s="50" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D71" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E71" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E71" s="10" t="s">
-        <v>139</v>
-      </c>
       <c r="F71" s="42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>28</v>
@@ -3803,17 +3819,17 @@
     </row>
     <row r="72" spans="1:12" ht="26">
       <c r="A72" s="50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E72" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>142</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>27</v>
@@ -3822,7 +3838,7 @@
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>28</v>
@@ -3831,26 +3847,26 @@
     </row>
     <row r="73" spans="1:12" ht="38.5">
       <c r="A73" s="50" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E73" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E73" s="10" t="s">
-        <v>145</v>
-      </c>
       <c r="F73" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>28</v>
@@ -3859,26 +3875,26 @@
     </row>
     <row r="74" spans="1:12" ht="26">
       <c r="A74" s="50" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E74" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E74" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="F74" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>28</v>
@@ -3887,17 +3903,17 @@
     </row>
     <row r="75" spans="1:12" ht="26">
       <c r="A75" s="50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E75" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="E75" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>26</v>
@@ -3906,7 +3922,7 @@
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>28</v>
@@ -3915,17 +3931,17 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B76" s="49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E76" s="30" t="s">
         <v>150</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>151</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>35</v>
@@ -3934,7 +3950,7 @@
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>28</v>
@@ -3943,17 +3959,17 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E77" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>35</v>
@@ -3962,7 +3978,7 @@
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>28</v>
@@ -3971,19 +3987,19 @@
     </row>
     <row r="78" spans="1:12" ht="38.5">
       <c r="A78" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D78" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="E78" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>35</v>
@@ -3992,7 +4008,7 @@
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>28</v>
@@ -4001,19 +4017,19 @@
     </row>
     <row r="79" spans="1:12" ht="26">
       <c r="A79" s="50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D79" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E79" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="E79" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>26</v>
@@ -4022,7 +4038,7 @@
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>28</v>
@@ -4031,19 +4047,19 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="E80" s="10" t="s">
         <v>160</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>161</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>35</v>
@@ -4052,7 +4068,7 @@
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>28</v>
@@ -4061,19 +4077,19 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D81" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E81" s="13" t="s">
         <v>162</v>
-      </c>
-      <c r="E81" s="13" t="s">
-        <v>163</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -4082,7 +4098,7 @@
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>28</v>
@@ -4091,19 +4107,19 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D82" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E82" s="27" t="s">
         <v>164</v>
-      </c>
-      <c r="E82" s="27" t="s">
-        <v>165</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>26</v>
@@ -4112,7 +4128,7 @@
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>28</v>
@@ -4121,19 +4137,19 @@
     </row>
     <row r="83" spans="1:12" ht="26">
       <c r="A83" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C83" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="E83" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="E83" s="13" t="s">
-        <v>168</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>27</v>
@@ -4142,7 +4158,7 @@
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>28</v>
@@ -4154,25 +4170,25 @@
         <v>16</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E84" s="31"/>
       <c r="F84" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G84" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>28</v>
@@ -4184,16 +4200,16 @@
         <v>17</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D85" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E85" s="27" t="s">
         <v>170</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>171</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>26</v>
@@ -4202,7 +4218,7 @@
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>28</v>
@@ -4211,17 +4227,17 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E86" s="32" t="s">
         <v>173</v>
-      </c>
-      <c r="E86" s="32" t="s">
-        <v>174</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>35</v>
@@ -4230,7 +4246,7 @@
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>28</v>
@@ -4239,14 +4255,14 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E87" s="9"/>
       <c r="F87" s="7" t="s">
@@ -4256,7 +4272,7 @@
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>28</v>
@@ -4265,17 +4281,17 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E88" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>27</v>
@@ -4284,7 +4300,7 @@
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>28</v>
@@ -4293,17 +4309,17 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E89" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>26</v>
@@ -4312,7 +4328,7 @@
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>28</v>
@@ -4321,17 +4337,17 @@
     </row>
     <row r="90" spans="1:12" ht="38.5">
       <c r="A90" s="50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E90" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="E90" s="13" t="s">
-        <v>181</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>27</v>
@@ -4340,7 +4356,7 @@
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>28</v>
@@ -4349,17 +4365,17 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="50" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C91" s="12"/>
       <c r="D91" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E91" s="27" t="s">
         <v>182</v>
-      </c>
-      <c r="E91" s="27" t="s">
-        <v>183</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>26</v>
@@ -4368,7 +4384,7 @@
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>28</v>
@@ -4377,17 +4393,17 @@
     </row>
     <row r="92" spans="1:12" ht="38.5">
       <c r="A92" s="50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C92" s="12"/>
       <c r="D92" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>184</v>
-      </c>
-      <c r="E92" s="13" t="s">
-        <v>185</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>26</v>
@@ -4396,7 +4412,7 @@
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
       <c r="J92" s="39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>28</v>
@@ -4405,28 +4421,28 @@
     </row>
     <row r="93" spans="1:12" ht="26">
       <c r="A93" s="50" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E93" s="10" t="s">
         <v>186</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>187</v>
       </c>
       <c r="F93" s="42" t="s">
         <v>42</v>
       </c>
       <c r="G93" s="42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>28</v>
@@ -4435,17 +4451,17 @@
     </row>
     <row r="94" spans="1:12" ht="26">
       <c r="A94" s="50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>188</v>
-      </c>
-      <c r="E94" s="13" t="s">
-        <v>189</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>27</v>
@@ -4454,7 +4470,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
       <c r="J94" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>28</v>
@@ -4463,17 +4479,17 @@
     </row>
     <row r="95" spans="1:12" ht="51">
       <c r="A95" s="50" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C95" s="33"/>
       <c r="D95" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E95" s="13" t="s">
         <v>190</v>
-      </c>
-      <c r="E95" s="13" t="s">
-        <v>191</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>26</v>
@@ -4482,7 +4498,7 @@
       <c r="H95" s="11"/>
       <c r="I95" s="15"/>
       <c r="J95" s="53" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>28</v>
@@ -4491,6 +4507,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
progress on OECD and UGCP
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8839BA-EE40-4FA7-8583-97975164AF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AAEB96-6D1D-4933-AAFE-1518139DC0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1000,9 +1000,6 @@
     <t>Custom - Rolling Window mit vorangestellter Freitext (oder List of Strings) Frage zu den Sektoren</t>
   </si>
   <si>
-    <t>Custom - Tabellencomponent?</t>
-  </si>
-  <si>
     <t>Akkreditierungen</t>
   </si>
   <si>
@@ -1067,6 +1064,9 @@
   </si>
   <si>
     <t>Nachhaltigkeitsberichte</t>
+  </si>
+  <si>
+    <t>Custom - Aufsplitten in mehrere Fragen</t>
   </si>
 </sst>
 </file>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -1811,10 +1811,10 @@
         <v>36</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>314</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>37</v>
@@ -1841,10 +1841,10 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>38</v>
@@ -1871,10 +1871,10 @@
         <v>36</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>39</v>
@@ -1901,10 +1901,10 @@
         <v>36</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>40</v>
@@ -1931,10 +1931,10 @@
         <v>36</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>312</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>41</v>
@@ -1963,10 +1963,10 @@
         <v>36</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>43</v>
@@ -1993,7 +1993,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>44</v>
@@ -2025,7 +2025,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>46</v>
@@ -2034,7 +2034,7 @@
         <v>47</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2055,7 +2055,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D12" s="42" t="s">
         <v>293</v>
@@ -2087,7 +2087,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>294</v>
@@ -2119,7 +2119,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>295</v>
@@ -2151,7 +2151,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>296</v>
@@ -2183,7 +2183,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>305</v>
@@ -2192,7 +2192,7 @@
         <v>301</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
@@ -2213,13 +2213,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>27</v>
@@ -2243,16 +2243,16 @@
         <v>36</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>322</v>
-      </c>
       <c r="F18" s="42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -2267,16 +2267,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="50" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B19" s="51" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>48</v>
@@ -2306,10 +2306,10 @@
         <v>49</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>27</v>
@@ -2336,13 +2336,13 @@
         <v>49</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="50" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>36</v>
@@ -3859,8 +3859,8 @@
       <c r="E73" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="F73" s="7" t="s">
-        <v>307</v>
+      <c r="F73" s="42" t="s">
+        <v>329</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
@@ -3887,7 +3887,7 @@
       <c r="E74" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F74" s="42" t="s">
         <v>304</v>
       </c>
       <c r="G74" s="11"/>
@@ -4239,8 +4239,8 @@
       <c r="E86" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="F86" s="7" t="s">
-        <v>35</v>
+      <c r="F86" s="42" t="s">
+        <v>329</v>
       </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
@@ -4512,12 +4512,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -4726,6 +4720,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4736,23 +4736,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4771,6 +4754,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Progress on reworking excel and fields
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AAEB96-6D1D-4933-AAFE-1518139DC0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ACDBF6-C585-4364-A080-D2F606531405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="342">
   <si>
     <t>Unit</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Ist das Unternehmen berichtspflichtig?</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>Allgemein</t>
   </si>
   <si>
@@ -313,15 +310,6 @@
   </si>
   <si>
     <t>Was waren die kritischen Punkte beim ESG-Rating?</t>
-  </si>
-  <si>
-    <t>Nachhaltigkeitsbezogenen Anleihen</t>
-  </si>
-  <si>
-    <t>Hat das Unternehmen „grüne“, „soziale“ und/oder „nachhaltige“ Schuldtitel begeben oder Sustainability Linked Debt („SLD“) emittiert?</t>
-  </si>
-  <si>
-    <t>Ausstehende Emissionen</t>
   </si>
   <si>
     <t>Bitte geben Sie Details zu den ausstehenden Emissionen für das letzte Jahr der Berichterstattung an (in Mio €).</t>
@@ -697,9 +685,6 @@
     <t>15</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -988,9 +973,6 @@
     <t>In welchen Zeitabständen werden die Berichte erstellt?</t>
   </si>
   <si>
-    <t>Custom - Sollte in mehrere Fragen aufgebrochen werden =&gt; Ausstehende Emissionen einmal für "Nachhaltige Emissionen" und für "SLD" =&gt; Dann kann beides jeweils ein DecimalField mit € als (feste) unit sein</t>
-  </si>
-  <si>
     <t>Custom - Rolling Window</t>
   </si>
   <si>
@@ -1067,6 +1049,60 @@
   </si>
   <si>
     <t>Custom - Aufsplitten in mehrere Fragen</t>
+  </si>
+  <si>
+    <t>Sonstige</t>
+  </si>
+  <si>
+    <t>Rechtsstreitigkeiten</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Anleihen</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Sustainibility Linked Debt</t>
+  </si>
+  <si>
+    <t>Custom - Reuse rolling window?</t>
+  </si>
+  <si>
+    <t>Führungsstandards</t>
+  </si>
+  <si>
+    <t>Risiken</t>
+  </si>
+  <si>
+    <t>Grüne, soziale und/oder nachhaltige Emissionen</t>
+  </si>
+  <si>
+    <t>Ausstehende grüne, soziale und/oder nachhaltige Emissionen</t>
+  </si>
+  <si>
+    <t>Ausstehende Sustainibility Linked Debt</t>
+  </si>
+  <si>
+    <t>Hat das Unternehmen „grüne“, „soziale“ und/oder „nachhaltige“ Schuldtitel begeben?</t>
+  </si>
+  <si>
+    <t>Hat das Unternehmen Sustainability Linked Debt („SLD“) emittiert?</t>
+  </si>
+  <si>
+    <t>16.1.1</t>
+  </si>
+  <si>
+    <t>16.2</t>
+  </si>
+  <si>
+    <t>16.2.1</t>
+  </si>
+  <si>
+    <t>Produktion</t>
   </si>
 </sst>
 </file>
@@ -1363,9 +1399,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1477,6 +1510,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1694,25 +1730,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="36"/>
+    <col min="1" max="1" width="12.54296875" style="35"/>
     <col min="3" max="3" width="22.26953125" customWidth="1"/>
     <col min="4" max="4" width="62.6328125" customWidth="1"/>
     <col min="5" max="5" width="85.54296875" customWidth="1"/>
     <col min="6" max="6" width="65.54296875" customWidth="1"/>
     <col min="7" max="7" width="31.6328125" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" style="36"/>
+    <col min="10" max="10" width="12.54296875" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1739,7 +1775,7 @@
       <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="36" t="s">
         <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1750,8 +1786,8 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="35" t="s">
-        <v>191</v>
+      <c r="A2" s="34" t="s">
+        <v>187</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1765,20 +1801,20 @@
       <c r="E2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="11"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="38"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="9"/>
-      <c r="L2" s="49" t="s">
+      <c r="L2" s="48" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1796,28 +1832,28 @@
       <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="42"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="38"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="9"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="26">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>27</v>
@@ -1825,8 +1861,8 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="39" t="s">
-        <v>191</v>
+      <c r="J4" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>28</v>
@@ -1834,20 +1870,20 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="41" t="s">
-        <v>192</v>
+      <c r="A5" s="40" t="s">
+        <v>188</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>26</v>
@@ -1855,7 +1891,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="38" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="9" t="s">
@@ -1864,20 +1900,20 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="26">
-      <c r="A6" s="35" t="s">
-        <v>193</v>
+      <c r="A6" s="34" t="s">
+        <v>189</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>26</v>
@@ -1885,7 +1921,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="38" t="s">
         <v>7</v>
       </c>
       <c r="K6" s="9" t="s">
@@ -1894,20 +1930,20 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="26">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>27</v>
@@ -1915,8 +1951,8 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="39" t="s">
-        <v>191</v>
+      <c r="J7" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>28</v>
@@ -1924,30 +1960,30 @@
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="26">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>263</v>
+      <c r="G8" s="47" t="s">
+        <v>258</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="38" t="s">
         <v>8</v>
       </c>
       <c r="K8" s="9" t="s">
@@ -1956,20 +1992,20 @@
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="35" t="s">
-        <v>194</v>
+      <c r="A9" s="34" t="s">
+        <v>190</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>27</v>
@@ -1977,8 +2013,8 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="39" t="s">
-        <v>191</v>
+      <c r="J9" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>28</v>
@@ -1986,31 +2022,31 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="42" t="s">
-        <v>258</v>
+      <c r="G10" s="41" t="s">
+        <v>253</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="39" t="s">
-        <v>194</v>
+      <c r="J10" s="38" t="s">
+        <v>190</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>28</v>
@@ -2018,187 +2054,187 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="34" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="49" t="s">
-        <v>316</v>
+      <c r="F11" s="48" t="s">
+        <v>310</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="49" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>294</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="50" t="s">
+      <c r="B15" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" ht="26">
+      <c r="A16" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="B12" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>307</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>297</v>
-      </c>
-      <c r="F12" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>307</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>294</v>
-      </c>
-      <c r="E13" s="52" t="s">
-        <v>298</v>
-      </c>
-      <c r="F13" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="50" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>307</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>295</v>
-      </c>
-      <c r="E14" s="52" t="s">
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="F14" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="50" t="s">
-        <v>198</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>307</v>
-      </c>
-      <c r="D15" s="42" t="s">
+      <c r="E16" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="E15" s="52" t="s">
-        <v>300</v>
-      </c>
-      <c r="F15" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" ht="26">
-      <c r="A16" s="50" t="s">
-        <v>199</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>307</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F16" s="42" t="s">
-        <v>316</v>
+      <c r="F16" s="41" t="s">
+        <v>310</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="39" t="s">
-        <v>191</v>
+      <c r="J16" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>28</v>
@@ -2206,29 +2242,29 @@
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" ht="26">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>322</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="F17" s="42" t="s">
+      <c r="B17" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>313</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>311</v>
+      </c>
+      <c r="F17" s="41" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="11"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="39" t="s">
-        <v>191</v>
+      <c r="J17" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>28</v>
@@ -2236,28 +2272,28 @@
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>322</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="F18" s="42" t="s">
+      <c r="B18" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="48" t="s">
         <v>316</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>315</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>310</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="38" t="s">
         <v>12</v>
       </c>
       <c r="K18" s="9" t="s">
@@ -2266,28 +2302,28 @@
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="50" t="s">
-        <v>326</v>
-      </c>
-      <c r="B19" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>322</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="42" t="s">
+      <c r="A19" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>312</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="41" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="11"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="38" t="s">
         <v>12</v>
       </c>
       <c r="K19" s="9" t="s">
@@ -2296,58 +2332,58 @@
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" ht="26">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="F20" s="42" t="s">
+      <c r="B20" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="F20" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="54" t="s">
-        <v>191</v>
-      </c>
-      <c r="K20" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" s="49"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="K20" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="48"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="50" t="s">
-        <v>200</v>
+      <c r="A21" s="49" t="s">
+        <v>196</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>316</v>
+        <v>35</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>310</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="38" t="s">
         <v>13</v>
       </c>
       <c r="K21" s="9" t="s">
@@ -2356,20 +2392,20 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="50" t="s">
-        <v>327</v>
+      <c r="A22" s="49" t="s">
+        <v>321</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>242</v>
-      </c>
-      <c r="E22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="48" t="s">
         <v>48</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>47</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>26</v>
@@ -2377,7 +2413,7 @@
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="39" t="s">
+      <c r="J22" s="38" t="s">
         <v>13</v>
       </c>
       <c r="K22" s="9" t="s">
@@ -2386,18 +2422,20 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" ht="38.5">
-      <c r="A23" s="50" t="s">
-        <v>201</v>
+      <c r="A23" s="49" t="s">
+        <v>197</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>324</v>
+      </c>
       <c r="D23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>26</v>
@@ -2405,8 +2443,8 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="39" t="s">
-        <v>191</v>
+      <c r="J23" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>28</v>
@@ -2414,18 +2452,20 @@
       <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12" ht="26">
-      <c r="A24" s="50" t="s">
-        <v>202</v>
+      <c r="A24" s="49" t="s">
+        <v>198</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>324</v>
+      </c>
       <c r="D24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>27</v>
@@ -2433,8 +2473,8 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="39" t="s">
-        <v>191</v>
+      <c r="J24" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>28</v>
@@ -2442,18 +2482,20 @@
       <c r="L24" s="9"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>324</v>
+      </c>
       <c r="D25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>26</v>
@@ -2461,8 +2503,8 @@
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="39" t="s">
-        <v>202</v>
+      <c r="J25" s="38" t="s">
+        <v>198</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>28</v>
@@ -2470,18 +2512,20 @@
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="50" t="s">
-        <v>203</v>
+      <c r="A26" s="49" t="s">
+        <v>199</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>331</v>
+      </c>
       <c r="D26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>57</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>27</v>
@@ -2489,8 +2533,8 @@
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="39" t="s">
-        <v>191</v>
+      <c r="J26" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>28</v>
@@ -2498,29 +2542,31 @@
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" ht="26">
-      <c r="A27" s="50" t="s">
-        <v>265</v>
+      <c r="A27" s="49" t="s">
+        <v>260</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>331</v>
+      </c>
       <c r="D27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="F27" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="46" t="s">
-        <v>257</v>
+        <v>44</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>252</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="39" t="s">
-        <v>203</v>
+      <c r="J27" s="38" t="s">
+        <v>199</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>28</v>
@@ -2528,29 +2574,31 @@
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="1:12" ht="26">
-      <c r="A28" s="50" t="s">
-        <v>266</v>
+      <c r="A28" s="49" t="s">
+        <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>331</v>
+      </c>
       <c r="D28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="F28" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>257</v>
+        <v>44</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>252</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="39" t="s">
-        <v>203</v>
+      <c r="J28" s="38" t="s">
+        <v>199</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>28</v>
@@ -2558,18 +2606,20 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" ht="26">
-      <c r="A29" s="50" t="s">
-        <v>204</v>
+      <c r="A29" s="49" t="s">
+        <v>200</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>325</v>
+      </c>
       <c r="D29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>27</v>
@@ -2577,8 +2627,8 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="39" t="s">
-        <v>191</v>
+      <c r="J29" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>28</v>
@@ -2586,18 +2636,20 @@
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="50" t="s">
-        <v>267</v>
+      <c r="A30" s="49" t="s">
+        <v>262</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="42" t="s">
-        <v>246</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>64</v>
+        <v>35</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>27</v>
@@ -2605,8 +2657,8 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="39" t="s">
-        <v>204</v>
+      <c r="J30" s="38" t="s">
+        <v>200</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>28</v>
@@ -2614,29 +2666,31 @@
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="50" t="s">
-        <v>268</v>
+      <c r="A31" s="49" t="s">
+        <v>263</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>325</v>
+      </c>
       <c r="D31" s="8" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="39" t="s">
-        <v>267</v>
+      <c r="J31" s="38" t="s">
+        <v>262</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>28</v>
@@ -2644,18 +2698,20 @@
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="50" t="s">
-        <v>269</v>
+      <c r="A32" s="49" t="s">
+        <v>264</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="42" t="s">
-        <v>243</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>66</v>
+        <v>35</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>26</v>
@@ -2663,8 +2719,8 @@
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
-      <c r="J32" s="39" t="s">
-        <v>267</v>
+      <c r="J32" s="38" t="s">
+        <v>262</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>28</v>
@@ -2672,18 +2728,20 @@
       <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="50" t="s">
-        <v>270</v>
+      <c r="A33" s="49" t="s">
+        <v>265</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>67</v>
+        <v>35</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>27</v>
@@ -2691,8 +2749,8 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="39" t="s">
-        <v>204</v>
+      <c r="J33" s="38" t="s">
+        <v>200</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>28</v>
@@ -2700,29 +2758,31 @@
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="50" t="s">
-        <v>271</v>
+      <c r="A34" s="49" t="s">
+        <v>266</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>325</v>
+      </c>
       <c r="D34" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>259</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="39" t="s">
-        <v>270</v>
+      <c r="J34" s="38" t="s">
+        <v>265</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>28</v>
@@ -2730,18 +2790,20 @@
       <c r="L34" s="9"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="50" t="s">
-        <v>272</v>
+      <c r="A35" s="49" t="s">
+        <v>267</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="42" t="s">
-        <v>244</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>66</v>
+        <v>35</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>26</v>
@@ -2749,8 +2811,8 @@
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="39" t="s">
-        <v>270</v>
+      <c r="J35" s="38" t="s">
+        <v>265</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>28</v>
@@ -2758,18 +2820,20 @@
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="50" t="s">
-        <v>273</v>
+      <c r="A36" s="49" t="s">
+        <v>268</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="42" t="s">
-        <v>248</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>27</v>
@@ -2777,8 +2841,8 @@
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
-      <c r="J36" s="39" t="s">
-        <v>204</v>
+      <c r="J36" s="38" t="s">
+        <v>200</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>28</v>
@@ -2786,29 +2850,31 @@
       <c r="L36" s="9"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="50" t="s">
-        <v>274</v>
+      <c r="A37" s="49" t="s">
+        <v>269</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>325</v>
+      </c>
       <c r="D37" s="8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
-      <c r="J37" s="39" t="s">
-        <v>273</v>
+      <c r="J37" s="38" t="s">
+        <v>268</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>28</v>
@@ -2816,18 +2882,20 @@
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="50" t="s">
-        <v>275</v>
+      <c r="A38" s="49" t="s">
+        <v>270</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="42" t="s">
-        <v>245</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>66</v>
+        <v>35</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>26</v>
@@ -2835,8 +2903,8 @@
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
-      <c r="J38" s="39" t="s">
-        <v>273</v>
+      <c r="J38" s="38" t="s">
+        <v>268</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>28</v>
@@ -2844,18 +2912,20 @@
       <c r="L38" s="9"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="50" t="s">
-        <v>205</v>
+      <c r="A39" s="49" t="s">
+        <v>201</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>326</v>
+      </c>
       <c r="D39" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>71</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>72</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>27</v>
@@ -2863,8 +2933,8 @@
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="39" t="s">
-        <v>191</v>
+      <c r="J39" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>28</v>
@@ -2872,18 +2942,20 @@
       <c r="L39" s="9"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="50" t="s">
-        <v>276</v>
+      <c r="A40" s="49" t="s">
+        <v>271</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>326</v>
+      </c>
       <c r="D40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>73</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>74</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>26</v>
@@ -2891,8 +2963,8 @@
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
-      <c r="J40" s="39" t="s">
-        <v>205</v>
+      <c r="J40" s="38" t="s">
+        <v>201</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>28</v>
@@ -2900,18 +2972,20 @@
       <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="50" t="s">
-        <v>277</v>
+      <c r="A41" s="49" t="s">
+        <v>272</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>326</v>
+      </c>
       <c r="D41" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>75</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>76</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>26</v>
@@ -2921,8 +2995,8 @@
       <c r="I41" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J41" s="39" t="s">
-        <v>205</v>
+      <c r="J41" s="38" t="s">
+        <v>201</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>28</v>
@@ -2930,18 +3004,20 @@
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="50" t="s">
-        <v>278</v>
+      <c r="A42" s="49" t="s">
+        <v>273</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>326</v>
+      </c>
       <c r="D42" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>26</v>
@@ -2949,27 +3025,29 @@
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
       <c r="I42" s="9"/>
-      <c r="J42" s="39" t="s">
-        <v>205</v>
+      <c r="J42" s="38" t="s">
+        <v>201</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L42" s="9"/>
     </row>
-    <row r="43" spans="1:12" ht="26">
-      <c r="A43" s="50" t="s">
-        <v>206</v>
+    <row r="43" spans="1:12">
+      <c r="A43" s="49" t="s">
+        <v>274</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="D43" s="8" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>80</v>
+        <v>336</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>27</v>
@@ -2977,8 +3055,8 @@
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
-      <c r="J43" s="39" t="s">
-        <v>191</v>
+      <c r="J43" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>28</v>
@@ -2986,55 +3064,59 @@
       <c r="L43" s="9"/>
     </row>
     <row r="44" spans="1:12" ht="26">
-      <c r="A44" s="50" t="s">
-        <v>279</v>
+      <c r="A44" s="49" t="s">
+        <v>338</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="D44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F44" s="42" t="s">
-        <v>303</v>
+        <v>334</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" s="41" t="s">
+        <v>328</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
-      <c r="J44" s="39" t="s">
-        <v>206</v>
+      <c r="J44" s="38" t="s">
+        <v>274</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="9"/>
     </row>
-    <row r="45" spans="1:12" ht="26">
-      <c r="A45" s="50" t="s">
-        <v>207</v>
+    <row r="45" spans="1:12">
+      <c r="A45" s="49" t="s">
+        <v>339</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="D45" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>84</v>
+        <v>329</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>337</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
-      <c r="J45" s="39" t="s">
-        <v>191</v>
+      <c r="J45" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>28</v>
@@ -3042,78 +3124,80 @@
       <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12" ht="26">
-      <c r="A46" s="50" t="s">
-        <v>208</v>
+      <c r="A46" s="49" t="s">
+        <v>340</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="D46" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>26</v>
+        <v>335</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" s="41" t="s">
+        <v>328</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
-      <c r="J46" s="39" t="s">
-        <v>191</v>
+      <c r="J46" s="38" t="s">
+        <v>339</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L46" s="9"/>
     </row>
-    <row r="47" spans="1:12" ht="51">
-      <c r="A47" s="50" t="s">
-        <v>209</v>
+    <row r="47" spans="1:12" ht="26">
+      <c r="A47" s="49" t="s">
+        <v>202</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>88</v>
+        <v>35</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>332</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F47" s="42" t="s">
-        <v>304</v>
+        <v>79</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
-      <c r="J47" s="39" t="s">
-        <v>191</v>
+      <c r="J47" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L47" s="9"/>
     </row>
-    <row r="48" spans="1:12" ht="38.5">
-      <c r="A48" s="50" t="s">
-        <v>210</v>
+    <row r="48" spans="1:12" ht="26">
+      <c r="A48" s="49" t="s">
+        <v>203</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>249</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>91</v>
+        <v>35</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>26</v>
@@ -3121,8 +3205,8 @@
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
-      <c r="J48" s="39" t="s">
-        <v>191</v>
+      <c r="J48" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>28</v>
@@ -3130,76 +3214,80 @@
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="51">
-      <c r="A49" s="50" t="s">
-        <v>211</v>
+      <c r="A49" s="49" t="s">
+        <v>204</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>26</v>
+        <v>85</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="41" t="s">
+        <v>298</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
-      <c r="J49" s="39" t="s">
-        <v>191</v>
+      <c r="J49" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L49" s="9"/>
     </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="50" t="s">
-        <v>212</v>
+    <row r="50" spans="1:12" ht="38.5">
+      <c r="A50" s="49" t="s">
+        <v>205</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E50" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>95</v>
-      </c>
       <c r="F50" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
-      <c r="J50" s="39" t="s">
-        <v>191</v>
+      <c r="J50" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="50" t="s">
-        <v>280</v>
+    <row r="51" spans="1:12" ht="51">
+      <c r="A51" s="49" t="s">
+        <v>206</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C51" s="12"/>
+        <v>83</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D51" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>26</v>
@@ -3207,27 +3295,29 @@
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
-      <c r="J51" s="39" t="s">
-        <v>212</v>
+      <c r="J51" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L51" s="9"/>
     </row>
-    <row r="52" spans="1:12" ht="26">
-      <c r="A52" s="50" t="s">
-        <v>213</v>
+    <row r="52" spans="1:12">
+      <c r="A52" s="49" t="s">
+        <v>207</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="12"/>
+        <v>83</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>341</v>
+      </c>
       <c r="D52" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>27</v>
@@ -3235,98 +3325,98 @@
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
-      <c r="J52" s="39" t="s">
-        <v>191</v>
+      <c r="J52" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="1:12" ht="42.5">
-      <c r="A53" s="50" t="s">
-        <v>214</v>
+    <row r="53" spans="1:12">
+      <c r="A53" s="49" t="s">
+        <v>275</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>100</v>
+        <v>83</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>341</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="F53" s="42" t="s">
-        <v>304</v>
+        <v>92</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
-      <c r="J53" s="39" t="s">
-        <v>191</v>
+      <c r="J53" s="38" t="s">
+        <v>207</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="1:12" ht="42.5">
-      <c r="A54" s="50" t="s">
-        <v>215</v>
+    <row r="54" spans="1:12" ht="26">
+      <c r="A54" s="49" t="s">
+        <v>208</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D54" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
-      <c r="J54" s="39" t="s">
-        <v>191</v>
+      <c r="J54" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L54" s="9"/>
     </row>
-    <row r="55" spans="1:12" ht="28.5">
-      <c r="A55" s="50" t="s">
-        <v>216</v>
+    <row r="55" spans="1:12" ht="42.5">
+      <c r="A55" s="49" t="s">
+        <v>209</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="F55" s="42" t="s">
-        <v>304</v>
+        <v>97</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F55" s="41" t="s">
+        <v>298</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
-      <c r="J55" s="39" t="s">
-        <v>191</v>
+      <c r="J55" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>28</v>
@@ -3334,20 +3424,20 @@
       <c r="L55" s="9"/>
     </row>
     <row r="56" spans="1:12" ht="42.5">
-      <c r="A56" s="50" t="s">
-        <v>217</v>
+      <c r="A56" s="49" t="s">
+        <v>210</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D56" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="E56" s="23" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="D56" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>26</v>
@@ -3355,38 +3445,38 @@
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
-      <c r="J56" s="39" t="s">
-        <v>191</v>
+      <c r="J56" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:12" ht="42.5">
-      <c r="A57" s="50" t="s">
-        <v>218</v>
+    <row r="57" spans="1:12" ht="28.5">
+      <c r="A57" s="49" t="s">
+        <v>211</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="E57" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F57" s="42" t="s">
-        <v>304</v>
+        <v>100</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="41" t="s">
+        <v>298</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
-      <c r="J57" s="39" t="s">
-        <v>191</v>
+      <c r="J57" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>28</v>
@@ -3394,20 +3484,20 @@
       <c r="L57" s="9"/>
     </row>
     <row r="58" spans="1:12" ht="42.5">
-      <c r="A58" s="50" t="s">
-        <v>219</v>
+      <c r="A58" s="49" t="s">
+        <v>212</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>250</v>
-      </c>
-      <c r="E58" s="23" t="s">
-        <v>103</v>
+        <v>247</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>26</v>
@@ -3415,59 +3505,59 @@
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
-      <c r="J58" s="39" t="s">
-        <v>191</v>
+      <c r="J58" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L58" s="9"/>
     </row>
-    <row r="59" spans="1:12" ht="56.5">
-      <c r="A59" s="50" t="s">
-        <v>220</v>
+    <row r="59" spans="1:12" ht="42.5">
+      <c r="A59" s="49" t="s">
+        <v>213</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F59" s="42" t="s">
-        <v>304</v>
+        <v>103</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F59" s="41" t="s">
+        <v>298</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
-      <c r="J59" s="39" t="s">
-        <v>191</v>
+      <c r="J59" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L59" s="9"/>
     </row>
-    <row r="60" spans="1:12">
-      <c r="A60" s="50" t="s">
-        <v>221</v>
+    <row r="60" spans="1:12" ht="42.5">
+      <c r="A60" s="49" t="s">
+        <v>214</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" s="45" t="s">
-        <v>253</v>
-      </c>
-      <c r="E60" s="24" t="s">
         <v>103</v>
+      </c>
+      <c r="D60" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>26</v>
@@ -3475,59 +3565,59 @@
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
-      <c r="J60" s="39" t="s">
-        <v>191</v>
+      <c r="J60" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:12" ht="38.5">
-      <c r="A61" s="50" t="s">
-        <v>222</v>
+    <row r="61" spans="1:12" ht="56.5">
+      <c r="A61" s="49" t="s">
+        <v>215</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E61" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="F61" s="42" t="s">
-        <v>304</v>
+        <v>106</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="41" t="s">
+        <v>298</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
-      <c r="J61" s="39" t="s">
-        <v>191</v>
+      <c r="J61" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L61" s="9"/>
     </row>
-    <row r="62" spans="1:12" ht="26">
-      <c r="A62" s="50" t="s">
-        <v>223</v>
+    <row r="62" spans="1:12">
+      <c r="A62" s="49" t="s">
+        <v>216</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>117</v>
+        <v>106</v>
+      </c>
+      <c r="D62" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>26</v>
@@ -3535,59 +3625,59 @@
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
-      <c r="J62" s="39" t="s">
-        <v>191</v>
+      <c r="J62" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L62" s="9"/>
     </row>
-    <row r="63" spans="1:12">
-      <c r="A63" s="50" t="s">
-        <v>224</v>
-      </c>
-      <c r="B63" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E63" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>27</v>
+    <row r="63" spans="1:12" ht="38.5">
+      <c r="A63" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" s="41" t="s">
+        <v>298</v>
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
-      <c r="J63" s="39" t="s">
-        <v>191</v>
+      <c r="J63" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L63" s="9"/>
     </row>
-    <row r="64" spans="1:12" ht="51">
-      <c r="A64" s="50" t="s">
-        <v>281</v>
+    <row r="64" spans="1:12" ht="26">
+      <c r="A64" s="49" t="s">
+        <v>218</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>26</v>
@@ -3595,8 +3685,8 @@
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
-      <c r="J64" s="39" t="s">
-        <v>224</v>
+      <c r="J64" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>28</v>
@@ -3604,20 +3694,20 @@
       <c r="L64" s="9"/>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="50" t="s">
-        <v>225</v>
-      </c>
-      <c r="B65" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="E65" s="29" t="s">
-        <v>124</v>
+      <c r="A65" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>27</v>
@@ -3625,8 +3715,8 @@
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
-      <c r="J65" s="39" t="s">
-        <v>191</v>
+      <c r="J65" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>28</v>
@@ -3634,20 +3724,20 @@
       <c r="L65" s="9"/>
     </row>
     <row r="66" spans="1:12" ht="51">
-      <c r="A66" s="50" t="s">
-        <v>282</v>
+      <c r="A66" s="49" t="s">
+        <v>276</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>26</v>
@@ -3655,29 +3745,29 @@
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
-      <c r="J66" s="39" t="s">
-        <v>225</v>
+      <c r="J66" s="38" t="s">
+        <v>219</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L66" s="9"/>
     </row>
-    <row r="67" spans="1:12" ht="38.5">
-      <c r="A67" s="50" t="s">
-        <v>226</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>129</v>
+    <row r="67" spans="1:12">
+      <c r="A67" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B67" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E67" s="28" t="s">
+        <v>120</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>27</v>
@@ -3685,188 +3775,192 @@
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
-      <c r="J67" s="39" t="s">
-        <v>191</v>
+      <c r="J67" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L67" s="9"/>
     </row>
-    <row r="68" spans="1:12" ht="42.5">
-      <c r="A68" s="50" t="s">
-        <v>142</v>
+    <row r="68" spans="1:12" ht="51">
+      <c r="A68" s="49" t="s">
+        <v>277</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E68" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F68" s="42" t="s">
-        <v>304</v>
+        <v>121</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
-      <c r="J68" s="39" t="s">
-        <v>226</v>
+      <c r="J68" s="38" t="s">
+        <v>220</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="9"/>
     </row>
-    <row r="69" spans="1:12">
-      <c r="A69" s="50" t="s">
-        <v>227</v>
+    <row r="69" spans="1:12" ht="38.5">
+      <c r="A69" s="49" t="s">
+        <v>221</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>134</v>
+        <v>124</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>262</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G69" s="11"/>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
-      <c r="J69" s="39" t="s">
-        <v>191</v>
+      <c r="J69" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L69" s="9"/>
     </row>
-    <row r="70" spans="1:12">
-      <c r="A70" s="50" t="s">
-        <v>228</v>
+    <row r="70" spans="1:12" ht="42.5">
+      <c r="A70" s="49" t="s">
+        <v>138</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>264</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="F70" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="G70" s="11"/>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
-      <c r="J70" s="39" t="s">
-        <v>191</v>
+      <c r="J70" s="38" t="s">
+        <v>221</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:12" ht="51">
-      <c r="A71" s="50" t="s">
-        <v>229</v>
+    <row r="71" spans="1:12">
+      <c r="A71" s="49" t="s">
+        <v>222</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F71" s="42" t="s">
-        <v>306</v>
-      </c>
-      <c r="G71" s="11"/>
+        <v>129</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>257</v>
+      </c>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
-      <c r="J71" s="39" t="s">
-        <v>191</v>
+      <c r="J71" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L71" s="9"/>
     </row>
-    <row r="72" spans="1:12" ht="26">
-      <c r="A72" s="50" t="s">
-        <v>230</v>
+    <row r="72" spans="1:12">
+      <c r="A72" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C72" s="12"/>
+        <v>83</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="D72" s="8" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G72" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>259</v>
+      </c>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
-      <c r="J72" s="39" t="s">
-        <v>191</v>
+      <c r="J72" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="9"/>
     </row>
-    <row r="73" spans="1:12" ht="38.5">
-      <c r="A73" s="50" t="s">
-        <v>283</v>
+    <row r="73" spans="1:12" ht="51">
+      <c r="A73" s="49" t="s">
+        <v>224</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C73" s="12"/>
+        <v>83</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="D73" s="8" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F73" s="42" t="s">
-        <v>329</v>
+        <v>134</v>
+      </c>
+      <c r="F73" s="41" t="s">
+        <v>300</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
-      <c r="J73" s="39" t="s">
-        <v>230</v>
+      <c r="J73" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>28</v>
@@ -3874,83 +3968,83 @@
       <c r="L73" s="9"/>
     </row>
     <row r="74" spans="1:12" ht="26">
-      <c r="A74" s="50" t="s">
-        <v>284</v>
+      <c r="A74" s="49" t="s">
+        <v>225</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F74" s="42" t="s">
-        <v>304</v>
+        <v>136</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
-      <c r="J74" s="39" t="s">
-        <v>230</v>
+      <c r="J74" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L74" s="9"/>
     </row>
-    <row r="75" spans="1:12" ht="26">
-      <c r="A75" s="50" t="s">
-        <v>231</v>
+    <row r="75" spans="1:12" ht="38.5">
+      <c r="A75" s="49" t="s">
+        <v>278</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E75" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>26</v>
+        <v>139</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F75" s="41" t="s">
+        <v>323</v>
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
-      <c r="J75" s="39" t="s">
-        <v>191</v>
+      <c r="J75" s="38" t="s">
+        <v>225</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L75" s="9"/>
     </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="50" t="s">
-        <v>232</v>
-      </c>
-      <c r="B76" s="49" t="s">
-        <v>139</v>
+    <row r="76" spans="1:12" ht="26">
+      <c r="A76" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>35</v>
+        <v>141</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F76" s="41" t="s">
+        <v>298</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
-      <c r="J76" s="39" t="s">
-        <v>191</v>
+      <c r="J76" s="38" t="s">
+        <v>225</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>28</v>
@@ -3958,57 +4052,55 @@
       <c r="L76" s="9"/>
     </row>
     <row r="77" spans="1:12" ht="26">
-      <c r="A77" s="50" t="s">
-        <v>233</v>
+      <c r="A77" s="49" t="s">
+        <v>226</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
-      <c r="J77" s="39" t="s">
-        <v>191</v>
+      <c r="J77" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L77" s="9"/>
     </row>
-    <row r="78" spans="1:12" ht="38.5">
-      <c r="A78" s="50" t="s">
-        <v>234</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>153</v>
-      </c>
+    <row r="78" spans="1:12">
+      <c r="A78" s="49" t="s">
+        <v>227</v>
+      </c>
+      <c r="B78" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="12"/>
       <c r="D78" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>35</v>
+        <v>145</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="F78" s="41" t="s">
+        <v>330</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
-      <c r="J78" s="39" t="s">
-        <v>191</v>
+      <c r="J78" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>28</v>
@@ -4016,80 +4108,78 @@
       <c r="L78" s="9"/>
     </row>
     <row r="79" spans="1:12" ht="26">
-      <c r="A79" s="50" t="s">
-        <v>235</v>
+      <c r="A79" s="49" t="s">
+        <v>228</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>153</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C79" s="12"/>
       <c r="D79" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E79" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>26</v>
+        <v>147</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F79" s="41" t="s">
+        <v>330</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
-      <c r="J79" s="39" t="s">
-        <v>191</v>
+      <c r="J79" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L79" s="9"/>
     </row>
-    <row r="80" spans="1:12" ht="26">
-      <c r="A80" s="50" t="s">
-        <v>236</v>
+    <row r="80" spans="1:12" ht="38.5">
+      <c r="A80" s="49" t="s">
+        <v>229</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>35</v>
+        <v>151</v>
+      </c>
+      <c r="F80" s="41" t="s">
+        <v>330</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
-      <c r="J80" s="39" t="s">
-        <v>191</v>
+      <c r="J80" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="9"/>
     </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="50" t="s">
-        <v>237</v>
+    <row r="81" spans="1:12" ht="26">
+      <c r="A81" s="49" t="s">
+        <v>230</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -4097,68 +4187,68 @@
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
-      <c r="J81" s="39" t="s">
-        <v>191</v>
+      <c r="J81" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L81" s="9"/>
     </row>
-    <row r="82" spans="1:12">
-      <c r="A82" s="50" t="s">
-        <v>238</v>
+    <row r="82" spans="1:12" ht="26">
+      <c r="A82" s="49" t="s">
+        <v>231</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E82" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>26</v>
+        <v>155</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F82" s="41" t="s">
+        <v>323</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
-      <c r="J82" s="39" t="s">
-        <v>191</v>
+      <c r="J82" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L82" s="9"/>
     </row>
-    <row r="83" spans="1:12" ht="26">
-      <c r="A83" s="50" t="s">
-        <v>239</v>
+    <row r="83" spans="1:12">
+      <c r="A83" s="49" t="s">
+        <v>232</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
-      <c r="J83" s="39" t="s">
-        <v>191</v>
+      <c r="J83" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>28</v>
@@ -4166,59 +4256,59 @@
       <c r="L83" s="9"/>
     </row>
     <row r="84" spans="1:12">
-      <c r="A84" s="50" t="s">
-        <v>16</v>
+      <c r="A84" s="49" t="s">
+        <v>233</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E84" s="31"/>
+        <v>159</v>
+      </c>
+      <c r="E84" s="26" t="s">
+        <v>160</v>
+      </c>
       <c r="F84" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G84" s="47" t="s">
-        <v>260</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
-      <c r="J84" s="39" t="s">
-        <v>239</v>
+      <c r="J84" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L84" s="9"/>
     </row>
-    <row r="85" spans="1:12">
-      <c r="A85" s="50" t="s">
-        <v>17</v>
+    <row r="85" spans="1:12" ht="26">
+      <c r="A85" s="49" t="s">
+        <v>234</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>170</v>
+        <v>162</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>163</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
-      <c r="J85" s="39" t="s">
-        <v>239</v>
+      <c r="J85" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>28</v>
@@ -4226,27 +4316,29 @@
       <c r="L85" s="9"/>
     </row>
     <row r="86" spans="1:12">
-      <c r="A86" s="50" t="s">
-        <v>240</v>
+      <c r="A86" s="49" t="s">
+        <v>16</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C86" s="12"/>
+        <v>135</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="D86" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E86" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="F86" s="42" t="s">
-        <v>329</v>
-      </c>
-      <c r="G86" s="11"/>
+        <v>164</v>
+      </c>
+      <c r="E86" s="30"/>
+      <c r="F86" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G86" s="46" t="s">
+        <v>255</v>
+      </c>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
-      <c r="J86" s="39" t="s">
-        <v>191</v>
+      <c r="J86" s="38" t="s">
+        <v>234</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>28</v>
@@ -4254,25 +4346,29 @@
       <c r="L86" s="9"/>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="50" t="s">
-        <v>241</v>
+      <c r="A87" s="49" t="s">
+        <v>17</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C87" s="12"/>
+        <v>135</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="D87" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E87" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="E87" s="26" t="s">
+        <v>166</v>
+      </c>
       <c r="F87" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
-      <c r="J87" s="39" t="s">
-        <v>191</v>
+      <c r="J87" s="38" t="s">
+        <v>234</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>28</v>
@@ -4280,27 +4376,27 @@
       <c r="L87" s="9"/>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="50" t="s">
-        <v>285</v>
+      <c r="A88" s="49" t="s">
+        <v>235</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>27</v>
+        <v>168</v>
+      </c>
+      <c r="E88" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="F88" s="41" t="s">
+        <v>323</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
-      <c r="J88" s="39" t="s">
-        <v>191</v>
+      <c r="J88" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>28</v>
@@ -4308,46 +4404,44 @@
       <c r="L88" s="9"/>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="50" t="s">
-        <v>286</v>
+      <c r="A89" s="49" t="s">
+        <v>236</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>178</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E89" s="9"/>
       <c r="F89" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
-      <c r="J89" s="39" t="s">
-        <v>285</v>
+      <c r="J89" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L89" s="9"/>
     </row>
-    <row r="90" spans="1:12" ht="38.5">
-      <c r="A90" s="50" t="s">
-        <v>287</v>
+    <row r="90" spans="1:12">
+      <c r="A90" s="49" t="s">
+        <v>280</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E90" s="13" t="s">
-        <v>180</v>
+        <v>171</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>27</v>
@@ -4355,8 +4449,8 @@
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
-      <c r="J90" s="39" t="s">
-        <v>191</v>
+      <c r="J90" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>28</v>
@@ -4364,18 +4458,18 @@
       <c r="L90" s="9"/>
     </row>
     <row r="91" spans="1:12">
-      <c r="A91" s="50" t="s">
-        <v>288</v>
+      <c r="A91" s="49" t="s">
+        <v>281</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C91" s="12"/>
-      <c r="D91" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E91" s="27" t="s">
-        <v>182</v>
+      <c r="D91" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>26</v>
@@ -4383,8 +4477,8 @@
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
-      <c r="J91" s="39" t="s">
-        <v>287</v>
+      <c r="J91" s="38" t="s">
+        <v>280</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>28</v>
@@ -4392,118 +4486,174 @@
       <c r="L91" s="9"/>
     </row>
     <row r="92" spans="1:12" ht="38.5">
-      <c r="A92" s="50" t="s">
-        <v>289</v>
+      <c r="A92" s="49" t="s">
+        <v>282</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C92" s="12"/>
       <c r="D92" s="8" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
-      <c r="J92" s="39" t="s">
-        <v>287</v>
+      <c r="J92" s="38" t="s">
+        <v>187</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L92" s="9"/>
     </row>
-    <row r="93" spans="1:12" ht="26">
-      <c r="A93" s="50" t="s">
-        <v>290</v>
+    <row r="93" spans="1:12">
+      <c r="A93" s="49" t="s">
+        <v>283</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C93" s="12"/>
-      <c r="D93" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="F93" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G93" s="42" t="s">
-        <v>261</v>
-      </c>
+      <c r="D93" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E93" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93" s="11"/>
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
-      <c r="J93" s="39" t="s">
-        <v>191</v>
+      <c r="J93" s="38" t="s">
+        <v>282</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L93" s="9"/>
     </row>
-    <row r="94" spans="1:12" ht="26">
-      <c r="A94" s="50" t="s">
-        <v>291</v>
+    <row r="94" spans="1:12" ht="38.5">
+      <c r="A94" s="49" t="s">
+        <v>284</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="8" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
-      <c r="J94" s="39" t="s">
-        <v>191</v>
+      <c r="J94" s="38" t="s">
+        <v>282</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L94" s="9"/>
     </row>
-    <row r="95" spans="1:12" ht="51">
-      <c r="A95" s="50" t="s">
-        <v>292</v>
+    <row r="95" spans="1:12" ht="26">
+      <c r="A95" s="49" t="s">
+        <v>285</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C95" s="33"/>
+        <v>167</v>
+      </c>
+      <c r="C95" s="12"/>
       <c r="D95" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E95" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="F95" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F95" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="G95" s="41" t="s">
+        <v>256</v>
+      </c>
+      <c r="H95" s="11"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L95" s="9"/>
+    </row>
+    <row r="96" spans="1:12" ht="26">
+      <c r="A96" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C96" s="12"/>
+      <c r="D96" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="K96" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L96" s="9"/>
+    </row>
+    <row r="97" spans="1:12" ht="51">
+      <c r="A97" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C97" s="32"/>
+      <c r="D97" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="F97" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="15"/>
-      <c r="J95" s="53" t="s">
-        <v>291</v>
-      </c>
-      <c r="K95" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L95" s="9"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="52" t="s">
+        <v>286</v>
+      </c>
+      <c r="K97" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L97" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4512,6 +4662,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -4720,12 +4876,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4736,6 +4886,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4754,23 +4921,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
progress on custom fields oecd and ungcp
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ACDBF6-C585-4364-A080-D2F606531405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DD210C-5E0D-4F70-8C56-C977959055EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="343">
   <si>
     <t>Unit</t>
   </si>
@@ -790,9 +790,6 @@
     <t>51</t>
   </si>
   <si>
-    <t>Erklärung OECD</t>
-  </si>
-  <si>
     <t>Einzelheiten zu den Rechtsstreitigkeiten zu E</t>
   </si>
   <si>
@@ -1015,15 +1012,6 @@
     <t>Verfügt das Unternehmen über Prozesse und Compliance-Mechanismen, um die Einhaltung der Prinzipien des UN Global Compact zu überwachen?</t>
   </si>
   <si>
-    <t xml:space="preserve">Erklärung der Einhaltung </t>
-  </si>
-  <si>
-    <t>Mechanismen zur Überwachung der Einhaltung der UN Global Compact Prinzipien</t>
-  </si>
-  <si>
-    <t>Richtlinien zur Einhaltung</t>
-  </si>
-  <si>
     <t>Bitte teilen Sie die Richtlinien mit uns die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der UN Global Compact Prinzipien überwacht.</t>
   </si>
   <si>
@@ -1103,6 +1091,21 @@
   </si>
   <si>
     <t>Produktion</t>
+  </si>
+  <si>
+    <t>Mechanismen zur Überwachung der Einhaltung der UNGCP</t>
+  </si>
+  <si>
+    <t>Richtlinien zur Einhaltung der UNGCP</t>
+  </si>
+  <si>
+    <t>Erklärung der Einhaltung der UNGCP</t>
+  </si>
+  <si>
+    <t>Richtlinien zur Einhaltung der OECD-Leitsätze</t>
+  </si>
+  <si>
+    <t>Erklärung der Einhaltung der OECD-Leitsätze</t>
   </si>
 </sst>
 </file>
@@ -1732,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -1847,10 +1850,10 @@
         <v>35</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>307</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>36</v>
@@ -1877,10 +1880,10 @@
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>37</v>
@@ -1907,10 +1910,10 @@
         <v>35</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>38</v>
@@ -1937,10 +1940,10 @@
         <v>35</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>39</v>
@@ -1967,10 +1970,10 @@
         <v>35</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>304</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>305</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>40</v>
@@ -1979,7 +1982,7 @@
         <v>41</v>
       </c>
       <c r="G8" s="47" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -1999,10 +2002,10 @@
         <v>35</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>42</v>
@@ -2029,19 +2032,19 @@
         <v>35</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>44</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
@@ -2061,7 +2064,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>45</v>
@@ -2070,7 +2073,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2091,13 +2094,13 @@
         <v>35</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E12" s="51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F12" s="48" t="s">
         <v>27</v>
@@ -2123,13 +2126,13 @@
         <v>35</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F13" s="48" t="s">
         <v>27</v>
@@ -2155,13 +2158,13 @@
         <v>35</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F14" s="48" t="s">
         <v>27</v>
@@ -2187,13 +2190,13 @@
         <v>35</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F15" s="48" t="s">
         <v>27</v>
@@ -2219,16 +2222,16 @@
         <v>35</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
@@ -2249,13 +2252,13 @@
         <v>35</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F17" s="41" t="s">
         <v>27</v>
@@ -2279,16 +2282,16 @@
         <v>35</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -2303,16 +2306,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="49" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="E19" s="54" t="s">
         <v>47</v>
@@ -2342,10 +2345,10 @@
         <v>48</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F20" s="41" t="s">
         <v>27</v>
@@ -2372,13 +2375,13 @@
         <v>48</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>314</v>
+        <v>341</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2393,7 +2396,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="49" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>35</v>
@@ -2402,7 +2405,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="E22" s="54" t="s">
         <v>47</v>
@@ -2429,7 +2432,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>49</v>
@@ -2459,7 +2462,7 @@
         <v>35</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>51</v>
@@ -2489,7 +2492,7 @@
         <v>35</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>53</v>
@@ -2519,7 +2522,7 @@
         <v>35</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>55</v>
@@ -2543,13 +2546,13 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>57</v>
@@ -2561,7 +2564,7 @@
         <v>44</v>
       </c>
       <c r="G27" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
@@ -2575,13 +2578,13 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>59</v>
@@ -2593,7 +2596,7 @@
         <v>44</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
@@ -2613,7 +2616,7 @@
         <v>35</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>61</v>
@@ -2637,16 +2640,16 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>63</v>
@@ -2667,16 +2670,16 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="49" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>64</v>
@@ -2685,12 +2688,12 @@
         <v>44</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>28</v>
@@ -2699,16 +2702,16 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>65</v>
@@ -2720,7 +2723,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>28</v>
@@ -2729,16 +2732,16 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>66</v>
@@ -2759,16 +2762,16 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>67</v>
@@ -2777,12 +2780,12 @@
         <v>44</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>28</v>
@@ -2791,16 +2794,16 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>65</v>
@@ -2812,7 +2815,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>28</v>
@@ -2821,16 +2824,16 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>68</v>
@@ -2851,16 +2854,16 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="49" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>69</v>
@@ -2869,12 +2872,12 @@
         <v>44</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>28</v>
@@ -2883,16 +2886,16 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>65</v>
@@ -2904,7 +2907,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>28</v>
@@ -2919,7 +2922,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>70</v>
@@ -2943,13 +2946,13 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>72</v>
@@ -2973,13 +2976,13 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>74</v>
@@ -3005,13 +3008,13 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>76</v>
@@ -3035,19 +3038,19 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="49" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>27</v>
@@ -3065,28 +3068,28 @@
     </row>
     <row r="44" spans="1:12" ht="26">
       <c r="A44" s="49" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>78</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>28</v>
@@ -3095,19 +3098,19 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="49" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>27</v>
@@ -3125,28 +3128,28 @@
     </row>
     <row r="46" spans="1:12" ht="26">
       <c r="A46" s="49" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>78</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="38" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>28</v>
@@ -3161,7 +3164,7 @@
         <v>35</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>79</v>
@@ -3191,7 +3194,7 @@
         <v>35</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>81</v>
@@ -3230,7 +3233,7 @@
         <v>86</v>
       </c>
       <c r="F49" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -3254,7 +3257,7 @@
         <v>84</v>
       </c>
       <c r="D50" s="41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>87</v>
@@ -3311,7 +3314,7 @@
         <v>83</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>90</v>
@@ -3335,13 +3338,13 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="49" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>92</v>
@@ -3371,7 +3374,7 @@
         <v>83</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>94</v>
@@ -3410,7 +3413,7 @@
         <v>98</v>
       </c>
       <c r="F55" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
@@ -3434,7 +3437,7 @@
         <v>96</v>
       </c>
       <c r="D56" s="41" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E56" s="21" t="s">
         <v>99</v>
@@ -3470,7 +3473,7 @@
         <v>102</v>
       </c>
       <c r="F57" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
@@ -3494,7 +3497,7 @@
         <v>100</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E58" s="22" t="s">
         <v>99</v>
@@ -3530,7 +3533,7 @@
         <v>105</v>
       </c>
       <c r="F59" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -3554,7 +3557,7 @@
         <v>103</v>
       </c>
       <c r="D60" s="42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E60" s="22" t="s">
         <v>99</v>
@@ -3590,7 +3593,7 @@
         <v>108</v>
       </c>
       <c r="F61" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
@@ -3614,7 +3617,7 @@
         <v>106</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E62" s="23" t="s">
         <v>99</v>
@@ -3650,7 +3653,7 @@
         <v>110</v>
       </c>
       <c r="F63" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -3725,7 +3728,7 @@
     </row>
     <row r="66" spans="1:12" ht="51">
       <c r="A66" s="49" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>83</v>
@@ -3785,7 +3788,7 @@
     </row>
     <row r="68" spans="1:12" ht="51">
       <c r="A68" s="49" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>83</v>
@@ -3860,7 +3863,7 @@
         <v>127</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
@@ -3893,7 +3896,7 @@
         <v>44</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
@@ -3925,7 +3928,7 @@
         <v>41</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
@@ -3954,7 +3957,7 @@
         <v>134</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
@@ -3997,7 +4000,7 @@
     </row>
     <row r="75" spans="1:12" ht="38.5">
       <c r="A75" s="49" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>135</v>
@@ -4010,7 +4013,7 @@
         <v>140</v>
       </c>
       <c r="F75" s="41" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
@@ -4025,7 +4028,7 @@
     </row>
     <row r="76" spans="1:12" ht="26">
       <c r="A76" s="49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>135</v>
@@ -4038,7 +4041,7 @@
         <v>142</v>
       </c>
       <c r="F76" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
@@ -4094,7 +4097,7 @@
         <v>146</v>
       </c>
       <c r="F78" s="41" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
@@ -4122,7 +4125,7 @@
         <v>148</v>
       </c>
       <c r="F79" s="41" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
@@ -4152,7 +4155,7 @@
         <v>151</v>
       </c>
       <c r="F80" s="41" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
@@ -4212,7 +4215,7 @@
         <v>156</v>
       </c>
       <c r="F82" s="41" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
@@ -4333,7 +4336,7 @@
         <v>44</v>
       </c>
       <c r="G86" s="46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
@@ -4390,7 +4393,7 @@
         <v>169</v>
       </c>
       <c r="F88" s="41" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -4431,7 +4434,7 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="49" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>167</v>
@@ -4459,7 +4462,7 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>167</v>
@@ -4478,7 +4481,7 @@
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>28</v>
@@ -4487,7 +4490,7 @@
     </row>
     <row r="92" spans="1:12" ht="38.5">
       <c r="A92" s="49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>167</v>
@@ -4515,7 +4518,7 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="49" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>167</v>
@@ -4534,7 +4537,7 @@
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>28</v>
@@ -4543,7 +4546,7 @@
     </row>
     <row r="94" spans="1:12" ht="38.5">
       <c r="A94" s="49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>167</v>
@@ -4562,7 +4565,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
       <c r="J94" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>28</v>
@@ -4571,7 +4574,7 @@
     </row>
     <row r="95" spans="1:12" ht="26">
       <c r="A95" s="49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>167</v>
@@ -4587,7 +4590,7 @@
         <v>41</v>
       </c>
       <c r="G95" s="41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H95" s="11"/>
       <c r="I95" s="9"/>
@@ -4601,7 +4604,7 @@
     </row>
     <row r="96" spans="1:12" ht="26">
       <c r="A96" s="49" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>167</v>
@@ -4629,7 +4632,7 @@
     </row>
     <row r="97" spans="1:12" ht="51">
       <c r="A97" s="49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>167</v>
@@ -4648,7 +4651,7 @@
       <c r="H97" s="11"/>
       <c r="I97" s="15"/>
       <c r="J97" s="52" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K97" s="9" t="s">
         <v>28</v>
@@ -4668,6 +4671,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -4876,15 +4888,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
@@ -4903,6 +4906,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4919,12 +4930,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
more structuring of subcategories
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DD210C-5E0D-4F70-8C56-C977959055EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292D799D-DF90-4362-90B2-784A8E9F1BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="341">
   <si>
     <t>Unit</t>
   </si>
@@ -412,9 +412,6 @@
 recyceltes wiederverwertetes Material) im Produktionsprozess für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre.</t>
   </si>
   <si>
-    <t>Gefährliche Abfälle</t>
-  </si>
-  <si>
     <t>Gefährlicher Abfall</t>
   </si>
   <si>
@@ -974,9 +971,6 @@
   </si>
   <si>
     <t>Weitere Akkreditierungen</t>
-  </si>
-  <si>
-    <t>Custom - Rolling Window mit vorangestellter Freitext (oder List of Strings) Frage zu den Sektoren</t>
   </si>
   <si>
     <t>Akkreditierungen</t>
@@ -1735,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -1790,7 +1784,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1850,10 +1844,10 @@
         <v>35</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>36</v>
@@ -1865,7 +1859,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>28</v>
@@ -1874,16 +1868,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>37</v>
@@ -1904,16 +1898,16 @@
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>307</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>38</v>
@@ -1940,10 +1934,10 @@
         <v>35</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>39</v>
@@ -1955,7 +1949,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>28</v>
@@ -1970,10 +1964,10 @@
         <v>35</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>40</v>
@@ -1982,7 +1976,7 @@
         <v>41</v>
       </c>
       <c r="G8" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -1996,16 +1990,16 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>42</v>
@@ -2017,7 +2011,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>28</v>
@@ -2032,24 +2026,24 @@
         <v>35</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>44</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>28</v>
@@ -2064,7 +2058,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>45</v>
@@ -2073,13 +2067,13 @@
         <v>46</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7"/>
       <c r="J11" s="38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>28</v>
@@ -2088,19 +2082,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E12" s="51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F12" s="48" t="s">
         <v>27</v>
@@ -2111,7 +2105,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>28</v>
@@ -2120,19 +2114,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F13" s="48" t="s">
         <v>27</v>
@@ -2143,7 +2137,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>28</v>
@@ -2152,19 +2146,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F14" s="48" t="s">
         <v>27</v>
@@ -2175,7 +2169,7 @@
         <v>29</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>28</v>
@@ -2184,19 +2178,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F15" s="48" t="s">
         <v>27</v>
@@ -2207,7 +2201,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>28</v>
@@ -2216,28 +2210,28 @@
     </row>
     <row r="16" spans="1:12" ht="26">
       <c r="A16" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
       <c r="I16" s="7"/>
       <c r="J16" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>28</v>
@@ -2252,13 +2246,13 @@
         <v>35</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F17" s="41" t="s">
         <v>27</v>
@@ -2267,7 +2261,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="7"/>
       <c r="J17" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>28</v>
@@ -2282,16 +2276,16 @@
         <v>35</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -2306,16 +2300,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="49" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E19" s="54" t="s">
         <v>47</v>
@@ -2345,10 +2339,10 @@
         <v>48</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F20" s="41" t="s">
         <v>27</v>
@@ -2357,7 +2351,7 @@
       <c r="H20" s="48"/>
       <c r="I20" s="48"/>
       <c r="J20" s="53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K20" s="48" t="s">
         <v>28</v>
@@ -2366,7 +2360,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>35</v>
@@ -2375,13 +2369,13 @@
         <v>48</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2396,7 +2390,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="49" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>35</v>
@@ -2405,7 +2399,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E22" s="54" t="s">
         <v>47</v>
@@ -2426,13 +2420,13 @@
     </row>
     <row r="23" spans="1:12" ht="38.5">
       <c r="A23" s="49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>49</v>
@@ -2447,7 +2441,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>28</v>
@@ -2456,13 +2450,13 @@
     </row>
     <row r="24" spans="1:12" ht="26">
       <c r="A24" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>51</v>
@@ -2477,7 +2471,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>28</v>
@@ -2492,7 +2486,7 @@
         <v>35</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>53</v>
@@ -2507,7 +2501,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>28</v>
@@ -2516,13 +2510,13 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>55</v>
@@ -2537,7 +2531,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>28</v>
@@ -2546,13 +2540,13 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="49" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>57</v>
@@ -2564,12 +2558,12 @@
         <v>44</v>
       </c>
       <c r="G27" s="45" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>28</v>
@@ -2578,13 +2572,13 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>59</v>
@@ -2596,12 +2590,12 @@
         <v>44</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>28</v>
@@ -2610,13 +2604,13 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>61</v>
@@ -2631,7 +2625,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>28</v>
@@ -2640,16 +2634,16 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>63</v>
@@ -2661,7 +2655,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>28</v>
@@ -2670,16 +2664,16 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>64</v>
@@ -2688,12 +2682,12 @@
         <v>44</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>28</v>
@@ -2702,16 +2696,16 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="49" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>65</v>
@@ -2723,7 +2717,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>28</v>
@@ -2732,16 +2726,16 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>66</v>
@@ -2753,7 +2747,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>28</v>
@@ -2762,16 +2756,16 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>67</v>
@@ -2780,12 +2774,12 @@
         <v>44</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>28</v>
@@ -2794,16 +2788,16 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>65</v>
@@ -2815,7 +2809,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>28</v>
@@ -2824,16 +2818,16 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>68</v>
@@ -2845,7 +2839,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>28</v>
@@ -2854,16 +2848,16 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>69</v>
@@ -2872,12 +2866,12 @@
         <v>44</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>28</v>
@@ -2886,16 +2880,16 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="49" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>65</v>
@@ -2907,7 +2901,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>28</v>
@@ -2916,13 +2910,13 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>70</v>
@@ -2937,7 +2931,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>28</v>
@@ -2946,13 +2940,13 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>72</v>
@@ -2967,7 +2961,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>28</v>
@@ -2976,13 +2970,13 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>74</v>
@@ -2999,7 +2993,7 @@
         <v>29</v>
       </c>
       <c r="J41" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>28</v>
@@ -3008,13 +3002,13 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>76</v>
@@ -3029,7 +3023,7 @@
       <c r="H42" s="11"/>
       <c r="I42" s="9"/>
       <c r="J42" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>28</v>
@@ -3038,19 +3032,19 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>27</v>
@@ -3059,7 +3053,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>28</v>
@@ -3068,28 +3062,28 @@
     </row>
     <row r="44" spans="1:12" ht="26">
       <c r="A44" s="49" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>78</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>28</v>
@@ -3098,19 +3092,19 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="49" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>325</v>
-      </c>
       <c r="E45" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>27</v>
@@ -3119,7 +3113,7 @@
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>28</v>
@@ -3128,28 +3122,28 @@
     </row>
     <row r="46" spans="1:12" ht="26">
       <c r="A46" s="49" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>78</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="38" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>28</v>
@@ -3158,13 +3152,13 @@
     </row>
     <row r="47" spans="1:12" ht="26">
       <c r="A47" s="49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>79</v>
@@ -3179,7 +3173,7 @@
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>28</v>
@@ -3188,13 +3182,13 @@
     </row>
     <row r="48" spans="1:12" ht="26">
       <c r="A48" s="49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>81</v>
@@ -3209,7 +3203,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>28</v>
@@ -3218,7 +3212,7 @@
     </row>
     <row r="49" spans="1:12" ht="51">
       <c r="A49" s="49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>83</v>
@@ -3233,13 +3227,13 @@
         <v>86</v>
       </c>
       <c r="F49" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>28</v>
@@ -3248,7 +3242,7 @@
     </row>
     <row r="50" spans="1:12" ht="38.5">
       <c r="A50" s="49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>83</v>
@@ -3257,7 +3251,7 @@
         <v>84</v>
       </c>
       <c r="D50" s="41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>87</v>
@@ -3269,7 +3263,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>28</v>
@@ -3278,7 +3272,7 @@
     </row>
     <row r="51" spans="1:12" ht="51">
       <c r="A51" s="49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>83</v>
@@ -3299,7 +3293,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>28</v>
@@ -3308,13 +3302,13 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>90</v>
@@ -3329,7 +3323,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>28</v>
@@ -3338,13 +3332,13 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="49" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>92</v>
@@ -3359,7 +3353,7 @@
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="38" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>28</v>
@@ -3368,13 +3362,13 @@
     </row>
     <row r="54" spans="1:12" ht="26">
       <c r="A54" s="49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>94</v>
@@ -3389,7 +3383,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>28</v>
@@ -3398,7 +3392,7 @@
     </row>
     <row r="55" spans="1:12" ht="42.5">
       <c r="A55" s="49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>83</v>
@@ -3413,13 +3407,13 @@
         <v>98</v>
       </c>
       <c r="F55" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>28</v>
@@ -3428,7 +3422,7 @@
     </row>
     <row r="56" spans="1:12" ht="42.5">
       <c r="A56" s="49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>83</v>
@@ -3437,7 +3431,7 @@
         <v>96</v>
       </c>
       <c r="D56" s="41" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E56" s="21" t="s">
         <v>99</v>
@@ -3449,7 +3443,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>28</v>
@@ -3458,7 +3452,7 @@
     </row>
     <row r="57" spans="1:12" ht="28.5">
       <c r="A57" s="49" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>83</v>
@@ -3473,13 +3467,13 @@
         <v>102</v>
       </c>
       <c r="F57" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>28</v>
@@ -3488,7 +3482,7 @@
     </row>
     <row r="58" spans="1:12" ht="42.5">
       <c r="A58" s="49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>83</v>
@@ -3497,7 +3491,7 @@
         <v>100</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E58" s="22" t="s">
         <v>99</v>
@@ -3509,7 +3503,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>28</v>
@@ -3518,7 +3512,7 @@
     </row>
     <row r="59" spans="1:12" ht="42.5">
       <c r="A59" s="49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>83</v>
@@ -3533,13 +3527,13 @@
         <v>105</v>
       </c>
       <c r="F59" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>28</v>
@@ -3548,7 +3542,7 @@
     </row>
     <row r="60" spans="1:12" ht="42.5">
       <c r="A60" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>83</v>
@@ -3557,7 +3551,7 @@
         <v>103</v>
       </c>
       <c r="D60" s="42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E60" s="22" t="s">
         <v>99</v>
@@ -3569,7 +3563,7 @@
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>28</v>
@@ -3578,7 +3572,7 @@
     </row>
     <row r="61" spans="1:12" ht="56.5">
       <c r="A61" s="49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>83</v>
@@ -3593,13 +3587,13 @@
         <v>108</v>
       </c>
       <c r="F61" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>28</v>
@@ -3608,7 +3602,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="49" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>83</v>
@@ -3617,7 +3611,7 @@
         <v>106</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E62" s="23" t="s">
         <v>99</v>
@@ -3629,7 +3623,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>28</v>
@@ -3638,7 +3632,7 @@
     </row>
     <row r="63" spans="1:12" ht="38.5">
       <c r="A63" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>83</v>
@@ -3653,13 +3647,13 @@
         <v>110</v>
       </c>
       <c r="F63" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>28</v>
@@ -3668,19 +3662,19 @@
     </row>
     <row r="64" spans="1:12" ht="26">
       <c r="A64" s="49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C64" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D64" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="E64" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>26</v>
@@ -3689,7 +3683,7 @@
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>28</v>
@@ -3698,19 +3692,19 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B65" s="48" t="s">
         <v>83</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D65" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="E65" s="27" t="s">
         <v>114</v>
-      </c>
-      <c r="E65" s="27" t="s">
-        <v>115</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>27</v>
@@ -3719,7 +3713,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>28</v>
@@ -3728,19 +3722,19 @@
     </row>
     <row r="66" spans="1:12" ht="51">
       <c r="A66" s="49" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="E66" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>118</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>26</v>
@@ -3749,7 +3743,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>28</v>
@@ -3758,19 +3752,19 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B67" s="48" t="s">
         <v>83</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D67" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" s="28" t="s">
         <v>119</v>
-      </c>
-      <c r="E67" s="28" t="s">
-        <v>120</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>27</v>
@@ -3779,7 +3773,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>28</v>
@@ -3788,19 +3782,19 @@
     </row>
     <row r="68" spans="1:12" ht="51">
       <c r="A68" s="49" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D68" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E68" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="E68" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>26</v>
@@ -3809,7 +3803,7 @@
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>28</v>
@@ -3818,19 +3812,19 @@
     </row>
     <row r="69" spans="1:12" ht="38.5">
       <c r="A69" s="49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="E69" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="E69" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>27</v>
@@ -3839,7 +3833,7 @@
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>28</v>
@@ -3848,28 +3842,28 @@
     </row>
     <row r="70" spans="1:12" ht="42.5">
       <c r="A70" s="49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D70" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="E70" s="20" t="s">
-        <v>127</v>
-      </c>
       <c r="F70" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>28</v>
@@ -3878,30 +3872,30 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="49" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="E71" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>130</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>44</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>28</v>
@@ -3910,30 +3904,30 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D72" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E72" s="13" t="s">
         <v>131</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>132</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>28</v>
@@ -3942,28 +3936,28 @@
     </row>
     <row r="73" spans="1:12" ht="51">
       <c r="A73" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D73" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E73" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="F73" s="41" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>28</v>
@@ -3972,17 +3966,17 @@
     </row>
     <row r="74" spans="1:12" ht="26">
       <c r="A74" s="49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E74" s="13" t="s">
         <v>136</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>137</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>27</v>
@@ -3991,7 +3985,7 @@
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>28</v>
@@ -4000,26 +3994,26 @@
     </row>
     <row r="75" spans="1:12" ht="38.5">
       <c r="A75" s="49" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E75" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E75" s="10" t="s">
-        <v>140</v>
-      </c>
       <c r="F75" s="41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>28</v>
@@ -4028,26 +4022,26 @@
     </row>
     <row r="76" spans="1:12" ht="26">
       <c r="A76" s="49" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E76" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E76" s="10" t="s">
-        <v>142</v>
-      </c>
       <c r="F76" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>28</v>
@@ -4056,17 +4050,17 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E77" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="E77" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>26</v>
@@ -4075,7 +4069,7 @@
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>28</v>
@@ -4084,26 +4078,26 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B78" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C78" s="12"/>
       <c r="D78" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E78" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="E78" s="29" t="s">
-        <v>146</v>
-      </c>
       <c r="F78" s="41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>28</v>
@@ -4112,26 +4106,26 @@
     </row>
     <row r="79" spans="1:12" ht="26">
       <c r="A79" s="49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C79" s="12"/>
       <c r="D79" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E79" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E79" s="10" t="s">
-        <v>148</v>
-      </c>
       <c r="F79" s="41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>28</v>
@@ -4140,28 +4134,28 @@
     </row>
     <row r="80" spans="1:12" ht="38.5">
       <c r="A80" s="49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="E80" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E80" s="10" t="s">
-        <v>151</v>
-      </c>
       <c r="F80" s="41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>28</v>
@@ -4170,19 +4164,19 @@
     </row>
     <row r="81" spans="1:12" ht="26">
       <c r="A81" s="49" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D81" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E81" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="E81" s="13" t="s">
-        <v>153</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -4191,7 +4185,7 @@
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>28</v>
@@ -4200,28 +4194,28 @@
     </row>
     <row r="82" spans="1:12" ht="26">
       <c r="A82" s="49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C82" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="E82" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E82" s="10" t="s">
-        <v>156</v>
-      </c>
       <c r="F82" s="41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>28</v>
@@ -4230,19 +4224,19 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D83" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E83" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="E83" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>26</v>
@@ -4251,7 +4245,7 @@
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>28</v>
@@ -4260,19 +4254,19 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D84" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E84" s="26" t="s">
         <v>159</v>
-      </c>
-      <c r="E84" s="26" t="s">
-        <v>160</v>
       </c>
       <c r="F84" s="7" t="s">
         <v>26</v>
@@ -4281,7 +4275,7 @@
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>28</v>
@@ -4290,19 +4284,19 @@
     </row>
     <row r="85" spans="1:12" ht="26">
       <c r="A85" s="49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="E85" s="13" t="s">
         <v>162</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>163</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>27</v>
@@ -4311,7 +4305,7 @@
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>28</v>
@@ -4323,25 +4317,25 @@
         <v>16</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E86" s="30"/>
       <c r="F86" s="7" t="s">
         <v>44</v>
       </c>
       <c r="G86" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="38" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>28</v>
@@ -4353,16 +4347,16 @@
         <v>17</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D87" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E87" s="26" t="s">
         <v>165</v>
-      </c>
-      <c r="E87" s="26" t="s">
-        <v>166</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>26</v>
@@ -4371,7 +4365,7 @@
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="38" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>28</v>
@@ -4380,26 +4374,26 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E88" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="E88" s="31" t="s">
-        <v>169</v>
-      </c>
       <c r="F88" s="41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>28</v>
@@ -4408,14 +4402,14 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E89" s="9"/>
       <c r="F89" s="7" t="s">
@@ -4425,7 +4419,7 @@
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>28</v>
@@ -4434,17 +4428,17 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>27</v>
@@ -4453,7 +4447,7 @@
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>28</v>
@@ -4462,17 +4456,17 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="49" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C91" s="12"/>
       <c r="D91" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E91" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>26</v>
@@ -4481,7 +4475,7 @@
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>28</v>
@@ -4490,17 +4484,17 @@
     </row>
     <row r="92" spans="1:12" ht="38.5">
       <c r="A92" s="49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C92" s="12"/>
       <c r="D92" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>175</v>
-      </c>
-      <c r="E92" s="13" t="s">
-        <v>176</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>27</v>
@@ -4509,7 +4503,7 @@
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
       <c r="J92" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>28</v>
@@ -4518,17 +4512,17 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="E93" s="26" t="s">
         <v>177</v>
-      </c>
-      <c r="E93" s="26" t="s">
-        <v>178</v>
       </c>
       <c r="F93" s="7" t="s">
         <v>26</v>
@@ -4537,7 +4531,7 @@
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>28</v>
@@ -4546,17 +4540,17 @@
     </row>
     <row r="94" spans="1:12" ht="38.5">
       <c r="A94" s="49" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>179</v>
-      </c>
-      <c r="E94" s="13" t="s">
-        <v>180</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>26</v>
@@ -4565,7 +4559,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
       <c r="J94" s="38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>28</v>
@@ -4574,28 +4568,28 @@
     </row>
     <row r="95" spans="1:12" ht="26">
       <c r="A95" s="49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C95" s="12"/>
       <c r="D95" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>182</v>
       </c>
       <c r="F95" s="41" t="s">
         <v>41</v>
       </c>
       <c r="G95" s="41" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H95" s="11"/>
       <c r="I95" s="9"/>
       <c r="J95" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>28</v>
@@ -4604,17 +4598,17 @@
     </row>
     <row r="96" spans="1:12" ht="26">
       <c r="A96" s="49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C96" s="12"/>
       <c r="D96" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E96" s="13" t="s">
         <v>183</v>
-      </c>
-      <c r="E96" s="13" t="s">
-        <v>184</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>27</v>
@@ -4623,7 +4617,7 @@
       <c r="H96" s="11"/>
       <c r="I96" s="9"/>
       <c r="J96" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K96" s="9" t="s">
         <v>28</v>
@@ -4632,17 +4626,17 @@
     </row>
     <row r="97" spans="1:12" ht="51">
       <c r="A97" s="49" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C97" s="32"/>
       <c r="D97" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E97" s="13" t="s">
         <v>185</v>
-      </c>
-      <c r="E97" s="13" t="s">
-        <v>186</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>26</v>
@@ -4651,7 +4645,7 @@
       <c r="H97" s="11"/>
       <c r="I97" s="15"/>
       <c r="J97" s="52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K97" s="9" t="s">
         <v>28</v>
@@ -4665,18 +4659,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4889,6 +4883,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4901,14 +4903,6 @@
     <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
lots of improvements and fixes on view + upload page
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E84520-C454-4FAE-90F3-C68B8CA92686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C10229C-0139-4879-9254-49C8520527A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="422">
   <si>
     <t>Unit</t>
   </si>
@@ -295,9 +295,6 @@
   </si>
   <si>
     <t>Ergebnis</t>
-  </si>
-  <si>
-    <t>Wie lautet das Rating (Ratingbericht bitte anfügen)?</t>
   </si>
   <si>
     <t>Kritische Punkte</t>
@@ -1334,6 +1331,18 @@
   </si>
   <si>
     <t>Sicherheit und Weiterbildung</t>
+  </si>
+  <si>
+    <t>15.4</t>
+  </si>
+  <si>
+    <t>Ratingbericht</t>
+  </si>
+  <si>
+    <t>Wie lautet das Rating?</t>
+  </si>
+  <si>
+    <t>Liegt ein Ratingbericht vor?</t>
   </si>
 </sst>
 </file>
@@ -2049,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
-  <dimension ref="A1:L120"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="E32" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -2107,7 +2116,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -2167,10 +2176,10 @@
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>291</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>34</v>
@@ -2182,7 +2191,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>26</v>
@@ -2191,16 +2200,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>35</v>
@@ -2221,16 +2230,16 @@
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>36</v>
@@ -2257,10 +2266,10 @@
         <v>33</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>37</v>
@@ -2272,7 +2281,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>26</v>
@@ -2287,10 +2296,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>289</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>290</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>38</v>
@@ -2299,7 +2308,7 @@
         <v>39</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -2313,16 +2322,16 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>40</v>
@@ -2334,7 +2343,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>26</v>
@@ -2349,24 +2358,24 @@
         <v>33</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>26</v>
@@ -2381,7 +2390,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>43</v>
@@ -2390,13 +2399,13 @@
         <v>44</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7"/>
       <c r="J11" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>26</v>
@@ -2405,19 +2414,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F12" s="46" t="s">
         <v>25</v>
@@ -2428,7 +2437,7 @@
         <v>27</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>26</v>
@@ -2437,19 +2446,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F13" s="46" t="s">
         <v>25</v>
@@ -2460,7 +2469,7 @@
         <v>27</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>26</v>
@@ -2469,19 +2478,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F14" s="46" t="s">
         <v>25</v>
@@ -2492,7 +2501,7 @@
         <v>27</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>26</v>
@@ -2501,19 +2510,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>25</v>
@@ -2524,7 +2533,7 @@
         <v>27</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>26</v>
@@ -2533,28 +2542,28 @@
     </row>
     <row r="16" spans="1:12" ht="26">
       <c r="A16" s="47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F16" s="39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
       <c r="I16" s="7"/>
       <c r="J16" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>26</v>
@@ -2569,13 +2578,13 @@
         <v>33</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F17" s="39" t="s">
         <v>25</v>
@@ -2584,7 +2593,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="7"/>
       <c r="J17" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>26</v>
@@ -2599,16 +2608,16 @@
         <v>33</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F18" s="39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -2623,16 +2632,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E19" s="51" t="s">
         <v>45</v>
@@ -2662,10 +2671,10 @@
         <v>46</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F20" s="39" t="s">
         <v>25</v>
@@ -2674,7 +2683,7 @@
       <c r="H20" s="46"/>
       <c r="I20" s="46"/>
       <c r="J20" s="50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K20" s="46" t="s">
         <v>26</v>
@@ -2683,7 +2692,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>33</v>
@@ -2692,13 +2701,13 @@
         <v>46</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2713,7 +2722,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>33</v>
@@ -2722,7 +2731,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E22" s="51" t="s">
         <v>45</v>
@@ -2743,13 +2752,13 @@
     </row>
     <row r="23" spans="1:12" ht="38.5">
       <c r="A23" s="47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>47</v>
@@ -2764,7 +2773,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>26</v>
@@ -2773,13 +2782,13 @@
     </row>
     <row r="24" spans="1:12" ht="26">
       <c r="A24" s="47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>49</v>
@@ -2794,7 +2803,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>26</v>
@@ -2809,7 +2818,7 @@
         <v>33</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>51</v>
@@ -2824,7 +2833,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>26</v>
@@ -2833,13 +2842,13 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>53</v>
@@ -2854,7 +2863,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>26</v>
@@ -2863,13 +2872,13 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>55</v>
@@ -2881,12 +2890,12 @@
         <v>42</v>
       </c>
       <c r="G27" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>26</v>
@@ -2895,13 +2904,13 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="47" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>57</v>
@@ -2913,12 +2922,12 @@
         <v>42</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>26</v>
@@ -2927,13 +2936,13 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>59</v>
@@ -2948,7 +2957,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>26</v>
@@ -2957,16 +2966,16 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>61</v>
@@ -2978,7 +2987,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>26</v>
@@ -2987,16 +2996,16 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>62</v>
@@ -3005,12 +3014,12 @@
         <v>42</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>26</v>
@@ -3019,16 +3028,16 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>63</v>
@@ -3040,7 +3049,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>26</v>
@@ -3049,16 +3058,16 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="47" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>64</v>
@@ -3070,7 +3079,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>26</v>
@@ -3079,16 +3088,16 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>65</v>
@@ -3097,12 +3106,12 @@
         <v>42</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="36" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>26</v>
@@ -3111,16 +3120,16 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="47" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>63</v>
@@ -3132,7 +3141,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="36" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>26</v>
@@ -3141,16 +3150,16 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="47" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>66</v>
@@ -3162,7 +3171,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>26</v>
@@ -3171,16 +3180,16 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>67</v>
@@ -3189,12 +3198,12 @@
         <v>42</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>26</v>
@@ -3203,16 +3212,16 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>63</v>
@@ -3224,7 +3233,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>26</v>
@@ -3233,13 +3242,13 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>68</v>
@@ -3254,7 +3263,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>26</v>
@@ -3263,13 +3272,13 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>70</v>
@@ -3284,7 +3293,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>26</v>
@@ -3293,30 +3302,28 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="47" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>73</v>
+        <v>420</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="I41" s="7"/>
       <c r="J41" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>26</v>
@@ -3325,28 +3332,30 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="47" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>74</v>
+        <v>419</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>75</v>
+        <v>421</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="9"/>
+      <c r="I42" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="J42" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>26</v>
@@ -3355,118 +3364,118 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="47" t="s">
-        <v>260</v>
+        <v>418</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>313</v>
+        <v>73</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>316</v>
+        <v>74</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="36" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L43" s="9"/>
     </row>
-    <row r="44" spans="1:12" ht="26">
+    <row r="44" spans="1:12">
       <c r="A44" s="47" t="s">
-        <v>318</v>
+        <v>259</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F44" s="39" t="s">
-        <v>309</v>
+        <v>312</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="36" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L44" s="9"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" ht="26">
       <c r="A45" s="47" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="39" t="s">
         <v>308</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="36" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L45" s="9"/>
     </row>
-    <row r="46" spans="1:12" ht="26">
+    <row r="46" spans="1:12">
       <c r="A46" s="47" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F46" s="39" t="s">
         <v>309</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="36" t="s">
-        <v>319</v>
+        <v>175</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>26</v>
@@ -3475,28 +3484,28 @@
     </row>
     <row r="47" spans="1:12" ht="26">
       <c r="A47" s="47" t="s">
-        <v>191</v>
+        <v>319</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>24</v>
+        <v>314</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F47" s="39" t="s">
+        <v>308</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="36" t="s">
-        <v>176</v>
+        <v>318</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>26</v>
@@ -3505,19 +3514,19 @@
     </row>
     <row r="48" spans="1:12" ht="26">
       <c r="A48" s="47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>24</v>
@@ -3526,88 +3535,88 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L48" s="9"/>
     </row>
-    <row r="49" spans="1:12" ht="51">
+    <row r="49" spans="1:12" ht="26">
       <c r="A49" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>82</v>
+        <v>33</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>311</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F49" s="39" t="s">
-        <v>284</v>
+        <v>78</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L49" s="9"/>
     </row>
-    <row r="50" spans="1:12" ht="38.5">
+    <row r="50" spans="1:12" ht="51">
       <c r="A50" s="47" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>24</v>
+      <c r="E50" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F50" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="1:12" ht="51">
+    <row r="51" spans="1:12" ht="38.5">
       <c r="A51" s="47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>87</v>
+      <c r="D51" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>24</v>
@@ -3616,37 +3625,37 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L51" s="9"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" ht="51">
       <c r="A52" s="47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>321</v>
-      </c>
       <c r="D52" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>26</v>
@@ -3655,88 +3664,88 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="47" t="s">
-        <v>261</v>
+        <v>195</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="36" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="1:12" ht="26">
+    <row r="54" spans="1:12">
       <c r="A54" s="47" t="s">
-        <v>197</v>
+        <v>260</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="36" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L54" s="9"/>
     </row>
-    <row r="55" spans="1:12" ht="42.5">
+    <row r="55" spans="1:12" ht="26">
       <c r="A55" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="39" t="s">
-        <v>284</v>
+        <v>91</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>26</v>
@@ -3745,88 +3754,88 @@
     </row>
     <row r="56" spans="1:12" ht="42.5">
       <c r="A56" s="47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>24</v>
+      <c r="E56" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:12" ht="28.5">
+    <row r="57" spans="1:12" ht="42.5">
       <c r="A57" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F57" s="39" t="s">
-        <v>284</v>
+        <v>93</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L57" s="9"/>
     </row>
-    <row r="58" spans="1:12" ht="42.5">
+    <row r="58" spans="1:12" ht="28.5">
       <c r="A58" s="47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D58" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>24</v>
+      <c r="E58" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F58" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>26</v>
@@ -3835,28 +3844,28 @@
     </row>
     <row r="59" spans="1:12" ht="42.5">
       <c r="A59" s="47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F59" s="39" t="s">
-        <v>284</v>
+        <v>97</v>
+      </c>
+      <c r="D59" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>26</v>
@@ -3865,360 +3874,358 @@
     </row>
     <row r="60" spans="1:12" ht="42.5">
       <c r="A60" s="47" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D60" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D60" s="40" t="s">
-        <v>231</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>24</v>
+      <c r="E60" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F60" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:12" ht="56.5">
+    <row r="61" spans="1:12" ht="42.5">
       <c r="A61" s="47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="F61" s="39" t="s">
-        <v>284</v>
+        <v>100</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L61" s="9"/>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" ht="56.5">
       <c r="A62" s="47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="42" t="s">
-        <v>234</v>
-      </c>
-      <c r="E62" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>24</v>
+      <c r="E62" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F62" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L62" s="9"/>
     </row>
-    <row r="63" spans="1:12" ht="38.5">
+    <row r="63" spans="1:12">
       <c r="A63" s="47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="E63" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F63" s="39" t="s">
-        <v>284</v>
+        <v>103</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L63" s="9"/>
     </row>
-    <row r="64" spans="1:12" ht="26">
+    <row r="64" spans="1:12" ht="38.5">
       <c r="A64" s="47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>24</v>
+        <v>103</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L64" s="9"/>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" ht="26">
       <c r="A65" s="47" t="s">
-        <v>208</v>
-      </c>
-      <c r="B65" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="D65" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E65" s="27" t="s">
-        <v>112</v>
+        <v>206</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L65" s="9"/>
     </row>
-    <row r="66" spans="1:12" ht="51">
+    <row r="66" spans="1:12">
       <c r="A66" s="47" t="s">
-        <v>262</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>115</v>
+        <v>207</v>
+      </c>
+      <c r="B66" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="36" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L66" s="9"/>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" ht="51">
       <c r="A67" s="47" t="s">
-        <v>209</v>
-      </c>
-      <c r="B67" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D67" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="E67" s="28" t="s">
-        <v>117</v>
+      <c r="E67" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="36" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L67" s="9"/>
     </row>
-    <row r="68" spans="1:12" ht="51">
+    <row r="68" spans="1:12">
       <c r="A68" s="47" t="s">
-        <v>263</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E68" s="13" t="s">
-        <v>119</v>
+        <v>208</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E68" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="36" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L68" s="9"/>
     </row>
-    <row r="69" spans="1:12" ht="38.5">
+    <row r="69" spans="1:12" ht="51">
       <c r="A69" s="47" t="s">
-        <v>210</v>
+        <v>262</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="36" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L69" s="9"/>
     </row>
-    <row r="70" spans="1:12" ht="42.5">
+    <row r="70" spans="1:12" ht="38.5">
       <c r="A70" s="47" t="s">
-        <v>134</v>
+        <v>209</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C70" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D70" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="F70" s="39" t="s">
-        <v>284</v>
+      <c r="E70" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="36" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" ht="42.5">
       <c r="A71" s="47" t="s">
-        <v>211</v>
+        <v>133</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>243</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F71" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="36" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>26</v>
@@ -4227,150 +4234,152 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="47" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D72" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>129</v>
+      <c r="E72" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>245</v>
+        <v>42</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L72" s="9"/>
     </row>
-    <row r="73" spans="1:12" ht="51">
+    <row r="73" spans="1:12">
       <c r="A73" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73" s="39" t="s">
-        <v>284</v>
-      </c>
-      <c r="G73" s="11"/>
+        <v>127</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>244</v>
+      </c>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L73" s="9"/>
     </row>
-    <row r="74" spans="1:12" ht="26">
+    <row r="74" spans="1:12" ht="51">
       <c r="A74" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C74" s="62" t="s">
-        <v>327</v>
-      </c>
-      <c r="D74" s="54" t="s">
-        <v>328</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>25</v>
+        <v>80</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F74" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L74" s="9"/>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" ht="26">
       <c r="A75" s="47" t="s">
-        <v>264</v>
+        <v>213</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="D75" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="E75" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="E75" s="13" t="s">
-        <v>334</v>
-      </c>
       <c r="F75" s="7" t="s">
-        <v>309</v>
+        <v>25</v>
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="36" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L75" s="9"/>
     </row>
-    <row r="76" spans="1:12" ht="26">
+    <row r="76" spans="1:12">
       <c r="A76" s="47" t="s">
-        <v>341</v>
+        <v>263</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E76" s="13" t="s">
         <v>333</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>26</v>
@@ -4379,88 +4388,88 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="47" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L77" s="9"/>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" ht="26">
       <c r="A78" s="47" t="s">
-        <v>265</v>
+        <v>341</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L78" s="9"/>
     </row>
-    <row r="79" spans="1:12" ht="26">
+    <row r="79" spans="1:12">
       <c r="A79" s="47" t="s">
-        <v>343</v>
+        <v>264</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>26</v>
@@ -4469,28 +4478,28 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="47" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>26</v>
@@ -4499,28 +4508,28 @@
     </row>
     <row r="81" spans="1:12" ht="26">
       <c r="A81" s="47" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F81" s="39" t="s">
-        <v>346</v>
+        <v>338</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>308</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>26</v>
@@ -4529,178 +4538,178 @@
     </row>
     <row r="82" spans="1:12" ht="26">
       <c r="A82" s="47" t="s">
-        <v>215</v>
+        <v>344</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C82" s="62" t="s">
-        <v>418</v>
+        <v>131</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>24</v>
+        <v>134</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F82" s="39" t="s">
+        <v>345</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="36" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L82" s="9"/>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" ht="26">
       <c r="A83" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="B83" s="46" t="s">
-        <v>132</v>
+        <v>214</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C83" s="62" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E83" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="F83" s="39" t="s">
-        <v>346</v>
+        <v>136</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L83" s="9"/>
     </row>
-    <row r="84" spans="1:12" ht="26">
+    <row r="84" spans="1:12">
       <c r="A84" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>132</v>
+        <v>215</v>
+      </c>
+      <c r="B84" s="46" t="s">
+        <v>131</v>
       </c>
       <c r="C84" s="62" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E84" s="10" t="s">
-        <v>142</v>
+        <v>138</v>
+      </c>
+      <c r="E84" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="F84" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L84" s="9"/>
     </row>
-    <row r="85" spans="1:12" ht="38.5">
+    <row r="85" spans="1:12" ht="26">
       <c r="A85" s="47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>143</v>
+        <v>131</v>
+      </c>
+      <c r="C85" s="62" t="s">
+        <v>417</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F85" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L85" s="9"/>
     </row>
-    <row r="86" spans="1:12" ht="26">
+    <row r="86" spans="1:12" ht="38.5">
       <c r="A86" s="47" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D86" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D86" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E86" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>24</v>
+      <c r="E86" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F86" s="39" t="s">
+        <v>345</v>
       </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L86" s="9"/>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" ht="26">
       <c r="A87" s="47" t="s">
-        <v>350</v>
+        <v>218</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E87" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="F87" s="39" t="s">
-        <v>309</v>
+        <v>145</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>26</v>
@@ -4712,25 +4721,25 @@
         <v>349</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="F88" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>26</v>
@@ -4738,29 +4747,29 @@
       <c r="L88" s="9"/>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="65" t="s">
-        <v>399</v>
+      <c r="A89" s="47" t="s">
+        <v>348</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F89" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>26</v>
@@ -4769,28 +4778,28 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="65" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F90" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>26</v>
@@ -4799,28 +4808,28 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="65" t="s">
-        <v>220</v>
+        <v>399</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="F91" s="7" t="s">
-        <v>24</v>
+        <v>354</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="F91" s="39" t="s">
+        <v>308</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>26</v>
@@ -4829,19 +4838,19 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="65" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C92" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D92" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D92" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E92" s="26" t="s">
-        <v>152</v>
+      <c r="E92" s="13" t="s">
+        <v>149</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>24</v>
@@ -4850,69 +4859,67 @@
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
       <c r="J92" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L92" s="9"/>
     </row>
-    <row r="93" spans="1:12" ht="26">
+    <row r="93" spans="1:12">
       <c r="A93" s="65" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
+      </c>
+      <c r="E93" s="26" t="s">
+        <v>151</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L93" s="9"/>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" ht="26">
       <c r="A94" s="65" t="s">
-        <v>401</v>
+        <v>221</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C94" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D94" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D94" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E94" s="30" t="s">
-        <v>357</v>
+      <c r="E94" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G94" s="44" t="s">
-        <v>241</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G94" s="11"/>
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
-      <c r="J94" s="56" t="s">
-        <v>222</v>
+      <c r="J94" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>26</v>
@@ -4921,28 +4928,30 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="65" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E95" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="E95" s="30" t="s">
+        <v>356</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G95" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="G95" s="44" t="s">
+        <v>240</v>
+      </c>
       <c r="H95" s="11"/>
       <c r="I95" s="9"/>
       <c r="J95" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>26</v>
@@ -4951,28 +4960,28 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="65" t="s">
-        <v>223</v>
+        <v>401</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>358</v>
+        <v>152</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="E96" s="52" t="s">
-        <v>360</v>
+        <v>156</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>157</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>309</v>
+        <v>24</v>
       </c>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
       <c r="I96" s="9"/>
-      <c r="J96" s="36" t="s">
-        <v>176</v>
+      <c r="J96" s="56" t="s">
+        <v>221</v>
       </c>
       <c r="K96" s="9" t="s">
         <v>26</v>
@@ -4981,28 +4990,28 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="65" t="s">
-        <v>403</v>
+        <v>222</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C97" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D97" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="D97" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="E97" s="53" t="s">
-        <v>380</v>
+      <c r="E97" s="52" t="s">
+        <v>359</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
       <c r="I97" s="9"/>
       <c r="J97" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K97" s="9" t="s">
         <v>26</v>
@@ -5011,28 +5020,28 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="65" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E98" s="52" t="s">
-        <v>363</v>
+        <v>360</v>
+      </c>
+      <c r="E98" s="53" t="s">
+        <v>379</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
       <c r="I98" s="9"/>
       <c r="J98" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K98" s="9" t="s">
         <v>26</v>
@@ -5041,28 +5050,28 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="65" t="s">
-        <v>266</v>
+        <v>403</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E99" s="52" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G99" s="11"/>
       <c r="H99" s="11"/>
       <c r="I99" s="9"/>
       <c r="J99" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K99" s="9" t="s">
         <v>26</v>
@@ -5071,28 +5080,28 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="65" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D100" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="D100" s="8" t="s">
-        <v>367</v>
-      </c>
       <c r="E100" s="52" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
       <c r="I100" s="9"/>
       <c r="J100" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K100" s="9" t="s">
         <v>26</v>
@@ -5101,28 +5110,28 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="65" t="s">
-        <v>405</v>
+        <v>266</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E101" s="52" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
       <c r="I101" s="9"/>
       <c r="J101" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K101" s="9" t="s">
         <v>26</v>
@@ -5131,28 +5140,28 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="65" t="s">
-        <v>268</v>
+        <v>404</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E102" s="53" t="s">
-        <v>376</v>
+        <v>367</v>
+      </c>
+      <c r="E102" s="52" t="s">
+        <v>368</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
       <c r="I102" s="9"/>
       <c r="J102" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K102" s="9" t="s">
         <v>26</v>
@@ -5161,28 +5170,28 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="65" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D103" s="54" t="s">
-        <v>377</v>
+        <v>369</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>372</v>
       </c>
       <c r="E103" s="53" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G103" s="11"/>
       <c r="H103" s="11"/>
       <c r="I103" s="9"/>
       <c r="J103" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K103" s="9" t="s">
         <v>26</v>
@@ -5191,28 +5200,28 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="65" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
+      </c>
+      <c r="D104" s="54" t="s">
+        <v>376</v>
       </c>
       <c r="E104" s="53" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
       <c r="I104" s="9"/>
       <c r="J104" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K104" s="9" t="s">
         <v>26</v>
@@ -5221,28 +5230,28 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="65" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="D105" s="54" t="s">
-        <v>374</v>
+        <v>369</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>367</v>
       </c>
       <c r="E105" s="53" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G105" s="11"/>
       <c r="H105" s="11"/>
       <c r="I105" s="9"/>
       <c r="J105" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K105" s="9" t="s">
         <v>26</v>
@@ -5251,28 +5260,28 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="65" t="s">
-        <v>406</v>
+        <v>270</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D106" s="54" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E106" s="53" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G106" s="11"/>
       <c r="H106" s="11"/>
       <c r="I106" s="9"/>
       <c r="J106" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K106" s="9" t="s">
         <v>26</v>
@@ -5281,28 +5290,28 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="65" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D107" s="54" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="E107" s="53" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
       <c r="I107" s="9"/>
       <c r="J107" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K107" s="9" t="s">
         <v>26</v>
@@ -5311,28 +5320,28 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="65" t="s">
-        <v>272</v>
+        <v>406</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D108" s="54" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="E108" s="53" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
       <c r="I108" s="9"/>
       <c r="J108" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K108" s="9" t="s">
         <v>26</v>
@@ -5341,28 +5350,28 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="65" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D109" s="54" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E109" s="53" t="s">
-        <v>390</v>
-      </c>
-      <c r="F109" s="39" t="s">
-        <v>309</v>
+        <v>386</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>308</v>
       </c>
       <c r="G109" s="11"/>
       <c r="H109" s="11"/>
       <c r="I109" s="9"/>
       <c r="J109" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K109" s="9" t="s">
         <v>26</v>
@@ -5371,86 +5380,86 @@
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="65" t="s">
-        <v>398</v>
+        <v>272</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D110" s="54" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="E110" s="53" t="s">
-        <v>391</v>
-      </c>
-      <c r="F110" s="55" t="s">
-        <v>309</v>
+        <v>389</v>
+      </c>
+      <c r="F110" s="39" t="s">
+        <v>308</v>
       </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
       <c r="I110" s="9"/>
-      <c r="J110" s="56" t="s">
-        <v>176</v>
-      </c>
-      <c r="K110" s="57" t="s">
+      <c r="J110" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="K110" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L110" s="9"/>
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="65" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C111" s="62" t="s">
-        <v>305</v>
-      </c>
-      <c r="D111" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E111" s="9"/>
-      <c r="F111" s="7" t="s">
-        <v>24</v>
+        <v>158</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D111" s="54" t="s">
+        <v>384</v>
+      </c>
+      <c r="E111" s="53" t="s">
+        <v>390</v>
+      </c>
+      <c r="F111" s="55" t="s">
+        <v>308</v>
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
       <c r="I111" s="9"/>
-      <c r="J111" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="K111" s="9" t="s">
+      <c r="J111" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="K111" s="57" t="s">
         <v>26</v>
       </c>
       <c r="L111" s="9"/>
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="65" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B112" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C112" s="62" t="s">
+        <v>304</v>
+      </c>
+      <c r="D112" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C112" s="62" t="s">
-        <v>305</v>
-      </c>
-      <c r="D112" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E112" s="7" t="s">
-        <v>162</v>
-      </c>
+      <c r="E112" s="9"/>
       <c r="F112" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
       <c r="I112" s="9"/>
-      <c r="J112" s="56" t="s">
-        <v>176</v>
+      <c r="J112" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="K112" s="9" t="s">
         <v>26</v>
@@ -5459,109 +5468,109 @@
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="65" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C113" s="62" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G113" s="11"/>
       <c r="H113" s="11"/>
       <c r="I113" s="9"/>
       <c r="J113" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="K113" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L113" s="9"/>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114" s="65" t="s">
         <v>409</v>
       </c>
-      <c r="K113" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L113" s="9"/>
-    </row>
-    <row r="114" spans="1:12" ht="38.5">
-      <c r="A114" s="65" t="s">
-        <v>411</v>
-      </c>
       <c r="B114" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C114" s="62" t="s">
-        <v>395</v>
+        <v>304</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E114" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G114" s="11"/>
       <c r="H114" s="11"/>
       <c r="I114" s="9"/>
       <c r="J114" s="56" t="s">
-        <v>176</v>
+        <v>408</v>
       </c>
       <c r="K114" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L114" s="9"/>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" ht="38.5">
       <c r="A115" s="65" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C115" s="62" t="s">
-        <v>395</v>
-      </c>
-      <c r="D115" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="E115" s="26" t="s">
-        <v>168</v>
+        <v>394</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G115" s="11"/>
       <c r="H115" s="11"/>
       <c r="I115" s="9"/>
       <c r="J115" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="K115" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L115" s="9"/>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="K115" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L115" s="9"/>
-    </row>
-    <row r="116" spans="1:12" ht="38.5">
-      <c r="A116" s="65" t="s">
-        <v>413</v>
-      </c>
       <c r="B116" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C116" s="62" t="s">
-        <v>395</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E116" s="13" t="s">
-        <v>170</v>
+        <v>394</v>
+      </c>
+      <c r="D116" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E116" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="F116" s="7" t="s">
         <v>24</v>
@@ -5570,39 +5579,37 @@
       <c r="H116" s="11"/>
       <c r="I116" s="9"/>
       <c r="J116" s="56" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K116" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L116" s="9"/>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" ht="38.5">
       <c r="A117" s="65" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C117" s="62" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="E117" s="59" t="s">
-        <v>392</v>
-      </c>
-      <c r="F117" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="G117" s="39" t="s">
-        <v>242</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="E117" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G117" s="11"/>
       <c r="H117" s="11"/>
       <c r="I117" s="9"/>
-      <c r="J117" s="36" t="s">
-        <v>176</v>
+      <c r="J117" s="56" t="s">
+        <v>410</v>
       </c>
       <c r="K117" s="9" t="s">
         <v>26</v>
@@ -5611,88 +5618,120 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="65" t="s">
+        <v>413</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C118" s="62" t="s">
+        <v>395</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E118" s="59" t="s">
+        <v>391</v>
+      </c>
+      <c r="F118" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="G118" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="H118" s="11"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="K118" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L118" s="9"/>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" s="65" t="s">
+        <v>414</v>
+      </c>
+      <c r="B119" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C119" s="62" t="s">
+        <v>395</v>
+      </c>
+      <c r="D119" s="54" t="s">
+        <v>393</v>
+      </c>
+      <c r="E119" s="59" t="s">
+        <v>392</v>
+      </c>
+      <c r="F119" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="G119" s="39"/>
+      <c r="H119" s="11"/>
+      <c r="I119" s="58"/>
+      <c r="J119" s="60" t="s">
+        <v>175</v>
+      </c>
+      <c r="K119" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="L119" s="9"/>
+    </row>
+    <row r="120" spans="1:12" ht="26">
+      <c r="A120" s="65" t="s">
         <v>415</v>
       </c>
-      <c r="B118" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="C118" s="62" t="s">
+      <c r="B120" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C120" s="62" t="s">
         <v>396</v>
       </c>
-      <c r="D118" s="54" t="s">
-        <v>394</v>
-      </c>
-      <c r="E118" s="59" t="s">
-        <v>393</v>
-      </c>
-      <c r="F118" s="55" t="s">
+      <c r="D120" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E120" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G120" s="11"/>
+      <c r="H120" s="11"/>
+      <c r="I120" s="15"/>
+      <c r="J120" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="K120" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L120" s="9"/>
+    </row>
+    <row r="121" spans="1:12" ht="51">
+      <c r="A121" s="63" t="s">
+        <v>416</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C121" s="62" t="s">
+        <v>396</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E121" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F121" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G118" s="39"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="58"/>
-      <c r="J118" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="K118" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="L118" s="9"/>
-    </row>
-    <row r="119" spans="1:12" ht="26">
-      <c r="A119" s="65" t="s">
-        <v>416</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C119" s="62" t="s">
-        <v>397</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E119" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="F119" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
-      <c r="I119" s="15"/>
-      <c r="J119" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="K119" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L119" s="9"/>
-    </row>
-    <row r="120" spans="1:12" ht="51">
-      <c r="A120" s="63" t="s">
-        <v>417</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C120" s="62" t="s">
-        <v>397</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E120" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F120" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G120" s="11"/>
-      <c r="J120" s="63" t="s">
-        <v>416</v>
-      </c>
-      <c r="K120" s="64" t="s">
+      <c r="G121" s="11"/>
+      <c r="J121" s="63" t="s">
+        <v>415</v>
+      </c>
+      <c r="K121" s="64" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5703,6 +5742,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -5911,36 +5965,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
-    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5963,9 +5991,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
+    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
better names for two fields (ceo + amtszeit)
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C10229C-0139-4879-9254-49C8520527A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEE534E-B3F2-45D9-AC39-288C16492F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -559,15 +559,9 @@
     <t>Wirtschaftsprüfer</t>
   </si>
   <si>
-    <t>CEO/Vorsitzender</t>
-  </si>
-  <si>
     <t>Hat sich das Unternehmen im aktuellen Jahr der Berichterstattung von CEO/Vorsitzenden getrennt?</t>
   </si>
   <si>
-    <t>Amtszeit</t>
-  </si>
-  <si>
     <t>Wieviele Jahre war der/die CEO/Vorsitzende(r) im Amt?</t>
   </si>
   <si>
@@ -1343,6 +1337,12 @@
   </si>
   <si>
     <t>Liegt ein Ratingbericht vor?</t>
+  </si>
+  <si>
+    <t>Trennung von CEO oder Vorsitzenden</t>
+  </si>
+  <si>
+    <t>Amtszeit bis zur Trennung</t>
   </si>
 </sst>
 </file>
@@ -2060,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E32" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -2176,10 +2176,10 @@
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>34</v>
@@ -2191,7 +2191,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>26</v>
@@ -2200,16 +2200,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>35</v>
@@ -2230,16 +2230,16 @@
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>290</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>36</v>
@@ -2266,10 +2266,10 @@
         <v>33</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>37</v>
@@ -2281,7 +2281,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>26</v>
@@ -2296,10 +2296,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>38</v>
@@ -2308,7 +2308,7 @@
         <v>39</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -2322,16 +2322,16 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>40</v>
@@ -2343,7 +2343,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>26</v>
@@ -2358,24 +2358,24 @@
         <v>33</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>26</v>
@@ -2390,7 +2390,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>43</v>
@@ -2399,13 +2399,13 @@
         <v>44</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7"/>
       <c r="J11" s="36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>26</v>
@@ -2414,19 +2414,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F12" s="46" t="s">
         <v>25</v>
@@ -2437,7 +2437,7 @@
         <v>27</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>26</v>
@@ -2446,19 +2446,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F13" s="46" t="s">
         <v>25</v>
@@ -2469,7 +2469,7 @@
         <v>27</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>26</v>
@@ -2478,19 +2478,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="47" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F14" s="46" t="s">
         <v>25</v>
@@ -2501,7 +2501,7 @@
         <v>27</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>26</v>
@@ -2510,19 +2510,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="47" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>25</v>
@@ -2533,7 +2533,7 @@
         <v>27</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>26</v>
@@ -2542,28 +2542,28 @@
     </row>
     <row r="16" spans="1:12" ht="26">
       <c r="A16" s="47" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F16" s="39" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
       <c r="I16" s="7"/>
       <c r="J16" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>26</v>
@@ -2578,13 +2578,13 @@
         <v>33</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F17" s="39" t="s">
         <v>25</v>
@@ -2593,7 +2593,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="7"/>
       <c r="J17" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>26</v>
@@ -2608,16 +2608,16 @@
         <v>33</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F18" s="39" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -2632,16 +2632,16 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="47" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E19" s="51" t="s">
         <v>45</v>
@@ -2671,10 +2671,10 @@
         <v>46</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F20" s="39" t="s">
         <v>25</v>
@@ -2683,7 +2683,7 @@
       <c r="H20" s="46"/>
       <c r="I20" s="46"/>
       <c r="J20" s="50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K20" s="46" t="s">
         <v>26</v>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="47" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>33</v>
@@ -2701,13 +2701,13 @@
         <v>46</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="47" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>33</v>
@@ -2731,7 +2731,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E22" s="51" t="s">
         <v>45</v>
@@ -2752,13 +2752,13 @@
     </row>
     <row r="23" spans="1:12" ht="38.5">
       <c r="A23" s="47" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>47</v>
@@ -2773,7 +2773,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>26</v>
@@ -2782,13 +2782,13 @@
     </row>
     <row r="24" spans="1:12" ht="26">
       <c r="A24" s="47" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>49</v>
@@ -2803,7 +2803,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>26</v>
@@ -2818,7 +2818,7 @@
         <v>33</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>51</v>
@@ -2833,7 +2833,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>26</v>
@@ -2842,13 +2842,13 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="47" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>53</v>
@@ -2863,7 +2863,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>26</v>
@@ -2872,13 +2872,13 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="47" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>55</v>
@@ -2890,12 +2890,12 @@
         <v>42</v>
       </c>
       <c r="G27" s="43" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>26</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="47" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>57</v>
@@ -2922,12 +2922,12 @@
         <v>42</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>26</v>
@@ -2936,13 +2936,13 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="47" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>59</v>
@@ -2957,7 +2957,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>26</v>
@@ -2966,16 +2966,16 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="47" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>61</v>
@@ -2987,7 +2987,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>26</v>
@@ -2996,16 +2996,16 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="47" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>62</v>
@@ -3014,12 +3014,12 @@
         <v>42</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="36" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>26</v>
@@ -3028,16 +3028,16 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="47" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>63</v>
@@ -3049,7 +3049,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="36" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>26</v>
@@ -3058,16 +3058,16 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="47" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>64</v>
@@ -3079,7 +3079,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>26</v>
@@ -3088,16 +3088,16 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="47" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>65</v>
@@ -3106,12 +3106,12 @@
         <v>42</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="36" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>26</v>
@@ -3120,16 +3120,16 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="47" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>63</v>
@@ -3141,7 +3141,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="36" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>26</v>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="47" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>66</v>
@@ -3171,7 +3171,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>26</v>
@@ -3180,16 +3180,16 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="47" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>67</v>
@@ -3198,12 +3198,12 @@
         <v>42</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="36" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>26</v>
@@ -3212,16 +3212,16 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>63</v>
@@ -3233,7 +3233,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="36" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>26</v>
@@ -3242,13 +3242,13 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="47" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>68</v>
@@ -3263,7 +3263,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>26</v>
@@ -3272,13 +3272,13 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>70</v>
@@ -3293,7 +3293,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>26</v>
@@ -3302,19 +3302,19 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="47" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>24</v>
@@ -3323,7 +3323,7 @@
       <c r="H41" s="11"/>
       <c r="I41" s="7"/>
       <c r="J41" s="36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>26</v>
@@ -3332,19 +3332,19 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="47" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D42" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>419</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>421</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>25</v>
@@ -3355,7 +3355,7 @@
         <v>27</v>
       </c>
       <c r="J42" s="36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>26</v>
@@ -3364,13 +3364,13 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="47" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>73</v>
@@ -3385,7 +3385,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>26</v>
@@ -3394,19 +3394,19 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="47" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>25</v>
@@ -3415,7 +3415,7 @@
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>26</v>
@@ -3424,28 +3424,28 @@
     </row>
     <row r="45" spans="1:12" ht="26">
       <c r="A45" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>75</v>
       </c>
       <c r="F45" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="36" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>26</v>
@@ -3454,19 +3454,19 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="47" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>309</v>
-      </c>
       <c r="E46" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>25</v>
@@ -3475,7 +3475,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>26</v>
@@ -3484,28 +3484,28 @@
     </row>
     <row r="47" spans="1:12" ht="26">
       <c r="A47" s="47" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>75</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="36" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>26</v>
@@ -3514,13 +3514,13 @@
     </row>
     <row r="48" spans="1:12" ht="26">
       <c r="A48" s="47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>76</v>
@@ -3535,7 +3535,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>26</v>
@@ -3544,13 +3544,13 @@
     </row>
     <row r="49" spans="1:12" ht="26">
       <c r="A49" s="47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>78</v>
@@ -3565,7 +3565,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>26</v>
@@ -3574,7 +3574,7 @@
     </row>
     <row r="50" spans="1:12" ht="51">
       <c r="A50" s="47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>80</v>
@@ -3589,13 +3589,13 @@
         <v>83</v>
       </c>
       <c r="F50" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>26</v>
@@ -3604,7 +3604,7 @@
     </row>
     <row r="51" spans="1:12" ht="38.5">
       <c r="A51" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>80</v>
@@ -3613,7 +3613,7 @@
         <v>81</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>84</v>
@@ -3625,7 +3625,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>26</v>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="52" spans="1:12" ht="51">
       <c r="A52" s="47" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>80</v>
@@ -3655,7 +3655,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>26</v>
@@ -3664,13 +3664,13 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>87</v>
@@ -3685,7 +3685,7 @@
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>26</v>
@@ -3694,13 +3694,13 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="47" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>89</v>
@@ -3715,7 +3715,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>26</v>
@@ -3724,13 +3724,13 @@
     </row>
     <row r="55" spans="1:12" ht="26">
       <c r="A55" s="47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>91</v>
@@ -3745,7 +3745,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>26</v>
@@ -3754,7 +3754,7 @@
     </row>
     <row r="56" spans="1:12" ht="42.5">
       <c r="A56" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>80</v>
@@ -3769,13 +3769,13 @@
         <v>95</v>
       </c>
       <c r="F56" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>26</v>
@@ -3784,7 +3784,7 @@
     </row>
     <row r="57" spans="1:12" ht="42.5">
       <c r="A57" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>80</v>
@@ -3793,7 +3793,7 @@
         <v>93</v>
       </c>
       <c r="D57" s="39" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E57" s="21" t="s">
         <v>96</v>
@@ -3805,7 +3805,7 @@
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>26</v>
@@ -3814,7 +3814,7 @@
     </row>
     <row r="58" spans="1:12" ht="28.5">
       <c r="A58" s="47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>80</v>
@@ -3829,13 +3829,13 @@
         <v>99</v>
       </c>
       <c r="F58" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>26</v>
@@ -3844,7 +3844,7 @@
     </row>
     <row r="59" spans="1:12" ht="42.5">
       <c r="A59" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>80</v>
@@ -3853,7 +3853,7 @@
         <v>97</v>
       </c>
       <c r="D59" s="41" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E59" s="22" t="s">
         <v>96</v>
@@ -3865,7 +3865,7 @@
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>26</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="60" spans="1:12" ht="42.5">
       <c r="A60" s="47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>80</v>
@@ -3889,13 +3889,13 @@
         <v>102</v>
       </c>
       <c r="F60" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>26</v>
@@ -3904,7 +3904,7 @@
     </row>
     <row r="61" spans="1:12" ht="42.5">
       <c r="A61" s="47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>80</v>
@@ -3913,7 +3913,7 @@
         <v>100</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E61" s="22" t="s">
         <v>96</v>
@@ -3925,7 +3925,7 @@
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>26</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="62" spans="1:12" ht="56.5">
       <c r="A62" s="47" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>80</v>
@@ -3949,13 +3949,13 @@
         <v>105</v>
       </c>
       <c r="F62" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>26</v>
@@ -3964,7 +3964,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>80</v>
@@ -3973,7 +3973,7 @@
         <v>103</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E63" s="23" t="s">
         <v>96</v>
@@ -3985,7 +3985,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>26</v>
@@ -3994,7 +3994,7 @@
     </row>
     <row r="64" spans="1:12" ht="38.5">
       <c r="A64" s="47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>80</v>
@@ -4009,13 +4009,13 @@
         <v>107</v>
       </c>
       <c r="F64" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>26</v>
@@ -4024,7 +4024,7 @@
     </row>
     <row r="65" spans="1:12" ht="26">
       <c r="A65" s="47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>80</v>
@@ -4045,7 +4045,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>26</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B66" s="46" t="s">
         <v>80</v>
@@ -4075,7 +4075,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>26</v>
@@ -4084,7 +4084,7 @@
     </row>
     <row r="67" spans="1:12" ht="51">
       <c r="A67" s="47" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>80</v>
@@ -4105,7 +4105,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>26</v>
@@ -4114,7 +4114,7 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="47" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B68" s="46" t="s">
         <v>80</v>
@@ -4135,7 +4135,7 @@
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>26</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="69" spans="1:12" ht="51">
       <c r="A69" s="47" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>80</v>
@@ -4165,7 +4165,7 @@
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="36" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>26</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="70" spans="1:12" ht="38.5">
       <c r="A70" s="47" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>80</v>
@@ -4195,7 +4195,7 @@
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>26</v>
@@ -4219,13 +4219,13 @@
         <v>123</v>
       </c>
       <c r="F71" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="36" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>26</v>
@@ -4234,7 +4234,7 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="47" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>80</v>
@@ -4252,12 +4252,12 @@
         <v>42</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>26</v>
@@ -4266,7 +4266,7 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="47" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>80</v>
@@ -4284,12 +4284,12 @@
         <v>39</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>26</v>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="74" spans="1:12" ht="51">
       <c r="A74" s="47" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>80</v>
@@ -4313,13 +4313,13 @@
         <v>130</v>
       </c>
       <c r="F74" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>26</v>
@@ -4328,16 +4328,16 @@
     </row>
     <row r="75" spans="1:12" ht="26">
       <c r="A75" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C75" s="62" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D75" s="54" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E75" s="13" t="s">
         <v>132</v>
@@ -4349,7 +4349,7 @@
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>26</v>
@@ -4358,28 +4358,28 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="47" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C76" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>328</v>
-      </c>
       <c r="E76" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>26</v>
@@ -4388,28 +4388,28 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="47" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>26</v>
@@ -4418,28 +4418,28 @@
     </row>
     <row r="78" spans="1:12" ht="26">
       <c r="A78" s="47" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>26</v>
@@ -4448,28 +4448,28 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="47" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>26</v>
@@ -4478,28 +4478,28 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="47" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>26</v>
@@ -4508,28 +4508,28 @@
     </row>
     <row r="81" spans="1:12" ht="26">
       <c r="A81" s="47" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>26</v>
@@ -4538,13 +4538,13 @@
     </row>
     <row r="82" spans="1:12" ht="26">
       <c r="A82" s="47" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>134</v>
@@ -4553,13 +4553,13 @@
         <v>135</v>
       </c>
       <c r="F82" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>26</v>
@@ -4568,13 +4568,13 @@
     </row>
     <row r="83" spans="1:12" ht="26">
       <c r="A83" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C83" s="62" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>136</v>
@@ -4589,7 +4589,7 @@
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>26</v>
@@ -4598,13 +4598,13 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="47" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B84" s="46" t="s">
         <v>131</v>
       </c>
       <c r="C84" s="62" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>138</v>
@@ -4613,13 +4613,13 @@
         <v>139</v>
       </c>
       <c r="F84" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>26</v>
@@ -4628,13 +4628,13 @@
     </row>
     <row r="85" spans="1:12" ht="26">
       <c r="A85" s="47" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C85" s="62" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>140</v>
@@ -4643,13 +4643,13 @@
         <v>141</v>
       </c>
       <c r="F85" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>26</v>
@@ -4658,7 +4658,7 @@
     </row>
     <row r="86" spans="1:12" ht="38.5">
       <c r="A86" s="47" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>131</v>
@@ -4673,13 +4673,13 @@
         <v>144</v>
       </c>
       <c r="F86" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>26</v>
@@ -4688,7 +4688,7 @@
     </row>
     <row r="87" spans="1:12" ht="26">
       <c r="A87" s="47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>131</v>
@@ -4709,7 +4709,7 @@
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>26</v>
@@ -4718,7 +4718,7 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="47" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>131</v>
@@ -4727,19 +4727,19 @@
         <v>147</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F88" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>26</v>
@@ -4748,7 +4748,7 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="47" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>131</v>
@@ -4757,19 +4757,19 @@
         <v>147</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F89" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>26</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="65" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>131</v>
@@ -4787,19 +4787,19 @@
         <v>147</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F90" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>26</v>
@@ -4808,7 +4808,7 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="65" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>131</v>
@@ -4817,19 +4817,19 @@
         <v>147</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F91" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>26</v>
@@ -4838,7 +4838,7 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="65" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>131</v>
@@ -4859,7 +4859,7 @@
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
       <c r="J92" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>26</v>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="65" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>131</v>
@@ -4889,7 +4889,7 @@
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>26</v>
@@ -4898,7 +4898,7 @@
     </row>
     <row r="94" spans="1:12" ht="26">
       <c r="A94" s="65" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>131</v>
@@ -4919,7 +4919,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
       <c r="J94" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>26</v>
@@ -4928,7 +4928,7 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="65" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>131</v>
@@ -4940,18 +4940,18 @@
         <v>155</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G95" s="44" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H95" s="11"/>
       <c r="I95" s="9"/>
       <c r="J95" s="56" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>26</v>
@@ -4960,7 +4960,7 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="65" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>131</v>
@@ -4981,7 +4981,7 @@
       <c r="H96" s="11"/>
       <c r="I96" s="9"/>
       <c r="J96" s="56" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K96" s="9" t="s">
         <v>26</v>
@@ -4990,28 +4990,28 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="65" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C97" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E97" s="52" t="s">
         <v>357</v>
       </c>
-      <c r="D97" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="E97" s="52" t="s">
-        <v>359</v>
-      </c>
       <c r="F97" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
       <c r="I97" s="9"/>
       <c r="J97" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K97" s="9" t="s">
         <v>26</v>
@@ -5020,28 +5020,28 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="65" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E98" s="53" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
       <c r="I98" s="9"/>
       <c r="J98" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K98" s="9" t="s">
         <v>26</v>
@@ -5050,28 +5050,28 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="65" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E99" s="52" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G99" s="11"/>
       <c r="H99" s="11"/>
       <c r="I99" s="9"/>
       <c r="J99" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K99" s="9" t="s">
         <v>26</v>
@@ -5080,28 +5080,28 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="65" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="E100" s="52" t="s">
         <v>363</v>
       </c>
-      <c r="D100" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="E100" s="52" t="s">
-        <v>365</v>
-      </c>
       <c r="F100" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
       <c r="I100" s="9"/>
       <c r="J100" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K100" s="9" t="s">
         <v>26</v>
@@ -5110,28 +5110,28 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E101" s="52" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
       <c r="I101" s="9"/>
       <c r="J101" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K101" s="9" t="s">
         <v>26</v>
@@ -5140,28 +5140,28 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="65" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E102" s="52" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
       <c r="I102" s="9"/>
       <c r="J102" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K102" s="9" t="s">
         <v>26</v>
@@ -5170,28 +5170,28 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="65" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E103" s="53" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G103" s="11"/>
       <c r="H103" s="11"/>
       <c r="I103" s="9"/>
       <c r="J103" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K103" s="9" t="s">
         <v>26</v>
@@ -5200,28 +5200,28 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="65" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D104" s="54" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E104" s="53" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
       <c r="I104" s="9"/>
       <c r="J104" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K104" s="9" t="s">
         <v>26</v>
@@ -5230,28 +5230,28 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="65" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E105" s="53" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G105" s="11"/>
       <c r="H105" s="11"/>
       <c r="I105" s="9"/>
       <c r="J105" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K105" s="9" t="s">
         <v>26</v>
@@ -5260,28 +5260,28 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="65" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D106" s="54" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E106" s="53" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G106" s="11"/>
       <c r="H106" s="11"/>
       <c r="I106" s="9"/>
       <c r="J106" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K106" s="9" t="s">
         <v>26</v>
@@ -5290,28 +5290,28 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="65" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D107" s="54" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E107" s="53" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
       <c r="I107" s="9"/>
       <c r="J107" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K107" s="9" t="s">
         <v>26</v>
@@ -5320,28 +5320,28 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="65" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D108" s="54" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E108" s="53" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
       <c r="I108" s="9"/>
       <c r="J108" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K108" s="9" t="s">
         <v>26</v>
@@ -5350,28 +5350,28 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="65" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D109" s="54" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E109" s="53" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G109" s="11"/>
       <c r="H109" s="11"/>
       <c r="I109" s="9"/>
       <c r="J109" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K109" s="9" t="s">
         <v>26</v>
@@ -5380,28 +5380,28 @@
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="65" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D110" s="54" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E110" s="53" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F110" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
       <c r="I110" s="9"/>
       <c r="J110" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K110" s="9" t="s">
         <v>26</v>
@@ -5410,28 +5410,28 @@
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="65" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D111" s="54" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E111" s="53" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F111" s="55" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
       <c r="I111" s="9"/>
       <c r="J111" s="56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K111" s="57" t="s">
         <v>26</v>
@@ -5440,13 +5440,13 @@
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="65" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C112" s="62" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>159</v>
@@ -5459,7 +5459,7 @@
       <c r="H112" s="11"/>
       <c r="I112" s="9"/>
       <c r="J112" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K112" s="9" t="s">
         <v>26</v>
@@ -5468,19 +5468,19 @@
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="65" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C113" s="62" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D113" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="E113" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>25</v>
@@ -5489,7 +5489,7 @@
       <c r="H113" s="11"/>
       <c r="I113" s="9"/>
       <c r="J113" s="56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K113" s="9" t="s">
         <v>26</v>
@@ -5498,19 +5498,19 @@
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="65" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C114" s="62" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>162</v>
+        <v>421</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>24</v>
@@ -5519,7 +5519,7 @@
       <c r="H114" s="11"/>
       <c r="I114" s="9"/>
       <c r="J114" s="56" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K114" s="9" t="s">
         <v>26</v>
@@ -5528,19 +5528,19 @@
     </row>
     <row r="115" spans="1:12" ht="38.5">
       <c r="A115" s="65" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C115" s="62" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F115" s="7" t="s">
         <v>25</v>
@@ -5549,7 +5549,7 @@
       <c r="H115" s="11"/>
       <c r="I115" s="9"/>
       <c r="J115" s="56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K115" s="9" t="s">
         <v>26</v>
@@ -5558,19 +5558,19 @@
     </row>
     <row r="116" spans="1:12">
       <c r="A116" s="65" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C116" s="62" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F116" s="7" t="s">
         <v>24</v>
@@ -5579,7 +5579,7 @@
       <c r="H116" s="11"/>
       <c r="I116" s="9"/>
       <c r="J116" s="56" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K116" s="9" t="s">
         <v>26</v>
@@ -5588,19 +5588,19 @@
     </row>
     <row r="117" spans="1:12" ht="38.5">
       <c r="A117" s="65" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C117" s="62" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F117" s="7" t="s">
         <v>24</v>
@@ -5609,7 +5609,7 @@
       <c r="H117" s="11"/>
       <c r="I117" s="9"/>
       <c r="J117" s="56" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K117" s="9" t="s">
         <v>26</v>
@@ -5618,30 +5618,30 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="65" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C118" s="62" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E118" s="59" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F118" s="39" t="s">
         <v>39</v>
       </c>
       <c r="G118" s="39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H118" s="11"/>
       <c r="I118" s="9"/>
       <c r="J118" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K118" s="9" t="s">
         <v>26</v>
@@ -5650,19 +5650,19 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="65" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B119" s="61" t="s">
         <v>158</v>
       </c>
       <c r="C119" s="62" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D119" s="54" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E119" s="59" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F119" s="55" t="s">
         <v>24</v>
@@ -5671,7 +5671,7 @@
       <c r="H119" s="11"/>
       <c r="I119" s="58"/>
       <c r="J119" s="60" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K119" s="57" t="s">
         <v>26</v>
@@ -5680,19 +5680,19 @@
     </row>
     <row r="120" spans="1:12" ht="26">
       <c r="A120" s="65" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C120" s="62" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F120" s="7" t="s">
         <v>25</v>
@@ -5701,7 +5701,7 @@
       <c r="H120" s="11"/>
       <c r="I120" s="15"/>
       <c r="J120" s="66" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K120" s="9" t="s">
         <v>26</v>
@@ -5710,26 +5710,26 @@
     </row>
     <row r="121" spans="1:12" ht="51">
       <c r="A121" s="63" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C121" s="62" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G121" s="11"/>
       <c r="J121" s="63" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="K121" s="64" t="s">
         <v>26</v>
@@ -5742,21 +5742,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -5965,10 +5950,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
+    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5991,20 +6002,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
-    <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adjust berichtspflicht question to consent the public display of dataset
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEE534E-B3F2-45D9-AC39-288C16492F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FD7222-F6C1-4527-9B41-B4B0ADA2F209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="422">
   <si>
     <t>Unit</t>
   </si>
@@ -169,12 +169,6 @@
   </si>
   <si>
     <t>Datum bis wann die Information gültig ist</t>
-  </si>
-  <si>
-    <t>Berichts-Pflicht</t>
-  </si>
-  <si>
-    <t>Ist das Unternehmen berichtspflichtig?</t>
   </si>
   <si>
     <t>Allgemein</t>
@@ -805,9 +799,6 @@
     <t>A; B; C; D; E; F; G; H; L</t>
   </si>
   <si>
-    <t>EuTaxonomyActivityOptions</t>
-  </si>
-  <si>
     <t>13.1</t>
   </si>
   <si>
@@ -1343,6 +1334,15 @@
   </si>
   <si>
     <t>Amtszeit bis zur Trennung</t>
+  </si>
+  <si>
+    <t>Custom - Multi-Select with EuTaxoActivites</t>
+  </si>
+  <si>
+    <t>Ist das Unternehmen berichtspflichtig und mit der Veröffentlichung des Datensatzes auf Dataland einverstanden? Andernfalls ist eine weitere Dateneingabe nicht möglich.</t>
+  </si>
+  <si>
+    <t>Berichtspflicht und Einwilligung zur Veröffentlichung</t>
   </si>
 </sst>
 </file>
@@ -2060,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
@@ -2114,9 +2114,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="26">
       <c r="A2" s="32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -2125,10 +2125,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>31</v>
+        <v>421</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>32</v>
+        <v>420</v>
       </c>
       <c r="F2" s="39" t="s">
         <v>25</v>
@@ -2173,16 +2173,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>25</v>
@@ -2191,7 +2191,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
       <c r="J4" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>26</v>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>24</v>
@@ -2230,19 +2230,19 @@
     </row>
     <row r="6" spans="1:12" ht="26">
       <c r="A6" s="32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>24</v>
@@ -2263,16 +2263,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>25</v>
@@ -2281,7 +2281,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
       <c r="J7" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>26</v>
@@ -2293,22 +2293,22 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
@@ -2322,19 +2322,19 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>25</v>
@@ -2343,7 +2343,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
       <c r="J9" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>26</v>
@@ -2355,27 +2355,27 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
       <c r="J10" s="36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>26</v>
@@ -2387,25 +2387,25 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7"/>
       <c r="J11" s="36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>26</v>
@@ -2414,19 +2414,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F12" s="46" t="s">
         <v>25</v>
@@ -2437,7 +2437,7 @@
         <v>27</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>26</v>
@@ -2446,19 +2446,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="47" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F13" s="46" t="s">
         <v>25</v>
@@ -2469,7 +2469,7 @@
         <v>27</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>26</v>
@@ -2478,19 +2478,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F14" s="46" t="s">
         <v>25</v>
@@ -2501,7 +2501,7 @@
         <v>27</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>26</v>
@@ -2510,19 +2510,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>25</v>
@@ -2533,7 +2533,7 @@
         <v>27</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>26</v>
@@ -2542,28 +2542,28 @@
     </row>
     <row r="16" spans="1:12" ht="26">
       <c r="A16" s="47" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F16" s="39" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
       <c r="I16" s="7"/>
       <c r="J16" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>26</v>
@@ -2575,16 +2575,16 @@
         <v>12</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F17" s="39" t="s">
         <v>25</v>
@@ -2593,7 +2593,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="7"/>
       <c r="J17" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>26</v>
@@ -2605,19 +2605,19 @@
         <v>15</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F18" s="39" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -2632,19 +2632,19 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="47" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F19" s="39" t="s">
         <v>24</v>
@@ -2665,16 +2665,16 @@
         <v>13</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F20" s="39" t="s">
         <v>25</v>
@@ -2683,7 +2683,7 @@
       <c r="H20" s="46"/>
       <c r="I20" s="46"/>
       <c r="J20" s="50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K20" s="46" t="s">
         <v>26</v>
@@ -2692,22 +2692,22 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="47" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2722,19 +2722,19 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="47" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>24</v>
@@ -2752,19 +2752,19 @@
     </row>
     <row r="23" spans="1:12" ht="38.5">
       <c r="A23" s="47" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>24</v>
@@ -2773,7 +2773,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>26</v>
@@ -2782,19 +2782,19 @@
     </row>
     <row r="24" spans="1:12" ht="26">
       <c r="A24" s="47" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>25</v>
@@ -2803,7 +2803,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>26</v>
@@ -2815,16 +2815,16 @@
         <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>24</v>
@@ -2833,7 +2833,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="36" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>26</v>
@@ -2842,19 +2842,19 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="47" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>25</v>
@@ -2863,7 +2863,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>26</v>
@@ -2872,30 +2872,30 @@
     </row>
     <row r="27" spans="1:12" ht="26">
       <c r="A27" s="47" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" s="43" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>26</v>
@@ -2904,30 +2904,30 @@
     </row>
     <row r="28" spans="1:12" ht="26">
       <c r="A28" s="47" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>26</v>
@@ -2936,19 +2936,19 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="47" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>25</v>
@@ -2957,7 +2957,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>26</v>
@@ -2966,19 +2966,19 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="47" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>25</v>
@@ -2987,7 +2987,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>26</v>
@@ -2996,30 +2996,30 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="47" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="36" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>26</v>
@@ -3028,19 +3028,19 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="47" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>24</v>
@@ -3049,7 +3049,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="36" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>26</v>
@@ -3058,19 +3058,19 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="47" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>25</v>
@@ -3079,7 +3079,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>26</v>
@@ -3088,30 +3088,30 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="47" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="36" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>26</v>
@@ -3120,19 +3120,19 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="47" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>24</v>
@@ -3141,7 +3141,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
       <c r="J35" s="36" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>26</v>
@@ -3150,19 +3150,19 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="47" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>25</v>
@@ -3171,7 +3171,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
       <c r="J36" s="36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>26</v>
@@ -3180,30 +3180,30 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="47" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
       <c r="J37" s="36" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>26</v>
@@ -3212,19 +3212,19 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="47" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>24</v>
@@ -3233,7 +3233,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
       <c r="J38" s="36" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>26</v>
@@ -3242,19 +3242,19 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="47" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>25</v>
@@ -3263,7 +3263,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
       <c r="J39" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>26</v>
@@ -3272,19 +3272,19 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>24</v>
@@ -3293,7 +3293,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
       <c r="J40" s="36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>26</v>
@@ -3302,19 +3302,19 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>24</v>
@@ -3323,7 +3323,7 @@
       <c r="H41" s="11"/>
       <c r="I41" s="7"/>
       <c r="J41" s="36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>26</v>
@@ -3332,19 +3332,19 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>25</v>
@@ -3355,7 +3355,7 @@
         <v>27</v>
       </c>
       <c r="J42" s="36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>26</v>
@@ -3364,19 +3364,19 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="47" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>24</v>
@@ -3385,7 +3385,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
       <c r="J43" s="36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>26</v>
@@ -3394,19 +3394,19 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D44" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>310</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>313</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>25</v>
@@ -3415,7 +3415,7 @@
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
       <c r="J44" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>26</v>
@@ -3424,28 +3424,28 @@
     </row>
     <row r="45" spans="1:12" ht="26">
       <c r="A45" s="47" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F45" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
       <c r="J45" s="36" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>26</v>
@@ -3454,19 +3454,19 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="47" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>25</v>
@@ -3475,7 +3475,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
       <c r="J46" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>26</v>
@@ -3484,28 +3484,28 @@
     </row>
     <row r="47" spans="1:12" ht="26">
       <c r="A47" s="47" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
       <c r="J47" s="36" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>26</v>
@@ -3514,19 +3514,19 @@
     </row>
     <row r="48" spans="1:12" ht="26">
       <c r="A48" s="47" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>24</v>
@@ -3535,7 +3535,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
       <c r="J48" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>26</v>
@@ -3544,19 +3544,19 @@
     </row>
     <row r="49" spans="1:12" ht="26">
       <c r="A49" s="47" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>24</v>
@@ -3565,7 +3565,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
       <c r="J49" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K49" s="9" t="s">
         <v>26</v>
@@ -3574,28 +3574,28 @@
     </row>
     <row r="50" spans="1:12" ht="51">
       <c r="A50" s="47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="E50" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>83</v>
-      </c>
       <c r="F50" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
       <c r="J50" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>26</v>
@@ -3604,19 +3604,19 @@
     </row>
     <row r="51" spans="1:12" ht="38.5">
       <c r="A51" s="47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>24</v>
@@ -3625,7 +3625,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
       <c r="J51" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>26</v>
@@ -3634,19 +3634,19 @@
     </row>
     <row r="52" spans="1:12" ht="51">
       <c r="A52" s="47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>24</v>
@@ -3655,7 +3655,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
       <c r="J52" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>26</v>
@@ -3664,19 +3664,19 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>25</v>
@@ -3685,7 +3685,7 @@
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
       <c r="J53" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>26</v>
@@ -3694,19 +3694,19 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="47" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>24</v>
@@ -3715,7 +3715,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
       <c r="J54" s="36" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>26</v>
@@ -3724,19 +3724,19 @@
     </row>
     <row r="55" spans="1:12" ht="26">
       <c r="A55" s="47" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>25</v>
@@ -3745,7 +3745,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
       <c r="J55" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K55" s="9" t="s">
         <v>26</v>
@@ -3754,28 +3754,28 @@
     </row>
     <row r="56" spans="1:12" ht="42.5">
       <c r="A56" s="47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D56" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>95</v>
-      </c>
       <c r="F56" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
       <c r="J56" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K56" s="9" t="s">
         <v>26</v>
@@ -3784,19 +3784,19 @@
     </row>
     <row r="57" spans="1:12" ht="42.5">
       <c r="A57" s="47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D57" s="39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>24</v>
@@ -3805,7 +3805,7 @@
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K57" s="9" t="s">
         <v>26</v>
@@ -3814,28 +3814,28 @@
     </row>
     <row r="58" spans="1:12" ht="28.5">
       <c r="A58" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C58" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E58" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>99</v>
-      </c>
       <c r="F58" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
       <c r="J58" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K58" s="9" t="s">
         <v>26</v>
@@ -3844,19 +3844,19 @@
     </row>
     <row r="59" spans="1:12" ht="42.5">
       <c r="A59" s="47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D59" s="41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>24</v>
@@ -3865,7 +3865,7 @@
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>26</v>
@@ -3874,28 +3874,28 @@
     </row>
     <row r="60" spans="1:12" ht="42.5">
       <c r="A60" s="47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E60" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D60" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>102</v>
-      </c>
       <c r="F60" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
       <c r="J60" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>26</v>
@@ -3904,19 +3904,19 @@
     </row>
     <row r="61" spans="1:12" ht="42.5">
       <c r="A61" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>24</v>
@@ -3925,7 +3925,7 @@
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
       <c r="J61" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>26</v>
@@ -3934,28 +3934,28 @@
     </row>
     <row r="62" spans="1:12" ht="56.5">
       <c r="A62" s="47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D62" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>105</v>
-      </c>
       <c r="F62" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
       <c r="J62" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>26</v>
@@ -3964,19 +3964,19 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>24</v>
@@ -3985,7 +3985,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K63" s="9" t="s">
         <v>26</v>
@@ -3994,28 +3994,28 @@
     </row>
     <row r="64" spans="1:12" ht="38.5">
       <c r="A64" s="47" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F64" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
       <c r="J64" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>26</v>
@@ -4024,19 +4024,19 @@
     </row>
     <row r="65" spans="1:12" ht="26">
       <c r="A65" s="47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>24</v>
@@ -4045,7 +4045,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
       <c r="J65" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>26</v>
@@ -4054,19 +4054,19 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C66" s="46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>25</v>
@@ -4075,7 +4075,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
       <c r="J66" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>26</v>
@@ -4084,19 +4084,19 @@
     </row>
     <row r="67" spans="1:12" ht="51">
       <c r="A67" s="47" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>24</v>
@@ -4105,7 +4105,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="36" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>26</v>
@@ -4114,19 +4114,19 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C68" s="46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>25</v>
@@ -4135,7 +4135,7 @@
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
       <c r="J68" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>26</v>
@@ -4144,19 +4144,19 @@
     </row>
     <row r="69" spans="1:12" ht="51">
       <c r="A69" s="47" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>24</v>
@@ -4165,7 +4165,7 @@
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
       <c r="J69" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>26</v>
@@ -4174,19 +4174,19 @@
     </row>
     <row r="70" spans="1:12" ht="38.5">
       <c r="A70" s="47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C70" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E70" s="13" t="s">
         <v>119</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>121</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>25</v>
@@ -4195,7 +4195,7 @@
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
       <c r="J70" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K70" s="9" t="s">
         <v>26</v>
@@ -4204,28 +4204,28 @@
     </row>
     <row r="71" spans="1:12" ht="42.5">
       <c r="A71" s="47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F71" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
       <c r="J71" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>26</v>
@@ -4234,30 +4234,30 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="47" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E72" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D72" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>126</v>
-      </c>
       <c r="F72" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>26</v>
@@ -4266,30 +4266,28 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="47" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>242</v>
-      </c>
+        <v>419</v>
+      </c>
+      <c r="G73" s="8"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>26</v>
@@ -4298,28 +4296,28 @@
     </row>
     <row r="74" spans="1:12" ht="51">
       <c r="A74" s="47" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F74" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
       <c r="J74" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>26</v>
@@ -4328,19 +4326,19 @@
     </row>
     <row r="75" spans="1:12" ht="26">
       <c r="A75" s="47" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C75" s="62" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D75" s="54" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>25</v>
@@ -4349,7 +4347,7 @@
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>26</v>
@@ -4358,28 +4356,28 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="47" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
       <c r="J76" s="36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K76" s="9" t="s">
         <v>26</v>
@@ -4388,28 +4386,28 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="47" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
       <c r="J77" s="36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K77" s="9" t="s">
         <v>26</v>
@@ -4418,28 +4416,28 @@
     </row>
     <row r="78" spans="1:12" ht="26">
       <c r="A78" s="47" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
       <c r="J78" s="36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K78" s="9" t="s">
         <v>26</v>
@@ -4448,28 +4446,28 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="47" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C79" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="D79" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="D79" s="8" t="s">
-        <v>327</v>
-      </c>
       <c r="E79" s="13" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
       <c r="J79" s="36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>26</v>
@@ -4478,28 +4476,28 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="47" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
       <c r="J80" s="36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K80" s="9" t="s">
         <v>26</v>
@@ -4508,28 +4506,28 @@
     </row>
     <row r="81" spans="1:12" ht="26">
       <c r="A81" s="47" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
       <c r="J81" s="36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K81" s="9" t="s">
         <v>26</v>
@@ -4538,28 +4536,28 @@
     </row>
     <row r="82" spans="1:12" ht="26">
       <c r="A82" s="47" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F82" s="39" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
       <c r="J82" s="36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K82" s="9" t="s">
         <v>26</v>
@@ -4568,19 +4566,19 @@
     </row>
     <row r="83" spans="1:12" ht="26">
       <c r="A83" s="47" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C83" s="62" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>24</v>
@@ -4589,7 +4587,7 @@
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
       <c r="J83" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>26</v>
@@ -4598,28 +4596,28 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B84" s="46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C84" s="62" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F84" s="39" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
       <c r="J84" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>26</v>
@@ -4628,28 +4626,28 @@
     </row>
     <row r="85" spans="1:12" ht="26">
       <c r="A85" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C85" s="62" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F85" s="39" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
       <c r="J85" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K85" s="9" t="s">
         <v>26</v>
@@ -4658,28 +4656,28 @@
     </row>
     <row r="86" spans="1:12" ht="38.5">
       <c r="A86" s="47" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C86" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E86" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D86" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E86" s="10" t="s">
-        <v>144</v>
-      </c>
       <c r="F86" s="39" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
       <c r="J86" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>26</v>
@@ -4688,19 +4686,19 @@
     </row>
     <row r="87" spans="1:12" ht="26">
       <c r="A87" s="47" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>24</v>
@@ -4709,7 +4707,7 @@
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
       <c r="J87" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>26</v>
@@ -4718,28 +4716,28 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="47" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F88" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
       <c r="J88" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>26</v>
@@ -4748,28 +4746,28 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="47" t="s">
+        <v>343</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E89" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>349</v>
-      </c>
       <c r="F89" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
       <c r="J89" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>26</v>
@@ -4778,28 +4776,28 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="65" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F90" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
       <c r="J90" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>26</v>
@@ -4808,28 +4806,28 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="65" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F91" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
       <c r="J91" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>26</v>
@@ -4838,19 +4836,19 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="65" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C92" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E92" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>24</v>
@@ -4859,7 +4857,7 @@
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
       <c r="J92" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K92" s="9" t="s">
         <v>26</v>
@@ -4868,19 +4866,19 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="65" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E93" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F93" s="7" t="s">
         <v>24</v>
@@ -4889,7 +4887,7 @@
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
       <c r="J93" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K93" s="9" t="s">
         <v>26</v>
@@ -4898,19 +4896,19 @@
     </row>
     <row r="94" spans="1:12" ht="26">
       <c r="A94" s="65" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C94" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E94" s="13" t="s">
-        <v>154</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>25</v>
@@ -4919,7 +4917,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
       <c r="J94" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K94" s="9" t="s">
         <v>26</v>
@@ -4928,30 +4926,30 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="65" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G95" s="44" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H95" s="11"/>
       <c r="I95" s="9"/>
       <c r="J95" s="56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>26</v>
@@ -4960,19 +4958,19 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="65" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>24</v>
@@ -4981,7 +4979,7 @@
       <c r="H96" s="11"/>
       <c r="I96" s="9"/>
       <c r="J96" s="56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K96" s="9" t="s">
         <v>26</v>
@@ -4990,28 +4988,28 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="65" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E97" s="52" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
       <c r="I97" s="9"/>
       <c r="J97" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K97" s="9" t="s">
         <v>26</v>
@@ -5020,28 +5018,28 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="65" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C98" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D98" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="D98" s="8" t="s">
-        <v>358</v>
-      </c>
       <c r="E98" s="53" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
       <c r="I98" s="9"/>
       <c r="J98" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K98" s="9" t="s">
         <v>26</v>
@@ -5050,28 +5048,28 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="65" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E99" s="52" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G99" s="11"/>
       <c r="H99" s="11"/>
       <c r="I99" s="9"/>
       <c r="J99" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K99" s="9" t="s">
         <v>26</v>
@@ -5080,28 +5078,28 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="65" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E100" s="52" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
       <c r="I100" s="9"/>
       <c r="J100" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K100" s="9" t="s">
         <v>26</v>
@@ -5110,28 +5108,28 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="65" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C101" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D101" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="D101" s="8" t="s">
-        <v>364</v>
-      </c>
       <c r="E101" s="52" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
       <c r="I101" s="9"/>
       <c r="J101" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K101" s="9" t="s">
         <v>26</v>
@@ -5140,28 +5138,28 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="65" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E102" s="52" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
       <c r="I102" s="9"/>
       <c r="J102" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K102" s="9" t="s">
         <v>26</v>
@@ -5170,28 +5168,28 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="65" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C103" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D103" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="D103" s="8" t="s">
+      <c r="E103" s="53" t="s">
         <v>370</v>
       </c>
-      <c r="E103" s="53" t="s">
-        <v>373</v>
-      </c>
       <c r="F103" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G103" s="11"/>
       <c r="H103" s="11"/>
       <c r="I103" s="9"/>
       <c r="J103" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K103" s="9" t="s">
         <v>26</v>
@@ -5200,28 +5198,28 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="65" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D104" s="54" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E104" s="53" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
       <c r="I104" s="9"/>
       <c r="J104" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K104" s="9" t="s">
         <v>26</v>
@@ -5230,28 +5228,28 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="65" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E105" s="53" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G105" s="11"/>
       <c r="H105" s="11"/>
       <c r="I105" s="9"/>
       <c r="J105" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K105" s="9" t="s">
         <v>26</v>
@@ -5260,28 +5258,28 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="65" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C106" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="D106" s="54" t="s">
         <v>368</v>
       </c>
-      <c r="D106" s="54" t="s">
-        <v>371</v>
-      </c>
       <c r="E106" s="53" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G106" s="11"/>
       <c r="H106" s="11"/>
       <c r="I106" s="9"/>
       <c r="J106" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K106" s="9" t="s">
         <v>26</v>
@@ -5290,28 +5288,28 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="65" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D107" s="54" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E107" s="53" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
       <c r="I107" s="9"/>
       <c r="J107" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K107" s="9" t="s">
         <v>26</v>
@@ -5320,28 +5318,28 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="65" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D108" s="54" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E108" s="53" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
       <c r="I108" s="9"/>
       <c r="J108" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K108" s="9" t="s">
         <v>26</v>
@@ -5350,28 +5348,28 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="65" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C109" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D109" s="54" t="s">
         <v>369</v>
       </c>
-      <c r="D109" s="54" t="s">
-        <v>372</v>
-      </c>
       <c r="E109" s="53" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G109" s="11"/>
       <c r="H109" s="11"/>
       <c r="I109" s="9"/>
       <c r="J109" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K109" s="9" t="s">
         <v>26</v>
@@ -5380,28 +5378,28 @@
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="65" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D110" s="54" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E110" s="53" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F110" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
       <c r="I110" s="9"/>
       <c r="J110" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K110" s="9" t="s">
         <v>26</v>
@@ -5410,28 +5408,28 @@
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="65" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D111" s="54" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E111" s="53" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F111" s="55" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
       <c r="I111" s="9"/>
       <c r="J111" s="56" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K111" s="57" t="s">
         <v>26</v>
@@ -5440,16 +5438,16 @@
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="65" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C112" s="62" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E112" s="9"/>
       <c r="F112" s="7" t="s">
@@ -5459,7 +5457,7 @@
       <c r="H112" s="11"/>
       <c r="I112" s="9"/>
       <c r="J112" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K112" s="9" t="s">
         <v>26</v>
@@ -5468,19 +5466,19 @@
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="65" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C113" s="62" t="s">
+        <v>299</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="E113" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="C113" s="62" t="s">
-        <v>302</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>25</v>
@@ -5489,7 +5487,7 @@
       <c r="H113" s="11"/>
       <c r="I113" s="9"/>
       <c r="J113" s="56" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K113" s="9" t="s">
         <v>26</v>
@@ -5498,19 +5496,19 @@
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="65" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C114" s="62" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>24</v>
@@ -5519,7 +5517,7 @@
       <c r="H114" s="11"/>
       <c r="I114" s="9"/>
       <c r="J114" s="56" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="K114" s="9" t="s">
         <v>26</v>
@@ -5528,19 +5526,19 @@
     </row>
     <row r="115" spans="1:12" ht="38.5">
       <c r="A115" s="65" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C115" s="62" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F115" s="7" t="s">
         <v>25</v>
@@ -5549,7 +5547,7 @@
       <c r="H115" s="11"/>
       <c r="I115" s="9"/>
       <c r="J115" s="56" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K115" s="9" t="s">
         <v>26</v>
@@ -5558,19 +5556,19 @@
     </row>
     <row r="116" spans="1:12">
       <c r="A116" s="65" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C116" s="62" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F116" s="7" t="s">
         <v>24</v>
@@ -5579,7 +5577,7 @@
       <c r="H116" s="11"/>
       <c r="I116" s="9"/>
       <c r="J116" s="56" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="K116" s="9" t="s">
         <v>26</v>
@@ -5588,19 +5586,19 @@
     </row>
     <row r="117" spans="1:12" ht="38.5">
       <c r="A117" s="65" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C117" s="62" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F117" s="7" t="s">
         <v>24</v>
@@ -5609,7 +5607,7 @@
       <c r="H117" s="11"/>
       <c r="I117" s="9"/>
       <c r="J117" s="56" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="K117" s="9" t="s">
         <v>26</v>
@@ -5618,30 +5616,30 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="65" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C118" s="62" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E118" s="59" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F118" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G118" s="39" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H118" s="11"/>
       <c r="I118" s="9"/>
       <c r="J118" s="36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K118" s="9" t="s">
         <v>26</v>
@@ -5650,19 +5648,19 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="65" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B119" s="61" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C119" s="62" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D119" s="54" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E119" s="59" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F119" s="55" t="s">
         <v>24</v>
@@ -5671,7 +5669,7 @@
       <c r="H119" s="11"/>
       <c r="I119" s="58"/>
       <c r="J119" s="60" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K119" s="57" t="s">
         <v>26</v>
@@ -5680,19 +5678,19 @@
     </row>
     <row r="120" spans="1:12" ht="26">
       <c r="A120" s="65" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C120" s="62" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F120" s="7" t="s">
         <v>25</v>
@@ -5701,7 +5699,7 @@
       <c r="H120" s="11"/>
       <c r="I120" s="15"/>
       <c r="J120" s="66" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K120" s="9" t="s">
         <v>26</v>
@@ -5710,26 +5708,26 @@
     </row>
     <row r="121" spans="1:12" ht="51">
       <c r="A121" s="63" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C121" s="62" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G121" s="11"/>
       <c r="J121" s="63" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="K121" s="64" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
switch to pipes as delimiter + add full text descriptions for nace code sector options
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FD7222-F6C1-4527-9B41-B4B0ADA2F209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8083A795-8FA4-4C7B-A38A-29AE07011EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="28" r:id="rId1"/>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -778,27 +778,6 @@
     <t>Status zu G</t>
   </si>
   <si>
-    <t>Nein; Ja, Aufsichtsrat; Ja, Geschäftsleitung; Ja, Aufsichtsrat und Geschäftsleitung</t>
-  </si>
-  <si>
-    <t>jährlich; halbjährlich; vierteljährlich; monatlich</t>
-  </si>
-  <si>
-    <t>offen; geklärt</t>
-  </si>
-  <si>
-    <t>Interne Anhörung; Prüfung durch Dritte; Sowohl intern als auch von Drittanbietern</t>
-  </si>
-  <si>
-    <t>Anti-Korruption; Verhaltenskodex; Interessenkonflikte; Datenschutz; Diversität &amp; Inklusion; Faire Behandlung von Kunden; Zwangsarbeit; Gesundheit und Sicherheit; Mgt von Umweltgefahren; Verantwortungsvolles Marketing; Whistleblowing; other</t>
-  </si>
-  <si>
-    <t>NFRD; CSRD</t>
-  </si>
-  <si>
-    <t>A; B; C; D; E; F; G; H; L</t>
-  </si>
-  <si>
     <t>13.1</t>
   </si>
   <si>
@@ -1343,13 +1322,34 @@
   </si>
   <si>
     <t>Berichtspflicht und Einwilligung zur Veröffentlichung</t>
+  </si>
+  <si>
+    <t>A - Landwirtschaft, Forstwirtschaft und Fischerei| B - Bergbau und Gewinnung von Steinen und Erden|C - Verarbeitendes Gewerbe / Herstellung von Waren|D - Energieversorgung|E - Wasserversorgung; Abwasser &amp; Abfallentsorgung; Beseitigungen von Umweltverschmutzungen|F - Baugewerbe/Bau|G - Handel; Instandhaltung und Reparatur von Kraftfahrzeugen|H - Verkehr und Lagerhaltung| L - Grundstücks- und Wohnungswesen</t>
+  </si>
+  <si>
+    <t>jährlich| halbjährlich| vierteljährlich| monatlich</t>
+  </si>
+  <si>
+    <t>Nein| Ja, Aufsichtsrat| Ja, Geschäftsleitung| Ja, Aufsichtsrat und Geschäftsleitung</t>
+  </si>
+  <si>
+    <t>offen| geklärt</t>
+  </si>
+  <si>
+    <t>NFRD| CSRD</t>
+  </si>
+  <si>
+    <t>Interne Anhörung| Prüfung durch Dritte| Sowohl intern als auch von Drittanbietern</t>
+  </si>
+  <si>
+    <t>Anti-Korruption| Verhaltenskodex| Interessenkonflikte| Datenschutz| Diversität &amp; Inklusion| Faire Behandlung von Kunden| Zwangsarbeit| Gesundheit und Sicherheit| Mgt von Umweltgefahren| Verantwortungsvolles Marketing| Whistleblowing| other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1448,6 +1448,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1640,13 +1646,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1696,9 +1703,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
@@ -1772,15 +1776,6 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1842,10 +1837,42 @@
     <xf numFmtId="49" fontId="14" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{9B196376-B27D-4F96-A613-CA22D98B6E9E}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{405B915E-5C8D-407D-94B3-32C9B8B2BBC9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2060,24 +2087,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB04CA-2866-4632-9649-41001AEF9A34}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="33"/>
+    <col min="1" max="1" width="12.54296875" style="32"/>
     <col min="2" max="2" width="30.1796875" customWidth="1"/>
     <col min="3" max="3" width="22.26953125" customWidth="1"/>
     <col min="4" max="4" width="62.6328125" customWidth="1"/>
     <col min="5" max="5" width="85.54296875" customWidth="1"/>
     <col min="6" max="6" width="26.26953125" customWidth="1"/>
-    <col min="7" max="7" width="31.6328125" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" style="33"/>
+    <col min="7" max="7" width="31.6328125" style="73" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2095,7 +2122,7 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="63" t="s">
         <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2104,7 +2131,7 @@
       <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="33" t="s">
         <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -2115,7 +2142,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="26">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>171</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2125,25 +2152,25 @@
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="F2" s="39" t="s">
+        <v>413</v>
+      </c>
+      <c r="F2" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="64"/>
       <c r="H2" s="11"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="35"/>
+      <c r="J2" s="34"/>
       <c r="K2" s="9"/>
-      <c r="L2" s="46" t="s">
+      <c r="L2" s="42" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2161,25 +2188,25 @@
       <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="39"/>
+      <c r="G3" s="65"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="35"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="9"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="26">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>32</v>
@@ -2187,10 +2214,10 @@
       <c r="F4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="66"/>
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K4" s="9" t="s">
@@ -2199,17 +2226,17 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>172</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>33</v>
@@ -2217,10 +2244,10 @@
       <c r="F5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="66"/>
       <c r="H5" s="11"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="35" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="9" t="s">
@@ -2229,17 +2256,17 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="26">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>173</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>34</v>
@@ -2247,10 +2274,10 @@
       <c r="F6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="11"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="35" t="s">
         <v>7</v>
       </c>
       <c r="K6" s="9" t="s">
@@ -2259,17 +2286,17 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="26">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>35</v>
@@ -2277,10 +2304,10 @@
       <c r="F7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="66"/>
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="36" t="s">
+      <c r="J7" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K7" s="9" t="s">
@@ -2289,17 +2316,17 @@
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="26">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>36</v>
@@ -2307,12 +2334,12 @@
       <c r="F8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="45" t="s">
-        <v>239</v>
+      <c r="G8" s="67" t="s">
+        <v>415</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="35" t="s">
         <v>8</v>
       </c>
       <c r="K8" s="9" t="s">
@@ -2321,17 +2348,17 @@
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>174</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>38</v>
@@ -2339,10 +2366,10 @@
       <c r="F9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="66"/>
       <c r="H9" s="11"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K9" s="9" t="s">
@@ -2351,30 +2378,30 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="39" t="s">
-        <v>234</v>
+      <c r="G10" s="65" t="s">
+        <v>416</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="35" t="s">
         <v>174</v>
       </c>
       <c r="K10" s="9" t="s">
@@ -2383,14 +2410,14 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>41</v>
@@ -2398,13 +2425,13 @@
       <c r="E11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="46" t="s">
-        <v>289</v>
-      </c>
-      <c r="G11" s="11"/>
+      <c r="F11" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="G11" s="66"/>
       <c r="H11" s="11"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="35" t="s">
         <v>174</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -2413,126 +2440,126 @@
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>280</v>
-      </c>
-      <c r="D12" s="39" t="s">
+      <c r="C12" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="68"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="68"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="68"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="E12" s="49" t="s">
-        <v>272</v>
-      </c>
-      <c r="F12" s="46" t="s">
+      <c r="F15" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="39" t="s">
+      <c r="G15" s="68"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="47" t="s">
-        <v>176</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>280</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>269</v>
-      </c>
-      <c r="E13" s="49" t="s">
-        <v>273</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>280</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="E14" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="F14" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>280</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="E15" s="49" t="s">
-        <v>275</v>
-      </c>
-      <c r="F15" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K15" s="9" t="s">
@@ -2541,28 +2568,28 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="26">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="43" t="s">
         <v>179</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="46" t="s">
-        <v>280</v>
+      <c r="C16" s="42" t="s">
+        <v>273</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>289</v>
-      </c>
-      <c r="G16" s="8"/>
+        <v>269</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="G16" s="64"/>
       <c r="H16" s="11"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="36" t="s">
+      <c r="J16" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K16" s="9" t="s">
@@ -2571,28 +2598,28 @@
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" ht="26">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="46" t="s">
-        <v>292</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>316</v>
-      </c>
-      <c r="E17" s="49" t="s">
-        <v>290</v>
-      </c>
-      <c r="F17" s="39" t="s">
+      <c r="C17" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="F17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="8"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="11"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="36" t="s">
+      <c r="J17" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K17" s="9" t="s">
@@ -2601,28 +2628,28 @@
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="46" t="s">
-        <v>292</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>317</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>291</v>
-      </c>
-      <c r="F18" s="39" t="s">
-        <v>289</v>
-      </c>
-      <c r="G18" s="8"/>
+      <c r="C18" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="G18" s="64"/>
       <c r="H18" s="11"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="36" t="s">
+      <c r="J18" s="35" t="s">
         <v>12</v>
       </c>
       <c r="K18" s="9" t="s">
@@ -2631,28 +2658,28 @@
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="47" t="s">
-        <v>296</v>
-      </c>
-      <c r="B19" s="48" t="s">
+      <c r="A19" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B19" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="46" t="s">
-        <v>292</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>318</v>
-      </c>
-      <c r="E19" s="51" t="s">
+      <c r="C19" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="E19" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="11"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="36" t="s">
+      <c r="J19" s="35" t="s">
         <v>12</v>
       </c>
       <c r="K19" s="9" t="s">
@@ -2661,58 +2688,58 @@
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" ht="26">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="E20" s="49" t="s">
-        <v>293</v>
-      </c>
-      <c r="F20" s="39" t="s">
+      <c r="D20" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="F20" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="K20" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="L20" s="46"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="K20" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="43" t="s">
         <v>180</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="39" t="s">
-        <v>319</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>289</v>
-      </c>
-      <c r="G21" s="11"/>
+      <c r="D21" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="G21" s="66"/>
       <c r="H21" s="11"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="36" t="s">
+      <c r="J21" s="35" t="s">
         <v>13</v>
       </c>
       <c r="K21" s="9" t="s">
@@ -2721,28 +2748,28 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="47" t="s">
-        <v>297</v>
+      <c r="A22" s="43" t="s">
+        <v>290</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="39" t="s">
-        <v>320</v>
-      </c>
-      <c r="E22" s="51" t="s">
+      <c r="D22" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="E22" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="66"/>
       <c r="H22" s="11"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="36" t="s">
+      <c r="J22" s="35" t="s">
         <v>13</v>
       </c>
       <c r="K22" s="9" t="s">
@@ -2751,14 +2778,14 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" ht="38.5">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="43" t="s">
         <v>181</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>45</v>
@@ -2769,10 +2796,10 @@
       <c r="F23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="11"/>
+      <c r="G23" s="66"/>
       <c r="H23" s="11"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="36" t="s">
+      <c r="J23" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K23" s="9" t="s">
@@ -2781,14 +2808,14 @@
       <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12" ht="26">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="43" t="s">
         <v>182</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>47</v>
@@ -2799,10 +2826,10 @@
       <c r="F24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="66"/>
       <c r="H24" s="11"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="36" t="s">
+      <c r="J24" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K24" s="9" t="s">
@@ -2811,14 +2838,14 @@
       <c r="L24" s="9"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>49</v>
@@ -2829,10 +2856,10 @@
       <c r="F25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="66"/>
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="36" t="s">
+      <c r="J25" s="35" t="s">
         <v>182</v>
       </c>
       <c r="K25" s="9" t="s">
@@ -2841,14 +2868,14 @@
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="43" t="s">
         <v>183</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>51</v>
@@ -2859,10 +2886,10 @@
       <c r="F26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="11"/>
+      <c r="G26" s="66"/>
       <c r="H26" s="11"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="36" t="s">
+      <c r="J26" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K26" s="9" t="s">
@@ -2871,14 +2898,14 @@
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" ht="26">
-      <c r="A27" s="47" t="s">
-        <v>240</v>
+      <c r="A27" s="43" t="s">
+        <v>233</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>53</v>
@@ -2889,12 +2916,12 @@
       <c r="F27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="43" t="s">
-        <v>233</v>
+      <c r="G27" s="69" t="s">
+        <v>417</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="36" t="s">
+      <c r="J27" s="35" t="s">
         <v>183</v>
       </c>
       <c r="K27" s="9" t="s">
@@ -2903,14 +2930,14 @@
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="1:12" ht="26">
-      <c r="A28" s="47" t="s">
-        <v>241</v>
+      <c r="A28" s="43" t="s">
+        <v>234</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>55</v>
@@ -2921,12 +2948,12 @@
       <c r="F28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="17" t="s">
-        <v>233</v>
+      <c r="G28" s="70" t="s">
+        <v>417</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="36" t="s">
+      <c r="J28" s="35" t="s">
         <v>183</v>
       </c>
       <c r="K28" s="9" t="s">
@@ -2935,14 +2962,14 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" ht="26">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="43" t="s">
         <v>184</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>57</v>
@@ -2953,10 +2980,10 @@
       <c r="F29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="11"/>
+      <c r="G29" s="66"/>
       <c r="H29" s="11"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="36" t="s">
+      <c r="J29" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K29" s="9" t="s">
@@ -2965,28 +2992,28 @@
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="47" t="s">
-        <v>242</v>
+      <c r="A30" s="43" t="s">
+        <v>235</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D30" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="D30" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="17" t="s">
         <v>59</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="11"/>
+      <c r="G30" s="66"/>
       <c r="H30" s="11"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="36" t="s">
+      <c r="J30" s="35" t="s">
         <v>184</v>
       </c>
       <c r="K30" s="9" t="s">
@@ -2995,14 +3022,14 @@
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="47" t="s">
-        <v>243</v>
+      <c r="A31" s="43" t="s">
+        <v>236</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>231</v>
@@ -3013,13 +3040,13 @@
       <c r="F31" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>235</v>
+      <c r="G31" s="64" t="s">
+        <v>418</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="36" t="s">
-        <v>242</v>
+      <c r="J31" s="35" t="s">
+        <v>235</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>26</v>
@@ -3027,29 +3054,29 @@
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="47" t="s">
-        <v>244</v>
+      <c r="A32" s="43" t="s">
+        <v>237</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D32" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="D32" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="17" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="11"/>
+      <c r="G32" s="66"/>
       <c r="H32" s="11"/>
       <c r="I32" s="9"/>
-      <c r="J32" s="36" t="s">
-        <v>242</v>
+      <c r="J32" s="35" t="s">
+        <v>235</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>26</v>
@@ -3057,28 +3084,28 @@
       <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="47" t="s">
-        <v>245</v>
+      <c r="A33" s="43" t="s">
+        <v>238</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D33" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="D33" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="17" t="s">
         <v>62</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="11"/>
+      <c r="G33" s="66"/>
       <c r="H33" s="11"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="36" t="s">
+      <c r="J33" s="35" t="s">
         <v>184</v>
       </c>
       <c r="K33" s="9" t="s">
@@ -3087,14 +3114,14 @@
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="47" t="s">
-        <v>246</v>
+      <c r="A34" s="43" t="s">
+        <v>239</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>230</v>
@@ -3105,13 +3132,13 @@
       <c r="F34" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G34" s="8" t="s">
-        <v>235</v>
+      <c r="G34" s="64" t="s">
+        <v>418</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="36" t="s">
-        <v>245</v>
+      <c r="J34" s="35" t="s">
+        <v>238</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>26</v>
@@ -3119,29 +3146,29 @@
       <c r="L34" s="9"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="47" t="s">
-        <v>247</v>
+      <c r="A35" s="43" t="s">
+        <v>240</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D35" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="D35" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="17" t="s">
         <v>61</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="11"/>
+      <c r="G35" s="66"/>
       <c r="H35" s="11"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="36" t="s">
-        <v>245</v>
+      <c r="J35" s="35" t="s">
+        <v>238</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>26</v>
@@ -3149,28 +3176,28 @@
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="47" t="s">
-        <v>248</v>
+      <c r="A36" s="43" t="s">
+        <v>241</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D36" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="D36" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="17" t="s">
         <v>64</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="11"/>
+      <c r="G36" s="66"/>
       <c r="H36" s="11"/>
       <c r="I36" s="9"/>
-      <c r="J36" s="36" t="s">
+      <c r="J36" s="35" t="s">
         <v>184</v>
       </c>
       <c r="K36" s="9" t="s">
@@ -3179,14 +3206,14 @@
       <c r="L36" s="9"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="47" t="s">
-        <v>249</v>
+      <c r="A37" s="43" t="s">
+        <v>242</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>232</v>
@@ -3197,13 +3224,13 @@
       <c r="F37" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G37" s="8" t="s">
-        <v>235</v>
+      <c r="G37" s="64" t="s">
+        <v>418</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
-      <c r="J37" s="36" t="s">
-        <v>248</v>
+      <c r="J37" s="35" t="s">
+        <v>241</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>26</v>
@@ -3211,29 +3238,29 @@
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="47" t="s">
-        <v>250</v>
+      <c r="A38" s="43" t="s">
+        <v>243</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D38" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="D38" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="17" t="s">
         <v>61</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="11"/>
+      <c r="G38" s="66"/>
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
-      <c r="J38" s="36" t="s">
-        <v>248</v>
+      <c r="J38" s="35" t="s">
+        <v>241</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>26</v>
@@ -3241,14 +3268,14 @@
       <c r="L38" s="9"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="43" t="s">
         <v>185</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>66</v>
@@ -3259,10 +3286,10 @@
       <c r="F39" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="11"/>
+      <c r="G39" s="66"/>
       <c r="H39" s="11"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="36" t="s">
+      <c r="J39" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K39" s="9" t="s">
@@ -3271,14 +3298,14 @@
       <c r="L39" s="9"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="47" t="s">
-        <v>251</v>
+      <c r="A40" s="43" t="s">
+        <v>244</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>68</v>
@@ -3289,10 +3316,10 @@
       <c r="F40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="11"/>
+      <c r="G40" s="66"/>
       <c r="H40" s="11"/>
       <c r="I40" s="9"/>
-      <c r="J40" s="36" t="s">
+      <c r="J40" s="35" t="s">
         <v>185</v>
       </c>
       <c r="K40" s="9" t="s">
@@ -3301,28 +3328,28 @@
       <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="47" t="s">
-        <v>252</v>
+      <c r="A41" s="43" t="s">
+        <v>245</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="11"/>
+      <c r="G41" s="66"/>
       <c r="H41" s="11"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="36" t="s">
+      <c r="J41" s="35" t="s">
         <v>185</v>
       </c>
       <c r="K41" s="9" t="s">
@@ -3331,30 +3358,30 @@
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="47" t="s">
-        <v>253</v>
+      <c r="A42" s="43" t="s">
+        <v>246</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="11"/>
+      <c r="G42" s="66"/>
       <c r="H42" s="11"/>
       <c r="I42" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J42" s="36" t="s">
+      <c r="J42" s="35" t="s">
         <v>185</v>
       </c>
       <c r="K42" s="9" t="s">
@@ -3363,14 +3390,14 @@
       <c r="L42" s="9"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="47" t="s">
-        <v>413</v>
+      <c r="A43" s="43" t="s">
+        <v>406</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>71</v>
@@ -3381,10 +3408,10 @@
       <c r="F43" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="11"/>
+      <c r="G43" s="66"/>
       <c r="H43" s="11"/>
       <c r="I43" s="9"/>
-      <c r="J43" s="36" t="s">
+      <c r="J43" s="35" t="s">
         <v>185</v>
       </c>
       <c r="K43" s="9" t="s">
@@ -3393,28 +3420,28 @@
       <c r="L43" s="9"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="47" t="s">
-        <v>254</v>
+      <c r="A44" s="43" t="s">
+        <v>247</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G44" s="11"/>
+      <c r="G44" s="66"/>
       <c r="H44" s="11"/>
       <c r="I44" s="9"/>
-      <c r="J44" s="36" t="s">
+      <c r="J44" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K44" s="9" t="s">
@@ -3423,29 +3450,29 @@
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12" ht="26">
-      <c r="A45" s="47" t="s">
-        <v>312</v>
+      <c r="A45" s="43" t="s">
+        <v>305</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="E45" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="E45" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F45" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="G45" s="11"/>
+      <c r="F45" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="G45" s="66"/>
       <c r="H45" s="11"/>
       <c r="I45" s="9"/>
-      <c r="J45" s="36" t="s">
-        <v>254</v>
+      <c r="J45" s="35" t="s">
+        <v>247</v>
       </c>
       <c r="K45" s="9" t="s">
         <v>26</v>
@@ -3453,28 +3480,28 @@
       <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="47" t="s">
-        <v>313</v>
+      <c r="A46" s="43" t="s">
+        <v>306</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D46" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>304</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>311</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G46" s="11"/>
+      <c r="G46" s="66"/>
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
-      <c r="J46" s="36" t="s">
+      <c r="J46" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K46" s="9" t="s">
@@ -3483,29 +3510,29 @@
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12" ht="26">
-      <c r="A47" s="47" t="s">
-        <v>314</v>
+      <c r="A47" s="43" t="s">
+        <v>307</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C47" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="G47" s="11"/>
+      <c r="F47" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="G47" s="66"/>
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
-      <c r="J47" s="36" t="s">
-        <v>313</v>
+      <c r="J47" s="35" t="s">
+        <v>306</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>26</v>
@@ -3513,28 +3540,28 @@
       <c r="L47" s="9"/>
     </row>
     <row r="48" spans="1:12" ht="26">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="43" t="s">
         <v>186</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="18" t="s">
+      <c r="E48" s="17" t="s">
         <v>75</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="11"/>
+      <c r="G48" s="66"/>
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
-      <c r="J48" s="36" t="s">
+      <c r="J48" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K48" s="9" t="s">
@@ -3543,14 +3570,14 @@
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="26">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="43" t="s">
         <v>187</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>76</v>
@@ -3561,10 +3588,10 @@
       <c r="F49" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="11"/>
+      <c r="G49" s="66"/>
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
-      <c r="J49" s="36" t="s">
+      <c r="J49" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K49" s="9" t="s">
@@ -3573,7 +3600,7 @@
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" ht="51">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="43" t="s">
         <v>188</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -3588,13 +3615,13 @@
       <c r="E50" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F50" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G50" s="11"/>
+      <c r="F50" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G50" s="66"/>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
-      <c r="J50" s="36" t="s">
+      <c r="J50" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K50" s="9" t="s">
@@ -3603,7 +3630,7 @@
       <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12" ht="38.5">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="43" t="s">
         <v>189</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -3612,19 +3639,19 @@
       <c r="C51" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="39" t="s">
+      <c r="D51" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="17" t="s">
         <v>82</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G51" s="11"/>
+      <c r="G51" s="66"/>
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
-      <c r="J51" s="36" t="s">
+      <c r="J51" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K51" s="9" t="s">
@@ -3633,7 +3660,7 @@
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" ht="51">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="43" t="s">
         <v>190</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -3651,10 +3678,10 @@
       <c r="F52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="11"/>
+      <c r="G52" s="66"/>
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
-      <c r="J52" s="36" t="s">
+      <c r="J52" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K52" s="9" t="s">
@@ -3663,14 +3690,14 @@
       <c r="L52" s="9"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="43" t="s">
         <v>191</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>85</v>
@@ -3681,10 +3708,10 @@
       <c r="F53" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G53" s="11"/>
+      <c r="G53" s="66"/>
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
-      <c r="J53" s="36" t="s">
+      <c r="J53" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K53" s="9" t="s">
@@ -3693,14 +3720,14 @@
       <c r="L53" s="9"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="A54" s="47" t="s">
-        <v>255</v>
+      <c r="A54" s="43" t="s">
+        <v>248</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>87</v>
@@ -3711,10 +3738,10 @@
       <c r="F54" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="11"/>
+      <c r="G54" s="66"/>
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
-      <c r="J54" s="36" t="s">
+      <c r="J54" s="35" t="s">
         <v>191</v>
       </c>
       <c r="K54" s="9" t="s">
@@ -3723,14 +3750,14 @@
       <c r="L54" s="9"/>
     </row>
     <row r="55" spans="1:12" ht="26">
-      <c r="A55" s="47" t="s">
+      <c r="A55" s="43" t="s">
         <v>192</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>89</v>
@@ -3741,10 +3768,10 @@
       <c r="F55" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G55" s="11"/>
+      <c r="G55" s="66"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
-      <c r="J55" s="36" t="s">
+      <c r="J55" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K55" s="9" t="s">
@@ -3753,7 +3780,7 @@
       <c r="L55" s="9"/>
     </row>
     <row r="56" spans="1:12" ht="42.5">
-      <c r="A56" s="47" t="s">
+      <c r="A56" s="43" t="s">
         <v>193</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3765,16 +3792,16 @@
       <c r="D56" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E56" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F56" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G56" s="11"/>
+      <c r="F56" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G56" s="66"/>
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
-      <c r="J56" s="36" t="s">
+      <c r="J56" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K56" s="9" t="s">
@@ -3783,7 +3810,7 @@
       <c r="L56" s="9"/>
     </row>
     <row r="57" spans="1:12" ht="42.5">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="43" t="s">
         <v>194</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -3792,19 +3819,19 @@
       <c r="C57" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D57" s="39" t="s">
+      <c r="D57" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="20" t="s">
         <v>94</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="11"/>
+      <c r="G57" s="66"/>
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
-      <c r="J57" s="36" t="s">
+      <c r="J57" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K57" s="9" t="s">
@@ -3813,7 +3840,7 @@
       <c r="L57" s="9"/>
     </row>
     <row r="58" spans="1:12" ht="28.5">
-      <c r="A58" s="47" t="s">
+      <c r="A58" s="43" t="s">
         <v>195</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -3825,16 +3852,16 @@
       <c r="D58" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E58" s="20" t="s">
+      <c r="E58" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F58" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G58" s="11"/>
+      <c r="F58" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G58" s="66"/>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
-      <c r="J58" s="36" t="s">
+      <c r="J58" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K58" s="9" t="s">
@@ -3843,7 +3870,7 @@
       <c r="L58" s="9"/>
     </row>
     <row r="59" spans="1:12" ht="42.5">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="43" t="s">
         <v>196</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -3852,19 +3879,19 @@
       <c r="C59" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="41" t="s">
+      <c r="D59" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="E59" s="22" t="s">
+      <c r="E59" s="21" t="s">
         <v>94</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G59" s="11"/>
+      <c r="G59" s="66"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
-      <c r="J59" s="36" t="s">
+      <c r="J59" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K59" s="9" t="s">
@@ -3873,7 +3900,7 @@
       <c r="L59" s="9"/>
     </row>
     <row r="60" spans="1:12" ht="42.5">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="43" t="s">
         <v>197</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -3885,16 +3912,16 @@
       <c r="D60" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E60" s="20" t="s">
+      <c r="E60" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F60" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G60" s="11"/>
+      <c r="F60" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G60" s="66"/>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
-      <c r="J60" s="36" t="s">
+      <c r="J60" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K60" s="9" t="s">
@@ -3903,7 +3930,7 @@
       <c r="L60" s="9"/>
     </row>
     <row r="61" spans="1:12" ht="42.5">
-      <c r="A61" s="47" t="s">
+      <c r="A61" s="43" t="s">
         <v>198</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -3912,19 +3939,19 @@
       <c r="C61" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D61" s="40" t="s">
+      <c r="D61" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="E61" s="22" t="s">
+      <c r="E61" s="21" t="s">
         <v>94</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="11"/>
+      <c r="G61" s="66"/>
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
-      <c r="J61" s="36" t="s">
+      <c r="J61" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K61" s="9" t="s">
@@ -3933,7 +3960,7 @@
       <c r="L61" s="9"/>
     </row>
     <row r="62" spans="1:12" ht="56.5">
-      <c r="A62" s="47" t="s">
+      <c r="A62" s="43" t="s">
         <v>199</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -3945,16 +3972,16 @@
       <c r="D62" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F62" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G62" s="11"/>
+      <c r="F62" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G62" s="66"/>
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
-      <c r="J62" s="36" t="s">
+      <c r="J62" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K62" s="9" t="s">
@@ -3963,7 +3990,7 @@
       <c r="L62" s="9"/>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="47" t="s">
+      <c r="A63" s="43" t="s">
         <v>200</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -3972,19 +3999,19 @@
       <c r="C63" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D63" s="42" t="s">
+      <c r="D63" s="41" t="s">
         <v>229</v>
       </c>
-      <c r="E63" s="23" t="s">
+      <c r="E63" s="22" t="s">
         <v>94</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G63" s="11"/>
+      <c r="G63" s="66"/>
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
-      <c r="J63" s="36" t="s">
+      <c r="J63" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K63" s="9" t="s">
@@ -3993,7 +4020,7 @@
       <c r="L63" s="9"/>
     </row>
     <row r="64" spans="1:12" ht="38.5">
-      <c r="A64" s="47" t="s">
+      <c r="A64" s="43" t="s">
         <v>201</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -4002,19 +4029,19 @@
       <c r="C64" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D64" s="24" t="s">
+      <c r="D64" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="E64" s="25" t="s">
+      <c r="E64" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="F64" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G64" s="11"/>
+      <c r="F64" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G64" s="66"/>
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
-      <c r="J64" s="36" t="s">
+      <c r="J64" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K64" s="9" t="s">
@@ -4023,7 +4050,7 @@
       <c r="L64" s="9"/>
     </row>
     <row r="65" spans="1:12" ht="26">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="43" t="s">
         <v>202</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -4041,10 +4068,10 @@
       <c r="F65" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G65" s="11"/>
+      <c r="G65" s="66"/>
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
-      <c r="J65" s="36" t="s">
+      <c r="J65" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K65" s="9" t="s">
@@ -4053,28 +4080,28 @@
       <c r="L65" s="9"/>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="47" t="s">
+      <c r="A66" s="43" t="s">
         <v>203</v>
       </c>
-      <c r="B66" s="46" t="s">
+      <c r="B66" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="46" t="s">
+      <c r="C66" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="D66" s="26" t="s">
+      <c r="D66" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E66" s="27" t="s">
+      <c r="E66" s="26" t="s">
         <v>109</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G66" s="11"/>
+      <c r="G66" s="66"/>
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
-      <c r="J66" s="36" t="s">
+      <c r="J66" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K66" s="9" t="s">
@@ -4083,8 +4110,8 @@
       <c r="L66" s="9"/>
     </row>
     <row r="67" spans="1:12" ht="51">
-      <c r="A67" s="47" t="s">
-        <v>256</v>
+      <c r="A67" s="43" t="s">
+        <v>249</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>78</v>
@@ -4101,10 +4128,10 @@
       <c r="F67" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G67" s="11"/>
+      <c r="G67" s="66"/>
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
-      <c r="J67" s="36" t="s">
+      <c r="J67" s="35" t="s">
         <v>203</v>
       </c>
       <c r="K67" s="9" t="s">
@@ -4113,28 +4140,28 @@
       <c r="L67" s="9"/>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="47" t="s">
+      <c r="A68" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="46" t="s">
+      <c r="C68" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="D68" s="26" t="s">
+      <c r="D68" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="28" t="s">
+      <c r="E68" s="27" t="s">
         <v>114</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G68" s="11"/>
+      <c r="G68" s="66"/>
       <c r="H68" s="11"/>
       <c r="I68" s="9"/>
-      <c r="J68" s="36" t="s">
+      <c r="J68" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K68" s="9" t="s">
@@ -4143,8 +4170,8 @@
       <c r="L68" s="9"/>
     </row>
     <row r="69" spans="1:12" ht="51">
-      <c r="A69" s="47" t="s">
-        <v>257</v>
+      <c r="A69" s="43" t="s">
+        <v>250</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>78</v>
@@ -4161,10 +4188,10 @@
       <c r="F69" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G69" s="11"/>
+      <c r="G69" s="66"/>
       <c r="H69" s="11"/>
       <c r="I69" s="9"/>
-      <c r="J69" s="36" t="s">
+      <c r="J69" s="35" t="s">
         <v>204</v>
       </c>
       <c r="K69" s="9" t="s">
@@ -4173,7 +4200,7 @@
       <c r="L69" s="9"/>
     </row>
     <row r="70" spans="1:12" ht="38.5">
-      <c r="A70" s="47" t="s">
+      <c r="A70" s="43" t="s">
         <v>205</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -4191,10 +4218,10 @@
       <c r="F70" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G70" s="11"/>
+      <c r="G70" s="66"/>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
-      <c r="J70" s="36" t="s">
+      <c r="J70" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K70" s="9" t="s">
@@ -4203,7 +4230,7 @@
       <c r="L70" s="9"/>
     </row>
     <row r="71" spans="1:12" ht="42.5">
-      <c r="A71" s="47" t="s">
+      <c r="A71" s="43" t="s">
         <v>131</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -4215,16 +4242,16 @@
       <c r="D71" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E71" s="20" t="s">
+      <c r="E71" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F71" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G71" s="11"/>
+      <c r="F71" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G71" s="66"/>
       <c r="H71" s="11"/>
       <c r="I71" s="9"/>
-      <c r="J71" s="36" t="s">
+      <c r="J71" s="35" t="s">
         <v>205</v>
       </c>
       <c r="K71" s="9" t="s">
@@ -4233,7 +4260,7 @@
       <c r="L71" s="9"/>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="47" t="s">
+      <c r="A72" s="43" t="s">
         <v>206</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -4251,12 +4278,12 @@
       <c r="F72" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G72" s="7" t="s">
-        <v>238</v>
+      <c r="G72" s="71" t="s">
+        <v>419</v>
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="9"/>
-      <c r="J72" s="36" t="s">
+      <c r="J72" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K72" s="9" t="s">
@@ -4265,7 +4292,7 @@
       <c r="L72" s="9"/>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="47" t="s">
+      <c r="A73" s="43" t="s">
         <v>207</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -4281,12 +4308,12 @@
         <v>126</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="G73" s="8"/>
+        <v>412</v>
+      </c>
+      <c r="G73" s="64"/>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
-      <c r="J73" s="36" t="s">
+      <c r="J73" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K73" s="9" t="s">
@@ -4295,7 +4322,7 @@
       <c r="L73" s="9"/>
     </row>
     <row r="74" spans="1:12" ht="51">
-      <c r="A74" s="47" t="s">
+      <c r="A74" s="43" t="s">
         <v>208</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -4310,13 +4337,13 @@
       <c r="E74" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F74" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="G74" s="11"/>
+      <c r="F74" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G74" s="66"/>
       <c r="H74" s="11"/>
       <c r="I74" s="9"/>
-      <c r="J74" s="36" t="s">
+      <c r="J74" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K74" s="9" t="s">
@@ -4325,17 +4352,17 @@
       <c r="L74" s="9"/>
     </row>
     <row r="75" spans="1:12" ht="26">
-      <c r="A75" s="47" t="s">
+      <c r="A75" s="43" t="s">
         <v>209</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C75" s="62" t="s">
-        <v>321</v>
-      </c>
-      <c r="D75" s="54" t="s">
-        <v>322</v>
+      <c r="C75" s="58" t="s">
+        <v>314</v>
+      </c>
+      <c r="D75" s="50" t="s">
+        <v>315</v>
       </c>
       <c r="E75" s="13" t="s">
         <v>130</v>
@@ -4343,10 +4370,10 @@
       <c r="F75" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G75" s="11"/>
+      <c r="G75" s="66"/>
       <c r="H75" s="11"/>
       <c r="I75" s="9"/>
-      <c r="J75" s="36" t="s">
+      <c r="J75" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K75" s="9" t="s">
@@ -4355,28 +4382,28 @@
       <c r="L75" s="9"/>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="47" t="s">
-        <v>258</v>
+      <c r="A76" s="43" t="s">
+        <v>251</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C76" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E76" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>328</v>
-      </c>
       <c r="F76" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G76" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G76" s="66"/>
       <c r="H76" s="11"/>
       <c r="I76" s="9"/>
-      <c r="J76" s="36" t="s">
+      <c r="J76" s="35" t="s">
         <v>209</v>
       </c>
       <c r="K76" s="9" t="s">
@@ -4385,28 +4412,28 @@
       <c r="L76" s="9"/>
     </row>
     <row r="77" spans="1:12" ht="26">
-      <c r="A77" s="47" t="s">
-        <v>335</v>
+      <c r="A77" s="43" t="s">
+        <v>328</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G77" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G77" s="66"/>
       <c r="H77" s="11"/>
       <c r="I77" s="9"/>
-      <c r="J77" s="36" t="s">
+      <c r="J77" s="35" t="s">
         <v>209</v>
       </c>
       <c r="K77" s="9" t="s">
@@ -4415,28 +4442,28 @@
       <c r="L77" s="9"/>
     </row>
     <row r="78" spans="1:12" ht="26">
-      <c r="A78" s="47" t="s">
-        <v>336</v>
+      <c r="A78" s="43" t="s">
+        <v>329</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G78" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G78" s="66"/>
       <c r="H78" s="11"/>
       <c r="I78" s="9"/>
-      <c r="J78" s="36" t="s">
+      <c r="J78" s="35" t="s">
         <v>209</v>
       </c>
       <c r="K78" s="9" t="s">
@@ -4445,28 +4472,28 @@
       <c r="L78" s="9"/>
     </row>
     <row r="79" spans="1:12">
-      <c r="A79" s="47" t="s">
-        <v>259</v>
+      <c r="A79" s="43" t="s">
+        <v>252</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G79" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G79" s="66"/>
       <c r="H79" s="11"/>
       <c r="I79" s="9"/>
-      <c r="J79" s="36" t="s">
+      <c r="J79" s="35" t="s">
         <v>209</v>
       </c>
       <c r="K79" s="9" t="s">
@@ -4475,28 +4502,28 @@
       <c r="L79" s="9"/>
     </row>
     <row r="80" spans="1:12" ht="26">
-      <c r="A80" s="47" t="s">
-        <v>337</v>
+      <c r="A80" s="43" t="s">
+        <v>330</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G80" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G80" s="66"/>
       <c r="H80" s="11"/>
       <c r="I80" s="9"/>
-      <c r="J80" s="36" t="s">
+      <c r="J80" s="35" t="s">
         <v>209</v>
       </c>
       <c r="K80" s="9" t="s">
@@ -4505,28 +4532,28 @@
       <c r="L80" s="9"/>
     </row>
     <row r="81" spans="1:12" ht="26">
-      <c r="A81" s="47" t="s">
-        <v>338</v>
+      <c r="A81" s="43" t="s">
+        <v>331</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G81" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G81" s="66"/>
       <c r="H81" s="11"/>
       <c r="I81" s="9"/>
-      <c r="J81" s="36" t="s">
+      <c r="J81" s="35" t="s">
         <v>209</v>
       </c>
       <c r="K81" s="9" t="s">
@@ -4535,14 +4562,14 @@
       <c r="L81" s="9"/>
     </row>
     <row r="82" spans="1:12" ht="26">
-      <c r="A82" s="47" t="s">
-        <v>339</v>
+      <c r="A82" s="43" t="s">
+        <v>332</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>132</v>
@@ -4550,13 +4577,13 @@
       <c r="E82" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F82" s="39" t="s">
-        <v>340</v>
-      </c>
-      <c r="G82" s="11"/>
+      <c r="F82" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="G82" s="66"/>
       <c r="H82" s="11"/>
       <c r="I82" s="9"/>
-      <c r="J82" s="36" t="s">
+      <c r="J82" s="35" t="s">
         <v>209</v>
       </c>
       <c r="K82" s="9" t="s">
@@ -4565,14 +4592,14 @@
       <c r="L82" s="9"/>
     </row>
     <row r="83" spans="1:12" ht="26">
-      <c r="A83" s="47" t="s">
+      <c r="A83" s="43" t="s">
         <v>210</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C83" s="62" t="s">
-        <v>412</v>
+      <c r="C83" s="58" t="s">
+        <v>405</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>134</v>
@@ -4583,10 +4610,10 @@
       <c r="F83" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G83" s="11"/>
+      <c r="G83" s="66"/>
       <c r="H83" s="11"/>
       <c r="I83" s="9"/>
-      <c r="J83" s="36" t="s">
+      <c r="J83" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K83" s="9" t="s">
@@ -4595,28 +4622,28 @@
       <c r="L83" s="9"/>
     </row>
     <row r="84" spans="1:12">
-      <c r="A84" s="47" t="s">
+      <c r="A84" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="B84" s="46" t="s">
+      <c r="B84" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="C84" s="62" t="s">
-        <v>412</v>
+      <c r="C84" s="58" t="s">
+        <v>405</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E84" s="29" t="s">
+      <c r="E84" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F84" s="39" t="s">
-        <v>340</v>
-      </c>
-      <c r="G84" s="11"/>
+      <c r="F84" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="G84" s="66"/>
       <c r="H84" s="11"/>
       <c r="I84" s="9"/>
-      <c r="J84" s="36" t="s">
+      <c r="J84" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K84" s="9" t="s">
@@ -4625,14 +4652,14 @@
       <c r="L84" s="9"/>
     </row>
     <row r="85" spans="1:12" ht="26">
-      <c r="A85" s="47" t="s">
+      <c r="A85" s="43" t="s">
         <v>212</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C85" s="62" t="s">
-        <v>412</v>
+      <c r="C85" s="58" t="s">
+        <v>405</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>138</v>
@@ -4640,13 +4667,13 @@
       <c r="E85" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F85" s="39" t="s">
-        <v>340</v>
-      </c>
-      <c r="G85" s="11"/>
+      <c r="F85" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="G85" s="66"/>
       <c r="H85" s="11"/>
       <c r="I85" s="9"/>
-      <c r="J85" s="36" t="s">
+      <c r="J85" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K85" s="9" t="s">
@@ -4655,7 +4682,7 @@
       <c r="L85" s="9"/>
     </row>
     <row r="86" spans="1:12" ht="38.5">
-      <c r="A86" s="47" t="s">
+      <c r="A86" s="43" t="s">
         <v>213</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -4670,13 +4697,13 @@
       <c r="E86" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="F86" s="39" t="s">
-        <v>340</v>
-      </c>
-      <c r="G86" s="11"/>
+      <c r="F86" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="G86" s="66"/>
       <c r="H86" s="11"/>
       <c r="I86" s="9"/>
-      <c r="J86" s="36" t="s">
+      <c r="J86" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K86" s="9" t="s">
@@ -4685,7 +4712,7 @@
       <c r="L86" s="9"/>
     </row>
     <row r="87" spans="1:12" ht="26">
-      <c r="A87" s="47" t="s">
+      <c r="A87" s="43" t="s">
         <v>214</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -4703,10 +4730,10 @@
       <c r="F87" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G87" s="11"/>
+      <c r="G87" s="66"/>
       <c r="H87" s="11"/>
       <c r="I87" s="9"/>
-      <c r="J87" s="36" t="s">
+      <c r="J87" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K87" s="9" t="s">
@@ -4715,8 +4742,8 @@
       <c r="L87" s="9"/>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="47" t="s">
-        <v>344</v>
+      <c r="A88" s="43" t="s">
+        <v>337</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>129</v>
@@ -4725,18 +4752,18 @@
         <v>145</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="F88" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="G88" s="11"/>
+        <v>334</v>
+      </c>
+      <c r="F88" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="G88" s="66"/>
       <c r="H88" s="11"/>
       <c r="I88" s="9"/>
-      <c r="J88" s="36" t="s">
+      <c r="J88" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K88" s="9" t="s">
@@ -4745,8 +4772,8 @@
       <c r="L88" s="9"/>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="47" t="s">
-        <v>343</v>
+      <c r="A89" s="43" t="s">
+        <v>336</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>129</v>
@@ -4755,18 +4782,18 @@
         <v>145</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="F89" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="G89" s="11"/>
+        <v>339</v>
+      </c>
+      <c r="F89" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="G89" s="66"/>
       <c r="H89" s="11"/>
       <c r="I89" s="9"/>
-      <c r="J89" s="36" t="s">
+      <c r="J89" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K89" s="9" t="s">
@@ -4775,8 +4802,8 @@
       <c r="L89" s="9"/>
     </row>
     <row r="90" spans="1:12">
-      <c r="A90" s="65" t="s">
-        <v>393</v>
+      <c r="A90" s="61" t="s">
+        <v>386</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>129</v>
@@ -4785,18 +4812,18 @@
         <v>145</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="F90" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="G90" s="11"/>
+        <v>341</v>
+      </c>
+      <c r="F90" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="G90" s="66"/>
       <c r="H90" s="11"/>
       <c r="I90" s="9"/>
-      <c r="J90" s="36" t="s">
+      <c r="J90" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K90" s="9" t="s">
@@ -4805,8 +4832,8 @@
       <c r="L90" s="9"/>
     </row>
     <row r="91" spans="1:12">
-      <c r="A91" s="65" t="s">
-        <v>394</v>
+      <c r="A91" s="61" t="s">
+        <v>387</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>129</v>
@@ -4815,18 +4842,18 @@
         <v>145</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="F91" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="G91" s="11"/>
+        <v>343</v>
+      </c>
+      <c r="F91" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="G91" s="66"/>
       <c r="H91" s="11"/>
       <c r="I91" s="9"/>
-      <c r="J91" s="36" t="s">
+      <c r="J91" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K91" s="9" t="s">
@@ -4835,7 +4862,7 @@
       <c r="L91" s="9"/>
     </row>
     <row r="92" spans="1:12">
-      <c r="A92" s="65" t="s">
+      <c r="A92" s="61" t="s">
         <v>215</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -4853,10 +4880,10 @@
       <c r="F92" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G92" s="11"/>
+      <c r="G92" s="66"/>
       <c r="H92" s="11"/>
       <c r="I92" s="9"/>
-      <c r="J92" s="36" t="s">
+      <c r="J92" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K92" s="9" t="s">
@@ -4865,7 +4892,7 @@
       <c r="L92" s="9"/>
     </row>
     <row r="93" spans="1:12">
-      <c r="A93" s="65" t="s">
+      <c r="A93" s="61" t="s">
         <v>216</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -4877,16 +4904,16 @@
       <c r="D93" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E93" s="26" t="s">
+      <c r="E93" s="25" t="s">
         <v>149</v>
       </c>
       <c r="F93" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G93" s="11"/>
+      <c r="G93" s="66"/>
       <c r="H93" s="11"/>
       <c r="I93" s="9"/>
-      <c r="J93" s="36" t="s">
+      <c r="J93" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K93" s="9" t="s">
@@ -4895,7 +4922,7 @@
       <c r="L93" s="9"/>
     </row>
     <row r="94" spans="1:12" ht="26">
-      <c r="A94" s="65" t="s">
+      <c r="A94" s="61" t="s">
         <v>217</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -4913,10 +4940,10 @@
       <c r="F94" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G94" s="11"/>
+      <c r="G94" s="66"/>
       <c r="H94" s="11"/>
       <c r="I94" s="9"/>
-      <c r="J94" s="36" t="s">
+      <c r="J94" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K94" s="9" t="s">
@@ -4925,8 +4952,8 @@
       <c r="L94" s="9"/>
     </row>
     <row r="95" spans="1:12">
-      <c r="A95" s="65" t="s">
-        <v>395</v>
+      <c r="A95" s="61" t="s">
+        <v>388</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>129</v>
@@ -4937,18 +4964,18 @@
       <c r="D95" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E95" s="30" t="s">
-        <v>351</v>
+      <c r="E95" s="29" t="s">
+        <v>344</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G95" s="44" t="s">
-        <v>236</v>
+      <c r="G95" s="72" t="s">
+        <v>420</v>
       </c>
       <c r="H95" s="11"/>
       <c r="I95" s="9"/>
-      <c r="J95" s="56" t="s">
+      <c r="J95" s="52" t="s">
         <v>217</v>
       </c>
       <c r="K95" s="9" t="s">
@@ -4957,8 +4984,8 @@
       <c r="L95" s="9"/>
     </row>
     <row r="96" spans="1:12">
-      <c r="A96" s="65" t="s">
-        <v>396</v>
+      <c r="A96" s="61" t="s">
+        <v>389</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>129</v>
@@ -4969,16 +4996,16 @@
       <c r="D96" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E96" s="26" t="s">
+      <c r="E96" s="25" t="s">
         <v>155</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G96" s="11"/>
+      <c r="G96" s="66"/>
       <c r="H96" s="11"/>
       <c r="I96" s="9"/>
-      <c r="J96" s="56" t="s">
+      <c r="J96" s="52" t="s">
         <v>217</v>
       </c>
       <c r="K96" s="9" t="s">
@@ -4987,28 +5014,28 @@
       <c r="L96" s="9"/>
     </row>
     <row r="97" spans="1:12">
-      <c r="A97" s="65" t="s">
+      <c r="A97" s="61" t="s">
         <v>218</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E97" s="52" t="s">
-        <v>354</v>
+        <v>346</v>
+      </c>
+      <c r="E97" s="48" t="s">
+        <v>347</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G97" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G97" s="66"/>
       <c r="H97" s="11"/>
       <c r="I97" s="9"/>
-      <c r="J97" s="36" t="s">
+      <c r="J97" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K97" s="9" t="s">
@@ -5017,28 +5044,28 @@
       <c r="L97" s="9"/>
     </row>
     <row r="98" spans="1:12">
-      <c r="A98" s="65" t="s">
-        <v>397</v>
+      <c r="A98" s="61" t="s">
+        <v>390</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="E98" s="53" t="s">
-        <v>374</v>
+        <v>348</v>
+      </c>
+      <c r="E98" s="49" t="s">
+        <v>367</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G98" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G98" s="66"/>
       <c r="H98" s="11"/>
       <c r="I98" s="9"/>
-      <c r="J98" s="36" t="s">
+      <c r="J98" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K98" s="9" t="s">
@@ -5047,28 +5074,28 @@
       <c r="L98" s="9"/>
     </row>
     <row r="99" spans="1:12">
-      <c r="A99" s="65" t="s">
-        <v>398</v>
+      <c r="A99" s="61" t="s">
+        <v>391</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="E99" s="52" t="s">
-        <v>357</v>
+        <v>349</v>
+      </c>
+      <c r="E99" s="48" t="s">
+        <v>350</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G99" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G99" s="66"/>
       <c r="H99" s="11"/>
       <c r="I99" s="9"/>
-      <c r="J99" s="36" t="s">
+      <c r="J99" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K99" s="9" t="s">
@@ -5077,28 +5104,28 @@
       <c r="L99" s="9"/>
     </row>
     <row r="100" spans="1:12">
-      <c r="A100" s="65" t="s">
-        <v>260</v>
+      <c r="A100" s="61" t="s">
+        <v>253</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="E100" s="52" t="s">
-        <v>360</v>
+        <v>352</v>
+      </c>
+      <c r="E100" s="48" t="s">
+        <v>353</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G100" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G100" s="66"/>
       <c r="H100" s="11"/>
       <c r="I100" s="9"/>
-      <c r="J100" s="36" t="s">
+      <c r="J100" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K100" s="9" t="s">
@@ -5107,28 +5134,28 @@
       <c r="L100" s="9"/>
     </row>
     <row r="101" spans="1:12">
-      <c r="A101" s="65" t="s">
-        <v>261</v>
+      <c r="A101" s="61" t="s">
+        <v>254</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="E101" s="52" t="s">
-        <v>375</v>
+        <v>354</v>
+      </c>
+      <c r="E101" s="48" t="s">
+        <v>368</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G101" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G101" s="66"/>
       <c r="H101" s="11"/>
       <c r="I101" s="9"/>
-      <c r="J101" s="36" t="s">
+      <c r="J101" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K101" s="9" t="s">
@@ -5137,28 +5164,28 @@
       <c r="L101" s="9"/>
     </row>
     <row r="102" spans="1:12">
-      <c r="A102" s="65" t="s">
-        <v>399</v>
+      <c r="A102" s="61" t="s">
+        <v>392</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E102" s="52" t="s">
-        <v>363</v>
+        <v>355</v>
+      </c>
+      <c r="E102" s="48" t="s">
+        <v>356</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G102" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G102" s="66"/>
       <c r="H102" s="11"/>
       <c r="I102" s="9"/>
-      <c r="J102" s="36" t="s">
+      <c r="J102" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K102" s="9" t="s">
@@ -5167,28 +5194,28 @@
       <c r="L102" s="9"/>
     </row>
     <row r="103" spans="1:12">
-      <c r="A103" s="65" t="s">
-        <v>262</v>
+      <c r="A103" s="61" t="s">
+        <v>255</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="E103" s="53" t="s">
-        <v>370</v>
+        <v>360</v>
+      </c>
+      <c r="E103" s="49" t="s">
+        <v>363</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G103" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G103" s="66"/>
       <c r="H103" s="11"/>
       <c r="I103" s="9"/>
-      <c r="J103" s="36" t="s">
+      <c r="J103" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K103" s="9" t="s">
@@ -5197,28 +5224,28 @@
       <c r="L103" s="9"/>
     </row>
     <row r="104" spans="1:12">
-      <c r="A104" s="65" t="s">
-        <v>263</v>
+      <c r="A104" s="61" t="s">
+        <v>256</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C104" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D104" s="50" t="s">
         <v>364</v>
       </c>
-      <c r="D104" s="54" t="s">
-        <v>371</v>
-      </c>
-      <c r="E104" s="53" t="s">
-        <v>376</v>
+      <c r="E104" s="49" t="s">
+        <v>369</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G104" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G104" s="66"/>
       <c r="H104" s="11"/>
       <c r="I104" s="9"/>
-      <c r="J104" s="36" t="s">
+      <c r="J104" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K104" s="9" t="s">
@@ -5227,28 +5254,28 @@
       <c r="L104" s="9"/>
     </row>
     <row r="105" spans="1:12">
-      <c r="A105" s="65" t="s">
-        <v>264</v>
+      <c r="A105" s="61" t="s">
+        <v>257</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E105" s="53" t="s">
-        <v>377</v>
+        <v>355</v>
+      </c>
+      <c r="E105" s="49" t="s">
+        <v>370</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G105" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G105" s="66"/>
       <c r="H105" s="11"/>
       <c r="I105" s="9"/>
-      <c r="J105" s="36" t="s">
+      <c r="J105" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K105" s="9" t="s">
@@ -5257,28 +5284,28 @@
       <c r="L105" s="9"/>
     </row>
     <row r="106" spans="1:12">
-      <c r="A106" s="65" t="s">
-        <v>265</v>
+      <c r="A106" s="61" t="s">
+        <v>258</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="D106" s="54" t="s">
-        <v>368</v>
-      </c>
-      <c r="E106" s="53" t="s">
-        <v>380</v>
+        <v>358</v>
+      </c>
+      <c r="D106" s="50" t="s">
+        <v>361</v>
+      </c>
+      <c r="E106" s="49" t="s">
+        <v>373</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G106" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G106" s="66"/>
       <c r="H106" s="11"/>
       <c r="I106" s="9"/>
-      <c r="J106" s="36" t="s">
+      <c r="J106" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K106" s="9" t="s">
@@ -5287,28 +5314,28 @@
       <c r="L106" s="9"/>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="65" t="s">
-        <v>400</v>
+      <c r="A107" s="61" t="s">
+        <v>393</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C107" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D107" s="50" t="s">
         <v>365</v>
       </c>
-      <c r="D107" s="54" t="s">
-        <v>372</v>
-      </c>
-      <c r="E107" s="53" t="s">
-        <v>382</v>
+      <c r="E107" s="49" t="s">
+        <v>375</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G107" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G107" s="66"/>
       <c r="H107" s="11"/>
       <c r="I107" s="9"/>
-      <c r="J107" s="36" t="s">
+      <c r="J107" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K107" s="9" t="s">
@@ -5317,28 +5344,28 @@
       <c r="L107" s="9"/>
     </row>
     <row r="108" spans="1:12">
-      <c r="A108" s="65" t="s">
-        <v>401</v>
+      <c r="A108" s="61" t="s">
+        <v>394</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="D108" s="54" t="s">
-        <v>378</v>
-      </c>
-      <c r="E108" s="53" t="s">
-        <v>383</v>
+        <v>358</v>
+      </c>
+      <c r="D108" s="50" t="s">
+        <v>371</v>
+      </c>
+      <c r="E108" s="49" t="s">
+        <v>376</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G108" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G108" s="66"/>
       <c r="H108" s="11"/>
       <c r="I108" s="9"/>
-      <c r="J108" s="36" t="s">
+      <c r="J108" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K108" s="9" t="s">
@@ -5347,28 +5374,28 @@
       <c r="L108" s="9"/>
     </row>
     <row r="109" spans="1:12">
-      <c r="A109" s="65" t="s">
-        <v>266</v>
+      <c r="A109" s="61" t="s">
+        <v>259</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="D109" s="54" t="s">
-        <v>369</v>
-      </c>
-      <c r="E109" s="53" t="s">
-        <v>381</v>
+        <v>359</v>
+      </c>
+      <c r="D109" s="50" t="s">
+        <v>362</v>
+      </c>
+      <c r="E109" s="49" t="s">
+        <v>374</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G109" s="11"/>
+        <v>296</v>
+      </c>
+      <c r="G109" s="66"/>
       <c r="H109" s="11"/>
       <c r="I109" s="9"/>
-      <c r="J109" s="36" t="s">
+      <c r="J109" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K109" s="9" t="s">
@@ -5377,28 +5404,28 @@
       <c r="L109" s="9"/>
     </row>
     <row r="110" spans="1:12">
-      <c r="A110" s="65" t="s">
-        <v>267</v>
+      <c r="A110" s="61" t="s">
+        <v>260</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C110" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D110" s="50" t="s">
         <v>366</v>
       </c>
-      <c r="D110" s="54" t="s">
-        <v>373</v>
-      </c>
-      <c r="E110" s="53" t="s">
-        <v>384</v>
-      </c>
-      <c r="F110" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="G110" s="11"/>
+      <c r="E110" s="49" t="s">
+        <v>377</v>
+      </c>
+      <c r="F110" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="G110" s="66"/>
       <c r="H110" s="11"/>
       <c r="I110" s="9"/>
-      <c r="J110" s="36" t="s">
+      <c r="J110" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K110" s="9" t="s">
@@ -5407,44 +5434,44 @@
       <c r="L110" s="9"/>
     </row>
     <row r="111" spans="1:12">
-      <c r="A111" s="65" t="s">
-        <v>392</v>
+      <c r="A111" s="61" t="s">
+        <v>385</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="D111" s="54" t="s">
-        <v>379</v>
-      </c>
-      <c r="E111" s="53" t="s">
-        <v>385</v>
-      </c>
-      <c r="F111" s="55" t="s">
-        <v>303</v>
-      </c>
-      <c r="G111" s="11"/>
+        <v>359</v>
+      </c>
+      <c r="D111" s="50" t="s">
+        <v>372</v>
+      </c>
+      <c r="E111" s="49" t="s">
+        <v>378</v>
+      </c>
+      <c r="F111" s="51" t="s">
+        <v>296</v>
+      </c>
+      <c r="G111" s="66"/>
       <c r="H111" s="11"/>
       <c r="I111" s="9"/>
-      <c r="J111" s="56" t="s">
-        <v>171</v>
-      </c>
-      <c r="K111" s="57" t="s">
+      <c r="J111" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="K111" s="53" t="s">
         <v>26</v>
       </c>
       <c r="L111" s="9"/>
     </row>
     <row r="112" spans="1:12">
-      <c r="A112" s="65" t="s">
-        <v>402</v>
+      <c r="A112" s="61" t="s">
+        <v>395</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C112" s="62" t="s">
-        <v>299</v>
+      <c r="C112" s="58" t="s">
+        <v>292</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>157</v>
@@ -5453,10 +5480,10 @@
       <c r="F112" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G112" s="11"/>
+      <c r="G112" s="66"/>
       <c r="H112" s="11"/>
       <c r="I112" s="9"/>
-      <c r="J112" s="36" t="s">
+      <c r="J112" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K112" s="9" t="s">
@@ -5465,17 +5492,17 @@
       <c r="L112" s="9"/>
     </row>
     <row r="113" spans="1:12">
-      <c r="A113" s="65" t="s">
-        <v>403</v>
+      <c r="A113" s="61" t="s">
+        <v>396</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C113" s="62" t="s">
-        <v>299</v>
+      <c r="C113" s="58" t="s">
+        <v>292</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>158</v>
@@ -5483,10 +5510,10 @@
       <c r="F113" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G113" s="11"/>
+      <c r="G113" s="66"/>
       <c r="H113" s="11"/>
       <c r="I113" s="9"/>
-      <c r="J113" s="56" t="s">
+      <c r="J113" s="52" t="s">
         <v>171</v>
       </c>
       <c r="K113" s="9" t="s">
@@ -5495,17 +5522,17 @@
       <c r="L113" s="9"/>
     </row>
     <row r="114" spans="1:12">
-      <c r="A114" s="65" t="s">
-        <v>404</v>
+      <c r="A114" s="61" t="s">
+        <v>397</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C114" s="62" t="s">
-        <v>299</v>
+      <c r="C114" s="58" t="s">
+        <v>292</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="E114" s="7" t="s">
         <v>159</v>
@@ -5513,11 +5540,11 @@
       <c r="F114" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G114" s="11"/>
+      <c r="G114" s="66"/>
       <c r="H114" s="11"/>
       <c r="I114" s="9"/>
-      <c r="J114" s="56" t="s">
-        <v>403</v>
+      <c r="J114" s="52" t="s">
+        <v>396</v>
       </c>
       <c r="K114" s="9" t="s">
         <v>26</v>
@@ -5525,14 +5552,14 @@
       <c r="L114" s="9"/>
     </row>
     <row r="115" spans="1:12" ht="38.5">
-      <c r="A115" s="65" t="s">
-        <v>405</v>
+      <c r="A115" s="61" t="s">
+        <v>398</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C115" s="62" t="s">
-        <v>389</v>
+      <c r="C115" s="58" t="s">
+        <v>382</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>160</v>
@@ -5543,10 +5570,10 @@
       <c r="F115" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G115" s="11"/>
+      <c r="G115" s="66"/>
       <c r="H115" s="11"/>
       <c r="I115" s="9"/>
-      <c r="J115" s="56" t="s">
+      <c r="J115" s="52" t="s">
         <v>171</v>
       </c>
       <c r="K115" s="9" t="s">
@@ -5555,29 +5582,29 @@
       <c r="L115" s="9"/>
     </row>
     <row r="116" spans="1:12">
-      <c r="A116" s="65" t="s">
-        <v>406</v>
+      <c r="A116" s="61" t="s">
+        <v>399</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C116" s="62" t="s">
-        <v>389</v>
-      </c>
-      <c r="D116" s="26" t="s">
+      <c r="C116" s="58" t="s">
+        <v>382</v>
+      </c>
+      <c r="D116" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="E116" s="26" t="s">
+      <c r="E116" s="25" t="s">
         <v>163</v>
       </c>
       <c r="F116" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G116" s="11"/>
+      <c r="G116" s="66"/>
       <c r="H116" s="11"/>
       <c r="I116" s="9"/>
-      <c r="J116" s="56" t="s">
-        <v>405</v>
+      <c r="J116" s="52" t="s">
+        <v>398</v>
       </c>
       <c r="K116" s="9" t="s">
         <v>26</v>
@@ -5585,14 +5612,14 @@
       <c r="L116" s="9"/>
     </row>
     <row r="117" spans="1:12" ht="38.5">
-      <c r="A117" s="65" t="s">
-        <v>407</v>
+      <c r="A117" s="61" t="s">
+        <v>400</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C117" s="62" t="s">
-        <v>389</v>
+      <c r="C117" s="58" t="s">
+        <v>382</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>164</v>
@@ -5603,11 +5630,11 @@
       <c r="F117" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G117" s="11"/>
+      <c r="G117" s="66"/>
       <c r="H117" s="11"/>
       <c r="I117" s="9"/>
-      <c r="J117" s="56" t="s">
-        <v>405</v>
+      <c r="J117" s="52" t="s">
+        <v>398</v>
       </c>
       <c r="K117" s="9" t="s">
         <v>26</v>
@@ -5615,30 +5642,30 @@
       <c r="L117" s="9"/>
     </row>
     <row r="118" spans="1:12">
-      <c r="A118" s="65" t="s">
-        <v>408</v>
+      <c r="A118" s="61" t="s">
+        <v>401</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C118" s="62" t="s">
-        <v>390</v>
+      <c r="C118" s="58" t="s">
+        <v>383</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="E118" s="59" t="s">
-        <v>386</v>
-      </c>
-      <c r="F118" s="39" t="s">
+      <c r="E118" s="55" t="s">
+        <v>379</v>
+      </c>
+      <c r="F118" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="G118" s="39" t="s">
-        <v>237</v>
+      <c r="G118" s="65" t="s">
+        <v>421</v>
       </c>
       <c r="H118" s="11"/>
       <c r="I118" s="9"/>
-      <c r="J118" s="36" t="s">
+      <c r="J118" s="35" t="s">
         <v>171</v>
       </c>
       <c r="K118" s="9" t="s">
@@ -5647,44 +5674,44 @@
       <c r="L118" s="9"/>
     </row>
     <row r="119" spans="1:12">
-      <c r="A119" s="65" t="s">
-        <v>409</v>
-      </c>
-      <c r="B119" s="61" t="s">
+      <c r="A119" s="61" t="s">
+        <v>402</v>
+      </c>
+      <c r="B119" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="C119" s="62" t="s">
-        <v>390</v>
-      </c>
-      <c r="D119" s="54" t="s">
-        <v>388</v>
-      </c>
-      <c r="E119" s="59" t="s">
-        <v>387</v>
-      </c>
-      <c r="F119" s="55" t="s">
+      <c r="C119" s="58" t="s">
+        <v>383</v>
+      </c>
+      <c r="D119" s="50" t="s">
+        <v>381</v>
+      </c>
+      <c r="E119" s="55" t="s">
+        <v>380</v>
+      </c>
+      <c r="F119" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="G119" s="39"/>
+      <c r="G119" s="65"/>
       <c r="H119" s="11"/>
-      <c r="I119" s="58"/>
-      <c r="J119" s="60" t="s">
-        <v>171</v>
-      </c>
-      <c r="K119" s="57" t="s">
+      <c r="I119" s="54"/>
+      <c r="J119" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="K119" s="53" t="s">
         <v>26</v>
       </c>
       <c r="L119" s="9"/>
     </row>
     <row r="120" spans="1:12" ht="26">
-      <c r="A120" s="65" t="s">
-        <v>410</v>
+      <c r="A120" s="61" t="s">
+        <v>403</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C120" s="62" t="s">
-        <v>391</v>
+      <c r="C120" s="58" t="s">
+        <v>384</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>167</v>
@@ -5695,10 +5722,10 @@
       <c r="F120" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G120" s="11"/>
+      <c r="G120" s="66"/>
       <c r="H120" s="11"/>
       <c r="I120" s="15"/>
-      <c r="J120" s="66" t="s">
+      <c r="J120" s="62" t="s">
         <v>171</v>
       </c>
       <c r="K120" s="9" t="s">
@@ -5707,14 +5734,14 @@
       <c r="L120" s="9"/>
     </row>
     <row r="121" spans="1:12" ht="51">
-      <c r="A121" s="63" t="s">
-        <v>411</v>
+      <c r="A121" s="59" t="s">
+        <v>404</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C121" s="62" t="s">
-        <v>391</v>
+      <c r="C121" s="58" t="s">
+        <v>384</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>169</v>
@@ -5725,11 +5752,11 @@
       <c r="F121" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G121" s="11"/>
-      <c r="J121" s="63" t="s">
-        <v>410</v>
-      </c>
-      <c r="K121" s="64" t="s">
+      <c r="G121" s="66"/>
+      <c r="J121" s="59" t="s">
+        <v>403</v>
+      </c>
+      <c r="K121" s="60" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5949,18 +5976,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5983,6 +6010,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5997,12 +6032,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
review comment - Baugewerbe / Bau
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB53F11-353F-41FE-BB0D-7FF8F14DC2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADDA1D5-2FB2-4A12-8235-2EA3F9E38F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -864,9 +864,6 @@
     <t>Auflistung der Sektoren</t>
   </si>
   <si>
-    <t>A - Landwirtschaft, Forstwirtschaft und Fischerei| B - Bergbau und Gewinnung von Steinen und Erden|C - Verarbeitendes Gewerbe / Herstellung von Waren|D - Energieversorgung|E - Wasserversorgung; Abwasser &amp; Abfallentsorgung; Beseitigungen von Umweltverschmutzungen|F - Baugewerbe/Bau|G - Handel; Instandhaltung und Reparatur von Kraftfahrzeugen|H - Verkehr und Lagerhaltung| L - Grundstücks- und Wohnungswesen</t>
-  </si>
-  <si>
     <t>ESG Berichte</t>
   </si>
   <si>
@@ -1351,6 +1348,9 @@
   </si>
   <si>
     <t>Ist das Unternehmen berichtspflichtig im Rahmen der CSRD-Richtlinie bzw. ist es gemäß den Offenlegungspflichten der Artikel 19a und 29a der Richtilinie 2023/34/EU zur Nachhaltigkeitsberichtserstattung verpflichtet? Ist das Unternehmen außerdem mit einer Veröffentlichung des Datensatzes auf Dataland einverstanden? Anderenfalls ist eine Dateneineingabe nicht möglich.</t>
+  </si>
+  <si>
+    <t>A - Landwirtschaft, Forstwirtschaft und Fischerei| B - Bergbau und Gewinnung von Steinen und Erden|C - Verarbeitendes Gewerbe / Herstellung von Waren|D - Energieversorgung|E - Wasserversorgung; Abwasser &amp; Abfallentsorgung; Beseitigungen von Umweltverschmutzungen|F - Baugewerbe / Bau|G - Handel; Instandhaltung und Reparatur von Kraftfahrzeugen|H - Verkehr und Lagerhaltung| L - Grundstücks- und Wohnungswesen</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2075,7 @@
   <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
@@ -2106,7 +2106,7 @@
         <v>58</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -2144,7 +2144,7 @@
         <v>252</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>64</v>
@@ -2324,7 +2324,7 @@
         <v>78</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>262</v>
+        <v>424</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="13"/>
@@ -2344,10 +2344,10 @@
         <v>71</v>
       </c>
       <c r="C9" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>263</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>264</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>80</v>
@@ -2374,19 +2374,19 @@
         <v>71</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>82</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="13"/>
@@ -2406,7 +2406,7 @@
         <v>71</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>83</v>
@@ -2415,7 +2415,7 @@
         <v>84</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -2439,10 +2439,10 @@
         <v>86</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>268</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>269</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>64</v>
@@ -2471,10 +2471,10 @@
         <v>86</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>270</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>271</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>64</v>
@@ -2503,10 +2503,10 @@
         <v>86</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>272</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>273</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>64</v>
@@ -2535,10 +2535,10 @@
         <v>86</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>274</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>275</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>64</v>
@@ -2567,13 +2567,13 @@
         <v>86</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>277</v>
-      </c>
       <c r="F16" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="12"/>
@@ -2594,13 +2594,13 @@
         <v>71</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="29" t="s">
         <v>279</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>280</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>64</v>
@@ -2624,16 +2624,16 @@
         <v>71</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="E18" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>282</v>
-      </c>
       <c r="F18" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="12"/>
@@ -2648,16 +2648,16 @@
     </row>
     <row r="19" spans="1:12" ht="14.5">
       <c r="A19" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>71</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E19" s="31" t="s">
         <v>88</v>
@@ -2687,10 +2687,10 @@
         <v>89</v>
       </c>
       <c r="D20" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>285</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>286</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>64</v>
@@ -2717,13 +2717,13 @@
         <v>89</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="E21" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="E21" s="30" t="s">
-        <v>288</v>
-      </c>
       <c r="F21" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -2738,7 +2738,7 @@
     </row>
     <row r="22" spans="1:12" ht="14.5">
       <c r="A22" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>71</v>
@@ -2747,7 +2747,7 @@
         <v>89</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E22" s="31" t="s">
         <v>88</v>
@@ -2774,7 +2774,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>91</v>
@@ -2804,7 +2804,7 @@
         <v>71</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>94</v>
@@ -2834,7 +2834,7 @@
         <v>71</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>96</v>
@@ -2864,7 +2864,7 @@
         <v>71</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>99</v>
@@ -2894,7 +2894,7 @@
         <v>71</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>101</v>
@@ -2906,7 +2906,7 @@
         <v>82</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="13"/>
@@ -2926,7 +2926,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>103</v>
@@ -2938,7 +2938,7 @@
         <v>82</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="13"/>
@@ -2958,7 +2958,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>105</v>
@@ -2988,10 +2988,10 @@
         <v>71</v>
       </c>
       <c r="C30" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>294</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>295</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>107</v>
@@ -3012,16 +3012,16 @@
     </row>
     <row r="31" spans="1:12" ht="14.5">
       <c r="A31" s="27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>108</v>
@@ -3030,7 +3030,7 @@
         <v>82</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="13"/>
@@ -3044,16 +3044,16 @@
     </row>
     <row r="32" spans="1:12" ht="14.5">
       <c r="A32" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E32" s="35" t="s">
         <v>109</v>
@@ -3080,10 +3080,10 @@
         <v>71</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>110</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="34" spans="1:12" ht="14.5">
       <c r="A34" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>112</v>
@@ -3122,7 +3122,7 @@
         <v>82</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13"/>
@@ -3136,16 +3136,16 @@
     </row>
     <row r="35" spans="1:12" ht="14.5">
       <c r="A35" s="27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E35" s="35" t="s">
         <v>109</v>
@@ -3172,10 +3172,10 @@
         <v>71</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E36" s="21" t="s">
         <v>113</v>
@@ -3196,16 +3196,16 @@
     </row>
     <row r="37" spans="1:12" ht="14.5">
       <c r="A37" s="27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>114</v>
@@ -3214,7 +3214,7 @@
         <v>82</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="13"/>
@@ -3228,16 +3228,16 @@
     </row>
     <row r="38" spans="1:12" ht="14.5">
       <c r="A38" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E38" s="35" t="s">
         <v>109</v>
@@ -3264,7 +3264,7 @@
         <v>71</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>116</v>
@@ -3294,7 +3294,7 @@
         <v>71</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>118</v>
@@ -3324,13 +3324,13 @@
         <v>71</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>120</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F41" s="19" t="s">
         <v>63</v>
@@ -3354,13 +3354,13 @@
         <v>71</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D42" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="E42" s="21" t="s">
         <v>313</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>314</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>64</v>
@@ -3386,7 +3386,7 @@
         <v>71</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>121</v>
@@ -3416,13 +3416,13 @@
         <v>71</v>
       </c>
       <c r="C44" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="E44" s="21" t="s">
         <v>316</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>317</v>
       </c>
       <c r="F44" s="19" t="s">
         <v>64</v>
@@ -3440,16 +3440,16 @@
     </row>
     <row r="45" spans="1:12" ht="26">
       <c r="A45" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E45" s="36" t="s">
         <v>124</v>
@@ -3476,13 +3476,13 @@
         <v>71</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D46" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="E46" s="21" t="s">
         <v>320</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>321</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>64</v>
@@ -3500,16 +3500,16 @@
     </row>
     <row r="47" spans="1:12" ht="26">
       <c r="A47" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E47" s="36" t="s">
         <v>124</v>
@@ -3536,7 +3536,7 @@
         <v>71</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>126</v>
@@ -3566,7 +3566,7 @@
         <v>71</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>129</v>
@@ -3602,10 +3602,10 @@
         <v>134</v>
       </c>
       <c r="E50" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="F50" s="11" t="s">
         <v>325</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>326</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
@@ -3629,10 +3629,10 @@
         <v>133</v>
       </c>
       <c r="D51" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>327</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>328</v>
       </c>
       <c r="F51" s="19" t="s">
         <v>257</v>
@@ -3686,7 +3686,7 @@
         <v>132</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>139</v>
@@ -3716,7 +3716,7 @@
         <v>132</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>141</v>
@@ -3746,7 +3746,7 @@
         <v>132</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>144</v>
@@ -3785,7 +3785,7 @@
         <v>149</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -3809,7 +3809,7 @@
         <v>147</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E57" s="38" t="s">
         <v>151</v>
@@ -3845,7 +3845,7 @@
         <v>155</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
@@ -3869,7 +3869,7 @@
         <v>153</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E59" s="39" t="s">
         <v>151</v>
@@ -3905,7 +3905,7 @@
         <v>160</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -3929,7 +3929,7 @@
         <v>158</v>
       </c>
       <c r="D61" s="41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E61" s="39" t="s">
         <v>151</v>
@@ -3965,7 +3965,7 @@
         <v>165</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
@@ -3989,7 +3989,7 @@
         <v>163</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E63" s="43" t="s">
         <v>151</v>
@@ -4022,10 +4022,10 @@
         <v>168</v>
       </c>
       <c r="E64" s="37" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="67" spans="1:12" ht="51">
       <c r="A67" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>132</v>
@@ -4235,7 +4235,7 @@
         <v>188</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
@@ -4268,7 +4268,7 @@
         <v>82</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
@@ -4297,7 +4297,7 @@
         <v>195</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G73" s="9"/>
       <c r="H73" s="12"/>
@@ -4327,7 +4327,7 @@
         <v>198</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G74" s="12"/>
       <c r="H74" s="12"/>
@@ -4348,10 +4348,10 @@
         <v>200</v>
       </c>
       <c r="C75" s="48" t="s">
+        <v>337</v>
+      </c>
+      <c r="D75" s="49" t="s">
         <v>338</v>
-      </c>
-      <c r="D75" s="49" t="s">
-        <v>339</v>
       </c>
       <c r="E75" s="21" t="s">
         <v>201</v>
@@ -4372,22 +4372,22 @@
     </row>
     <row r="76" spans="1:12" ht="14.5">
       <c r="A76" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D76" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E76" s="21" t="s">
         <v>341</v>
       </c>
-      <c r="E76" s="21" t="s">
+      <c r="F76" s="19" t="s">
         <v>342</v>
-      </c>
-      <c r="F76" s="19" t="s">
-        <v>343</v>
       </c>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
@@ -4402,22 +4402,22 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C77" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D77" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E77" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="E77" s="21" t="s">
-        <v>346</v>
-      </c>
       <c r="F77" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G77" s="12"/>
       <c r="H77" s="12"/>
@@ -4432,22 +4432,22 @@
     </row>
     <row r="78" spans="1:12" ht="26">
       <c r="A78" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D78" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="E78" s="21" t="s">
         <v>348</v>
       </c>
-      <c r="E78" s="21" t="s">
-        <v>349</v>
-      </c>
       <c r="F78" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
@@ -4462,22 +4462,22 @@
     </row>
     <row r="79" spans="1:12" ht="14.5">
       <c r="A79" s="27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D79" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="E79" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="E79" s="21" t="s">
-        <v>352</v>
-      </c>
       <c r="F79" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
@@ -4492,22 +4492,22 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D80" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E80" s="21" t="s">
         <v>354</v>
       </c>
-      <c r="E80" s="21" t="s">
-        <v>355</v>
-      </c>
       <c r="F80" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
@@ -4522,22 +4522,22 @@
     </row>
     <row r="81" spans="1:12" ht="26">
       <c r="A81" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D81" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="E81" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="E81" s="21" t="s">
-        <v>358</v>
-      </c>
       <c r="F81" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
@@ -4552,13 +4552,13 @@
     </row>
     <row r="82" spans="1:12" ht="26">
       <c r="A82" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>200</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>203</v>
@@ -4567,7 +4567,7 @@
         <v>204</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
@@ -4588,7 +4588,7 @@
         <v>200</v>
       </c>
       <c r="C83" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>206</v>
@@ -4618,7 +4618,7 @@
         <v>200</v>
       </c>
       <c r="C84" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>209</v>
@@ -4627,7 +4627,7 @@
         <v>210</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
@@ -4648,7 +4648,7 @@
         <v>200</v>
       </c>
       <c r="C85" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>212</v>
@@ -4657,7 +4657,7 @@
         <v>213</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
@@ -4687,7 +4687,7 @@
         <v>217</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
@@ -4741,13 +4741,13 @@
         <v>222</v>
       </c>
       <c r="D88" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E88" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="E88" s="10" t="s">
-        <v>363</v>
-      </c>
       <c r="F88" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
@@ -4771,13 +4771,13 @@
         <v>222</v>
       </c>
       <c r="D89" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E89" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="E89" s="10" t="s">
-        <v>365</v>
-      </c>
       <c r="F89" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
@@ -4801,13 +4801,13 @@
         <v>222</v>
       </c>
       <c r="D90" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="E90" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="E90" s="10" t="s">
-        <v>367</v>
-      </c>
       <c r="F90" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
@@ -4831,13 +4831,13 @@
         <v>222</v>
       </c>
       <c r="D91" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="E91" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="E91" s="10" t="s">
-        <v>369</v>
-      </c>
       <c r="F91" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
@@ -4954,13 +4954,13 @@
         <v>233</v>
       </c>
       <c r="E95" s="52" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F95" s="19" t="s">
         <v>82</v>
       </c>
       <c r="G95" s="53" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
@@ -5010,16 +5010,16 @@
         <v>236</v>
       </c>
       <c r="C97" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="D97" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="D97" s="9" t="s">
+      <c r="E97" s="55" t="s">
         <v>373</v>
       </c>
-      <c r="E97" s="55" t="s">
-        <v>374</v>
-      </c>
       <c r="F97" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
@@ -5040,16 +5040,16 @@
         <v>236</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D98" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="E98" s="56" t="s">
         <v>375</v>
       </c>
-      <c r="E98" s="56" t="s">
-        <v>376</v>
-      </c>
       <c r="F98" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -5070,16 +5070,16 @@
         <v>236</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D99" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="E99" s="55" t="s">
         <v>377</v>
       </c>
-      <c r="E99" s="55" t="s">
-        <v>378</v>
-      </c>
       <c r="F99" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
@@ -5094,22 +5094,22 @@
     </row>
     <row r="100" spans="1:12" ht="14.5">
       <c r="A100" s="51" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B100" s="7" t="s">
         <v>236</v>
       </c>
       <c r="C100" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D100" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="D100" s="9" t="s">
+      <c r="E100" s="55" t="s">
         <v>381</v>
       </c>
-      <c r="E100" s="55" t="s">
-        <v>382</v>
-      </c>
       <c r="F100" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
@@ -5130,16 +5130,16 @@
         <v>236</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D101" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="E101" s="55" t="s">
         <v>383</v>
       </c>
-      <c r="E101" s="55" t="s">
-        <v>384</v>
-      </c>
       <c r="F101" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
@@ -5160,16 +5160,16 @@
         <v>236</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D102" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="E102" s="55" t="s">
         <v>385</v>
       </c>
-      <c r="E102" s="55" t="s">
-        <v>386</v>
-      </c>
       <c r="F102" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
@@ -5190,16 +5190,16 @@
         <v>236</v>
       </c>
       <c r="C103" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="D103" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="D103" s="9" t="s">
+      <c r="E103" s="56" t="s">
         <v>388</v>
       </c>
-      <c r="E103" s="56" t="s">
-        <v>389</v>
-      </c>
       <c r="F103" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
@@ -5220,16 +5220,16 @@
         <v>236</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D104" s="49" t="s">
+        <v>389</v>
+      </c>
+      <c r="E104" s="56" t="s">
         <v>390</v>
       </c>
-      <c r="E104" s="56" t="s">
-        <v>391</v>
-      </c>
       <c r="F104" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
@@ -5250,16 +5250,16 @@
         <v>236</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E105" s="56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
@@ -5280,16 +5280,16 @@
         <v>236</v>
       </c>
       <c r="C106" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="D106" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="D106" s="49" t="s">
+      <c r="E106" s="56" t="s">
         <v>394</v>
       </c>
-      <c r="E106" s="56" t="s">
-        <v>395</v>
-      </c>
       <c r="F106" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
@@ -5310,16 +5310,16 @@
         <v>236</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D107" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="E107" s="56" t="s">
         <v>396</v>
       </c>
-      <c r="E107" s="56" t="s">
-        <v>397</v>
-      </c>
       <c r="F107" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
@@ -5334,22 +5334,22 @@
     </row>
     <row r="108" spans="1:12" ht="14.5">
       <c r="A108" s="51" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>236</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D108" s="49" t="s">
+        <v>398</v>
+      </c>
+      <c r="E108" s="56" t="s">
         <v>399</v>
       </c>
-      <c r="E108" s="56" t="s">
-        <v>400</v>
-      </c>
       <c r="F108" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
@@ -5370,16 +5370,16 @@
         <v>236</v>
       </c>
       <c r="C109" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D109" s="49" t="s">
         <v>401</v>
       </c>
-      <c r="D109" s="49" t="s">
+      <c r="E109" s="56" t="s">
         <v>402</v>
       </c>
-      <c r="E109" s="56" t="s">
-        <v>403</v>
-      </c>
       <c r="F109" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
@@ -5400,16 +5400,16 @@
         <v>236</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D110" s="49" t="s">
+        <v>403</v>
+      </c>
+      <c r="E110" s="56" t="s">
         <v>404</v>
       </c>
-      <c r="E110" s="56" t="s">
-        <v>405</v>
-      </c>
       <c r="F110" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
@@ -5424,22 +5424,22 @@
     </row>
     <row r="111" spans="1:12" ht="14.5">
       <c r="A111" s="51" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>236</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D111" s="49" t="s">
+        <v>406</v>
+      </c>
+      <c r="E111" s="56" t="s">
         <v>407</v>
       </c>
-      <c r="E111" s="56" t="s">
-        <v>408</v>
-      </c>
       <c r="F111" s="57" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
@@ -5460,7 +5460,7 @@
         <v>236</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>237</v>
@@ -5488,13 +5488,13 @@
         <v>236</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D113" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E113" s="19" t="s">
         <v>409</v>
-      </c>
-      <c r="E113" s="19" t="s">
-        <v>410</v>
       </c>
       <c r="F113" s="19" t="s">
         <v>64</v>
@@ -5512,26 +5512,26 @@
     </row>
     <row r="114" spans="1:12" ht="14.5">
       <c r="A114" s="51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>236</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D114" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="E114" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="E114" s="19" t="s">
-        <v>413</v>
-      </c>
       <c r="F114" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G114" s="12"/>
       <c r="H114" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I114" s="13"/>
       <c r="J114" s="54" t="s">
@@ -5550,13 +5550,13 @@
         <v>236</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E115" s="21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F115" s="19" t="s">
         <v>64</v>
@@ -5580,7 +5580,7 @@
         <v>236</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D116" s="45" t="s">
         <v>241</v>
@@ -5610,7 +5610,7 @@
         <v>236</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>243</v>
@@ -5640,19 +5640,19 @@
         <v>236</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>246</v>
       </c>
       <c r="E118" s="59" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F118" s="11" t="s">
         <v>78</v>
       </c>
       <c r="G118" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
@@ -5672,13 +5672,13 @@
         <v>236</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D119" s="49" t="s">
+        <v>419</v>
+      </c>
+      <c r="E119" s="59" t="s">
         <v>420</v>
-      </c>
-      <c r="E119" s="59" t="s">
-        <v>421</v>
       </c>
       <c r="F119" s="57" t="s">
         <v>63</v>
@@ -5702,7 +5702,7 @@
         <v>236</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>248</v>
@@ -5732,7 +5732,7 @@
         <v>236</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>250</v>
@@ -5764,6 +5764,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010004229DD89C10BE4886C46C745EFFC03E" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="608cdcb1ec278c666435d1194397a6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee3db34d-9953-4a90-95a5-b9c1d5f232f6" xmlns:ns3="7a52d84a-254c-4bf4-af91-7c6121d880be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4117238668c99f2d4b94a932e7145cc6" ns2:_="" ns3:_="">
     <xsd:import namespace="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
@@ -5972,15 +5981,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
@@ -5999,6 +5999,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6785EBB6-36D4-401E-B674-CC51897F6E00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6015,12 +6023,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803D8F69-730E-465C-932E-EF76BE31F70E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
review comment (switch from String field to FreeText field) + data dictionary update by Julia
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
+++ b/dataland-framework-toolbox/inputs/gdv/dataDictionary-GDV-VOEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\gdv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADDA1D5-2FB2-4A12-8235-2EA3F9E38F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07768A13-8C52-46EF-ABDB-576B4FF16D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="GDV-VÖB ESG questionnaire" sheetId="30" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'GDV-VÖB ESG questionnaire'!$A$1:$L$1</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -49,9 +50,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Display Filter" guid="{E1BAD6F3-699C-4A2D-8747-B0545874A2E1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{A1A164E1-D3DD-4135-A59C-2A6B8062CD43}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{020AF4D7-5EC4-4308-B8F9-6EF8545A24CC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -459,9 +460,6 @@
     <t>Wichtigste E-, S- und G-Risiken und Bewertung</t>
   </si>
   <si>
-    <t>Welches sind die wichtigsten von der Gruppe identifizierten E-, S- und G-Risiken? Bitte geben Sie die Details / Bewertung der identifizierten Risiken an.</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
@@ -525,9 +523,6 @@
     <t>Berichterstattung Energieverbrauch</t>
   </si>
   <si>
-    <t>Bitte geben Sie den Energieverbrauch (in GWh), sowie den Verbrauch erneuerbaren Energien (%) und, falls zutreffend, die Erzeugung erneuerbaren Energien (%) für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre an.</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
@@ -543,9 +538,6 @@
     <t>Berichterstattung Energieverbrauch von Immobilienvermögen</t>
   </si>
   <si>
-    <t>Bitte geben Sie den Anteil an energieeffizienten Immobilienanlagen (%) für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre an.</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
@@ -558,9 +550,6 @@
     <t>Berichterstattung Wasserverbrauch</t>
   </si>
   <si>
-    <t>Bitte geben Sie den Wasserverbrauch (in l), sowie die Emissionen in Wasser (in Tonnen) für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre an.</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
@@ -573,9 +562,6 @@
     <t>Berichterstattung Abfallproduktion</t>
   </si>
   <si>
-    <t>Bitte geben Sie die gesamte Abfallmenge (in Tonnen), sowie den Anteil (%) der gesamten Abfallmenge, der recyclet wird, sowie den Anteil (%) gefährlicher Abfall der gesamten Abfallmenge für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre an.</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -642,9 +628,6 @@
     <t>Berichterstattung Einnahmen aus fossilen Brennstoffen</t>
   </si>
   <si>
-    <t>Bitte geben Sie den Anteil (%) der Einnahmen aus fossilen Brennstoffen aus den gesamten Einnahmen für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre an.</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
@@ -672,9 +655,6 @@
     <t>Umsatz/Investitionsaufwand für nachhaltige Aktivitäten</t>
   </si>
   <si>
-    <t>Wie hoch ist der Umsatz/Investitionsaufwand des Unternehmens aus nachhaltigen Aktivitäten (Mio. €) gemäß einer Definition der EU-Taxonomie? Bitte machen Sie Angaben zu den betrachteten Sektoren und gegebenenfalls zu den Annahmen bzgl. Taxonomie-konformen (aligned) Aktivitäten für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre an.</t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
@@ -864,6 +844,9 @@
     <t>Auflistung der Sektoren</t>
   </si>
   <si>
+    <t>A - Landwirtschaft, Forstwirtschaft und Fischerei| B - Bergbau und Gewinnung von Steinen und Erden|C - Verarbeitendes Gewerbe / Herstellung von Waren|D - Energieversorgung|E - Wasserversorgung; Abwasser &amp; Abfallentsorgung; Beseitigungen von Umweltverschmutzungen|F - Baugewerbe / Bau|G - Handel; Instandhaltung und Reparatur von Kraftfahrzeugen|H - Verkehr und Lagerhaltung| L - Grundstücks- und Wohnungswesen</t>
+  </si>
+  <si>
     <t>ESG Berichte</t>
   </si>
   <si>
@@ -1050,7 +1033,10 @@
     <t>Risiken</t>
   </si>
   <si>
-    <t>Welche Treibhausgasinformationen werden derzeit auf Unternehmens-/Konzernebene berichtet und prognostiziert? Bitte geben Sie die Scope 1, Scope 2 und Scope 3 Emissionen für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre an (in tCO2-Äquiv.).</t>
+    <t>Welche sind die wichtigsten von der Gruppe identifizierten E-, S- und G-Risiken? Bitte geben Sie die Details / Bewertung der identifizierten Risiken an.</t>
+  </si>
+  <si>
+    <t>Welche Treibhausgasinformationen werden derzeit auf Unternehmens-/Konzernebene berichtet und prognostiziert? Bitte geben Sie die Scope 1, Scope 2 und Scope 3 Emissionen für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre an (in tCO2-Äquiv.).</t>
   </si>
   <si>
     <t>Custom - Rolling Window</t>
@@ -1065,30 +1051,48 @@
     <t>Produktion</t>
   </si>
   <si>
+    <t>Bitte geben Sie den Energieverbrauch (in GWh), sowie den Verbrauch erneuerbaren Energien (%) und, falls zutreffend, die Erzeugung erneuerbaren Energien (%) für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre an.</t>
+  </si>
+  <si>
     <t>Unternehmens/Gruppen Strategie bzgl Energieverbrauch</t>
   </si>
   <si>
+    <t>Bitte geben Sie den Anteil an energieeffizienten Immobilienanlagen (%) für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre an.</t>
+  </si>
+  <si>
     <t>Unternehmens/Gruppen Strategie bzgl energieeffizienten Immobilienanlagen</t>
   </si>
   <si>
+    <t>Bitte geben Sie den Wasserverbrauch (in l), sowie die Emissionen in Wasser (in Tonnen) für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre an.</t>
+  </si>
+  <si>
     <t>Unternehmens/Gruppen Strategie bzgl Wasserverbrauch</t>
   </si>
   <si>
+    <t>Bitte geben Sie die gesamte Abfallmenge (in Tonnen), sowie den Anteil (%) der gesamten Abfallmenge, der recyclet wird, sowie den Anteil (%) gefährlicher Abfall der gesamten Abfallmenge für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre an.</t>
+  </si>
+  <si>
     <t>Unternehmens/Gruppen Strategie bzgl Abfallproduktion</t>
   </si>
   <si>
-    <t>Bitte geben Sie an, wie hoch der Anteil an Recyclaten (bereits recyceltes wiederverwertetes Material) im Produktionsprozess für das aktuelle Kalenderjahr, die letzten drei Jahren sowie die Prognosen für die kommenden drei Jahre.</t>
+    <t>Bitte geben Sie an, wie hoch der Anteil an Recyclaten (bereits recyceltes wiederverwertetes Material) im Produktionsprozess für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre ist.</t>
   </si>
   <si>
     <t>34.1</t>
   </si>
   <si>
+    <t>Bitte geben Sie den Anteil (%) der Einnahmen aus fossilen Brennstoffen aus den gesamten Einnahmen für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre an.</t>
+  </si>
+  <si>
     <t>NFRD| CSRD</t>
   </si>
   <si>
     <t>Custom - Multi-Select with EuTaxoActivites</t>
   </si>
   <si>
+    <t>Wie hoch ist der Umsatz/Investitionsaufwand des Unternehmens aus nachhaltigen Aktivitäten (Mio. €) gemäß einer Definition der EU-Taxonomie? Bitte machen Sie Angaben zu den betrachteten Sektoren und gegebenenfalls zu den Annahmen bzgl. Taxonomie-konformen (aligned) Aktivitäten für das aktuelle Kalenderjahr, die letzten drei Jahre sowie die Prognosen für die kommenden drei Jahre an.</t>
+  </si>
+  <si>
     <t>Unternehmensstrukturänderungen</t>
   </si>
   <si>
@@ -1348,9 +1352,6 @@
   </si>
   <si>
     <t>Ist das Unternehmen berichtspflichtig im Rahmen der CSRD-Richtlinie bzw. ist es gemäß den Offenlegungspflichten der Artikel 19a und 29a der Richtilinie 2023/34/EU zur Nachhaltigkeitsberichtserstattung verpflichtet? Ist das Unternehmen außerdem mit einer Veröffentlichung des Datensatzes auf Dataland einverstanden? Anderenfalls ist eine Dateneineingabe nicht möglich.</t>
-  </si>
-  <si>
-    <t>A - Landwirtschaft, Forstwirtschaft und Fischerei| B - Bergbau und Gewinnung von Steinen und Erden|C - Verarbeitendes Gewerbe / Herstellung von Waren|D - Energieversorgung|E - Wasserversorgung; Abwasser &amp; Abfallentsorgung; Beseitigungen von Umweltverschmutzungen|F - Baugewerbe / Bau|G - Handel; Instandhaltung und Reparatur von Kraftfahrzeugen|H - Verkehr und Lagerhaltung| L - Grundstücks- und Wohnungswesen</t>
   </si>
 </sst>
 </file>
@@ -1661,7 +1662,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1796,12 +1797,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1850,11 +1845,11 @@
     <xf numFmtId="49" fontId="14" fillId="10" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2074,21 +2069,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2497CF0-0CBF-4E39-94FC-8209193EBA68}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="66"/>
-    <col min="2" max="2" width="30.1796875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="63"/>
+    <col min="2" max="2" width="18.26953125" style="5" customWidth="1"/>
     <col min="3" max="3" width="22.26953125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="62.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="39.54296875" style="5" customWidth="1"/>
     <col min="5" max="5" width="85.54296875" style="5" customWidth="1"/>
     <col min="6" max="6" width="26.26953125" style="5" customWidth="1"/>
     <col min="7" max="7" width="31.54296875" style="5" customWidth="1"/>
     <col min="8" max="9" width="12.54296875" style="5"/>
-    <col min="10" max="10" width="12.54296875" style="66"/>
+    <col min="10" max="10" width="12.54296875" style="63"/>
     <col min="11" max="16384" width="12.54296875" style="5"/>
   </cols>
   <sheetData>
@@ -2106,7 +2101,7 @@
         <v>58</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -2141,10 +2136,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>64</v>
@@ -2192,13 +2187,13 @@
         <v>71</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>64</v>
@@ -2222,16 +2217,16 @@
         <v>71</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -2252,16 +2247,16 @@
         <v>71</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>75</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -2282,10 +2277,10 @@
         <v>71</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>76</v>
@@ -2312,10 +2307,10 @@
         <v>71</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>77</v>
@@ -2324,7 +2319,7 @@
         <v>78</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>424</v>
+        <v>255</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="13"/>
@@ -2344,10 +2339,10 @@
         <v>71</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>80</v>
@@ -2374,19 +2369,19 @@
         <v>71</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>82</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="13"/>
@@ -2406,7 +2401,7 @@
         <v>71</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>83</v>
@@ -2415,7 +2410,7 @@
         <v>84</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -2439,10 +2434,10 @@
         <v>86</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>64</v>
@@ -2471,10 +2466,10 @@
         <v>86</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>64</v>
@@ -2503,10 +2498,10 @@
         <v>86</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>64</v>
@@ -2535,10 +2530,10 @@
         <v>86</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>64</v>
@@ -2567,13 +2562,13 @@
         <v>86</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="12"/>
@@ -2594,13 +2589,13 @@
         <v>71</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>64</v>
@@ -2624,16 +2619,16 @@
         <v>71</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="12"/>
@@ -2648,22 +2643,22 @@
     </row>
     <row r="19" spans="1:12" ht="14.5">
       <c r="A19" s="27" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>71</v>
       </c>
       <c r="C19" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>277</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>283</v>
       </c>
       <c r="E19" s="31" t="s">
         <v>88</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="12"/>
@@ -2687,10 +2682,10 @@
         <v>89</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>64</v>
@@ -2717,13 +2712,13 @@
         <v>89</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -2738,7 +2733,7 @@
     </row>
     <row r="22" spans="1:12" ht="14.5">
       <c r="A22" s="27" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>71</v>
@@ -2747,13 +2742,13 @@
         <v>89</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E22" s="31" t="s">
         <v>88</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -2774,7 +2769,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>91</v>
@@ -2783,7 +2778,7 @@
         <v>92</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
@@ -2804,7 +2799,7 @@
         <v>71</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>94</v>
@@ -2834,7 +2829,7 @@
         <v>71</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>96</v>
@@ -2843,7 +2838,7 @@
         <v>97</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
@@ -2864,7 +2859,7 @@
         <v>71</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>99</v>
@@ -2894,7 +2889,7 @@
         <v>71</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>101</v>
@@ -2906,7 +2901,7 @@
         <v>82</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="13"/>
@@ -2926,7 +2921,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>103</v>
@@ -2938,7 +2933,7 @@
         <v>82</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="13"/>
@@ -2952,13 +2947,13 @@
     </row>
     <row r="29" spans="1:12" ht="26">
       <c r="A29" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>105</v>
@@ -2988,10 +2983,10 @@
         <v>71</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>107</v>
@@ -3003,7 +2998,7 @@
       <c r="H30" s="12"/>
       <c r="I30" s="13"/>
       <c r="J30" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K30" s="13" t="s">
         <v>65</v>
@@ -3012,16 +3007,16 @@
     </row>
     <row r="31" spans="1:12" ht="14.5">
       <c r="A31" s="27" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>108</v>
@@ -3030,7 +3025,7 @@
         <v>82</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="13"/>
@@ -3044,22 +3039,22 @@
     </row>
     <row r="32" spans="1:12" ht="14.5">
       <c r="A32" s="27" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C32" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>293</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>299</v>
       </c>
       <c r="E32" s="35" t="s">
         <v>109</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
@@ -3080,10 +3075,10 @@
         <v>71</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>110</v>
@@ -3095,7 +3090,7 @@
       <c r="H33" s="12"/>
       <c r="I33" s="13"/>
       <c r="J33" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K33" s="13" t="s">
         <v>65</v>
@@ -3104,16 +3099,16 @@
     </row>
     <row r="34" spans="1:12" ht="14.5">
       <c r="A34" s="27" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>112</v>
@@ -3122,7 +3117,7 @@
         <v>82</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="13"/>
@@ -3136,22 +3131,22 @@
     </row>
     <row r="35" spans="1:12" ht="14.5">
       <c r="A35" s="27" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E35" s="35" t="s">
         <v>109</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -3172,10 +3167,10 @@
         <v>71</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E36" s="21" t="s">
         <v>113</v>
@@ -3187,7 +3182,7 @@
       <c r="H36" s="12"/>
       <c r="I36" s="13"/>
       <c r="J36" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K36" s="13" t="s">
         <v>65</v>
@@ -3196,16 +3191,16 @@
     </row>
     <row r="37" spans="1:12" ht="14.5">
       <c r="A37" s="27" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>114</v>
@@ -3214,7 +3209,7 @@
         <v>82</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="13"/>
@@ -3228,22 +3223,22 @@
     </row>
     <row r="38" spans="1:12" ht="14.5">
       <c r="A38" s="27" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E38" s="35" t="s">
         <v>109</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
@@ -3258,13 +3253,13 @@
     </row>
     <row r="39" spans="1:12" ht="14.5">
       <c r="A39" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>116</v>
@@ -3294,7 +3289,7 @@
         <v>71</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>118</v>
@@ -3309,7 +3304,7 @@
       <c r="H40" s="12"/>
       <c r="I40" s="13"/>
       <c r="J40" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K40" s="13" t="s">
         <v>65</v>
@@ -3324,13 +3319,13 @@
         <v>71</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>120</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="F41" s="19" t="s">
         <v>63</v>
@@ -3339,7 +3334,7 @@
       <c r="H41" s="12"/>
       <c r="I41" s="19"/>
       <c r="J41" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K41" s="13" t="s">
         <v>65</v>
@@ -3354,13 +3349,13 @@
         <v>71</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>64</v>
@@ -3371,7 +3366,7 @@
         <v>66</v>
       </c>
       <c r="J42" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K42" s="13" t="s">
         <v>65</v>
@@ -3386,7 +3381,7 @@
         <v>71</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>121</v>
@@ -3395,13 +3390,13 @@
         <v>122</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="13"/>
       <c r="J43" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K43" s="13" t="s">
         <v>65</v>
@@ -3416,13 +3411,13 @@
         <v>71</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F44" s="19" t="s">
         <v>64</v>
@@ -3440,16 +3435,16 @@
     </row>
     <row r="45" spans="1:12" ht="26">
       <c r="A45" s="27" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E45" s="36" t="s">
         <v>124</v>
@@ -3476,13 +3471,13 @@
         <v>71</v>
       </c>
       <c r="C46" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E46" s="21" t="s">
         <v>314</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>320</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>64</v>
@@ -3500,16 +3495,16 @@
     </row>
     <row r="47" spans="1:12" ht="26">
       <c r="A47" s="27" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E47" s="36" t="s">
         <v>124</v>
@@ -3530,22 +3525,22 @@
     </row>
     <row r="48" spans="1:12" ht="26">
       <c r="A48" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>126</v>
       </c>
       <c r="E48" s="35" t="s">
-        <v>127</v>
+        <v>318</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
@@ -3560,22 +3555,22 @@
     </row>
     <row r="49" spans="1:12" ht="26">
       <c r="A49" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D49" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E49" s="21" t="s">
-        <v>130</v>
-      </c>
       <c r="F49" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
@@ -3590,22 +3585,22 @@
     </row>
     <row r="50" spans="1:12" ht="51">
       <c r="A50" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="D50" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>134</v>
-      </c>
       <c r="E50" s="10" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
@@ -3620,22 +3615,22 @@
     </row>
     <row r="51" spans="1:12" ht="38.5">
       <c r="A51" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="D51" s="11" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
@@ -3650,22 +3645,22 @@
     </row>
     <row r="52" spans="1:12" ht="51">
       <c r="A52" s="27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="D52" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="E52" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="F52" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
@@ -3680,19 +3675,19 @@
     </row>
     <row r="53" spans="1:12" ht="14.5">
       <c r="A53" s="27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D53" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="F53" s="19" t="s">
         <v>64</v>
@@ -3713,25 +3708,25 @@
         <v>45</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D54" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="E54" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="F54" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
       <c r="J54" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K54" s="13" t="s">
         <v>65</v>
@@ -3740,19 +3735,19 @@
     </row>
     <row r="55" spans="1:12" ht="26">
       <c r="A55" s="27" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D55" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="21" t="s">
         <v>144</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>145</v>
       </c>
       <c r="F55" s="19" t="s">
         <v>64</v>
@@ -3768,24 +3763,24 @@
       </c>
       <c r="L55" s="13"/>
     </row>
-    <row r="56" spans="1:12" ht="42.5">
+    <row r="56" spans="1:12" ht="72" customHeight="1">
       <c r="A56" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>148</v>
-      </c>
       <c r="E56" s="37" t="s">
-        <v>149</v>
+        <v>324</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -3800,22 +3795,22 @@
     </row>
     <row r="57" spans="1:12" ht="42.5">
       <c r="A57" s="27" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E57" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -3828,24 +3823,24 @@
       </c>
       <c r="L57" s="13"/>
     </row>
-    <row r="58" spans="1:12" ht="28.5">
+    <row r="58" spans="1:12" ht="55.5" customHeight="1">
       <c r="A58" s="27" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E58" s="37" t="s">
-        <v>155</v>
+        <v>326</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
@@ -3860,22 +3855,22 @@
     </row>
     <row r="59" spans="1:12" ht="42.5">
       <c r="A59" s="27" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
@@ -3890,22 +3885,22 @@
     </row>
     <row r="60" spans="1:12" ht="42.5">
       <c r="A60" s="27" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E60" s="37" t="s">
-        <v>160</v>
+        <v>328</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -3920,22 +3915,22 @@
     </row>
     <row r="61" spans="1:12" ht="42.5">
       <c r="A61" s="27" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D61" s="41" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
@@ -3950,22 +3945,22 @@
     </row>
     <row r="62" spans="1:12" ht="56.5">
       <c r="A62" s="27" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E62" s="37" t="s">
-        <v>165</v>
+        <v>330</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
@@ -3980,22 +3975,22 @@
     </row>
     <row r="63" spans="1:12" ht="14.5">
       <c r="A63" s="27" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
@@ -4010,22 +4005,22 @@
     </row>
     <row r="64" spans="1:12" ht="42.5">
       <c r="A64" s="27" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C64" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D64" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="D64" s="44" t="s">
-        <v>168</v>
-      </c>
       <c r="E64" s="37" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -4040,22 +4035,22 @@
     </row>
     <row r="65" spans="1:12" ht="26">
       <c r="A65" s="27" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
@@ -4068,21 +4063,21 @@
       </c>
       <c r="L65" s="13"/>
     </row>
-    <row r="66" spans="1:12" ht="14.5">
+    <row r="66" spans="1:12" ht="26">
       <c r="A66" s="27" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="E66" s="46" t="s">
-        <v>174</v>
+        <v>168</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="F66" s="19" t="s">
         <v>64</v>
@@ -4100,49 +4095,49 @@
     </row>
     <row r="67" spans="1:12" ht="51">
       <c r="A67" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
       <c r="J67" s="22" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="K67" s="13" t="s">
         <v>65</v>
       </c>
       <c r="L67" s="13"/>
     </row>
-    <row r="68" spans="1:12" ht="14.5">
+    <row r="68" spans="1:12" ht="26">
       <c r="A68" s="27" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C68" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E68" s="21" t="s">
         <v>175</v>
-      </c>
-      <c r="D68" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="E68" s="47" t="s">
-        <v>180</v>
       </c>
       <c r="F68" s="19" t="s">
         <v>64</v>
@@ -4163,25 +4158,25 @@
         <v>46</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G69" s="12"/>
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
       <c r="J69" s="22" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="K69" s="13" t="s">
         <v>65</v>
@@ -4190,19 +4185,19 @@
     </row>
     <row r="70" spans="1:12" ht="38.5">
       <c r="A70" s="27" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F70" s="19" t="s">
         <v>64</v>
@@ -4220,28 +4215,28 @@
     </row>
     <row r="71" spans="1:12" ht="42.5">
       <c r="A71" s="27" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E71" s="37" t="s">
-        <v>188</v>
+        <v>334</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
       <c r="J71" s="22" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>65</v>
@@ -4250,19 +4245,19 @@
     </row>
     <row r="72" spans="1:12" ht="14.5">
       <c r="A72" s="27" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F72" s="19" t="s">
         <v>82</v>
@@ -4282,19 +4277,19 @@
     </row>
     <row r="73" spans="1:12" ht="14.5">
       <c r="A73" s="27" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F73" s="19" t="s">
         <v>336</v>
@@ -4312,22 +4307,22 @@
     </row>
     <row r="74" spans="1:12" ht="51">
       <c r="A74" s="27" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>198</v>
+        <v>337</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G74" s="12"/>
       <c r="H74" s="12"/>
@@ -4342,19 +4337,19 @@
     </row>
     <row r="75" spans="1:12" ht="26">
       <c r="A75" s="27" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C75" s="48" t="s">
-        <v>337</v>
-      </c>
-      <c r="D75" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="C75" s="46" t="s">
         <v>338</v>
       </c>
+      <c r="D75" s="47" t="s">
+        <v>339</v>
+      </c>
       <c r="E75" s="21" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F75" s="19" t="s">
         <v>64</v>
@@ -4372,28 +4367,28 @@
     </row>
     <row r="76" spans="1:12" ht="14.5">
       <c r="A76" s="27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
       <c r="J76" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K76" s="13" t="s">
         <v>65</v>
@@ -4402,28 +4397,28 @@
     </row>
     <row r="77" spans="1:12" ht="26">
       <c r="A77" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="E77" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="F77" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="E77" s="21" t="s">
-        <v>345</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>342</v>
       </c>
       <c r="G77" s="12"/>
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
       <c r="J77" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K77" s="13" t="s">
         <v>65</v>
@@ -4432,28 +4427,28 @@
     </row>
     <row r="78" spans="1:12" ht="26">
       <c r="A78" s="27" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
       <c r="J78" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K78" s="13" t="s">
         <v>65</v>
@@ -4462,28 +4457,28 @@
     </row>
     <row r="79" spans="1:12" ht="14.5">
       <c r="A79" s="27" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
       <c r="J79" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K79" s="13" t="s">
         <v>65</v>
@@ -4492,28 +4487,28 @@
     </row>
     <row r="80" spans="1:12" ht="26">
       <c r="A80" s="27" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
       <c r="J80" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K80" s="13" t="s">
         <v>65</v>
@@ -4522,28 +4517,28 @@
     </row>
     <row r="81" spans="1:12" ht="26">
       <c r="A81" s="27" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E81" s="21" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
       <c r="J81" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K81" s="13" t="s">
         <v>65</v>
@@ -4552,28 +4547,28 @@
     </row>
     <row r="82" spans="1:12" ht="26">
       <c r="A82" s="27" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
       <c r="J82" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="K82" s="13" t="s">
         <v>65</v>
@@ -4582,22 +4577,22 @@
     </row>
     <row r="83" spans="1:12" ht="26">
       <c r="A83" s="27" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B83" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E83" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="C83" s="48" t="s">
-        <v>360</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E83" s="21" t="s">
-        <v>207</v>
-      </c>
       <c r="F83" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -4612,22 +4607,22 @@
     </row>
     <row r="84" spans="1:12" ht="14.5">
       <c r="A84" s="27" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C84" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E84" s="48" t="s">
+        <v>203</v>
+      </c>
+      <c r="F84" s="11" t="s">
         <v>360</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="E84" s="50" t="s">
-        <v>210</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>359</v>
       </c>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
@@ -4642,22 +4637,22 @@
     </row>
     <row r="85" spans="1:12" ht="26">
       <c r="A85" s="27" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C85" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F85" s="11" t="s">
         <v>360</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>359</v>
       </c>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
@@ -4672,22 +4667,22 @@
     </row>
     <row r="86" spans="1:12" ht="38.5">
       <c r="A86" s="27" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
@@ -4702,22 +4697,22 @@
     </row>
     <row r="87" spans="1:12" ht="26">
       <c r="A87" s="27" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
@@ -4735,19 +4730,19 @@
         <v>10</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F88" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
@@ -4765,19 +4760,19 @@
         <v>47</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
@@ -4791,23 +4786,23 @@
       <c r="L89" s="13"/>
     </row>
     <row r="90" spans="1:12" ht="14.5">
-      <c r="A90" s="51" t="s">
+      <c r="A90" s="49" t="s">
         <v>48</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
@@ -4821,23 +4816,23 @@
       <c r="L90" s="13"/>
     </row>
     <row r="91" spans="1:12" ht="14.5">
-      <c r="A91" s="51" t="s">
+      <c r="A91" s="49" t="s">
         <v>49</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
@@ -4851,23 +4846,23 @@
       <c r="L91" s="13"/>
     </row>
     <row r="92" spans="1:12" ht="14.5">
-      <c r="A92" s="51" t="s">
-        <v>238</v>
+      <c r="A92" s="49" t="s">
+        <v>231</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
@@ -4881,23 +4876,23 @@
       <c r="L92" s="13"/>
     </row>
     <row r="93" spans="1:12" ht="14.5">
-      <c r="A93" s="51" t="s">
-        <v>239</v>
+      <c r="A93" s="49" t="s">
+        <v>232</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E93" s="45" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
@@ -4911,20 +4906,20 @@
       <c r="L93" s="13"/>
     </row>
     <row r="94" spans="1:12" ht="26">
-      <c r="A94" s="51" t="s">
-        <v>245</v>
+      <c r="A94" s="49" t="s">
+        <v>238</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E94" s="21" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F94" s="19" t="s">
         <v>64</v>
@@ -4941,31 +4936,31 @@
       <c r="L94" s="13"/>
     </row>
     <row r="95" spans="1:12" ht="14.5">
-      <c r="A95" s="51" t="s">
+      <c r="A95" s="49" t="s">
         <v>50</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E95" s="52" t="s">
-        <v>369</v>
+        <v>226</v>
+      </c>
+      <c r="E95" s="50" t="s">
+        <v>370</v>
       </c>
       <c r="F95" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G95" s="53" t="s">
-        <v>370</v>
+      <c r="G95" s="51" t="s">
+        <v>371</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
-      <c r="J95" s="54" t="s">
-        <v>245</v>
+      <c r="J95" s="52" t="s">
+        <v>238</v>
       </c>
       <c r="K95" s="13" t="s">
         <v>65</v>
@@ -4973,29 +4968,29 @@
       <c r="L95" s="13"/>
     </row>
     <row r="96" spans="1:12" ht="14.5">
-      <c r="A96" s="51" t="s">
+      <c r="A96" s="49" t="s">
         <v>51</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E96" s="45" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F96" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
-      <c r="J96" s="54" t="s">
-        <v>245</v>
+      <c r="J96" s="52" t="s">
+        <v>238</v>
       </c>
       <c r="K96" s="13" t="s">
         <v>65</v>
@@ -5003,23 +4998,23 @@
       <c r="L96" s="13"/>
     </row>
     <row r="97" spans="1:12" ht="14.5">
-      <c r="A97" s="51" t="s">
-        <v>247</v>
+      <c r="A97" s="49" t="s">
+        <v>240</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="E97" s="55" t="s">
         <v>373</v>
       </c>
+      <c r="E97" s="53" t="s">
+        <v>374</v>
+      </c>
       <c r="F97" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
@@ -5033,23 +5028,23 @@
       <c r="L97" s="13"/>
     </row>
     <row r="98" spans="1:12" ht="14.5">
-      <c r="A98" s="51" t="s">
+      <c r="A98" s="49" t="s">
         <v>52</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="E98" s="56" t="s">
         <v>375</v>
       </c>
+      <c r="E98" s="54" t="s">
+        <v>376</v>
+      </c>
       <c r="F98" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -5063,23 +5058,23 @@
       <c r="L98" s="13"/>
     </row>
     <row r="99" spans="1:12" ht="14.5">
-      <c r="A99" s="51" t="s">
+      <c r="A99" s="49" t="s">
         <v>53</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>376</v>
-      </c>
-      <c r="E99" s="55" t="s">
         <v>377</v>
       </c>
+      <c r="E99" s="53" t="s">
+        <v>378</v>
+      </c>
       <c r="F99" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
@@ -5093,23 +5088,23 @@
       <c r="L99" s="13"/>
     </row>
     <row r="100" spans="1:12" ht="14.5">
-      <c r="A100" s="51" t="s">
-        <v>378</v>
+      <c r="A100" s="49" t="s">
+        <v>379</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>380</v>
-      </c>
-      <c r="E100" s="55" t="s">
         <v>381</v>
       </c>
+      <c r="E100" s="53" t="s">
+        <v>382</v>
+      </c>
       <c r="F100" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
@@ -5123,23 +5118,23 @@
       <c r="L100" s="13"/>
     </row>
     <row r="101" spans="1:12" ht="14.5">
-      <c r="A101" s="51" t="s">
+      <c r="A101" s="49" t="s">
         <v>54</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="E101" s="55" t="s">
         <v>383</v>
       </c>
+      <c r="E101" s="53" t="s">
+        <v>384</v>
+      </c>
       <c r="F101" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
@@ -5153,23 +5148,23 @@
       <c r="L101" s="13"/>
     </row>
     <row r="102" spans="1:12" ht="14.5">
-      <c r="A102" s="51" t="s">
+      <c r="A102" s="49" t="s">
         <v>55</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="E102" s="55" t="s">
         <v>385</v>
       </c>
+      <c r="E102" s="53" t="s">
+        <v>386</v>
+      </c>
       <c r="F102" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
@@ -5183,23 +5178,23 @@
       <c r="L102" s="13"/>
     </row>
     <row r="103" spans="1:12" ht="14.5">
-      <c r="A103" s="51" t="s">
+      <c r="A103" s="49" t="s">
         <v>11</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="E103" s="56" t="s">
         <v>388</v>
       </c>
+      <c r="E103" s="54" t="s">
+        <v>389</v>
+      </c>
       <c r="F103" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
@@ -5213,23 +5208,23 @@
       <c r="L103" s="13"/>
     </row>
     <row r="104" spans="1:12" ht="14.5">
-      <c r="A104" s="51" t="s">
+      <c r="A104" s="49" t="s">
         <v>12</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="D104" s="49" t="s">
-        <v>389</v>
-      </c>
-      <c r="E104" s="56" t="s">
+        <v>387</v>
+      </c>
+      <c r="D104" s="47" t="s">
         <v>390</v>
       </c>
+      <c r="E104" s="54" t="s">
+        <v>391</v>
+      </c>
       <c r="F104" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
@@ -5243,23 +5238,23 @@
       <c r="L104" s="13"/>
     </row>
     <row r="105" spans="1:12" ht="14.5">
-      <c r="A105" s="51" t="s">
+      <c r="A105" s="49" t="s">
         <v>13</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="E105" s="56" t="s">
-        <v>391</v>
+        <v>385</v>
+      </c>
+      <c r="E105" s="54" t="s">
+        <v>392</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
@@ -5273,23 +5268,23 @@
       <c r="L105" s="13"/>
     </row>
     <row r="106" spans="1:12" ht="14.5">
-      <c r="A106" s="51" t="s">
+      <c r="A106" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="D106" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="E106" s="56" t="s">
+      <c r="D106" s="47" t="s">
         <v>394</v>
       </c>
+      <c r="E106" s="54" t="s">
+        <v>395</v>
+      </c>
       <c r="F106" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
@@ -5303,23 +5298,23 @@
       <c r="L106" s="13"/>
     </row>
     <row r="107" spans="1:12" ht="14.5">
-      <c r="A107" s="51" t="s">
+      <c r="A107" s="49" t="s">
         <v>15</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="D107" s="49" t="s">
-        <v>395</v>
-      </c>
-      <c r="E107" s="56" t="s">
+        <v>393</v>
+      </c>
+      <c r="D107" s="47" t="s">
         <v>396</v>
       </c>
+      <c r="E107" s="54" t="s">
+        <v>397</v>
+      </c>
       <c r="F107" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
@@ -5333,23 +5328,23 @@
       <c r="L107" s="13"/>
     </row>
     <row r="108" spans="1:12" ht="14.5">
-      <c r="A108" s="51" t="s">
-        <v>397</v>
+      <c r="A108" s="49" t="s">
+        <v>398</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="D108" s="49" t="s">
-        <v>398</v>
-      </c>
-      <c r="E108" s="56" t="s">
+        <v>393</v>
+      </c>
+      <c r="D108" s="47" t="s">
         <v>399</v>
       </c>
+      <c r="E108" s="54" t="s">
+        <v>400</v>
+      </c>
       <c r="F108" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
@@ -5363,23 +5358,23 @@
       <c r="L108" s="13"/>
     </row>
     <row r="109" spans="1:12" ht="14.5">
-      <c r="A109" s="51" t="s">
+      <c r="A109" s="49" t="s">
         <v>16</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="D109" s="49" t="s">
         <v>401</v>
       </c>
-      <c r="E109" s="56" t="s">
+      <c r="D109" s="47" t="s">
         <v>402</v>
       </c>
+      <c r="E109" s="54" t="s">
+        <v>403</v>
+      </c>
       <c r="F109" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
@@ -5393,23 +5388,23 @@
       <c r="L109" s="13"/>
     </row>
     <row r="110" spans="1:12" ht="14.5">
-      <c r="A110" s="51" t="s">
+      <c r="A110" s="49" t="s">
         <v>17</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="D110" s="49" t="s">
-        <v>403</v>
-      </c>
-      <c r="E110" s="56" t="s">
+        <v>401</v>
+      </c>
+      <c r="D110" s="47" t="s">
         <v>404</v>
       </c>
+      <c r="E110" s="54" t="s">
+        <v>405</v>
+      </c>
       <c r="F110" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
@@ -5423,49 +5418,49 @@
       <c r="L110" s="13"/>
     </row>
     <row r="111" spans="1:12" ht="14.5">
-      <c r="A111" s="51" t="s">
-        <v>405</v>
+      <c r="A111" s="49" t="s">
+        <v>406</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="D111" s="49" t="s">
-        <v>406</v>
-      </c>
-      <c r="E111" s="56" t="s">
+        <v>401</v>
+      </c>
+      <c r="D111" s="47" t="s">
         <v>407</v>
       </c>
-      <c r="F111" s="57" t="s">
-        <v>342</v>
+      <c r="E111" s="54" t="s">
+        <v>408</v>
+      </c>
+      <c r="F111" s="55" t="s">
+        <v>343</v>
       </c>
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
-      <c r="J111" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="K111" s="58" t="s">
+      <c r="J111" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="K111" s="56" t="s">
         <v>65</v>
       </c>
       <c r="L111" s="13"/>
     </row>
     <row r="112" spans="1:12" ht="14.5">
-      <c r="A112" s="51" t="s">
+      <c r="A112" s="49" t="s">
         <v>18</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C112" s="48" t="s">
-        <v>290</v>
+        <v>229</v>
+      </c>
+      <c r="C112" s="46" t="s">
+        <v>284</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="E112" s="13"/>
+        <v>230</v>
+      </c>
+      <c r="E112" s="54"/>
       <c r="F112" s="19" t="s">
         <v>63</v>
       </c>
@@ -5481,20 +5476,20 @@
       <c r="L112" s="13"/>
     </row>
     <row r="113" spans="1:12" ht="14.5">
-      <c r="A113" s="51" t="s">
+      <c r="A113" s="49" t="s">
         <v>19</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C113" s="48" t="s">
-        <v>290</v>
+        <v>229</v>
+      </c>
+      <c r="C113" s="46" t="s">
+        <v>284</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="E113" s="19" t="s">
         <v>409</v>
+      </c>
+      <c r="E113" s="54" t="s">
+        <v>410</v>
       </c>
       <c r="F113" s="19" t="s">
         <v>64</v>
@@ -5502,7 +5497,7 @@
       <c r="G113" s="12"/>
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
-      <c r="J113" s="54" t="s">
+      <c r="J113" s="52" t="s">
         <v>68</v>
       </c>
       <c r="K113" s="13" t="s">
@@ -5511,30 +5506,30 @@
       <c r="L113" s="13"/>
     </row>
     <row r="114" spans="1:12" ht="14.5">
-      <c r="A114" s="51" t="s">
-        <v>410</v>
+      <c r="A114" s="49" t="s">
+        <v>411</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C114" s="48" t="s">
-        <v>290</v>
+        <v>229</v>
+      </c>
+      <c r="C114" s="46" t="s">
+        <v>284</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="E114" s="19" t="s">
         <v>412</v>
       </c>
+      <c r="E114" s="54" t="s">
+        <v>413</v>
+      </c>
       <c r="F114" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G114" s="12"/>
       <c r="H114" s="12" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="I114" s="13"/>
-      <c r="J114" s="54" t="s">
+      <c r="J114" s="52" t="s">
         <v>19</v>
       </c>
       <c r="K114" s="13" t="s">
@@ -5543,20 +5538,20 @@
       <c r="L114" s="13"/>
     </row>
     <row r="115" spans="1:12" ht="14.5">
-      <c r="A115" s="51" t="s">
+      <c r="A115" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C115" s="48" t="s">
-        <v>414</v>
+        <v>229</v>
+      </c>
+      <c r="C115" s="46" t="s">
+        <v>415</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="E115" s="21" t="s">
-        <v>415</v>
+        <v>233</v>
+      </c>
+      <c r="E115" s="54" t="s">
+        <v>416</v>
       </c>
       <c r="F115" s="19" t="s">
         <v>64</v>
@@ -5564,7 +5559,7 @@
       <c r="G115" s="12"/>
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
-      <c r="J115" s="54" t="s">
+      <c r="J115" s="52" t="s">
         <v>68</v>
       </c>
       <c r="K115" s="13" t="s">
@@ -5573,28 +5568,28 @@
       <c r="L115" s="13"/>
     </row>
     <row r="116" spans="1:12" ht="14.5">
-      <c r="A116" s="51" t="s">
+      <c r="A116" s="49" t="s">
         <v>21</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C116" s="48" t="s">
-        <v>414</v>
+        <v>229</v>
+      </c>
+      <c r="C116" s="46" t="s">
+        <v>415</v>
       </c>
       <c r="D116" s="45" t="s">
-        <v>241</v>
-      </c>
-      <c r="E116" s="45" t="s">
-        <v>242</v>
+        <v>234</v>
+      </c>
+      <c r="E116" s="54" t="s">
+        <v>235</v>
       </c>
       <c r="F116" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G116" s="12"/>
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
-      <c r="J116" s="54" t="s">
+      <c r="J116" s="52" t="s">
         <v>20</v>
       </c>
       <c r="K116" s="13" t="s">
@@ -5603,28 +5598,28 @@
       <c r="L116" s="13"/>
     </row>
     <row r="117" spans="1:12" ht="38.5">
-      <c r="A117" s="51" t="s">
+      <c r="A117" s="49" t="s">
         <v>22</v>
       </c>
       <c r="B117" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C117" s="46" t="s">
+        <v>415</v>
+      </c>
+      <c r="D117" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C117" s="48" t="s">
-        <v>414</v>
-      </c>
-      <c r="D117" s="9" t="s">
-        <v>243</v>
-      </c>
       <c r="E117" s="21" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="F117" s="19" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
-      <c r="J117" s="54" t="s">
+      <c r="J117" s="52" t="s">
         <v>20</v>
       </c>
       <c r="K117" s="13" t="s">
@@ -5633,26 +5628,26 @@
       <c r="L117" s="13"/>
     </row>
     <row r="118" spans="1:12" ht="14.5">
-      <c r="A118" s="51" t="s">
+      <c r="A118" s="49" t="s">
         <v>23</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C118" s="48" t="s">
-        <v>416</v>
+        <v>229</v>
+      </c>
+      <c r="C118" s="46" t="s">
+        <v>417</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E118" s="59" t="s">
-        <v>417</v>
+        <v>239</v>
+      </c>
+      <c r="E118" s="57" t="s">
+        <v>418</v>
       </c>
       <c r="F118" s="11" t="s">
         <v>78</v>
       </c>
       <c r="G118" s="11" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
@@ -5665,50 +5660,50 @@
       <c r="L118" s="13"/>
     </row>
     <row r="119" spans="1:12" ht="14.5">
-      <c r="A119" s="51" t="s">
+      <c r="A119" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B119" s="60" t="s">
-        <v>236</v>
-      </c>
-      <c r="C119" s="48" t="s">
-        <v>416</v>
-      </c>
-      <c r="D119" s="49" t="s">
-        <v>419</v>
-      </c>
-      <c r="E119" s="59" t="s">
+      <c r="B119" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C119" s="46" t="s">
+        <v>417</v>
+      </c>
+      <c r="D119" s="47" t="s">
         <v>420</v>
       </c>
-      <c r="F119" s="57" t="s">
-        <v>63</v>
+      <c r="E119" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="F119" s="55" t="s">
+        <v>250</v>
       </c>
       <c r="G119" s="11"/>
       <c r="H119" s="12"/>
-      <c r="I119" s="61"/>
-      <c r="J119" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="K119" s="58" t="s">
+      <c r="I119" s="59"/>
+      <c r="J119" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="K119" s="56" t="s">
         <v>65</v>
       </c>
       <c r="L119" s="13"/>
     </row>
     <row r="120" spans="1:12" ht="26">
-      <c r="A120" s="51" t="s">
+      <c r="A120" s="49" t="s">
         <v>25</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C120" s="48" t="s">
-        <v>421</v>
+        <v>229</v>
+      </c>
+      <c r="C120" s="46" t="s">
+        <v>422</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E120" s="21" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F120" s="19" t="s">
         <v>64</v>
@@ -5716,7 +5711,7 @@
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
       <c r="I120" s="26"/>
-      <c r="J120" s="63" t="s">
+      <c r="J120" s="61" t="s">
         <v>68</v>
       </c>
       <c r="K120" s="13" t="s">
@@ -5729,29 +5724,30 @@
         <v>26</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C121" s="48" t="s">
-        <v>421</v>
+        <v>229</v>
+      </c>
+      <c r="C121" s="46" t="s">
+        <v>422</v>
       </c>
       <c r="D121" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E121" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F121" s="19" t="s">
         <v>250</v>
-      </c>
-      <c r="E121" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="F121" s="19" t="s">
-        <v>257</v>
       </c>
       <c r="G121" s="12"/>
       <c r="J121" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="K121" s="65" t="s">
+      <c r="K121" s="62" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L121" xr:uid="{A2497CF0-0CBF-4E39-94FC-8209193EBA68}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5984,13 +5980,13 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BC9FA66-D047-4A51-8063-2C795F417984}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ee3db34d-9953-4a90-95a5-b9c1d5f232f6"/>
     <ds:schemaRef ds:uri="7a52d84a-254c-4bf4-af91-7c6121d880be"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>

</xml_diff>